<commit_message>
Bom updated: Missing components added, page references added.
</commit_message>
<xml_diff>
--- a/PumaBom-WithMods-Element14.xlsx
+++ b/PumaBom-WithMods-Element14.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="10515" windowHeight="4680" tabRatio="710"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="10515" windowHeight="4680" tabRatio="710" firstSheet="1" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Primary Puma Parts" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="384">
   <si>
     <t>MCU</t>
   </si>
@@ -130,9 +130,6 @@
     <t>D92</t>
   </si>
   <si>
-    <t>IN4148</t>
-  </si>
-  <si>
     <t>U20</t>
   </si>
   <si>
@@ -283,9 +280,6 @@
     <t>Schottky</t>
   </si>
   <si>
-    <t>1N4148</t>
-  </si>
-  <si>
     <t>R49</t>
   </si>
   <si>
@@ -415,9 +409,6 @@
     <t>1nF</t>
   </si>
   <si>
-    <t>Fuel Pump</t>
-  </si>
-  <si>
     <t>LED</t>
   </si>
   <si>
@@ -433,9 +424,6 @@
     <t>100K</t>
   </si>
   <si>
-    <t>Cylinder Head Temperature</t>
-  </si>
-  <si>
     <t>C75</t>
   </si>
   <si>
@@ -580,9 +568,6 @@
     <t>D10</t>
   </si>
   <si>
-    <t>5.1v Zener</t>
-  </si>
-  <si>
     <t>Mini usb connector</t>
   </si>
   <si>
@@ -643,9 +628,6 @@
     <t xml:space="preserve"> Pressure Sensor with Barb</t>
   </si>
   <si>
-    <t>Presure sensor NO barb</t>
-  </si>
-  <si>
     <t>R25</t>
   </si>
   <si>
@@ -754,9 +736,6 @@
     <t>CRYSTAL, TSX-3225, 16MHZ, 10PPM, 9PF</t>
   </si>
   <si>
-    <t>DIODE, ZENER, 5.1V, SOD-123, 0.5W</t>
-  </si>
-  <si>
     <t>(Avaliblity - 2k used instead of 2.4k)</t>
   </si>
   <si>
@@ -784,9 +763,6 @@
     <t>LED, SMD, 0805, ORANGE</t>
   </si>
   <si>
-    <t>DIODE, SWITCH, 100V, 0.4W, SOD123</t>
-  </si>
-  <si>
     <t>Free EMS Brain</t>
   </si>
   <si>
@@ -1000,9 +976,6 @@
     <t>C122</t>
   </si>
   <si>
-    <t>Change to zener diode</t>
-  </si>
-  <si>
     <t>D76</t>
   </si>
   <si>
@@ -1048,9 +1021,6 @@
     <t>C124</t>
   </si>
   <si>
-    <t>1.6K</t>
-  </si>
-  <si>
     <t>XOR logic</t>
   </si>
   <si>
@@ -1067,6 +1037,147 @@
   </si>
   <si>
     <t>Not used</t>
+  </si>
+  <si>
+    <t>Barbed, No Tabs</t>
+  </si>
+  <si>
+    <t>Presure sensor No barb, No Tabs</t>
+  </si>
+  <si>
+    <t>Coolant Head Temperature</t>
+  </si>
+  <si>
+    <t>Q8</t>
+  </si>
+  <si>
+    <t>Fuel Pump   ---- note this is on sheet 51 of schematics "general_drive1.sch"</t>
+  </si>
+  <si>
+    <t>R160</t>
+  </si>
+  <si>
+    <t>R164</t>
+  </si>
+  <si>
+    <t>C86</t>
+  </si>
+  <si>
+    <t>D61</t>
+  </si>
+  <si>
+    <t>D60</t>
+  </si>
+  <si>
+    <t>R159</t>
+  </si>
+  <si>
+    <t>R163</t>
+  </si>
+  <si>
+    <t>C85</t>
+  </si>
+  <si>
+    <t>D58</t>
+  </si>
+  <si>
+    <t>D59</t>
+  </si>
+  <si>
+    <t>R170</t>
+  </si>
+  <si>
+    <t>R174</t>
+  </si>
+  <si>
+    <t>C92</t>
+  </si>
+  <si>
+    <t>D72</t>
+  </si>
+  <si>
+    <t>D73</t>
+  </si>
+  <si>
+    <t>jumper</t>
+  </si>
+  <si>
+    <t>Schematic pages: 1, 48, 55</t>
+  </si>
+  <si>
+    <t>Schematic pages: 1, 48, 56</t>
+  </si>
+  <si>
+    <t>Schematic pages: 1, ??, 44</t>
+  </si>
+  <si>
+    <t>Schematic pages: 53</t>
+  </si>
+  <si>
+    <t>Schematic pages: 1, ??, 43</t>
+  </si>
+  <si>
+    <t>Schematic pages: 1, 14</t>
+  </si>
+  <si>
+    <t>Schematic pages: 15</t>
+  </si>
+  <si>
+    <t>Schematic pages: 33</t>
+  </si>
+  <si>
+    <t>Schematic pages: 34</t>
+  </si>
+  <si>
+    <t>Schematic pages: 18, 45</t>
+  </si>
+  <si>
+    <t>Schematic pages: 17, 46</t>
+  </si>
+  <si>
+    <t>Schematic pages: 1, 24, 26</t>
+  </si>
+  <si>
+    <t>Schematic pages: 1, 48</t>
+  </si>
+  <si>
+    <t>Schematic pages: 1, 27</t>
+  </si>
+  <si>
+    <t>Schematic pages: 1, 28</t>
+  </si>
+  <si>
+    <t>Schematic pages: 1, 29</t>
+  </si>
+  <si>
+    <t>Schematic pages: 1, 30</t>
+  </si>
+  <si>
+    <t>Schematic pages: 1, 31</t>
+  </si>
+  <si>
+    <t>Schematic pages: 1, 32</t>
+  </si>
+  <si>
+    <t>Schematic pages: 1, 20</t>
+  </si>
+  <si>
+    <t>Schematic pages: 1, 19</t>
+  </si>
+  <si>
+    <t>Schematic pages: 1</t>
+  </si>
+  <si>
+    <t>Schematic pages: 1, 35, 42</t>
+  </si>
+  <si>
+    <t>Schematic pages: 1, 36, 41</t>
+  </si>
+  <si>
+    <t>Schematic pages: 1, 37, 40</t>
+  </si>
+  <si>
+    <t>Schematic pages: 1, 38, 39</t>
   </si>
 </sst>
 </file>
@@ -1518,7 +1629,9 @@
   </sheetPr>
   <dimension ref="A1:L74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J53" sqref="J53"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1535,14 +1648,14 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="C2" s="19"/>
       <c r="D2" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="H2" s="23" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="I2" s="23"/>
       <c r="J2" s="23"/>
@@ -1551,10 +1664,10 @@
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C3" s="20"/>
       <c r="D3" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="H3" s="22" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="I3" s="23"/>
       <c r="J3" s="23"/>
@@ -1563,7 +1676,7 @@
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C4" s="21"/>
       <c r="D4" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25"/>
@@ -1576,11 +1689,13 @@
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
+      <c r="I6" s="4" t="s">
+        <v>363</v>
+      </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
@@ -1590,13 +1705,13 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="F7" s="5">
         <v>1380343</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1610,7 +1725,7 @@
         <v>1809302</v>
       </c>
       <c r="G8" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1624,7 +1739,7 @@
         <v>1809302</v>
       </c>
       <c r="G9" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1638,7 +1753,7 @@
         <v>1809302</v>
       </c>
       <c r="G10" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1652,7 +1767,7 @@
         <v>1809302</v>
       </c>
       <c r="G11" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1663,14 +1778,14 @@
         <v>3</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="D12" s="16"/>
       <c r="F12" s="5">
         <v>1809302</v>
       </c>
       <c r="G12" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1684,7 +1799,7 @@
         <v>8820120</v>
       </c>
       <c r="G13" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1698,7 +1813,7 @@
         <v>1650875</v>
       </c>
       <c r="G14" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1712,7 +1827,7 @@
         <v>1702127</v>
       </c>
       <c r="G15" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1726,7 +1841,7 @@
         <v>1887296</v>
       </c>
       <c r="G16" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1740,7 +1855,7 @@
         <v>1414676</v>
       </c>
       <c r="G17" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -1751,13 +1866,13 @@
         <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="F18" s="5">
         <v>1174062</v>
       </c>
       <c r="G18" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -1771,7 +1886,7 @@
         <v>1712841</v>
       </c>
       <c r="G19" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -1785,7 +1900,7 @@
         <v>8820120</v>
       </c>
       <c r="G20" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -1799,7 +1914,7 @@
         <v>8820120</v>
       </c>
       <c r="G21" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -1807,16 +1922,16 @@
         <v>23</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="F22" s="5">
         <v>1809300</v>
       </c>
       <c r="G22" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -1830,7 +1945,7 @@
         <v>8820120</v>
       </c>
       <c r="G23" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -1844,7 +1959,7 @@
         <v>8820120</v>
       </c>
       <c r="G24" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -1858,7 +1973,7 @@
         <v>8820120</v>
       </c>
       <c r="G25" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25"/>
@@ -1874,28 +1989,30 @@
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
-      <c r="I28" s="4"/>
+      <c r="I28" s="4" t="s">
+        <v>364</v>
+      </c>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" t="s">
         <v>35</v>
-      </c>
-      <c r="B29" t="s">
-        <v>36</v>
       </c>
       <c r="F29" s="5">
         <v>1146032</v>
       </c>
       <c r="G29" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B30" t="s">
         <v>22</v>
@@ -1904,21 +2021,21 @@
         <v>8820120</v>
       </c>
       <c r="G30" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="17"/>
       <c r="B31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C31" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B32" t="s">
         <v>8</v>
@@ -1927,112 +2044,112 @@
         <v>8820120</v>
       </c>
       <c r="G32" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" t="s">
         <v>40</v>
-      </c>
-      <c r="B33" t="s">
-        <v>41</v>
       </c>
       <c r="F33" s="5">
         <v>9334084</v>
       </c>
       <c r="G33" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F34" s="5">
         <v>9406352</v>
       </c>
       <c r="G34" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B35" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="F35" s="5">
         <v>1355761</v>
       </c>
       <c r="G35" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B36" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F36" s="5">
         <v>1226390</v>
       </c>
       <c r="G36" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B37" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F37" s="5">
         <v>1465996</v>
       </c>
       <c r="G37" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B38" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F38" s="5">
         <v>1809376</v>
       </c>
       <c r="G38" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B39" t="s">
         <v>50</v>
-      </c>
-      <c r="B39" t="s">
-        <v>51</v>
       </c>
       <c r="F39" s="5">
         <v>1809376</v>
       </c>
       <c r="G39" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -2041,7 +2158,9 @@
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
-      <c r="I42" s="4"/>
+      <c r="I42" s="4" t="s">
+        <v>365</v>
+      </c>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
       <c r="L42" s="4"/>
@@ -2057,7 +2176,7 @@
         <v>1556741</v>
       </c>
       <c r="G43" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
@@ -2071,7 +2190,7 @@
         <v>9229272</v>
       </c>
       <c r="G44" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
@@ -2085,7 +2204,7 @@
         <v>8820120</v>
       </c>
       <c r="G45" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
@@ -2093,59 +2212,59 @@
         <v>33</v>
       </c>
       <c r="B46" t="s">
-        <v>34</v>
+        <v>83</v>
       </c>
       <c r="F46" s="5">
-        <v>1776392</v>
+        <v>9556915</v>
       </c>
       <c r="G46" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B47" t="s">
         <v>53</v>
-      </c>
-      <c r="B47" t="s">
-        <v>54</v>
       </c>
       <c r="F47" s="5">
         <v>1617365</v>
       </c>
       <c r="G47" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B48" t="s">
         <v>55</v>
-      </c>
-      <c r="B48" t="s">
-        <v>56</v>
       </c>
       <c r="F48" s="5">
         <v>8820120</v>
       </c>
       <c r="G48" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="C49" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="C49" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25"/>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -2154,94 +2273,97 @@
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I52" s="4" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C53" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C53" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="10" t="s">
+      <c r="B54" s="1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="9" t="s">
+      <c r="B55" t="s">
         <v>62</v>
-      </c>
-      <c r="B55" t="s">
-        <v>63</v>
       </c>
       <c r="F55" s="5">
         <v>9486038</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="H55" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="10" t="s">
+      <c r="B57" s="1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="10" t="s">
+      <c r="B58" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F58" s="5"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="F58" s="5"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="10" t="s">
+      <c r="B59" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F59" s="5"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="F59" s="5"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="9" t="s">
-        <v>68</v>
-      </c>
       <c r="B60" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F60" s="5">
         <v>1617365</v>
       </c>
       <c r="G60" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B61" t="s">
         <v>22</v>
@@ -2250,57 +2372,57 @@
         <v>8820120</v>
       </c>
       <c r="G61" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B62" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F62" s="5">
         <v>1324152</v>
       </c>
       <c r="G62" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B63" t="s">
         <v>31</v>
       </c>
       <c r="D63" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="F63" s="5">
         <v>9229272</v>
       </c>
       <c r="G63" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B64" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F64" s="5">
         <v>8812519</v>
       </c>
       <c r="G64" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B65" t="s">
         <v>22</v>
@@ -2309,7 +2431,7 @@
         <v>8820120</v>
       </c>
       <c r="G65" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25"/>
@@ -2360,18 +2482,18 @@
     <hyperlink ref="F14" r:id="rId29" display="http://nz.element14.com/kemet/c0805c331j5gac-tu/capacitor-ceramic-multilayer/dp/1650875"/>
     <hyperlink ref="F15" r:id="rId30" display="http://nz.element14.com/kemet/c0805c332kcractu/capacitor-0805-3-3nf-500v-x7r/dp/1702127"/>
     <hyperlink ref="F17" r:id="rId31" display="http://nz.element14.com/kemet/c0805c220j1gactu/capacitor-0805-22pf-100v-np0/dp/1414676"/>
-    <hyperlink ref="F46" r:id="rId32" display="http://nz.element14.com/diodes-inc/1n4148w-7-f/diode-switch-100v-0-4w-sod123/dp/1776392"/>
-    <hyperlink ref="F47" r:id="rId33" display="http://nz.element14.com/vishay-sprague/199d106x9035d1v1e3/capacitor-tant-10uf-35v-radial/dp/1617365"/>
-    <hyperlink ref="F60" r:id="rId34" display="http://nz.element14.com/vishay-sprague/199d106x9035d1v1e3/capacitor-tant-10uf-35v-radial/dp/1617365"/>
-    <hyperlink ref="F63" r:id="rId35" display="http://nz.element14.com/kemet/t495d226k035ate300/capacitor-22uf-35v/dp/9229272"/>
-    <hyperlink ref="F44" r:id="rId36" display="http://nz.element14.com/kemet/t495d226k035ate300/capacitor-22uf-35v/dp/9229272"/>
-    <hyperlink ref="F62" r:id="rId37" display="http://nz.element14.com/fairchild-semiconductor/1n4007/bridge-rectifier-rohs-compliant/dp/9109625"/>
-    <hyperlink ref="F64" r:id="rId38" display="http://nz.element14.com/nichicon/upm1e222mhd/capacitor-2200uf-25v/dp/8812519"/>
-    <hyperlink ref="F18" r:id="rId39" display="http://nz.element14.com/te-connectivity-cgs/rh73u2a10mjtd/resistor-0805-10m/dp/1174062"/>
-    <hyperlink ref="F12" r:id="rId40" display="http://nz.element14.com/koa/rk73b2attd103j/resistor-0805-10k-ohm-5/dp/1809302"/>
-    <hyperlink ref="F22" r:id="rId41" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
-    <hyperlink ref="F34" r:id="rId42" display="http://nz.element14.com/multicomp/u0805r103kct/capacitor-0805-10nf-50v/dp/9406352"/>
-    <hyperlink ref="H3" r:id="rId43"/>
+    <hyperlink ref="F47" r:id="rId32" display="http://nz.element14.com/vishay-sprague/199d106x9035d1v1e3/capacitor-tant-10uf-35v-radial/dp/1617365"/>
+    <hyperlink ref="F60" r:id="rId33" display="http://nz.element14.com/vishay-sprague/199d106x9035d1v1e3/capacitor-tant-10uf-35v-radial/dp/1617365"/>
+    <hyperlink ref="F63" r:id="rId34" display="http://nz.element14.com/kemet/t495d226k035ate300/capacitor-22uf-35v/dp/9229272"/>
+    <hyperlink ref="F44" r:id="rId35" display="http://nz.element14.com/kemet/t495d226k035ate300/capacitor-22uf-35v/dp/9229272"/>
+    <hyperlink ref="F62" r:id="rId36" display="http://nz.element14.com/fairchild-semiconductor/1n4007/bridge-rectifier-rohs-compliant/dp/9109625"/>
+    <hyperlink ref="F64" r:id="rId37" display="http://nz.element14.com/nichicon/upm1e222mhd/capacitor-2200uf-25v/dp/8812519"/>
+    <hyperlink ref="F18" r:id="rId38" display="http://nz.element14.com/te-connectivity-cgs/rh73u2a10mjtd/resistor-0805-10m/dp/1174062"/>
+    <hyperlink ref="F12" r:id="rId39" display="http://nz.element14.com/koa/rk73b2attd103j/resistor-0805-10k-ohm-5/dp/1809302"/>
+    <hyperlink ref="F22" r:id="rId40" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
+    <hyperlink ref="F34" r:id="rId41" display="http://nz.element14.com/multicomp/u0805r103kct/capacitor-0805-10nf-50v/dp/9406352"/>
+    <hyperlink ref="H3" r:id="rId42"/>
+    <hyperlink ref="F46" r:id="rId43" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId44"/>
@@ -2386,7 +2508,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A10:XFD16"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -2398,7 +2520,7 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -2407,28 +2529,30 @@
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
+      <c r="I2" s="4" t="s">
+        <v>370</v>
+      </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F3" s="5">
         <v>1809376</v>
       </c>
       <c r="G3" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B4" t="s">
         <v>22</v>
@@ -2437,35 +2561,35 @@
         <v>8820120</v>
       </c>
       <c r="G4" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F5" s="5">
         <v>9556915</v>
       </c>
       <c r="G5" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>159</v>
+      <c r="A6" s="14" t="s">
+        <v>155</v>
       </c>
       <c r="B6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F6" s="5">
-        <v>1776392</v>
+        <v>9556915</v>
       </c>
       <c r="G6" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25"/>
@@ -2482,8 +2606,8 @@
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1" display="http://nz.element14.com/koa/rk73b2attd471j/resistor-0805-470-ohm-5/dp/1809376"/>
     <hyperlink ref="F4" r:id="rId2" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
-    <hyperlink ref="F6" r:id="rId3" display="http://nz.element14.com/diodes-inc/1n4148w-7-f/diode-switch-100v-0-4w-sod123/dp/1776392"/>
-    <hyperlink ref="F5" r:id="rId4" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
+    <hyperlink ref="F5" r:id="rId3" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
+    <hyperlink ref="F6" r:id="rId4" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2496,8 +2620,8 @@
   </sheetPr>
   <dimension ref="A1:L69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="I50" sqref="I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -2510,7 +2634,7 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -2519,100 +2643,102 @@
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
+      <c r="I2" s="4" t="s">
+        <v>371</v>
+      </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F3" s="5">
         <v>1809300</v>
       </c>
       <c r="G3" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F4" s="5">
         <v>1809376</v>
       </c>
       <c r="G4" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F5" s="5">
         <v>1465996</v>
       </c>
       <c r="G5" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B6" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B7" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="F7" s="5">
         <v>1775617</v>
       </c>
       <c r="G7" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="H7" s="5"/>
       <c r="K7" s="5">
         <v>1017798</v>
       </c>
       <c r="L7" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B8" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -2621,99 +2747,101 @@
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
+      <c r="I10" s="4" t="s">
+        <v>372</v>
+      </c>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="B11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F11" s="5">
         <v>1809300</v>
       </c>
       <c r="G11" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="B12" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F12" s="5">
         <v>1809376</v>
       </c>
       <c r="G12" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="B13" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F13" s="5">
         <v>1465996</v>
       </c>
       <c r="G13" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="B14" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="B15" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="F15" s="5">
         <v>1775617</v>
       </c>
       <c r="G15" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="K15" s="5">
         <v>1017798</v>
       </c>
       <c r="L15" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="B16" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -2722,99 +2850,101 @@
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
+      <c r="I18" s="4" t="s">
+        <v>373</v>
+      </c>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="B19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F19" s="5">
         <v>1809300</v>
       </c>
       <c r="G19" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="B20" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F20" s="5">
         <v>1809376</v>
       </c>
       <c r="G20" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="B21" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F21" s="5">
         <v>1465996</v>
       </c>
       <c r="G21" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="B22" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="K22" s="9" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="B23" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="F23" s="5">
         <v>1775617</v>
       </c>
       <c r="G23" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="K23" s="5">
         <v>1017798</v>
       </c>
       <c r="L23" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="B24" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -2823,99 +2953,101 @@
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
+      <c r="I26" s="4" t="s">
+        <v>374</v>
+      </c>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="B27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F27" s="5">
         <v>1809300</v>
       </c>
       <c r="G27" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="B28" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F28" s="5">
         <v>1809376</v>
       </c>
       <c r="G28" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="B29" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F29" s="5">
         <v>1465996</v>
       </c>
       <c r="G29" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="B30" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="K30" s="9" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="B31" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="F31" s="5">
         <v>1775617</v>
       </c>
       <c r="G31" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="K31" s="5">
         <v>1017798</v>
       </c>
       <c r="L31" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="B32" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -2924,99 +3056,101 @@
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
+      <c r="I34" s="4" t="s">
+        <v>375</v>
+      </c>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="B35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F35" s="5">
         <v>1809300</v>
       </c>
       <c r="G35" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="B36" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F36" s="5">
         <v>1809376</v>
       </c>
       <c r="G36" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="B37" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F37" s="5">
         <v>1465996</v>
       </c>
       <c r="G37" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="B38" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="K38" s="9" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="B39" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="F39" s="5">
         <v>1775617</v>
       </c>
       <c r="G39" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="K39" s="5">
         <v>1017798</v>
       </c>
       <c r="L39" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="18" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="B40" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -3025,99 +3159,101 @@
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
       <c r="H42" s="4"/>
-      <c r="I42" s="4"/>
+      <c r="I42" s="4" t="s">
+        <v>376</v>
+      </c>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
       <c r="L42" s="4"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="B43" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F43" s="5">
         <v>1809300</v>
       </c>
       <c r="G43" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="B44" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F44" s="5">
         <v>1809376</v>
       </c>
       <c r="G44" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="B45" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F45" s="5">
         <v>1465996</v>
       </c>
       <c r="G45" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="B46" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="K46" s="9" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="B47" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="F47" s="5">
         <v>1775617</v>
       </c>
       <c r="G47" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="K47" s="5">
         <v>1017798</v>
       </c>
       <c r="L47" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="18" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="B48" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -3126,93 +3262,95 @@
       <c r="F50" s="4"/>
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
-      <c r="I50" s="4"/>
+      <c r="I50" s="4" t="s">
+        <v>377</v>
+      </c>
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
       <c r="L50" s="4"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="B51" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F51" s="5">
         <v>1809300</v>
       </c>
       <c r="G51" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="B52" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F52" s="5">
         <v>1809376</v>
       </c>
       <c r="G52" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="B53" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F53" s="5">
         <v>1465996</v>
       </c>
       <c r="G53" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="B54" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F54" s="9" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="K54" s="9" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="B55" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="F55" s="5">
         <v>1775617</v>
       </c>
       <c r="G55" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="K55" s="5">
         <v>1017798</v>
       </c>
       <c r="L55" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="18" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="B56" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
@@ -3225,7 +3363,7 @@
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -3234,93 +3372,95 @@
       <c r="F58" s="4"/>
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
-      <c r="I58" s="4"/>
+      <c r="I58" s="4" t="s">
+        <v>378</v>
+      </c>
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
       <c r="L58" s="4"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="B59" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F59" s="5">
         <v>1809300</v>
       </c>
       <c r="G59" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="B60" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F60" s="5">
         <v>1809376</v>
       </c>
       <c r="G60" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="B61" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F61" s="5">
         <v>1465996</v>
       </c>
       <c r="G61" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="B62" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F62" s="9" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="K62" s="9" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="B63" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="F63" s="5">
         <v>1775617</v>
       </c>
       <c r="G63" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="K63" s="5">
         <v>1017798</v>
       </c>
       <c r="L63" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="18" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="B64" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
     </row>
     <row r="65" x14ac:dyDescent="0.25"/>
@@ -3382,8 +3522,8 @@
   </sheetPr>
   <dimension ref="A1:L68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G59" sqref="G59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -3396,7 +3536,7 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -3405,70 +3545,72 @@
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
+      <c r="I2" s="4" t="s">
+        <v>379</v>
+      </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="B3" t="s">
-        <v>340</v>
+        <v>77</v>
       </c>
       <c r="F3" s="5">
-        <v>1809321</v>
+        <v>1809300</v>
       </c>
       <c r="G3" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="B4" t="s">
-        <v>340</v>
+        <v>77</v>
       </c>
       <c r="F4" s="5">
-        <v>1809321</v>
+        <v>1809300</v>
       </c>
       <c r="G4" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="B5" t="s">
-        <v>340</v>
+        <v>77</v>
       </c>
       <c r="F5" s="5">
-        <v>1809321</v>
+        <v>1809300</v>
       </c>
       <c r="G5" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="B6" t="s">
-        <v>340</v>
+        <v>77</v>
       </c>
       <c r="F6" s="5">
-        <v>1809321</v>
+        <v>1809300</v>
       </c>
       <c r="G6" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
@@ -3477,12 +3619,12 @@
         <v>1809302</v>
       </c>
       <c r="G7" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
@@ -3491,12 +3633,12 @@
         <v>1809302</v>
       </c>
       <c r="G8" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="B9" t="s">
         <v>22</v>
@@ -3505,27 +3647,27 @@
         <v>8820120</v>
       </c>
       <c r="G9" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
       <c r="B10" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
       <c r="F10" s="5">
         <v>1740035</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -3534,140 +3676,142 @@
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
+      <c r="I12" s="4" t="s">
+        <v>380</v>
+      </c>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="F13" s="5">
         <v>9334084</v>
       </c>
       <c r="G13" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B14" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F14" s="5">
         <v>1686068</v>
       </c>
       <c r="G14" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B15" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="F15" s="5">
         <v>1017798</v>
       </c>
       <c r="G15" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B16" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F17" s="5">
         <v>1809596</v>
       </c>
       <c r="G17" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F18" s="5">
         <v>1809303</v>
       </c>
       <c r="G18" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F19" s="5">
         <v>1809300</v>
       </c>
       <c r="G19" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B20" t="s">
-        <v>184</v>
+        <v>83</v>
       </c>
       <c r="F20" s="5">
-        <v>1431273</v>
+        <v>9556915</v>
       </c>
       <c r="G20" t="s">
-        <v>242</v>
+        <v>253</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B21" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B22" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -3676,142 +3820,144 @@
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
+      <c r="I24" s="4" t="s">
+        <v>381</v>
+      </c>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C25" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="F25" s="5">
         <v>9334084</v>
       </c>
       <c r="G25" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="B26" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F26" s="5">
         <v>1686068</v>
       </c>
       <c r="G26" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="B27" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="F27" s="5">
         <v>1017798</v>
       </c>
       <c r="G27" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="B28" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="B29" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F29" s="5">
         <v>1809596</v>
       </c>
       <c r="G29" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="B30" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F30" s="5">
         <v>1809303</v>
       </c>
       <c r="G30" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F31" s="5">
         <v>1809300</v>
       </c>
       <c r="G31" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="B32" t="s">
-        <v>184</v>
+        <v>83</v>
       </c>
       <c r="F32" s="5">
-        <v>1431273</v>
+        <v>9556915</v>
       </c>
       <c r="G32" t="s">
-        <v>242</v>
+        <v>253</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="B33" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
       <c r="F33" s="5"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="B34" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
       <c r="F34" s="5"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -3820,157 +3966,159 @@
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
+      <c r="I36" s="4" t="s">
+        <v>382</v>
+      </c>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
       <c r="L36" s="4"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="B37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C37" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="F37" s="5">
         <v>9334084</v>
       </c>
       <c r="G37" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="B38" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F38" s="5">
         <v>1686068</v>
       </c>
       <c r="G38" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="9"/>
       <c r="F39" s="9" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="K39" s="9" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B40" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="F40" s="5">
         <v>1775617</v>
       </c>
       <c r="G40" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="K40" s="5">
         <v>1017798</v>
       </c>
       <c r="L40" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B41" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="B42" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F42" s="5">
         <v>1809596</v>
       </c>
       <c r="G42" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B43" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F43" s="5">
         <v>1809303</v>
       </c>
       <c r="G43" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F44" s="5">
         <v>1809300</v>
       </c>
       <c r="G44" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="B45" t="s">
-        <v>184</v>
+        <v>83</v>
       </c>
       <c r="F45" s="5">
-        <v>1431273</v>
+        <v>9556915</v>
       </c>
       <c r="G45" t="s">
-        <v>242</v>
+        <v>253</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="B46" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
       <c r="F46" s="5"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="B47" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
       <c r="F47" s="5"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
@@ -3979,150 +4127,152 @@
       <c r="F49" s="4"/>
       <c r="G49" s="4"/>
       <c r="H49" s="4"/>
-      <c r="I49" s="4"/>
+      <c r="I49" s="4" t="s">
+        <v>383</v>
+      </c>
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
       <c r="L49" s="4"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="B50" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C50" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="F50" s="5">
         <v>9334084</v>
       </c>
       <c r="G50" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B51" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F51" s="5">
         <v>1686068</v>
       </c>
       <c r="G51" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="9"/>
       <c r="F52" s="9" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="K52" s="9" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="B53" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="F53" s="5">
         <v>1775617</v>
       </c>
       <c r="G53" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="K53" s="5">
         <v>1017798</v>
       </c>
       <c r="L53" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="B54" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="B55" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F55" s="5">
         <v>1809596</v>
       </c>
       <c r="G55" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F56" s="5">
         <v>1809303</v>
       </c>
       <c r="G56" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F57" s="5">
         <v>1809300</v>
       </c>
       <c r="G57" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="B58" t="s">
-        <v>184</v>
+        <v>83</v>
       </c>
       <c r="F58" s="5">
-        <v>1431273</v>
+        <v>9556915</v>
       </c>
       <c r="G58" t="s">
-        <v>242</v>
+        <v>253</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="B59" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
       <c r="F59" s="5"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="B60" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
       <c r="F60" s="5"/>
     </row>
@@ -4140,40 +4290,40 @@
     <hyperlink ref="F29" r:id="rId2" display="http://nz.element14.com/koa/rk73z2attd/resistor-0805-0-ohm-jumper/dp/1809596"/>
     <hyperlink ref="F42" r:id="rId3" display="http://nz.element14.com/koa/rk73z2attd/resistor-0805-0-ohm-jumper/dp/1809596"/>
     <hyperlink ref="F55" r:id="rId4" display="http://nz.element14.com/koa/rk73z2attd/resistor-0805-0-ohm-jumper/dp/1809596"/>
-    <hyperlink ref="F58" r:id="rId5" display="http://nz.element14.com/on-semiconductor/mmsz5231bt1g/diode-zener-5-1v-0-5w/dp/1431273"/>
-    <hyperlink ref="F45" r:id="rId6" display="http://nz.element14.com/on-semiconductor/mmsz5231bt1g/diode-zener-5-1v-0-5w/dp/1431273"/>
-    <hyperlink ref="F32" r:id="rId7" display="http://nz.element14.com/on-semiconductor/mmsz5231bt1g/diode-zener-5-1v-0-5w/dp/1431273"/>
-    <hyperlink ref="F20" r:id="rId8" display="http://nz.element14.com/on-semiconductor/mmsz5231bt1g/diode-zener-5-1v-0-5w/dp/1431273"/>
-    <hyperlink ref="F50" r:id="rId9" display="http://nz.element14.com/multicomp/mc-0-1w-0805-5-2k/resistor-0805-2k/dp/9334084"/>
-    <hyperlink ref="F37" r:id="rId10" display="http://nz.element14.com/multicomp/mc-0-1w-0805-5-2k/resistor-0805-2k/dp/9334084"/>
-    <hyperlink ref="F25" r:id="rId11" display="http://nz.element14.com/multicomp/mc-0-1w-0805-5-2k/resistor-0805-2k/dp/9334084"/>
-    <hyperlink ref="F13" r:id="rId12" display="http://nz.element14.com/multicomp/mc-0-1w-0805-5-2k/resistor-0805-2k/dp/9334084"/>
-    <hyperlink ref="F14" r:id="rId13" display="http://nz.element14.com/kingbright/kphcm-2012seck/led-smd-0805-orange/dp/1686068"/>
-    <hyperlink ref="F26" r:id="rId14" display="http://nz.element14.com/kingbright/kphcm-2012seck/led-smd-0805-orange/dp/1686068"/>
-    <hyperlink ref="F38" r:id="rId15" display="http://nz.element14.com/kingbright/kphcm-2012seck/led-smd-0805-orange/dp/1686068"/>
-    <hyperlink ref="F51" r:id="rId16" display="http://nz.element14.com/kingbright/kphcm-2012seck/led-smd-0805-orange/dp/1686068"/>
-    <hyperlink ref="F56" r:id="rId17" display="http://nz.element14.com/koa/rk73b2attd104j/resistor-0805-100k-ohm-5/dp/1809303"/>
-    <hyperlink ref="F43" r:id="rId18" display="http://nz.element14.com/koa/rk73b2attd104j/resistor-0805-100k-ohm-5/dp/1809303"/>
-    <hyperlink ref="F30" r:id="rId19" display="http://nz.element14.com/koa/rk73b2attd104j/resistor-0805-100k-ohm-5/dp/1809303"/>
-    <hyperlink ref="F18" r:id="rId20" display="http://nz.element14.com/koa/rk73b2attd104j/resistor-0805-100k-ohm-5/dp/1809303"/>
-    <hyperlink ref="F27" r:id="rId21" display="http://nz.element14.com/fairchild-semiconductor/rfp30n06le/mosfet-n-logic-to-220/dp/1017798"/>
-    <hyperlink ref="F53" r:id="rId22" display="http://nz.element14.com/infineon/ipp037n08n3-g/mosfet-n-ch-100a-80v-pg-to220-3/dp/1775617"/>
-    <hyperlink ref="K53" r:id="rId23" display="http://nz.element14.com/fairchild-semiconductor/rfp30n06le/mosfet-n-logic-to-220/dp/1017798"/>
-    <hyperlink ref="F40" r:id="rId24" display="http://nz.element14.com/infineon/ipp037n08n3-g/mosfet-n-ch-100a-80v-pg-to220-3/dp/1775617"/>
-    <hyperlink ref="K40" r:id="rId25" display="http://nz.element14.com/fairchild-semiconductor/rfp30n06le/mosfet-n-logic-to-220/dp/1017798"/>
-    <hyperlink ref="F15" r:id="rId26" display="http://nz.element14.com/fairchild-semiconductor/rfp30n06le/mosfet-n-logic-to-220/dp/1017798"/>
-    <hyperlink ref="F9" r:id="rId27" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
-    <hyperlink ref="F6" r:id="rId28" display="http://nz.element14.com/koa/rk73b2attd162j/resistor-0805-1k6-ohm-5/dp/1809321"/>
-    <hyperlink ref="F5" r:id="rId29" display="http://nz.element14.com/koa/rk73b2attd162j/resistor-0805-1k6-ohm-5/dp/1809321"/>
-    <hyperlink ref="F4" r:id="rId30" display="http://nz.element14.com/koa/rk73b2attd162j/resistor-0805-1k6-ohm-5/dp/1809321"/>
-    <hyperlink ref="F3" r:id="rId31" display="http://nz.element14.com/koa/rk73b2attd162j/resistor-0805-1k6-ohm-5/dp/1809321"/>
-    <hyperlink ref="F7" r:id="rId32" display="http://nz.element14.com/koa/rk73b2attd103j/resistor-0805-10k-ohm-5/dp/1809302"/>
-    <hyperlink ref="F8" r:id="rId33" display="http://nz.element14.com/koa/rk73b2attd103j/resistor-0805-10k-ohm-5/dp/1809302"/>
-    <hyperlink ref="F10" r:id="rId34" display="http://nz.element14.com/texas-instruments/sn74ls86ad/logic-quad-2-in-ex-or-gate-14soic/dp/1740035?Ntt=74ls86"/>
-    <hyperlink ref="F19" r:id="rId35" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
-    <hyperlink ref="F31" r:id="rId36" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
-    <hyperlink ref="F44" r:id="rId37" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
-    <hyperlink ref="F57" r:id="rId38" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
+    <hyperlink ref="F50" r:id="rId5" display="http://nz.element14.com/multicomp/mc-0-1w-0805-5-2k/resistor-0805-2k/dp/9334084"/>
+    <hyperlink ref="F37" r:id="rId6" display="http://nz.element14.com/multicomp/mc-0-1w-0805-5-2k/resistor-0805-2k/dp/9334084"/>
+    <hyperlink ref="F25" r:id="rId7" display="http://nz.element14.com/multicomp/mc-0-1w-0805-5-2k/resistor-0805-2k/dp/9334084"/>
+    <hyperlink ref="F13" r:id="rId8" display="http://nz.element14.com/multicomp/mc-0-1w-0805-5-2k/resistor-0805-2k/dp/9334084"/>
+    <hyperlink ref="F14" r:id="rId9" display="http://nz.element14.com/kingbright/kphcm-2012seck/led-smd-0805-orange/dp/1686068"/>
+    <hyperlink ref="F26" r:id="rId10" display="http://nz.element14.com/kingbright/kphcm-2012seck/led-smd-0805-orange/dp/1686068"/>
+    <hyperlink ref="F38" r:id="rId11" display="http://nz.element14.com/kingbright/kphcm-2012seck/led-smd-0805-orange/dp/1686068"/>
+    <hyperlink ref="F51" r:id="rId12" display="http://nz.element14.com/kingbright/kphcm-2012seck/led-smd-0805-orange/dp/1686068"/>
+    <hyperlink ref="F56" r:id="rId13" display="http://nz.element14.com/koa/rk73b2attd104j/resistor-0805-100k-ohm-5/dp/1809303"/>
+    <hyperlink ref="F43" r:id="rId14" display="http://nz.element14.com/koa/rk73b2attd104j/resistor-0805-100k-ohm-5/dp/1809303"/>
+    <hyperlink ref="F30" r:id="rId15" display="http://nz.element14.com/koa/rk73b2attd104j/resistor-0805-100k-ohm-5/dp/1809303"/>
+    <hyperlink ref="F18" r:id="rId16" display="http://nz.element14.com/koa/rk73b2attd104j/resistor-0805-100k-ohm-5/dp/1809303"/>
+    <hyperlink ref="F27" r:id="rId17" display="http://nz.element14.com/fairchild-semiconductor/rfp30n06le/mosfet-n-logic-to-220/dp/1017798"/>
+    <hyperlink ref="F53" r:id="rId18" display="http://nz.element14.com/infineon/ipp037n08n3-g/mosfet-n-ch-100a-80v-pg-to220-3/dp/1775617"/>
+    <hyperlink ref="K53" r:id="rId19" display="http://nz.element14.com/fairchild-semiconductor/rfp30n06le/mosfet-n-logic-to-220/dp/1017798"/>
+    <hyperlink ref="F40" r:id="rId20" display="http://nz.element14.com/infineon/ipp037n08n3-g/mosfet-n-ch-100a-80v-pg-to220-3/dp/1775617"/>
+    <hyperlink ref="K40" r:id="rId21" display="http://nz.element14.com/fairchild-semiconductor/rfp30n06le/mosfet-n-logic-to-220/dp/1017798"/>
+    <hyperlink ref="F15" r:id="rId22" display="http://nz.element14.com/fairchild-semiconductor/rfp30n06le/mosfet-n-logic-to-220/dp/1017798"/>
+    <hyperlink ref="F9" r:id="rId23" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
+    <hyperlink ref="F7" r:id="rId24" display="http://nz.element14.com/koa/rk73b2attd103j/resistor-0805-10k-ohm-5/dp/1809302"/>
+    <hyperlink ref="F8" r:id="rId25" display="http://nz.element14.com/koa/rk73b2attd103j/resistor-0805-10k-ohm-5/dp/1809302"/>
+    <hyperlink ref="F10" r:id="rId26" display="http://nz.element14.com/texas-instruments/sn74ls86ad/logic-quad-2-in-ex-or-gate-14soic/dp/1740035?Ntt=74ls86"/>
+    <hyperlink ref="F19" r:id="rId27" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
+    <hyperlink ref="F31" r:id="rId28" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
+    <hyperlink ref="F44" r:id="rId29" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
+    <hyperlink ref="F57" r:id="rId30" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
+    <hyperlink ref="F3" r:id="rId31" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
+    <hyperlink ref="F4" r:id="rId32" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
+    <hyperlink ref="F5" r:id="rId33" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
+    <hyperlink ref="F6" r:id="rId34" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
+    <hyperlink ref="F20" r:id="rId35" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
+    <hyperlink ref="F32" r:id="rId36" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
+    <hyperlink ref="F45" r:id="rId37" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
+    <hyperlink ref="F58" r:id="rId38" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId39"/>
@@ -4202,7 +4352,7 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A12:XFD13"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -4214,7 +4364,7 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -4223,14 +4373,16 @@
       <c r="F2" s="3"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
+      <c r="I2" s="4" t="s">
+        <v>361</v>
+      </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
@@ -4239,40 +4391,40 @@
         <v>1887296</v>
       </c>
       <c r="G3" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" t="s">
         <v>77</v>
-      </c>
-      <c r="B4" t="s">
-        <v>78</v>
       </c>
       <c r="F4" s="5">
         <v>1506077</v>
       </c>
       <c r="G4" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" t="s">
         <v>79</v>
-      </c>
-      <c r="B5" t="s">
-        <v>80</v>
       </c>
       <c r="F5" s="5">
         <v>1809596</v>
       </c>
       <c r="G5" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B6" t="s">
         <v>22</v>
@@ -4281,51 +4433,51 @@
         <v>8820120</v>
       </c>
       <c r="G6" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="I6" s="5"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F7" s="5">
         <v>9556915</v>
       </c>
       <c r="G7" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" t="s">
         <v>83</v>
       </c>
-      <c r="B8" t="s">
-        <v>85</v>
-      </c>
       <c r="F8" s="5">
-        <v>1776392</v>
+        <v>9556915</v>
       </c>
       <c r="G8" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5">
         <v>1809376</v>
       </c>
       <c r="G9" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25"/>
@@ -4341,8 +4493,8 @@
     <hyperlink ref="F6" r:id="rId3" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
     <hyperlink ref="F4" r:id="rId4" display="http://nz.element14.com/welwyn/pcf0805p-r-1k-bt1/resistor-1k-25ppm-0-1-0805/dp/1506077"/>
     <hyperlink ref="F3" r:id="rId5" display="http://nz.element14.com/multicomp/mcpwr05ftew3901/resistor-0805-3-9k-1-0-125w/dp/1887296"/>
-    <hyperlink ref="F8" r:id="rId6" display="http://nz.element14.com/diodes-inc/1n4148w-7-f/diode-switch-100v-0-4w-sod123/dp/1776392"/>
-    <hyperlink ref="F7" r:id="rId7" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
+    <hyperlink ref="F7" r:id="rId6" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
+    <hyperlink ref="F8" r:id="rId7" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4356,7 +4508,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A15:XFD16"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -4368,7 +4520,7 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -4377,34 +4529,36 @@
       <c r="F2" s="3"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
+      <c r="I2" s="4" t="s">
+        <v>360</v>
+      </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F3" s="5">
         <v>1457153</v>
       </c>
       <c r="G3" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B4" t="s">
         <v>22</v>
@@ -4413,101 +4567,101 @@
         <v>8820120</v>
       </c>
       <c r="G4" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" t="s">
         <v>90</v>
-      </c>
-      <c r="B5" t="s">
-        <v>92</v>
       </c>
       <c r="F5" s="5">
         <v>1759199</v>
       </c>
       <c r="G5" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" t="s">
         <v>91</v>
-      </c>
-      <c r="B6" t="s">
-        <v>93</v>
       </c>
       <c r="F6" s="5">
         <v>1759172</v>
       </c>
       <c r="G6" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F7" s="5">
         <v>1809376</v>
       </c>
       <c r="G7" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F8" s="5">
         <v>1809596</v>
       </c>
       <c r="G8" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F9" s="5">
         <v>1809596</v>
       </c>
       <c r="G9" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" t="s">
         <v>99</v>
-      </c>
-      <c r="B12" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25"/>
@@ -4537,7 +4691,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A14:XFD16"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -4549,7 +4703,7 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -4558,28 +4712,36 @@
       <c r="F2" s="3"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
+      <c r="I2" s="4" t="s">
+        <v>362</v>
+      </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F3" s="5">
         <v>1555602</v>
       </c>
       <c r="G3" t="s">
-        <v>205</v>
+        <v>338</v>
+      </c>
+      <c r="J3" s="5">
+        <v>1703477</v>
+      </c>
+      <c r="K3" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B4" t="s">
         <v>22</v>
@@ -4588,88 +4750,88 @@
         <v>8820120</v>
       </c>
       <c r="G4" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F5" s="5">
         <v>1759199</v>
       </c>
       <c r="G5" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F7" s="5">
         <v>1809376</v>
       </c>
       <c r="G7" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F8" s="5">
         <v>1759172</v>
       </c>
       <c r="G8" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F11" s="5">
         <v>1809596</v>
       </c>
       <c r="G11" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25"/>
@@ -4685,8 +4847,10 @@
     <hyperlink ref="F4" r:id="rId4" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
     <hyperlink ref="F5" r:id="rId5" display="http://nz.element14.com/multicomp/mcca000326/mlcc-0805-np0-50v-47pf/dp/1759199"/>
     <hyperlink ref="F8" r:id="rId6" display="http://nz.element14.com/multicomp/mcca000301/mlcc-0805-x7r-25v-220nf/dp/1759172"/>
+    <hyperlink ref="J3" r:id="rId7" display="http://nz.element14.com/freescale-semiconductor/mpx4100as/ic-pressure-sensor-6-867e/dp/1703477"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -4698,7 +4862,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A19:XFD21"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -4712,7 +4876,7 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -4721,38 +4885,40 @@
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
+      <c r="I2" s="4" t="s">
+        <v>367</v>
+      </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="12">
         <v>1845719</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="8" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="L3" s="8"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -4761,12 +4927,12 @@
         <v>1809302</v>
       </c>
       <c r="G4" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B5" t="s">
         <v>22</v>
@@ -4775,61 +4941,61 @@
         <v>8820120</v>
       </c>
       <c r="G5" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F6" s="5">
         <v>1414659</v>
       </c>
       <c r="G6" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="F7" s="5">
         <v>1618242</v>
       </c>
       <c r="G7" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="F8" s="5">
         <v>1618242</v>
       </c>
       <c r="G8" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -4838,38 +5004,40 @@
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
+      <c r="I10" s="4" t="s">
+        <v>368</v>
+      </c>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="12">
         <v>1845719</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="8" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="L11" s="8"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
@@ -4878,12 +5046,12 @@
         <v>1809302</v>
       </c>
       <c r="G12" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B13" t="s">
         <v>22</v>
@@ -4892,55 +5060,55 @@
         <v>8820120</v>
       </c>
       <c r="G13" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B14" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F14" s="5">
         <v>1414659</v>
       </c>
       <c r="G14" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B15" t="s">
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="F15" s="5">
         <v>1618242</v>
       </c>
       <c r="G15" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B16" t="s">
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="F16" s="5">
         <v>1618242</v>
       </c>
       <c r="G16" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
     </row>
     <row r="17" x14ac:dyDescent="0.25"/>
@@ -4974,10 +5142,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:G4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -4989,7 +5157,7 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>129</v>
+        <v>341</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -5003,99 +5171,115 @@
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
-        <v>232</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="C3" t="s">
-        <v>132</v>
-      </c>
+    <row r="3" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>340</v>
+      </c>
+      <c r="B3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C3"/>
       <c r="F3" s="5">
-        <v>1465996</v>
+        <v>1017798</v>
       </c>
       <c r="G3" t="s">
-        <v>196</v>
+        <v>319</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C4" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="F4" s="5">
+        <v>1465996</v>
+      </c>
+      <c r="G4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" t="s">
+        <v>130</v>
+      </c>
+      <c r="F5" s="5">
         <v>1809376</v>
       </c>
-      <c r="G4" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="B5" t="s">
-        <v>134</v>
-      </c>
-      <c r="F5" s="5">
-        <v>1809303</v>
-      </c>
       <c r="G5" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="B6" t="s">
-        <v>78</v>
+        <v>131</v>
       </c>
       <c r="F6" s="5">
+        <v>1809303</v>
+      </c>
+      <c r="G6" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="B7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F7" s="5">
         <v>1809300</v>
       </c>
-      <c r="G6" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>236</v>
-      </c>
-      <c r="B7" t="s">
-        <v>101</v>
+      <c r="G7" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="B8" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="B9" t="s">
+        <v>99</v>
+      </c>
+    </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="17" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="18" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F4" r:id="rId1" display="http://nz.element14.com/koa/rk73b2attd471j/resistor-0805-470-ohm-5/dp/1809376"/>
-    <hyperlink ref="F3" r:id="rId2" display="http://nz.element14.com/dialight/5988170107f/led-0805-green/dp/1465996"/>
-    <hyperlink ref="F6" r:id="rId3" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
-    <hyperlink ref="F5" r:id="rId4" display="http://nz.element14.com/koa/rk73b2attd104j/resistor-0805-100k-ohm-5/dp/1809303"/>
+    <hyperlink ref="F5" r:id="rId1" display="http://nz.element14.com/koa/rk73b2attd471j/resistor-0805-470-ohm-5/dp/1809376"/>
+    <hyperlink ref="F4" r:id="rId2" display="http://nz.element14.com/dialight/5988170107f/led-0805-green/dp/1465996"/>
+    <hyperlink ref="F7" r:id="rId3" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
+    <hyperlink ref="F6" r:id="rId4" display="http://nz.element14.com/koa/rk73b2attd104j/resistor-0805-100k-ohm-5/dp/1809303"/>
+    <hyperlink ref="F3" r:id="rId5" display="http://nz.element14.com/fairchild-semiconductor/rfp30n06le/mosfet-n-logic-to-220/dp/1017798"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5106,10 +5290,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="F14" sqref="F14:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -5121,7 +5305,7 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>135</v>
+        <v>339</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -5130,14 +5314,16 @@
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
+      <c r="I2" s="4" t="s">
+        <v>358</v>
+      </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B3" t="s">
         <v>22</v>
@@ -5146,26 +5332,26 @@
         <v>8820120</v>
       </c>
       <c r="G3" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F4" s="5">
         <v>1809376</v>
       </c>
       <c r="G4" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B5" t="s">
         <v>22</v>
@@ -5174,60 +5360,123 @@
         <v>8820120</v>
       </c>
       <c r="G5" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>139</v>
+      <c r="A6" s="14" t="s">
+        <v>342</v>
       </c>
       <c r="B6" t="s">
-        <v>101</v>
+        <v>357</v>
+      </c>
+      <c r="F6" s="5">
+        <v>1809596</v>
+      </c>
+      <c r="G6" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>324</v>
+      <c r="A7" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="B7" t="s">
+        <v>357</v>
       </c>
       <c r="F7" s="5">
-        <v>1431273</v>
+        <v>1809596</v>
       </c>
       <c r="G7" t="s">
-        <v>242</v>
+        <v>224</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="C8" s="2"/>
+        <v>346</v>
+      </c>
+      <c r="B8" t="s">
+        <v>83</v>
+      </c>
       <c r="F8" s="5">
-        <v>1809376</v>
+        <v>9556915</v>
       </c>
       <c r="G8" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
+        <v>253</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>345</v>
+      </c>
+      <c r="B9" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" s="5">
+        <v>9556915</v>
+      </c>
+      <c r="G9" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F10" s="5">
+        <v>1887290</v>
+      </c>
+      <c r="G10" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="B11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>344</v>
+      </c>
+      <c r="B12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="B13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="17" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="18" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="19" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="20" x14ac:dyDescent="0.25"/>
+    <row r="21" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F4" r:id="rId1" display="http://nz.element14.com/koa/rk73b2attd471j/resistor-0805-470-ohm-5/dp/1809376"/>
     <hyperlink ref="F3" r:id="rId2" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
     <hyperlink ref="F5" r:id="rId3" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
-    <hyperlink ref="F8" r:id="rId4" display="http://nz.element14.com/koa/rk73b2attd471j/resistor-0805-470-ohm-5/dp/1809376"/>
-    <hyperlink ref="F7" r:id="rId5" display="http://nz.element14.com/on-semiconductor/mmsz5231bt1g/diode-zener-5-1v-0-5w/dp/1431273"/>
+    <hyperlink ref="F9" r:id="rId4" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
+    <hyperlink ref="F8" r:id="rId5" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
+    <hyperlink ref="F6" r:id="rId6" display="http://nz.element14.com/koa/rk73z2attd/resistor-0805-0-ohm-jumper/dp/1809596"/>
+    <hyperlink ref="F7" r:id="rId7" display="http://nz.element14.com/koa/rk73z2attd/resistor-0805-0-ohm-jumper/dp/1809596"/>
+    <hyperlink ref="F10" r:id="rId8" display="http://nz.element14.com/multicomp/mcpwr05ftew2401/resistor-0805-2-4k-1-0-125w/dp/1887290"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5238,10 +5487,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="F14" sqref="F14:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -5253,7 +5502,7 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -5262,14 +5511,16 @@
       <c r="F2" s="3"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
+      <c r="I2" s="4" t="s">
+        <v>369</v>
+      </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B3" t="s">
         <v>22</v>
@@ -5278,26 +5529,26 @@
         <v>8820120</v>
       </c>
       <c r="G3" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F4" s="5">
         <v>1809376</v>
       </c>
       <c r="G4" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B5" t="s">
         <v>22</v>
@@ -5306,61 +5557,124 @@
         <v>8820120</v>
       </c>
       <c r="G5" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>145</v>
+      <c r="A6" s="14" t="s">
+        <v>352</v>
       </c>
       <c r="B6" t="s">
-        <v>101</v>
+        <v>357</v>
+      </c>
+      <c r="F6" s="5">
+        <v>1809596</v>
+      </c>
+      <c r="G6" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>324</v>
+      <c r="A7" s="14" t="s">
+        <v>353</v>
+      </c>
+      <c r="B7" t="s">
+        <v>357</v>
       </c>
       <c r="F7" s="5">
-        <v>1431273</v>
+        <v>1809596</v>
       </c>
       <c r="G7" t="s">
-        <v>242</v>
+        <v>224</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="C8" s="2"/>
+        <v>355</v>
+      </c>
+      <c r="B8" t="s">
+        <v>83</v>
+      </c>
       <c r="F8" s="5">
-        <v>1809376</v>
+        <v>9556915</v>
       </c>
       <c r="G8" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
+        <v>253</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="B9" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" s="5">
+        <v>9556915</v>
+      </c>
+      <c r="G9" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F10" s="5">
+        <v>1887290</v>
+      </c>
+      <c r="G10" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="B11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="B12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>354</v>
+      </c>
+      <c r="B13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25"/>
+    <row r="17" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="18" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="19" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="20" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="21" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="22" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F4" r:id="rId1" display="http://nz.element14.com/koa/rk73b2attd471j/resistor-0805-470-ohm-5/dp/1809376"/>
     <hyperlink ref="F3" r:id="rId2" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
     <hyperlink ref="F5" r:id="rId3" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
-    <hyperlink ref="F7" r:id="rId4" display="http://nz.element14.com/on-semiconductor/mmsz5231bt1g/diode-zener-5-1v-0-5w/dp/1431273"/>
-    <hyperlink ref="F8" r:id="rId5" display="http://nz.element14.com/koa/rk73b2attd471j/resistor-0805-470-ohm-5/dp/1809376"/>
+    <hyperlink ref="F9" r:id="rId4" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
+    <hyperlink ref="F8" r:id="rId5" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
+    <hyperlink ref="F6" r:id="rId6" display="http://nz.element14.com/koa/rk73z2attd/resistor-0805-0-ohm-jumper/dp/1809596"/>
+    <hyperlink ref="F7" r:id="rId7" display="http://nz.element14.com/koa/rk73z2attd/resistor-0805-0-ohm-jumper/dp/1809596"/>
+    <hyperlink ref="F10" r:id="rId8" display="http://nz.element14.com/multicomp/mcpwr05ftew2401/resistor-0805-2-4k-1-0-125w/dp/1887290"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5371,10 +5685,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="F14" sqref="F14:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -5386,7 +5700,7 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -5395,14 +5709,16 @@
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
+      <c r="I2" s="4" t="s">
+        <v>359</v>
+      </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B3" t="s">
         <v>22</v>
@@ -5411,26 +5727,26 @@
         <v>8820120</v>
       </c>
       <c r="G3" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F4" s="5">
         <v>1809376</v>
       </c>
       <c r="G4" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B5" t="s">
         <v>22</v>
@@ -5439,61 +5755,125 @@
         <v>8820120</v>
       </c>
       <c r="G5" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>152</v>
+      <c r="A6" s="14" t="s">
+        <v>347</v>
       </c>
       <c r="B6" t="s">
-        <v>101</v>
+        <v>357</v>
+      </c>
+      <c r="F6" s="5">
+        <v>1809596</v>
+      </c>
+      <c r="G6" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>324</v>
+      <c r="A7" s="14" t="s">
+        <v>348</v>
+      </c>
+      <c r="B7" t="s">
+        <v>357</v>
       </c>
       <c r="F7" s="5">
-        <v>1431273</v>
+        <v>1809596</v>
       </c>
       <c r="G7" t="s">
-        <v>242</v>
+        <v>224</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>154</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="C8" s="2"/>
+        <v>350</v>
+      </c>
+      <c r="B8" t="s">
+        <v>83</v>
+      </c>
       <c r="F8" s="5">
-        <v>1809376</v>
+        <v>9556915</v>
       </c>
       <c r="G8" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
+        <v>253</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>351</v>
+      </c>
+      <c r="B9" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" s="5">
+        <v>9556915</v>
+      </c>
+      <c r="G9" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F10" s="5">
+        <v>1887290</v>
+      </c>
+      <c r="G10" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="B11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="B12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>349</v>
+      </c>
+      <c r="B13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25"/>
+    <row r="17" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="18" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="19" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="20" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="21" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="22" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F4" r:id="rId1" display="http://nz.element14.com/koa/rk73b2attd471j/resistor-0805-470-ohm-5/dp/1809376"/>
     <hyperlink ref="F3" r:id="rId2" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
     <hyperlink ref="F5" r:id="rId3" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
-    <hyperlink ref="F7" r:id="rId4" display="http://nz.element14.com/on-semiconductor/mmsz5231bt1g/diode-zener-5-1v-0-5w/dp/1431273"/>
-    <hyperlink ref="F8" r:id="rId5" display="http://nz.element14.com/koa/rk73b2attd471j/resistor-0805-470-ohm-5/dp/1809376"/>
+    <hyperlink ref="F9" r:id="rId4" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
+    <hyperlink ref="F8" r:id="rId5" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
+    <hyperlink ref="F6" r:id="rId6" display="http://nz.element14.com/koa/rk73z2attd/resistor-0805-0-ohm-jumper/dp/1809596"/>
+    <hyperlink ref="F7" r:id="rId7" display="http://nz.element14.com/koa/rk73z2attd/resistor-0805-0-ohm-jumper/dp/1809596"/>
+    <hyperlink ref="F10" r:id="rId8" display="http://nz.element14.com/multicomp/mcpwr05ftew2401/resistor-0805-2-4k-1-0-125w/dp/1887290"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added page numbers to MAP and AAP, updated ign and inj components to Omnifet. Some other minor changes made
</commit_message>
<xml_diff>
--- a/PumaBom-WithMods-Element14.xlsx
+++ b/PumaBom-WithMods-Element14.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="10515" windowHeight="4680" tabRatio="710" firstSheet="1" activeTab="11"/>
+    <workbookView xWindow="30" yWindow="0" windowWidth="19155" windowHeight="5160" tabRatio="710" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Primary Puma Parts" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="387">
   <si>
     <t>MCU</t>
   </si>
@@ -328,9 +328,6 @@
     <t>Not used no connection</t>
   </si>
   <si>
-    <t>Altitude Air Pressure</t>
-  </si>
-  <si>
     <t>MPX4100A</t>
   </si>
   <si>
@@ -607,9 +604,6 @@
     <t>Mini USB - type b</t>
   </si>
   <si>
-    <t>MOSFET, N CH, 100A, 80V, PG-TO220-3</t>
-  </si>
-  <si>
     <t>Not needed wire jumper</t>
   </si>
   <si>
@@ -1108,15 +1102,9 @@
     <t>Schematic pages: 1, 48, 56</t>
   </si>
   <si>
-    <t>Schematic pages: 1, ??, 44</t>
-  </si>
-  <si>
     <t>Schematic pages: 53</t>
   </si>
   <si>
-    <t>Schematic pages: 1, ??, 43</t>
-  </si>
-  <si>
     <t>Schematic pages: 1, 14</t>
   </si>
   <si>
@@ -1178,6 +1166,27 @@
   </si>
   <si>
     <t>Schematic pages: 1, 38, 39</t>
+  </si>
+  <si>
+    <t>Schematic pages: 1, 24, 44</t>
+  </si>
+  <si>
+    <t>Schematic pages: 1, 47, 43</t>
+  </si>
+  <si>
+    <t>Atmospheric Absolute Pressure</t>
+  </si>
+  <si>
+    <t>511-VNP14NV04-E</t>
+  </si>
+  <si>
+    <t>Mouser  N-Ch 40V 14A OmniFET</t>
+  </si>
+  <si>
+    <t>686-8518P</t>
+  </si>
+  <si>
+    <t>RS components VNP10N07 Omnifet</t>
   </si>
 </sst>
 </file>
@@ -1629,7 +1638,7 @@
   </sheetPr>
   <dimension ref="A1:L74"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J53" sqref="J53"/>
     </sheetView>
   </sheetViews>
@@ -1648,14 +1657,14 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C2" s="19"/>
       <c r="D2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="H2" s="23" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="I2" s="23"/>
       <c r="J2" s="23"/>
@@ -1664,10 +1673,10 @@
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C3" s="20"/>
       <c r="D3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H3" s="22" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="I3" s="23"/>
       <c r="J3" s="23"/>
@@ -1676,7 +1685,7 @@
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C4" s="21"/>
       <c r="D4" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25"/>
@@ -1689,12 +1698,12 @@
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
@@ -1705,13 +1714,13 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F7" s="5">
         <v>1380343</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1725,7 +1734,7 @@
         <v>1809302</v>
       </c>
       <c r="G8" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1739,7 +1748,7 @@
         <v>1809302</v>
       </c>
       <c r="G9" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1753,7 +1762,7 @@
         <v>1809302</v>
       </c>
       <c r="G10" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1767,7 +1776,7 @@
         <v>1809302</v>
       </c>
       <c r="G11" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1778,14 +1787,14 @@
         <v>3</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D12" s="16"/>
       <c r="F12" s="5">
         <v>1809302</v>
       </c>
       <c r="G12" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1799,7 +1808,7 @@
         <v>8820120</v>
       </c>
       <c r="G13" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1813,7 +1822,7 @@
         <v>1650875</v>
       </c>
       <c r="G14" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1827,7 +1836,7 @@
         <v>1702127</v>
       </c>
       <c r="G15" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1841,7 +1850,7 @@
         <v>1887296</v>
       </c>
       <c r="G16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1855,7 +1864,7 @@
         <v>1414676</v>
       </c>
       <c r="G17" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -1866,13 +1875,13 @@
         <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F18" s="5">
         <v>1174062</v>
       </c>
       <c r="G18" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -1886,7 +1895,7 @@
         <v>1712841</v>
       </c>
       <c r="G19" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -1900,7 +1909,7 @@
         <v>8820120</v>
       </c>
       <c r="G20" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -1914,7 +1923,7 @@
         <v>8820120</v>
       </c>
       <c r="G21" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -1925,13 +1934,13 @@
         <v>77</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F22" s="5">
         <v>1809300</v>
       </c>
       <c r="G22" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -1945,7 +1954,7 @@
         <v>8820120</v>
       </c>
       <c r="G23" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -1959,7 +1968,7 @@
         <v>8820120</v>
       </c>
       <c r="G24" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -1973,7 +1982,7 @@
         <v>8820120</v>
       </c>
       <c r="G25" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25"/>
@@ -1990,7 +1999,7 @@
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="4" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
@@ -2007,7 +2016,7 @@
         <v>1146032</v>
       </c>
       <c r="G29" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -2021,7 +2030,7 @@
         <v>8820120</v>
       </c>
       <c r="G30" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -2030,7 +2039,7 @@
         <v>38</v>
       </c>
       <c r="C31" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -2044,7 +2053,7 @@
         <v>8820120</v>
       </c>
       <c r="G32" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -2058,7 +2067,7 @@
         <v>9334084</v>
       </c>
       <c r="G33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -2072,7 +2081,7 @@
         <v>9406352</v>
       </c>
       <c r="G34" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -2080,13 +2089,13 @@
         <v>42</v>
       </c>
       <c r="B35" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F35" s="5">
         <v>1355761</v>
       </c>
       <c r="G35" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -2100,7 +2109,7 @@
         <v>1226390</v>
       </c>
       <c r="G36" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -2114,7 +2123,7 @@
         <v>1465996</v>
       </c>
       <c r="G37" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -2128,7 +2137,7 @@
         <v>1809376</v>
       </c>
       <c r="G38" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -2142,7 +2151,7 @@
         <v>1809376</v>
       </c>
       <c r="G39" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25"/>
@@ -2159,7 +2168,7 @@
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
       <c r="I42" s="4" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
@@ -2176,7 +2185,7 @@
         <v>1556741</v>
       </c>
       <c r="G43" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
@@ -2190,7 +2199,7 @@
         <v>9229272</v>
       </c>
       <c r="G44" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
@@ -2204,7 +2213,7 @@
         <v>8820120</v>
       </c>
       <c r="G45" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
@@ -2218,7 +2227,7 @@
         <v>9556915</v>
       </c>
       <c r="G46" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
@@ -2232,7 +2241,7 @@
         <v>1617365</v>
       </c>
       <c r="G47" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
@@ -2246,7 +2255,7 @@
         <v>8820120</v>
       </c>
       <c r="G48" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -2257,7 +2266,7 @@
         <v>57</v>
       </c>
       <c r="C49" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25"/>
@@ -2274,7 +2283,7 @@
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
       <c r="I52" s="4" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -2285,7 +2294,7 @@
         <v>57</v>
       </c>
       <c r="C53" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -2293,7 +2302,7 @@
         <v>60</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -2307,10 +2316,10 @@
         <v>9486038</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H55" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -2318,7 +2327,7 @@
         <v>63</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -2326,7 +2335,7 @@
         <v>64</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -2334,7 +2343,7 @@
         <v>65</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="F58" s="5"/>
     </row>
@@ -2343,7 +2352,7 @@
         <v>66</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="F59" s="5"/>
     </row>
@@ -2358,7 +2367,7 @@
         <v>1617365</v>
       </c>
       <c r="G60" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -2372,7 +2381,7 @@
         <v>8820120</v>
       </c>
       <c r="G61" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -2386,7 +2395,7 @@
         <v>1324152</v>
       </c>
       <c r="G62" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -2397,13 +2406,13 @@
         <v>31</v>
       </c>
       <c r="D63" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="F63" s="5">
         <v>9229272</v>
       </c>
       <c r="G63" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -2417,7 +2426,7 @@
         <v>8812519</v>
       </c>
       <c r="G64" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -2431,7 +2440,7 @@
         <v>8820120</v>
       </c>
       <c r="G65" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25"/>
@@ -2520,7 +2529,7 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -2530,7 +2539,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -2538,7 +2547,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B3" t="s">
         <v>50</v>
@@ -2547,12 +2556,12 @@
         <v>1809376</v>
       </c>
       <c r="G3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B4" t="s">
         <v>22</v>
@@ -2561,12 +2570,12 @@
         <v>8820120</v>
       </c>
       <c r="G4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B5" t="s">
         <v>83</v>
@@ -2575,12 +2584,12 @@
         <v>9556915</v>
       </c>
       <c r="G5" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B6" t="s">
         <v>83</v>
@@ -2589,7 +2598,7 @@
         <v>9556915</v>
       </c>
       <c r="G6" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25"/>
@@ -2618,23 +2627,23 @@
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:L69"/>
+  <dimension ref="A1:O69"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="I50" sqref="I50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="11" width="9.140625" customWidth="1"/>
-    <col min="12" max="12" width="27.28515625" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" hidden="1"/>
+    <col min="1" max="13" width="9.140625" customWidth="1"/>
+    <col min="14" max="14" width="27.28515625" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -2644,15 +2653,17 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B3" t="s">
         <v>77</v>
@@ -2661,84 +2672,88 @@
         <v>1809300</v>
       </c>
       <c r="G3" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F4" s="5">
         <v>1809376</v>
       </c>
       <c r="G4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F5" s="5">
         <v>1465996</v>
       </c>
       <c r="G5" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="B6" t="s">
         <v>160</v>
       </c>
-      <c r="B6" t="s">
+      <c r="F6" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="F6" s="9" t="s">
-        <v>321</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="B7" t="s">
         <v>162</v>
       </c>
-      <c r="B7" t="s">
+      <c r="F7" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="G7" t="s">
+        <v>386</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="M7" t="s">
+        <v>384</v>
+      </c>
+      <c r="O7" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="F7" s="5">
-        <v>1775617</v>
-      </c>
-      <c r="G7" t="s">
-        <v>193</v>
-      </c>
-      <c r="H7" s="5"/>
-      <c r="K7" s="5">
-        <v>1017798</v>
-      </c>
-      <c r="L7" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
+      <c r="B8" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>164</v>
-      </c>
-      <c r="B8" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>165</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -2748,15 +2763,17 @@
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B11" t="s">
         <v>77</v>
@@ -2765,83 +2782,88 @@
         <v>1809300</v>
       </c>
       <c r="G11" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F12" s="5">
         <v>1809376</v>
       </c>
       <c r="G12" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F13" s="5">
         <v>1465996</v>
       </c>
       <c r="G13" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B15" t="s">
-        <v>163</v>
-      </c>
-      <c r="F15" s="5">
-        <v>1775617</v>
+        <v>162</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>385</v>
       </c>
       <c r="G15" t="s">
-        <v>193</v>
-      </c>
-      <c r="K15" s="5">
-        <v>1017798</v>
-      </c>
-      <c r="L15" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+        <v>386</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="M15" t="s">
+        <v>384</v>
+      </c>
+      <c r="N15" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
+        <v>268</v>
+      </c>
+      <c r="B16" t="s">
         <v>270</v>
       </c>
-      <c r="B16" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -2851,15 +2873,17 @@
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B19" t="s">
         <v>77</v>
@@ -2868,83 +2892,88 @@
         <v>1809300</v>
       </c>
       <c r="G19" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F20" s="5">
         <v>1809376</v>
       </c>
       <c r="G20" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F21" s="5">
         <v>1465996</v>
       </c>
       <c r="G21" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B22" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="K22" s="9" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B23" t="s">
-        <v>163</v>
-      </c>
-      <c r="F23" s="5">
-        <v>1775617</v>
+        <v>162</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>385</v>
       </c>
       <c r="G23" t="s">
-        <v>193</v>
-      </c>
-      <c r="K23" s="5">
-        <v>1017798</v>
-      </c>
-      <c r="L23" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+        <v>386</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="M23" t="s">
+        <v>384</v>
+      </c>
+      <c r="N23" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B24" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -2954,15 +2983,17 @@
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
       <c r="I26" s="4" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B27" t="s">
         <v>77</v>
@@ -2971,83 +3002,88 @@
         <v>1809300</v>
       </c>
       <c r="G27" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B28" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F28" s="5">
         <v>1809376</v>
       </c>
       <c r="G28" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B29" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F29" s="5">
         <v>1465996</v>
       </c>
       <c r="G29" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B30" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="K30" s="9" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="B31" t="s">
+        <v>162</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="G31" t="s">
+        <v>386</v>
+      </c>
+      <c r="K31" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="M31" t="s">
+        <v>384</v>
+      </c>
+      <c r="N31" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="18" t="s">
+        <v>280</v>
+      </c>
+      <c r="B32" t="s">
         <v>281</v>
       </c>
-      <c r="B31" t="s">
-        <v>163</v>
-      </c>
-      <c r="F31" s="5">
-        <v>1775617</v>
-      </c>
-      <c r="G31" t="s">
-        <v>193</v>
-      </c>
-      <c r="K31" s="5">
-        <v>1017798</v>
-      </c>
-      <c r="L31" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="18" t="s">
-        <v>282</v>
-      </c>
-      <c r="B32" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25"/>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -3057,15 +3093,17 @@
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
       <c r="I34" s="4" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M34" s="4"/>
+      <c r="N34" s="4"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B35" t="s">
         <v>77</v>
@@ -3074,83 +3112,88 @@
         <v>1809300</v>
       </c>
       <c r="G35" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B36" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F36" s="5">
         <v>1809376</v>
       </c>
       <c r="G36" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B37" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F37" s="5">
         <v>1465996</v>
       </c>
       <c r="G37" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B38" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="K38" s="9" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+      <c r="L38" s="9"/>
+      <c r="M38" s="9"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B39" t="s">
-        <v>163</v>
-      </c>
-      <c r="F39" s="5">
-        <v>1775617</v>
+        <v>162</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>385</v>
       </c>
       <c r="G39" t="s">
-        <v>193</v>
-      </c>
-      <c r="K39" s="5">
-        <v>1017798</v>
-      </c>
-      <c r="L39" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+        <v>386</v>
+      </c>
+      <c r="K39" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="M39" t="s">
+        <v>384</v>
+      </c>
+      <c r="N39" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="18" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B40" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -3160,15 +3203,17 @@
       <c r="G42" s="4"/>
       <c r="H42" s="4"/>
       <c r="I42" s="4" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
       <c r="L42" s="4"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M42" s="4"/>
+      <c r="N42" s="4"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B43" t="s">
         <v>77</v>
@@ -3177,83 +3222,88 @@
         <v>1809300</v>
       </c>
       <c r="G43" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B44" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F44" s="5">
         <v>1809376</v>
       </c>
       <c r="G44" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B45" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F45" s="5">
         <v>1465996</v>
       </c>
       <c r="G45" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B46" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="K46" s="9" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+      <c r="L46" s="9"/>
+      <c r="M46" s="9"/>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B47" t="s">
-        <v>163</v>
-      </c>
-      <c r="F47" s="5">
-        <v>1775617</v>
+        <v>162</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>385</v>
       </c>
       <c r="G47" t="s">
-        <v>193</v>
-      </c>
-      <c r="K47" s="5">
-        <v>1017798</v>
-      </c>
-      <c r="L47" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+        <v>386</v>
+      </c>
+      <c r="K47" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="M47" t="s">
+        <v>384</v>
+      </c>
+      <c r="N47" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="18" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B48" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25"/>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -3263,15 +3313,17 @@
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
       <c r="I50" s="4" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
       <c r="L50" s="4"/>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M50" s="4"/>
+      <c r="N50" s="4"/>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B51" t="s">
         <v>77</v>
@@ -3280,90 +3332,97 @@
         <v>1809300</v>
       </c>
       <c r="G51" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B52" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F52" s="5">
         <v>1809376</v>
       </c>
       <c r="G52" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B53" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F53" s="5">
         <v>1465996</v>
       </c>
       <c r="G53" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B54" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F54" s="9" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="K54" s="9" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+      <c r="L54" s="9"/>
+      <c r="M54" s="9"/>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B55" t="s">
-        <v>163</v>
-      </c>
-      <c r="F55" s="5">
-        <v>1775617</v>
+        <v>162</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>385</v>
       </c>
       <c r="G55" t="s">
-        <v>193</v>
-      </c>
-      <c r="K55" s="5">
-        <v>1017798</v>
-      </c>
-      <c r="L55" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+        <v>386</v>
+      </c>
+      <c r="K55" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="M55" t="s">
+        <v>384</v>
+      </c>
+      <c r="N55" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="18" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B56" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
       <c r="K57" s="2"/>
       <c r="L57" s="2"/>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M57" s="2"/>
+      <c r="N57" s="2"/>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -3373,15 +3432,17 @@
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
       <c r="I58" s="4" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
       <c r="L58" s="4"/>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M58" s="4"/>
+      <c r="N58" s="4"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B59" t="s">
         <v>77</v>
@@ -3390,77 +3451,82 @@
         <v>1809300</v>
       </c>
       <c r="G59" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B60" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F60" s="5">
         <v>1809376</v>
       </c>
       <c r="G60" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B61" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F61" s="5">
         <v>1465996</v>
       </c>
       <c r="G61" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B62" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F62" s="9" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="K62" s="9" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+      <c r="L62" s="9"/>
+      <c r="M62" s="9"/>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B63" t="s">
-        <v>163</v>
-      </c>
-      <c r="F63" s="5">
-        <v>1775617</v>
+        <v>162</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>385</v>
       </c>
       <c r="G63" t="s">
-        <v>193</v>
-      </c>
-      <c r="K63" s="5">
-        <v>1017798</v>
-      </c>
-      <c r="L63" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+        <v>386</v>
+      </c>
+      <c r="K63" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="M63" t="s">
+        <v>384</v>
+      </c>
+      <c r="N63" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="18" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B64" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="65" x14ac:dyDescent="0.25"/>
@@ -3471,47 +3537,48 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F4" r:id="rId1" display="http://nz.element14.com/koa/rk73b2attd471j/resistor-0805-470-ohm-5/dp/1809376"/>
-    <hyperlink ref="F7" r:id="rId2" display="http://nz.element14.com/infineon/ipp037n08n3-g/mosfet-n-ch-100a-80v-pg-to220-3/dp/1775617"/>
-    <hyperlink ref="F12" r:id="rId3" display="http://nz.element14.com/koa/rk73b2attd471j/resistor-0805-470-ohm-5/dp/1809376"/>
-    <hyperlink ref="F20" r:id="rId4" display="http://nz.element14.com/koa/rk73b2attd471j/resistor-0805-470-ohm-5/dp/1809376"/>
-    <hyperlink ref="F28" r:id="rId5" display="http://nz.element14.com/koa/rk73b2attd471j/resistor-0805-470-ohm-5/dp/1809376"/>
-    <hyperlink ref="F36" r:id="rId6" display="http://nz.element14.com/koa/rk73b2attd471j/resistor-0805-470-ohm-5/dp/1809376"/>
-    <hyperlink ref="F44" r:id="rId7" display="http://nz.element14.com/koa/rk73b2attd471j/resistor-0805-470-ohm-5/dp/1809376"/>
-    <hyperlink ref="F52" r:id="rId8" display="http://nz.element14.com/koa/rk73b2attd471j/resistor-0805-470-ohm-5/dp/1809376"/>
-    <hyperlink ref="F60" r:id="rId9" display="http://nz.element14.com/koa/rk73b2attd471j/resistor-0805-470-ohm-5/dp/1809376"/>
-    <hyperlink ref="F5" r:id="rId10" display="http://nz.element14.com/dialight/5988170107f/led-0805-green/dp/1465996"/>
-    <hyperlink ref="F13" r:id="rId11" display="http://nz.element14.com/dialight/5988170107f/led-0805-green/dp/1465996"/>
-    <hyperlink ref="F21" r:id="rId12" display="http://nz.element14.com/dialight/5988170107f/led-0805-green/dp/1465996"/>
-    <hyperlink ref="F29" r:id="rId13" display="http://nz.element14.com/dialight/5988170107f/led-0805-green/dp/1465996"/>
-    <hyperlink ref="F37" r:id="rId14" display="http://nz.element14.com/dialight/5988170107f/led-0805-green/dp/1465996"/>
-    <hyperlink ref="F45" r:id="rId15" display="http://nz.element14.com/dialight/5988170107f/led-0805-green/dp/1465996"/>
-    <hyperlink ref="F53" r:id="rId16" display="http://nz.element14.com/dialight/5988170107f/led-0805-green/dp/1465996"/>
-    <hyperlink ref="F61" r:id="rId17" display="http://nz.element14.com/dialight/5988170107f/led-0805-green/dp/1465996"/>
-    <hyperlink ref="F3" r:id="rId18" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
-    <hyperlink ref="F11" r:id="rId19" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
-    <hyperlink ref="F19" r:id="rId20" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
-    <hyperlink ref="F27" r:id="rId21" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
-    <hyperlink ref="F35" r:id="rId22" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
-    <hyperlink ref="F43" r:id="rId23" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
-    <hyperlink ref="F51" r:id="rId24" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
-    <hyperlink ref="F15" r:id="rId25" display="http://nz.element14.com/infineon/ipp037n08n3-g/mosfet-n-ch-100a-80v-pg-to220-3/dp/1775617"/>
-    <hyperlink ref="F23" r:id="rId26" display="http://nz.element14.com/infineon/ipp037n08n3-g/mosfet-n-ch-100a-80v-pg-to220-3/dp/1775617"/>
-    <hyperlink ref="F31" r:id="rId27" display="http://nz.element14.com/infineon/ipp037n08n3-g/mosfet-n-ch-100a-80v-pg-to220-3/dp/1775617"/>
-    <hyperlink ref="F39" r:id="rId28" display="http://nz.element14.com/infineon/ipp037n08n3-g/mosfet-n-ch-100a-80v-pg-to220-3/dp/1775617"/>
-    <hyperlink ref="F47" r:id="rId29" display="http://nz.element14.com/infineon/ipp037n08n3-g/mosfet-n-ch-100a-80v-pg-to220-3/dp/1775617"/>
-    <hyperlink ref="F55" r:id="rId30" display="http://nz.element14.com/infineon/ipp037n08n3-g/mosfet-n-ch-100a-80v-pg-to220-3/dp/1775617"/>
-    <hyperlink ref="F63" r:id="rId31" display="http://nz.element14.com/infineon/ipp037n08n3-g/mosfet-n-ch-100a-80v-pg-to220-3/dp/1775617"/>
-    <hyperlink ref="F59" r:id="rId32" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
-    <hyperlink ref="K23" r:id="rId33" display="http://nz.element14.com/fairchild-semiconductor/rfp30n06le/mosfet-n-logic-to-220/dp/1017798"/>
-    <hyperlink ref="K15" r:id="rId34" display="http://nz.element14.com/fairchild-semiconductor/rfp30n06le/mosfet-n-logic-to-220/dp/1017798"/>
-    <hyperlink ref="K7" r:id="rId35" display="http://nz.element14.com/fairchild-semiconductor/rfp30n06le/mosfet-n-logic-to-220/dp/1017798"/>
-    <hyperlink ref="K31" r:id="rId36" display="http://nz.element14.com/fairchild-semiconductor/rfp30n06le/mosfet-n-logic-to-220/dp/1017798"/>
-    <hyperlink ref="K39" r:id="rId37" display="http://nz.element14.com/fairchild-semiconductor/rfp30n06le/mosfet-n-logic-to-220/dp/1017798"/>
-    <hyperlink ref="K47" r:id="rId38" display="http://nz.element14.com/fairchild-semiconductor/rfp30n06le/mosfet-n-logic-to-220/dp/1017798"/>
-    <hyperlink ref="K55" r:id="rId39" display="http://nz.element14.com/fairchild-semiconductor/rfp30n06le/mosfet-n-logic-to-220/dp/1017798"/>
-    <hyperlink ref="K63" r:id="rId40" display="http://nz.element14.com/fairchild-semiconductor/rfp30n06le/mosfet-n-logic-to-220/dp/1017798"/>
+    <hyperlink ref="F12" r:id="rId2" display="http://nz.element14.com/koa/rk73b2attd471j/resistor-0805-470-ohm-5/dp/1809376"/>
+    <hyperlink ref="F20" r:id="rId3" display="http://nz.element14.com/koa/rk73b2attd471j/resistor-0805-470-ohm-5/dp/1809376"/>
+    <hyperlink ref="F28" r:id="rId4" display="http://nz.element14.com/koa/rk73b2attd471j/resistor-0805-470-ohm-5/dp/1809376"/>
+    <hyperlink ref="F36" r:id="rId5" display="http://nz.element14.com/koa/rk73b2attd471j/resistor-0805-470-ohm-5/dp/1809376"/>
+    <hyperlink ref="F44" r:id="rId6" display="http://nz.element14.com/koa/rk73b2attd471j/resistor-0805-470-ohm-5/dp/1809376"/>
+    <hyperlink ref="F52" r:id="rId7" display="http://nz.element14.com/koa/rk73b2attd471j/resistor-0805-470-ohm-5/dp/1809376"/>
+    <hyperlink ref="F60" r:id="rId8" display="http://nz.element14.com/koa/rk73b2attd471j/resistor-0805-470-ohm-5/dp/1809376"/>
+    <hyperlink ref="F5" r:id="rId9" display="http://nz.element14.com/dialight/5988170107f/led-0805-green/dp/1465996"/>
+    <hyperlink ref="F13" r:id="rId10" display="http://nz.element14.com/dialight/5988170107f/led-0805-green/dp/1465996"/>
+    <hyperlink ref="F21" r:id="rId11" display="http://nz.element14.com/dialight/5988170107f/led-0805-green/dp/1465996"/>
+    <hyperlink ref="F29" r:id="rId12" display="http://nz.element14.com/dialight/5988170107f/led-0805-green/dp/1465996"/>
+    <hyperlink ref="F37" r:id="rId13" display="http://nz.element14.com/dialight/5988170107f/led-0805-green/dp/1465996"/>
+    <hyperlink ref="F45" r:id="rId14" display="http://nz.element14.com/dialight/5988170107f/led-0805-green/dp/1465996"/>
+    <hyperlink ref="F53" r:id="rId15" display="http://nz.element14.com/dialight/5988170107f/led-0805-green/dp/1465996"/>
+    <hyperlink ref="F61" r:id="rId16" display="http://nz.element14.com/dialight/5988170107f/led-0805-green/dp/1465996"/>
+    <hyperlink ref="F3" r:id="rId17" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
+    <hyperlink ref="F11" r:id="rId18" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
+    <hyperlink ref="F19" r:id="rId19" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
+    <hyperlink ref="F27" r:id="rId20" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
+    <hyperlink ref="F35" r:id="rId21" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
+    <hyperlink ref="F43" r:id="rId22" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
+    <hyperlink ref="F51" r:id="rId23" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
+    <hyperlink ref="F59" r:id="rId24" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
+    <hyperlink ref="K7" r:id="rId25" tooltip="Click to view additional information on this product." display="http://nz.mouser.com/ProductDetail/STMicroelectronics/VNP14NV04-E/?qs=sGAEpiMZZMuCmTIBzycWfOPiiwtMaP0Fv4CVvoRPcP8%3d"/>
+    <hyperlink ref="K15" r:id="rId26" tooltip="Click to view additional information on this product." display="http://nz.mouser.com/ProductDetail/STMicroelectronics/VNP14NV04-E/?qs=sGAEpiMZZMuCmTIBzycWfOPiiwtMaP0Fv4CVvoRPcP8%3d"/>
+    <hyperlink ref="K23" r:id="rId27" tooltip="Click to view additional information on this product." display="http://nz.mouser.com/ProductDetail/STMicroelectronics/VNP14NV04-E/?qs=sGAEpiMZZMuCmTIBzycWfOPiiwtMaP0Fv4CVvoRPcP8%3d"/>
+    <hyperlink ref="K31" r:id="rId28" tooltip="Click to view additional information on this product." display="http://nz.mouser.com/ProductDetail/STMicroelectronics/VNP14NV04-E/?qs=sGAEpiMZZMuCmTIBzycWfOPiiwtMaP0Fv4CVvoRPcP8%3d"/>
+    <hyperlink ref="K39" r:id="rId29" tooltip="Click to view additional information on this product." display="http://nz.mouser.com/ProductDetail/STMicroelectronics/VNP14NV04-E/?qs=sGAEpiMZZMuCmTIBzycWfOPiiwtMaP0Fv4CVvoRPcP8%3d"/>
+    <hyperlink ref="K47" r:id="rId30" tooltip="Click to view additional information on this product." display="http://nz.mouser.com/ProductDetail/STMicroelectronics/VNP14NV04-E/?qs=sGAEpiMZZMuCmTIBzycWfOPiiwtMaP0Fv4CVvoRPcP8%3d"/>
+    <hyperlink ref="K55" r:id="rId31" tooltip="Click to view additional information on this product." display="http://nz.mouser.com/ProductDetail/STMicroelectronics/VNP14NV04-E/?qs=sGAEpiMZZMuCmTIBzycWfOPiiwtMaP0Fv4CVvoRPcP8%3d"/>
+    <hyperlink ref="K63" r:id="rId32" tooltip="Click to view additional information on this product." display="http://nz.mouser.com/ProductDetail/STMicroelectronics/VNP14NV04-E/?qs=sGAEpiMZZMuCmTIBzycWfOPiiwtMaP0Fv4CVvoRPcP8%3d"/>
+    <hyperlink ref="F31" r:id="rId33" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
+    <hyperlink ref="F39" r:id="rId34" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
+    <hyperlink ref="F47" r:id="rId35" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
+    <hyperlink ref="F55" r:id="rId36" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
+    <hyperlink ref="F63" r:id="rId37" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
+    <hyperlink ref="F23" r:id="rId38" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
+    <hyperlink ref="F15" r:id="rId39" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
+    <hyperlink ref="F7" r:id="rId40" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId41"/>
 </worksheet>
 </file>
 
@@ -3520,23 +3587,23 @@
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:L68"/>
+  <dimension ref="A1:R70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="11" width="9.140625" customWidth="1"/>
-    <col min="12" max="12" width="27.28515625" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" hidden="1"/>
+    <col min="1" max="13" width="9.140625" customWidth="1"/>
+    <col min="14" max="14" width="27.28515625" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -3546,15 +3613,17 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B3" t="s">
         <v>77</v>
@@ -3563,12 +3632,12 @@
         <v>1809300</v>
       </c>
       <c r="G3" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B4" t="s">
         <v>77</v>
@@ -3577,12 +3646,12 @@
         <v>1809300</v>
       </c>
       <c r="G4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B5" t="s">
         <v>77</v>
@@ -3591,12 +3660,12 @@
         <v>1809300</v>
       </c>
       <c r="G5" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B6" t="s">
         <v>77</v>
@@ -3605,12 +3674,12 @@
         <v>1809300</v>
       </c>
       <c r="G6" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
@@ -3619,12 +3688,12 @@
         <v>1809302</v>
       </c>
       <c r="G7" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
@@ -3633,12 +3702,12 @@
         <v>1809302</v>
       </c>
       <c r="G8" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B9" t="s">
         <v>22</v>
@@ -3647,27 +3716,27 @@
         <v>8820120</v>
       </c>
       <c r="G9" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B10" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="F10" s="5">
         <v>1740035</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -3677,656 +3746,707 @@
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B13" t="s">
         <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F13" s="5">
         <v>9334084</v>
       </c>
       <c r="G13" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F14" s="5">
         <v>1686068</v>
       </c>
       <c r="G14" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="9"/>
+      <c r="F15" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="L15" s="9"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B16" t="s">
         <v>174</v>
       </c>
-      <c r="B15" t="s">
+      <c r="F16" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="G16" t="s">
+        <v>386</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="L16" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="F15" s="5">
-        <v>1017798</v>
-      </c>
-      <c r="G15" t="s">
+      <c r="B17" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="B18" t="s">
+        <v>98</v>
+      </c>
+      <c r="F18" s="5">
+        <v>1809596</v>
+      </c>
+      <c r="G18" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F19" s="5">
+        <v>1809303</v>
+      </c>
+      <c r="G19" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F20" s="5">
+        <v>1809300</v>
+      </c>
+      <c r="G20" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="B21" t="s">
+        <v>83</v>
+      </c>
+      <c r="F21" s="5">
+        <v>9556915</v>
+      </c>
+      <c r="G21" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="B22" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="B23" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="B26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" t="s">
+        <v>234</v>
+      </c>
+      <c r="F26" s="5">
+        <v>9334084</v>
+      </c>
+      <c r="G26" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="B27" t="s">
+        <v>126</v>
+      </c>
+      <c r="F27" s="5">
+        <v>1686068</v>
+      </c>
+      <c r="G27" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="9"/>
+      <c r="F28" s="9" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="B16" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="K28" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="L28" s="9"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="B29" t="s">
+        <v>174</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="G29" t="s">
+        <v>386</v>
+      </c>
+      <c r="K29" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="L29" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="B30" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="B31" t="s">
         <v>98</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F31" s="5">
         <v>1809596</v>
       </c>
-      <c r="G17" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="F18" s="5">
+      <c r="G31" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="B32" t="s">
+        <v>130</v>
+      </c>
+      <c r="F32" s="5">
         <v>1809303</v>
       </c>
-      <c r="G18" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
+      <c r="G32" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A33" s="14" t="s">
         <v>204</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F33" s="5">
         <v>1809300</v>
       </c>
-      <c r="G19" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="G33" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="B34" t="s">
         <v>83</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F34" s="5">
         <v>9556915</v>
       </c>
-      <c r="G20" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
-        <v>177</v>
-      </c>
-      <c r="B21" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
-        <v>179</v>
-      </c>
-      <c r="B22" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+      <c r="G34" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="B35" t="s">
+        <v>334</v>
+      </c>
+      <c r="F35" s="5"/>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="B36" t="s">
+        <v>334</v>
+      </c>
+      <c r="F36" s="5"/>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4" t="s">
-        <v>381</v>
-      </c>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
-        <v>200</v>
-      </c>
-      <c r="B25" t="s">
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="J38" s="4"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="4"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="4"/>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A39" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="B39" t="s">
         <v>40</v>
       </c>
-      <c r="C25" t="s">
-        <v>236</v>
-      </c>
-      <c r="F25" s="5">
+      <c r="C39" t="s">
+        <v>234</v>
+      </c>
+      <c r="F39" s="5">
         <v>9334084</v>
       </c>
-      <c r="G25" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="B26" t="s">
-        <v>127</v>
-      </c>
-      <c r="F26" s="5">
+      <c r="G39" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A40" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="B40" t="s">
+        <v>126</v>
+      </c>
+      <c r="F40" s="5">
         <v>1686068</v>
       </c>
-      <c r="G26" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="B27" t="s">
-        <v>175</v>
-      </c>
-      <c r="F27" s="5">
-        <v>1017798</v>
-      </c>
-      <c r="G27" t="s">
+      <c r="G40" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A41" s="9"/>
+      <c r="F41" s="9" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="B28" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
+      <c r="K41" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="L41" s="9"/>
+      <c r="M41" s="9"/>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="B42" t="s">
+        <v>174</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="G42" t="s">
+        <v>386</v>
+      </c>
+      <c r="K42" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="L42" t="s">
+        <v>386</v>
+      </c>
+      <c r="P42" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="R42" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A43" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="B43" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="B44" t="s">
+        <v>98</v>
+      </c>
+      <c r="F44" s="5">
+        <v>1809596</v>
+      </c>
+      <c r="G44" t="s">
         <v>222</v>
       </c>
-      <c r="B29" t="s">
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A45" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="B45" t="s">
+        <v>130</v>
+      </c>
+      <c r="F45" s="5">
+        <v>1809303</v>
+      </c>
+      <c r="G45" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A46" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F46" s="5">
+        <v>1809300</v>
+      </c>
+      <c r="G46" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A47" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="B47" t="s">
+        <v>83</v>
+      </c>
+      <c r="F47" s="5">
+        <v>9556915</v>
+      </c>
+      <c r="G47" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A48" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="B48" t="s">
+        <v>334</v>
+      </c>
+      <c r="F48" s="5"/>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A49" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="B49" t="s">
+        <v>334</v>
+      </c>
+      <c r="F49" s="5"/>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="J51" s="4"/>
+      <c r="K51" s="4"/>
+      <c r="L51" s="4"/>
+      <c r="M51" s="4"/>
+      <c r="N51" s="4"/>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A52" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="B52" t="s">
+        <v>40</v>
+      </c>
+      <c r="C52" t="s">
+        <v>234</v>
+      </c>
+      <c r="F52" s="5">
+        <v>9334084</v>
+      </c>
+      <c r="G52" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A53" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="B53" t="s">
+        <v>126</v>
+      </c>
+      <c r="F53" s="5">
+        <v>1686068</v>
+      </c>
+      <c r="G53" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A54" s="9"/>
+      <c r="F54" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="K54" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="L54" s="9"/>
+      <c r="M54" s="9"/>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A55" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="G55" t="s">
+        <v>386</v>
+      </c>
+      <c r="K55" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="L55" t="s">
+        <v>386</v>
+      </c>
+      <c r="M55" s="5"/>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A56" s="10" t="s">
+        <v>314</v>
+      </c>
+      <c r="B56" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A57" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="B57" t="s">
         <v>98</v>
       </c>
-      <c r="F29" s="5">
+      <c r="F57" s="5">
         <v>1809596</v>
       </c>
-      <c r="G29" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="14" t="s">
-        <v>205</v>
-      </c>
-      <c r="B30" t="s">
-        <v>131</v>
-      </c>
-      <c r="F30" s="5">
+      <c r="G57" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A58" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F58" s="5">
         <v>1809303</v>
       </c>
-      <c r="G30" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="14" t="s">
-        <v>206</v>
-      </c>
-      <c r="B31" s="2" t="s">
+      <c r="G58" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A59" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F31" s="5">
+      <c r="F59" s="5">
         <v>1809300</v>
       </c>
-      <c r="G31" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
+      <c r="G59" t="s">
         <v>223</v>
       </c>
-      <c r="B32" t="s">
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A60" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="B60" t="s">
         <v>83</v>
       </c>
-      <c r="F32" s="5">
+      <c r="F60" s="5">
         <v>9556915</v>
       </c>
-      <c r="G32" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="B33" t="s">
-        <v>336</v>
-      </c>
-      <c r="F33" s="5"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="10" t="s">
-        <v>223</v>
-      </c>
-      <c r="B34" t="s">
-        <v>336</v>
-      </c>
-      <c r="F34" s="5"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4" t="s">
-        <v>382</v>
-      </c>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="B37" t="s">
-        <v>40</v>
-      </c>
-      <c r="C37" t="s">
-        <v>236</v>
-      </c>
-      <c r="F37" s="5">
-        <v>9334084</v>
-      </c>
-      <c r="G37" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="B38" t="s">
-        <v>127</v>
-      </c>
-      <c r="F38" s="5">
-        <v>1686068</v>
-      </c>
-      <c r="G38" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="9"/>
-      <c r="F39" s="9" t="s">
-        <v>321</v>
-      </c>
-      <c r="K39" s="9" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="B40" t="s">
-        <v>175</v>
-      </c>
-      <c r="F40" s="5">
-        <v>1775617</v>
-      </c>
-      <c r="G40" t="s">
-        <v>193</v>
-      </c>
-      <c r="K40" s="5">
-        <v>1017798</v>
-      </c>
-      <c r="L40" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="10" t="s">
-        <v>210</v>
-      </c>
-      <c r="B41" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="B42" t="s">
-        <v>98</v>
-      </c>
-      <c r="F42" s="5">
-        <v>1809596</v>
-      </c>
-      <c r="G42" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="14" t="s">
-        <v>211</v>
-      </c>
-      <c r="B43" t="s">
-        <v>131</v>
-      </c>
-      <c r="F43" s="5">
-        <v>1809303</v>
-      </c>
-      <c r="G43" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="14" t="s">
-        <v>212</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="F44" s="5">
-        <v>1809300</v>
-      </c>
-      <c r="G44" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="B45" t="s">
-        <v>83</v>
-      </c>
-      <c r="F45" s="5">
-        <v>9556915</v>
-      </c>
-      <c r="G45" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="B46" t="s">
-        <v>336</v>
-      </c>
-      <c r="F46" s="5"/>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="B47" t="s">
-        <v>336</v>
-      </c>
-      <c r="F47" s="5"/>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25"/>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4"/>
-      <c r="G49" s="4"/>
-      <c r="H49" s="4"/>
-      <c r="I49" s="4" t="s">
-        <v>383</v>
-      </c>
-      <c r="J49" s="4"/>
-      <c r="K49" s="4"/>
-      <c r="L49" s="4"/>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A50" s="9" t="s">
-        <v>213</v>
-      </c>
-      <c r="B50" t="s">
-        <v>40</v>
-      </c>
-      <c r="C50" t="s">
-        <v>236</v>
-      </c>
-      <c r="F50" s="5">
-        <v>9334084</v>
-      </c>
-      <c r="G50" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="B51" t="s">
-        <v>127</v>
-      </c>
-      <c r="F51" s="5">
-        <v>1686068</v>
-      </c>
-      <c r="G51" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A52" s="9"/>
-      <c r="F52" s="9" t="s">
-        <v>321</v>
-      </c>
-      <c r="K52" s="9" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A53" s="9" t="s">
-        <v>215</v>
-      </c>
-      <c r="B53" t="s">
-        <v>175</v>
-      </c>
-      <c r="F53" s="5">
-        <v>1775617</v>
-      </c>
-      <c r="G53" t="s">
-        <v>193</v>
-      </c>
-      <c r="K53" s="5">
-        <v>1017798</v>
-      </c>
-      <c r="L53" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A54" s="10" t="s">
-        <v>316</v>
-      </c>
-      <c r="B54" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A55" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="B55" t="s">
-        <v>98</v>
-      </c>
-      <c r="F55" s="5">
-        <v>1809596</v>
-      </c>
-      <c r="G55" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A56" s="14" t="s">
+      <c r="G60" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A61" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="B56" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="F56" s="5">
-        <v>1809303</v>
-      </c>
-      <c r="G56" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A57" s="14" t="s">
+      <c r="B61" t="s">
+        <v>334</v>
+      </c>
+      <c r="F61" s="5"/>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A62" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="B57" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="F57" s="5">
-        <v>1809300</v>
-      </c>
-      <c r="G57" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A58" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="B58" t="s">
-        <v>83</v>
-      </c>
-      <c r="F58" s="5">
-        <v>9556915</v>
-      </c>
-      <c r="G58" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A59" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="B59" t="s">
-        <v>336</v>
-      </c>
-      <c r="F59" s="5"/>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A60" s="10" t="s">
-        <v>219</v>
-      </c>
-      <c r="B60" t="s">
-        <v>336</v>
-      </c>
-      <c r="F60" s="5"/>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="63" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
+      <c r="B62" t="s">
+        <v>334</v>
+      </c>
+      <c r="F62" s="5"/>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="1:14" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="65" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="66" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="67" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="68" x14ac:dyDescent="0.25"/>
+    <row r="68" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="69" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="70" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F17" r:id="rId1" display="http://nz.element14.com/koa/rk73z2attd/resistor-0805-0-ohm-jumper/dp/1809596"/>
-    <hyperlink ref="F29" r:id="rId2" display="http://nz.element14.com/koa/rk73z2attd/resistor-0805-0-ohm-jumper/dp/1809596"/>
-    <hyperlink ref="F42" r:id="rId3" display="http://nz.element14.com/koa/rk73z2attd/resistor-0805-0-ohm-jumper/dp/1809596"/>
-    <hyperlink ref="F55" r:id="rId4" display="http://nz.element14.com/koa/rk73z2attd/resistor-0805-0-ohm-jumper/dp/1809596"/>
-    <hyperlink ref="F50" r:id="rId5" display="http://nz.element14.com/multicomp/mc-0-1w-0805-5-2k/resistor-0805-2k/dp/9334084"/>
-    <hyperlink ref="F37" r:id="rId6" display="http://nz.element14.com/multicomp/mc-0-1w-0805-5-2k/resistor-0805-2k/dp/9334084"/>
-    <hyperlink ref="F25" r:id="rId7" display="http://nz.element14.com/multicomp/mc-0-1w-0805-5-2k/resistor-0805-2k/dp/9334084"/>
+    <hyperlink ref="F18" r:id="rId1" display="http://nz.element14.com/koa/rk73z2attd/resistor-0805-0-ohm-jumper/dp/1809596"/>
+    <hyperlink ref="F31" r:id="rId2" display="http://nz.element14.com/koa/rk73z2attd/resistor-0805-0-ohm-jumper/dp/1809596"/>
+    <hyperlink ref="F44" r:id="rId3" display="http://nz.element14.com/koa/rk73z2attd/resistor-0805-0-ohm-jumper/dp/1809596"/>
+    <hyperlink ref="F57" r:id="rId4" display="http://nz.element14.com/koa/rk73z2attd/resistor-0805-0-ohm-jumper/dp/1809596"/>
+    <hyperlink ref="F52" r:id="rId5" display="http://nz.element14.com/multicomp/mc-0-1w-0805-5-2k/resistor-0805-2k/dp/9334084"/>
+    <hyperlink ref="F39" r:id="rId6" display="http://nz.element14.com/multicomp/mc-0-1w-0805-5-2k/resistor-0805-2k/dp/9334084"/>
+    <hyperlink ref="F26" r:id="rId7" display="http://nz.element14.com/multicomp/mc-0-1w-0805-5-2k/resistor-0805-2k/dp/9334084"/>
     <hyperlink ref="F13" r:id="rId8" display="http://nz.element14.com/multicomp/mc-0-1w-0805-5-2k/resistor-0805-2k/dp/9334084"/>
     <hyperlink ref="F14" r:id="rId9" display="http://nz.element14.com/kingbright/kphcm-2012seck/led-smd-0805-orange/dp/1686068"/>
-    <hyperlink ref="F26" r:id="rId10" display="http://nz.element14.com/kingbright/kphcm-2012seck/led-smd-0805-orange/dp/1686068"/>
-    <hyperlink ref="F38" r:id="rId11" display="http://nz.element14.com/kingbright/kphcm-2012seck/led-smd-0805-orange/dp/1686068"/>
-    <hyperlink ref="F51" r:id="rId12" display="http://nz.element14.com/kingbright/kphcm-2012seck/led-smd-0805-orange/dp/1686068"/>
-    <hyperlink ref="F56" r:id="rId13" display="http://nz.element14.com/koa/rk73b2attd104j/resistor-0805-100k-ohm-5/dp/1809303"/>
-    <hyperlink ref="F43" r:id="rId14" display="http://nz.element14.com/koa/rk73b2attd104j/resistor-0805-100k-ohm-5/dp/1809303"/>
-    <hyperlink ref="F30" r:id="rId15" display="http://nz.element14.com/koa/rk73b2attd104j/resistor-0805-100k-ohm-5/dp/1809303"/>
-    <hyperlink ref="F18" r:id="rId16" display="http://nz.element14.com/koa/rk73b2attd104j/resistor-0805-100k-ohm-5/dp/1809303"/>
-    <hyperlink ref="F27" r:id="rId17" display="http://nz.element14.com/fairchild-semiconductor/rfp30n06le/mosfet-n-logic-to-220/dp/1017798"/>
-    <hyperlink ref="F53" r:id="rId18" display="http://nz.element14.com/infineon/ipp037n08n3-g/mosfet-n-ch-100a-80v-pg-to220-3/dp/1775617"/>
-    <hyperlink ref="K53" r:id="rId19" display="http://nz.element14.com/fairchild-semiconductor/rfp30n06le/mosfet-n-logic-to-220/dp/1017798"/>
-    <hyperlink ref="F40" r:id="rId20" display="http://nz.element14.com/infineon/ipp037n08n3-g/mosfet-n-ch-100a-80v-pg-to220-3/dp/1775617"/>
-    <hyperlink ref="K40" r:id="rId21" display="http://nz.element14.com/fairchild-semiconductor/rfp30n06le/mosfet-n-logic-to-220/dp/1017798"/>
-    <hyperlink ref="F15" r:id="rId22" display="http://nz.element14.com/fairchild-semiconductor/rfp30n06le/mosfet-n-logic-to-220/dp/1017798"/>
-    <hyperlink ref="F9" r:id="rId23" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
-    <hyperlink ref="F7" r:id="rId24" display="http://nz.element14.com/koa/rk73b2attd103j/resistor-0805-10k-ohm-5/dp/1809302"/>
-    <hyperlink ref="F8" r:id="rId25" display="http://nz.element14.com/koa/rk73b2attd103j/resistor-0805-10k-ohm-5/dp/1809302"/>
-    <hyperlink ref="F10" r:id="rId26" display="http://nz.element14.com/texas-instruments/sn74ls86ad/logic-quad-2-in-ex-or-gate-14soic/dp/1740035?Ntt=74ls86"/>
-    <hyperlink ref="F19" r:id="rId27" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
-    <hyperlink ref="F31" r:id="rId28" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
-    <hyperlink ref="F44" r:id="rId29" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
-    <hyperlink ref="F57" r:id="rId30" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
-    <hyperlink ref="F3" r:id="rId31" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
-    <hyperlink ref="F4" r:id="rId32" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
-    <hyperlink ref="F5" r:id="rId33" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
-    <hyperlink ref="F6" r:id="rId34" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
-    <hyperlink ref="F20" r:id="rId35" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
-    <hyperlink ref="F32" r:id="rId36" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
-    <hyperlink ref="F45" r:id="rId37" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
-    <hyperlink ref="F58" r:id="rId38" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
+    <hyperlink ref="F27" r:id="rId10" display="http://nz.element14.com/kingbright/kphcm-2012seck/led-smd-0805-orange/dp/1686068"/>
+    <hyperlink ref="F40" r:id="rId11" display="http://nz.element14.com/kingbright/kphcm-2012seck/led-smd-0805-orange/dp/1686068"/>
+    <hyperlink ref="F53" r:id="rId12" display="http://nz.element14.com/kingbright/kphcm-2012seck/led-smd-0805-orange/dp/1686068"/>
+    <hyperlink ref="F58" r:id="rId13" display="http://nz.element14.com/koa/rk73b2attd104j/resistor-0805-100k-ohm-5/dp/1809303"/>
+    <hyperlink ref="F45" r:id="rId14" display="http://nz.element14.com/koa/rk73b2attd104j/resistor-0805-100k-ohm-5/dp/1809303"/>
+    <hyperlink ref="F32" r:id="rId15" display="http://nz.element14.com/koa/rk73b2attd104j/resistor-0805-100k-ohm-5/dp/1809303"/>
+    <hyperlink ref="F19" r:id="rId16" display="http://nz.element14.com/koa/rk73b2attd104j/resistor-0805-100k-ohm-5/dp/1809303"/>
+    <hyperlink ref="F9" r:id="rId17" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
+    <hyperlink ref="F7" r:id="rId18" display="http://nz.element14.com/koa/rk73b2attd103j/resistor-0805-10k-ohm-5/dp/1809302"/>
+    <hyperlink ref="F8" r:id="rId19" display="http://nz.element14.com/koa/rk73b2attd103j/resistor-0805-10k-ohm-5/dp/1809302"/>
+    <hyperlink ref="F10" r:id="rId20" display="http://nz.element14.com/texas-instruments/sn74ls86ad/logic-quad-2-in-ex-or-gate-14soic/dp/1740035?Ntt=74ls86"/>
+    <hyperlink ref="F20" r:id="rId21" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
+    <hyperlink ref="F33" r:id="rId22" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
+    <hyperlink ref="F46" r:id="rId23" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
+    <hyperlink ref="F59" r:id="rId24" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
+    <hyperlink ref="F3" r:id="rId25" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
+    <hyperlink ref="F4" r:id="rId26" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
+    <hyperlink ref="F5" r:id="rId27" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
+    <hyperlink ref="F6" r:id="rId28" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
+    <hyperlink ref="F21" r:id="rId29" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
+    <hyperlink ref="F34" r:id="rId30" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
+    <hyperlink ref="F47" r:id="rId31" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
+    <hyperlink ref="F60" r:id="rId32" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
+    <hyperlink ref="F42" r:id="rId33" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
+    <hyperlink ref="P42" r:id="rId34" tooltip="Click to view additional information on this product." display="http://nz.mouser.com/ProductDetail/STMicroelectronics/VNP14NV04-E/?qs=sGAEpiMZZMuCmTIBzycWfOPiiwtMaP0Fv4CVvoRPcP8%3d"/>
+    <hyperlink ref="K42" r:id="rId35" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
+    <hyperlink ref="F29" r:id="rId36" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
+    <hyperlink ref="K29" r:id="rId37" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
+    <hyperlink ref="F16" r:id="rId38" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
+    <hyperlink ref="K16" r:id="rId39" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
+    <hyperlink ref="F55" r:id="rId40" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
+    <hyperlink ref="K55" r:id="rId41" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId39"/>
+  <pageSetup orientation="portrait" r:id="rId42"/>
 </worksheet>
 </file>
 
@@ -4374,7 +4494,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -4391,7 +4511,7 @@
         <v>1887296</v>
       </c>
       <c r="G3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -4405,7 +4525,7 @@
         <v>1506077</v>
       </c>
       <c r="G4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -4419,7 +4539,7 @@
         <v>1809596</v>
       </c>
       <c r="G5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -4433,7 +4553,7 @@
         <v>8820120</v>
       </c>
       <c r="G6" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="I6" s="5"/>
     </row>
@@ -4448,7 +4568,7 @@
         <v>9556915</v>
       </c>
       <c r="G7" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -4462,7 +4582,7 @@
         <v>9556915</v>
       </c>
       <c r="G8" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -4477,7 +4597,7 @@
         <v>1809376</v>
       </c>
       <c r="G9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25"/>
@@ -4520,7 +4640,7 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -4530,7 +4650,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4" t="s">
-        <v>360</v>
+        <v>380</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -4547,13 +4667,13 @@
         <v>1457153</v>
       </c>
       <c r="G3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -4567,7 +4687,7 @@
         <v>8820120</v>
       </c>
       <c r="G4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -4581,7 +4701,7 @@
         <v>1759199</v>
       </c>
       <c r="G5" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -4595,7 +4715,7 @@
         <v>1759172</v>
       </c>
       <c r="G6" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -4609,7 +4729,7 @@
         <v>1809376</v>
       </c>
       <c r="G7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -4623,7 +4743,7 @@
         <v>1809596</v>
       </c>
       <c r="G8" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -4637,7 +4757,7 @@
         <v>1809596</v>
       </c>
       <c r="G9" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -4691,7 +4811,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -4703,7 +4823,7 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>100</v>
+        <v>382</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -4713,7 +4833,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4" t="s">
-        <v>362</v>
+        <v>381</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -4721,27 +4841,27 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F3" s="5">
         <v>1555602</v>
       </c>
       <c r="G3" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="J3" s="5">
         <v>1703477</v>
       </c>
       <c r="K3" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B4" t="s">
         <v>22</v>
@@ -4750,12 +4870,12 @@
         <v>8820120</v>
       </c>
       <c r="G4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B5" t="s">
         <v>90</v>
@@ -4764,12 +4884,12 @@
         <v>1759199</v>
       </c>
       <c r="G5" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B6" t="s">
         <v>99</v>
@@ -4778,7 +4898,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B7" t="s">
         <v>50</v>
@@ -4787,12 +4907,12 @@
         <v>1809376</v>
       </c>
       <c r="G7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B8" t="s">
         <v>91</v>
@@ -4801,12 +4921,12 @@
         <v>1759172</v>
       </c>
       <c r="G8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B9" t="s">
         <v>99</v>
@@ -4814,7 +4934,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B10" t="s">
         <v>99</v>
@@ -4822,7 +4942,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B11" t="s">
         <v>98</v>
@@ -4831,7 +4951,7 @@
         <v>1809596</v>
       </c>
       <c r="G11" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25"/>
@@ -4876,7 +4996,7 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -4886,7 +5006,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -4894,31 +5014,31 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="12">
         <v>1845719</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="8" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="L3" s="8"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -4927,12 +5047,12 @@
         <v>1809302</v>
       </c>
       <c r="G4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B5" t="s">
         <v>22</v>
@@ -4941,61 +5061,61 @@
         <v>8820120</v>
       </c>
       <c r="G5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F6" s="5">
         <v>1414659</v>
       </c>
       <c r="G6" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F7" s="5">
         <v>1618242</v>
       </c>
       <c r="G7" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F8" s="5">
         <v>1618242</v>
       </c>
       <c r="G8" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -5005,7 +5125,7 @@
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
@@ -5013,31 +5133,31 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="12">
         <v>1845719</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="8" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="L11" s="8"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
@@ -5046,12 +5166,12 @@
         <v>1809302</v>
       </c>
       <c r="G12" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B13" t="s">
         <v>22</v>
@@ -5060,55 +5180,55 @@
         <v>8820120</v>
       </c>
       <c r="G13" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F14" s="5">
         <v>1414659</v>
       </c>
       <c r="G14" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B15" t="s">
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F15" s="5">
         <v>1618242</v>
       </c>
       <c r="G15" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B16" t="s">
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F16" s="5">
         <v>1618242</v>
       </c>
       <c r="G16" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="17" x14ac:dyDescent="0.25"/>
@@ -5157,7 +5277,7 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -5173,70 +5293,70 @@
     </row>
     <row r="3" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C3"/>
       <c r="F3" s="5">
         <v>1017798</v>
       </c>
       <c r="G3" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F4" s="5">
         <v>1465996</v>
       </c>
       <c r="G4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F5" s="5">
         <v>1809376</v>
       </c>
       <c r="G5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F6" s="5">
         <v>1809303</v>
       </c>
       <c r="G6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B7" t="s">
         <v>77</v>
@@ -5245,12 +5365,12 @@
         <v>1809300</v>
       </c>
       <c r="G7" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B8" t="s">
         <v>99</v>
@@ -5258,7 +5378,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B9" t="s">
         <v>99</v>
@@ -5305,7 +5425,7 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -5315,7 +5435,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -5323,7 +5443,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B3" t="s">
         <v>22</v>
@@ -5332,12 +5452,12 @@
         <v>8820120</v>
       </c>
       <c r="G3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B4" t="s">
         <v>50</v>
@@ -5346,12 +5466,12 @@
         <v>1809376</v>
       </c>
       <c r="G4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B5" t="s">
         <v>22</v>
@@ -5360,40 +5480,40 @@
         <v>8820120</v>
       </c>
       <c r="G5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B6" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="F6" s="5">
         <v>1809596</v>
       </c>
       <c r="G6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B7" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="F7" s="5">
         <v>1809596</v>
       </c>
       <c r="G7" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B8" t="s">
         <v>83</v>
@@ -5402,12 +5522,12 @@
         <v>9556915</v>
       </c>
       <c r="G8" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B9" t="s">
         <v>83</v>
@@ -5416,26 +5536,26 @@
         <v>9556915</v>
       </c>
       <c r="G9" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F10" s="5">
         <v>1887290</v>
       </c>
       <c r="G10" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B11" t="s">
         <v>99</v>
@@ -5443,7 +5563,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B12" t="s">
         <v>99</v>
@@ -5451,7 +5571,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B13" t="s">
         <v>99</v>
@@ -5502,7 +5622,7 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -5512,7 +5632,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -5520,7 +5640,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B3" t="s">
         <v>22</v>
@@ -5529,12 +5649,12 @@
         <v>8820120</v>
       </c>
       <c r="G3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B4" t="s">
         <v>50</v>
@@ -5543,12 +5663,12 @@
         <v>1809376</v>
       </c>
       <c r="G4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B5" t="s">
         <v>22</v>
@@ -5557,40 +5677,40 @@
         <v>8820120</v>
       </c>
       <c r="G5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B6" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="F6" s="5">
         <v>1809596</v>
       </c>
       <c r="G6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B7" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="F7" s="5">
         <v>1809596</v>
       </c>
       <c r="G7" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B8" t="s">
         <v>83</v>
@@ -5599,12 +5719,12 @@
         <v>9556915</v>
       </c>
       <c r="G8" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B9" t="s">
         <v>83</v>
@@ -5613,26 +5733,26 @@
         <v>9556915</v>
       </c>
       <c r="G9" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F10" s="5">
         <v>1887290</v>
       </c>
       <c r="G10" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B11" t="s">
         <v>99</v>
@@ -5640,7 +5760,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B12" t="s">
         <v>99</v>
@@ -5648,7 +5768,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B13" t="s">
         <v>99</v>
@@ -5700,7 +5820,7 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -5710,7 +5830,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -5718,7 +5838,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B3" t="s">
         <v>22</v>
@@ -5727,12 +5847,12 @@
         <v>8820120</v>
       </c>
       <c r="G3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B4" t="s">
         <v>50</v>
@@ -5741,12 +5861,12 @@
         <v>1809376</v>
       </c>
       <c r="G4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B5" t="s">
         <v>22</v>
@@ -5755,40 +5875,40 @@
         <v>8820120</v>
       </c>
       <c r="G5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B6" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="F6" s="5">
         <v>1809596</v>
       </c>
       <c r="G6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B7" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="F7" s="5">
         <v>1809596</v>
       </c>
       <c r="G7" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B8" t="s">
         <v>83</v>
@@ -5797,12 +5917,12 @@
         <v>9556915</v>
       </c>
       <c r="G8" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B9" t="s">
         <v>83</v>
@@ -5811,26 +5931,26 @@
         <v>9556915</v>
       </c>
       <c r="G9" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F10" s="5">
         <v>1887290</v>
       </c>
       <c r="G10" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B11" t="s">
         <v>99</v>
@@ -5838,7 +5958,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B12" t="s">
         <v>99</v>
@@ -5846,7 +5966,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B13" t="s">
         <v>99</v>

</xml_diff>

<commit_message>
Added Off board sensor options, upated changed component value colours.
</commit_message>
<xml_diff>
--- a/PumaBom-WithMods-Element14.xlsx
+++ b/PumaBom-WithMods-Element14.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="0" windowWidth="19155" windowHeight="5160" tabRatio="710" activeTab="10"/>
+    <workbookView xWindow="30" yWindow="0" windowWidth="19155" windowHeight="5160" tabRatio="710"/>
   </bookViews>
   <sheets>
     <sheet name="Primary Puma Parts" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="389">
   <si>
     <t>MCU</t>
   </si>
@@ -1187,6 +1187,12 @@
   </si>
   <si>
     <t>RS components VNP10N07 Omnifet</t>
+  </si>
+  <si>
+    <t>Off Board Manifold Air Pressure (Use this and NOT the above if you plan on having off board MAP sensor : ie OEM MAP)</t>
+  </si>
+  <si>
+    <t>Atmospheric Absolute Pressure (Use this and NOT the above you plan on having off board AAP sensor : ie OEM AAP)</t>
   </si>
 </sst>
 </file>
@@ -1224,7 +1230,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1273,6 +1279,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1302,7 +1320,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1331,6 +1349,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1638,8 +1662,8 @@
   </sheetPr>
   <dimension ref="A1:L74"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J53" sqref="J53"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -2629,8 +2653,8 @@
   </sheetPr>
   <dimension ref="A1:O69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -2786,7 +2810,7 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="16" t="s">
         <v>265</v>
       </c>
       <c r="B12" t="s">
@@ -2896,7 +2920,7 @@
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="16" t="s">
         <v>272</v>
       </c>
       <c r="B20" t="s">
@@ -3006,7 +3030,7 @@
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="16" t="s">
         <v>277</v>
       </c>
       <c r="B28" t="s">
@@ -3116,7 +3140,7 @@
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="A36" s="16" t="s">
         <v>288</v>
       </c>
       <c r="B36" t="s">
@@ -3226,7 +3250,7 @@
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="A44" s="16" t="s">
         <v>293</v>
       </c>
       <c r="B44" t="s">
@@ -3336,7 +3360,7 @@
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="A52" s="16" t="s">
         <v>308</v>
       </c>
       <c r="B52" t="s">
@@ -3455,7 +3479,7 @@
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+      <c r="A60" s="16" t="s">
         <v>309</v>
       </c>
       <c r="B60" t="s">
@@ -3589,7 +3613,7 @@
   </sheetPr>
   <dimension ref="A1:R70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
@@ -4625,10 +4649,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -4675,6 +4699,7 @@
       <c r="K3" s="11" t="s">
         <v>249</v>
       </c>
+      <c r="L3" s="8"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
@@ -4784,10 +4809,225 @@
         <v>99</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
+    </row>
+    <row r="14" spans="1:12" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="24" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="29">
+        <v>1457153</v>
+      </c>
+      <c r="G15" s="28" t="s">
+        <v>197</v>
+      </c>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="K15" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="L15" s="8"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="29">
+        <v>8820120</v>
+      </c>
+      <c r="G16" s="28" t="s">
+        <v>232</v>
+      </c>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="29">
+        <v>1759199</v>
+      </c>
+      <c r="G17" s="28" t="s">
+        <v>236</v>
+      </c>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="29">
+        <v>1759172</v>
+      </c>
+      <c r="G18" s="28" t="s">
+        <v>237</v>
+      </c>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="29">
+        <v>1809376</v>
+      </c>
+      <c r="G19" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="28"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="29">
+        <v>1809596</v>
+      </c>
+      <c r="G20" s="28" t="s">
+        <v>222</v>
+      </c>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="28"/>
+      <c r="L20" s="28"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="29">
+        <v>1809596</v>
+      </c>
+      <c r="G21" s="28" t="s">
+        <v>222</v>
+      </c>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="28"/>
+      <c r="L21" s="28"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="28"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="28"/>
+      <c r="J22" s="28"/>
+      <c r="K22" s="28"/>
+      <c r="L22" s="28"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
+      <c r="I23" s="28"/>
+      <c r="J23" s="28"/>
+      <c r="K23" s="28"/>
+      <c r="L23" s="28"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="28"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="28"/>
+      <c r="L24" s="28"/>
+    </row>
+    <row r="25" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1" display="http://nz.element14.com/freescale-semiconductor/mpx4250ap/ic-sensor-abs-press-36-3-psi/dp/1457153"/>
@@ -4798,6 +5038,14 @@
     <hyperlink ref="F5" r:id="rId6" display="http://nz.element14.com/multicomp/mcca000326/mlcc-0805-np0-50v-47pf/dp/1759199"/>
     <hyperlink ref="F6" r:id="rId7" display="http://nz.element14.com/multicomp/mcca000301/mlcc-0805-x7r-25v-220nf/dp/1759172"/>
     <hyperlink ref="K3" r:id="rId8" tooltip="Click to view additional information on this product." display="http://nz.mouser.com/ProductDetail/Freescale-Semiconductor/MPX4250AP/?qs=sGAEpiMZZMvhQj7WZhFIALpLlyV3lh9LDMe%2fRQPZbUw%3d"/>
+    <hyperlink ref="F15" r:id="rId9" display="http://nz.element14.com/freescale-semiconductor/mpx4250ap/ic-sensor-abs-press-36-3-psi/dp/1457153"/>
+    <hyperlink ref="F19" r:id="rId10" display="http://nz.element14.com/koa/rk73b2attd471j/resistor-0805-470-ohm-5/dp/1809376"/>
+    <hyperlink ref="F20" r:id="rId11" display="http://nz.element14.com/koa/rk73z2attd/resistor-0805-0-ohm-jumper/dp/1809596"/>
+    <hyperlink ref="F21" r:id="rId12" display="http://nz.element14.com/koa/rk73z2attd/resistor-0805-0-ohm-jumper/dp/1809596"/>
+    <hyperlink ref="F16" r:id="rId13" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
+    <hyperlink ref="F17" r:id="rId14" display="http://nz.element14.com/multicomp/mcca000326/mlcc-0805-np0-50v-47pf/dp/1759199"/>
+    <hyperlink ref="F18" r:id="rId15" display="http://nz.element14.com/multicomp/mcca000301/mlcc-0805-x7r-25v-220nf/dp/1759172"/>
+    <hyperlink ref="K15" r:id="rId16" tooltip="Click to view additional information on this product." display="http://nz.mouser.com/ProductDetail/Freescale-Semiconductor/MPX4250AP/?qs=sGAEpiMZZMvhQj7WZhFIALpLlyV3lh9LDMe%2fRQPZbUw%3d"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4808,10 +5056,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -4852,12 +5100,13 @@
       <c r="G3" t="s">
         <v>336</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="11">
         <v>1703477</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="8" t="s">
         <v>335</v>
       </c>
+      <c r="L3" s="8"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
@@ -4954,11 +5203,225 @@
         <v>222</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:12" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="24" t="s">
+        <v>388</v>
+      </c>
+      <c r="F14" s="26"/>
+    </row>
+    <row r="15" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="29">
+        <v>1555602</v>
+      </c>
+      <c r="G15" s="28" t="s">
+        <v>336</v>
+      </c>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="11">
+        <v>1703477</v>
+      </c>
+      <c r="K15" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="L15" s="8"/>
+    </row>
+    <row r="16" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="29">
+        <v>8820120</v>
+      </c>
+      <c r="G16" s="28" t="s">
+        <v>232</v>
+      </c>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
+    </row>
+    <row r="17" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="B17" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="29">
+        <v>1759199</v>
+      </c>
+      <c r="G17" s="28" t="s">
+        <v>236</v>
+      </c>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+    </row>
+    <row r="18" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="B18" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+    </row>
+    <row r="19" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="29">
+        <v>1809376</v>
+      </c>
+      <c r="G19" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="28"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="29">
+        <v>1759172</v>
+      </c>
+      <c r="G20" s="28" t="s">
+        <v>237</v>
+      </c>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="28"/>
+      <c r="L20" s="28"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="B21" s="28"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="28"/>
+      <c r="L21" s="28"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="B22" s="28"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="28"/>
+      <c r="J22" s="28"/>
+      <c r="K22" s="28"/>
+      <c r="L22" s="28"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="B23" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="29">
+        <v>1809596</v>
+      </c>
+      <c r="G23" s="28" t="s">
+        <v>222</v>
+      </c>
+      <c r="H23" s="28"/>
+      <c r="I23" s="28"/>
+      <c r="J23" s="28"/>
+      <c r="K23" s="28"/>
+      <c r="L23" s="28"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="27"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="28"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="28"/>
+      <c r="L24" s="28"/>
+    </row>
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1" display="http://nz.element14.com/freescale-semiconductor/mpx4100a/ic-pressure-sensor/dp/1555602"/>
@@ -4968,9 +5431,16 @@
     <hyperlink ref="F5" r:id="rId5" display="http://nz.element14.com/multicomp/mcca000326/mlcc-0805-np0-50v-47pf/dp/1759199"/>
     <hyperlink ref="F8" r:id="rId6" display="http://nz.element14.com/multicomp/mcca000301/mlcc-0805-x7r-25v-220nf/dp/1759172"/>
     <hyperlink ref="J3" r:id="rId7" display="http://nz.element14.com/freescale-semiconductor/mpx4100as/ic-pressure-sensor-6-867e/dp/1703477"/>
+    <hyperlink ref="F15" r:id="rId8" display="http://nz.element14.com/freescale-semiconductor/mpx4100a/ic-pressure-sensor/dp/1555602"/>
+    <hyperlink ref="F19" r:id="rId9" display="http://nz.element14.com/koa/rk73b2attd471j/resistor-0805-470-ohm-5/dp/1809376"/>
+    <hyperlink ref="F23" r:id="rId10" display="http://nz.element14.com/koa/rk73z2attd/resistor-0805-0-ohm-jumper/dp/1809596"/>
+    <hyperlink ref="F16" r:id="rId11" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
+    <hyperlink ref="F17" r:id="rId12" display="http://nz.element14.com/multicomp/mcca000326/mlcc-0805-np0-50v-47pf/dp/1759199"/>
+    <hyperlink ref="F20" r:id="rId13" display="http://nz.element14.com/multicomp/mcca000301/mlcc-0805-x7r-25v-220nf/dp/1759172"/>
+    <hyperlink ref="J15" r:id="rId14" display="http://nz.element14.com/freescale-semiconductor/mpx4100as/ic-pressure-sensor-6-867e/dp/1703477"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add components to MAP and AAP, corrected errors to page numbers, corrected component references on MAP, AAP and updated components attached to MCU
</commit_message>
<xml_diff>
--- a/PumaBom-WithMods-Element14.xlsx
+++ b/PumaBom-WithMods-Element14.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="390">
   <si>
     <t>MCU</t>
   </si>
@@ -1168,12 +1168,6 @@
     <t>Schematic pages: 1, 38, 39</t>
   </si>
   <si>
-    <t>Schematic pages: 1, 24, 44</t>
-  </si>
-  <si>
-    <t>Schematic pages: 1, 47, 43</t>
-  </si>
-  <si>
     <t>Atmospheric Absolute Pressure</t>
   </si>
   <si>
@@ -1193,6 +1187,15 @@
   </si>
   <si>
     <t>Atmospheric Absolute Pressure (Use this and NOT the above you plan on having off board AAP sensor : ie OEM AAP)</t>
+  </si>
+  <si>
+    <t>Schotty</t>
+  </si>
+  <si>
+    <t>Schematic pages: 1, 44, 47</t>
+  </si>
+  <si>
+    <t>Schematic pages: 1, 43, 47</t>
   </si>
 </sst>
 </file>
@@ -1343,18 +1346,18 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1662,9 +1665,7 @@
   </sheetPr>
   <dimension ref="A1:L74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1687,24 +1688,24 @@
       <c r="D2" t="s">
         <v>256</v>
       </c>
-      <c r="H2" s="23" t="s">
+      <c r="H2" s="29" t="s">
         <v>320</v>
       </c>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C3" s="20"/>
       <c r="D3" t="s">
         <v>257</v>
       </c>
-      <c r="H3" s="22" t="s">
+      <c r="H3" s="28" t="s">
         <v>321</v>
       </c>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C4" s="21"/>
@@ -1755,10 +1756,10 @@
         <v>3</v>
       </c>
       <c r="F8" s="5">
-        <v>1809302</v>
+        <v>1652909</v>
       </c>
       <c r="G8" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1769,10 +1770,10 @@
         <v>3</v>
       </c>
       <c r="F9" s="5">
-        <v>1809302</v>
+        <v>1652909</v>
       </c>
       <c r="G9" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1783,10 +1784,10 @@
         <v>3</v>
       </c>
       <c r="F10" s="5">
-        <v>1809302</v>
+        <v>1652909</v>
       </c>
       <c r="G10" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1797,10 +1798,10 @@
         <v>3</v>
       </c>
       <c r="F11" s="5">
-        <v>1809302</v>
+        <v>1652909</v>
       </c>
       <c r="G11" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1815,10 +1816,10 @@
       </c>
       <c r="D12" s="16"/>
       <c r="F12" s="5">
-        <v>1809302</v>
+        <v>1652909</v>
       </c>
       <c r="G12" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -2091,7 +2092,7 @@
         <v>9334084</v>
       </c>
       <c r="G33" t="s">
-        <v>187</v>
+        <v>223</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -2161,7 +2162,7 @@
         <v>1809376</v>
       </c>
       <c r="G38" t="s">
-        <v>187</v>
+        <v>223</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -2175,7 +2176,7 @@
         <v>1809376</v>
       </c>
       <c r="G39" t="s">
-        <v>187</v>
+        <v>223</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25"/>
@@ -2495,38 +2496,38 @@
     <hyperlink ref="F55" r:id="rId9" display="http://nz.element14.com/national-semiconductor/lm2937-5-0/ic-v-reg-ldo-5-0v-2937-to-220-3/dp/9486038"/>
     <hyperlink ref="F16" r:id="rId10" display="http://nz.element14.com/multicomp/mcpwr05ftew3901/resistor-0805-3-9k-1-0-125w/dp/1887296"/>
     <hyperlink ref="F43" r:id="rId11" display="http://nz.element14.com/micrel-semiconductor/mic2954-02ws/ic-reg-ldo-250ma-5v-0-5/dp/1556741"/>
-    <hyperlink ref="F8" r:id="rId12" display="http://nz.element14.com/koa/rk73b2attd103j/resistor-0805-10k-ohm-5/dp/1809302"/>
-    <hyperlink ref="F9" r:id="rId13" display="http://nz.element14.com/koa/rk73b2attd103j/resistor-0805-10k-ohm-5/dp/1809302"/>
-    <hyperlink ref="F10" r:id="rId14" display="http://nz.element14.com/koa/rk73b2attd103j/resistor-0805-10k-ohm-5/dp/1809302"/>
-    <hyperlink ref="F11" r:id="rId15" display="http://nz.element14.com/koa/rk73b2attd103j/resistor-0805-10k-ohm-5/dp/1809302"/>
-    <hyperlink ref="F61" r:id="rId16" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
-    <hyperlink ref="F65" r:id="rId17" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
-    <hyperlink ref="F48" r:id="rId18" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
-    <hyperlink ref="F45" r:id="rId19" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
-    <hyperlink ref="F30" r:id="rId20" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
-    <hyperlink ref="F23" r:id="rId21" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
-    <hyperlink ref="F24" r:id="rId22" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
-    <hyperlink ref="F25" r:id="rId23" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
-    <hyperlink ref="F20" r:id="rId24" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
-    <hyperlink ref="F21" r:id="rId25" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
-    <hyperlink ref="F13" r:id="rId26" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
-    <hyperlink ref="F32" r:id="rId27" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
-    <hyperlink ref="F19" r:id="rId28" display="http://nz.element14.com/epson-toyocom/tsx-3225-16mhz-10ppm-9pf/crystal-tsx-3225-16mhz-10ppm-9pf/dp/1712841"/>
-    <hyperlink ref="F14" r:id="rId29" display="http://nz.element14.com/kemet/c0805c331j5gac-tu/capacitor-ceramic-multilayer/dp/1650875"/>
-    <hyperlink ref="F15" r:id="rId30" display="http://nz.element14.com/kemet/c0805c332kcractu/capacitor-0805-3-3nf-500v-x7r/dp/1702127"/>
-    <hyperlink ref="F17" r:id="rId31" display="http://nz.element14.com/kemet/c0805c220j1gactu/capacitor-0805-22pf-100v-np0/dp/1414676"/>
-    <hyperlink ref="F47" r:id="rId32" display="http://nz.element14.com/vishay-sprague/199d106x9035d1v1e3/capacitor-tant-10uf-35v-radial/dp/1617365"/>
-    <hyperlink ref="F60" r:id="rId33" display="http://nz.element14.com/vishay-sprague/199d106x9035d1v1e3/capacitor-tant-10uf-35v-radial/dp/1617365"/>
-    <hyperlink ref="F63" r:id="rId34" display="http://nz.element14.com/kemet/t495d226k035ate300/capacitor-22uf-35v/dp/9229272"/>
-    <hyperlink ref="F44" r:id="rId35" display="http://nz.element14.com/kemet/t495d226k035ate300/capacitor-22uf-35v/dp/9229272"/>
-    <hyperlink ref="F62" r:id="rId36" display="http://nz.element14.com/fairchild-semiconductor/1n4007/bridge-rectifier-rohs-compliant/dp/9109625"/>
-    <hyperlink ref="F64" r:id="rId37" display="http://nz.element14.com/nichicon/upm1e222mhd/capacitor-2200uf-25v/dp/8812519"/>
-    <hyperlink ref="F18" r:id="rId38" display="http://nz.element14.com/te-connectivity-cgs/rh73u2a10mjtd/resistor-0805-10m/dp/1174062"/>
-    <hyperlink ref="F12" r:id="rId39" display="http://nz.element14.com/koa/rk73b2attd103j/resistor-0805-10k-ohm-5/dp/1809302"/>
-    <hyperlink ref="F22" r:id="rId40" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
-    <hyperlink ref="F34" r:id="rId41" display="http://nz.element14.com/multicomp/u0805r103kct/capacitor-0805-10nf-50v/dp/9406352"/>
-    <hyperlink ref="H3" r:id="rId42"/>
-    <hyperlink ref="F46" r:id="rId43" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
+    <hyperlink ref="F61" r:id="rId12" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
+    <hyperlink ref="F65" r:id="rId13" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
+    <hyperlink ref="F48" r:id="rId14" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
+    <hyperlink ref="F45" r:id="rId15" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
+    <hyperlink ref="F30" r:id="rId16" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
+    <hyperlink ref="F23" r:id="rId17" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
+    <hyperlink ref="F24" r:id="rId18" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
+    <hyperlink ref="F25" r:id="rId19" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
+    <hyperlink ref="F20" r:id="rId20" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
+    <hyperlink ref="F21" r:id="rId21" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
+    <hyperlink ref="F13" r:id="rId22" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
+    <hyperlink ref="F32" r:id="rId23" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
+    <hyperlink ref="F19" r:id="rId24" display="http://nz.element14.com/epson-toyocom/tsx-3225-16mhz-10ppm-9pf/crystal-tsx-3225-16mhz-10ppm-9pf/dp/1712841"/>
+    <hyperlink ref="F14" r:id="rId25" display="http://nz.element14.com/kemet/c0805c331j5gac-tu/capacitor-ceramic-multilayer/dp/1650875"/>
+    <hyperlink ref="F15" r:id="rId26" display="http://nz.element14.com/kemet/c0805c332kcractu/capacitor-0805-3-3nf-500v-x7r/dp/1702127"/>
+    <hyperlink ref="F17" r:id="rId27" display="http://nz.element14.com/kemet/c0805c220j1gactu/capacitor-0805-22pf-100v-np0/dp/1414676"/>
+    <hyperlink ref="F47" r:id="rId28" display="http://nz.element14.com/vishay-sprague/199d106x9035d1v1e3/capacitor-tant-10uf-35v-radial/dp/1617365"/>
+    <hyperlink ref="F60" r:id="rId29" display="http://nz.element14.com/vishay-sprague/199d106x9035d1v1e3/capacitor-tant-10uf-35v-radial/dp/1617365"/>
+    <hyperlink ref="F63" r:id="rId30" display="http://nz.element14.com/kemet/t495d226k035ate300/capacitor-22uf-35v/dp/9229272"/>
+    <hyperlink ref="F44" r:id="rId31" display="http://nz.element14.com/kemet/t495d226k035ate300/capacitor-22uf-35v/dp/9229272"/>
+    <hyperlink ref="F62" r:id="rId32" display="http://nz.element14.com/fairchild-semiconductor/1n4007/bridge-rectifier-rohs-compliant/dp/9109625"/>
+    <hyperlink ref="F64" r:id="rId33" display="http://nz.element14.com/nichicon/upm1e222mhd/capacitor-2200uf-25v/dp/8812519"/>
+    <hyperlink ref="F18" r:id="rId34" display="http://nz.element14.com/te-connectivity-cgs/rh73u2a10mjtd/resistor-0805-10m/dp/1174062"/>
+    <hyperlink ref="F22" r:id="rId35" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
+    <hyperlink ref="F34" r:id="rId36" display="http://nz.element14.com/multicomp/u0805r103kct/capacitor-0805-10nf-50v/dp/9406352"/>
+    <hyperlink ref="H3" r:id="rId37"/>
+    <hyperlink ref="F46" r:id="rId38" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
+    <hyperlink ref="F8" r:id="rId39" display="http://nz.element14.com/vishay-draloric/crcw080510k0fkta/thick-film-chip-resistor/dp/1652909"/>
+    <hyperlink ref="F9" r:id="rId40" display="http://nz.element14.com/vishay-draloric/crcw080510k0fkta/thick-film-chip-resistor/dp/1652909"/>
+    <hyperlink ref="F10" r:id="rId41" display="http://nz.element14.com/vishay-draloric/crcw080510k0fkta/thick-film-chip-resistor/dp/1652909"/>
+    <hyperlink ref="F11" r:id="rId42" display="http://nz.element14.com/vishay-draloric/crcw080510k0fkta/thick-film-chip-resistor/dp/1652909"/>
+    <hyperlink ref="F12" r:id="rId43" display="http://nz.element14.com/vishay-draloric/crcw080510k0fkta/thick-film-chip-resistor/dp/1652909"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId44"/>
@@ -2653,9 +2654,7 @@
   </sheetPr>
   <dimension ref="A1:O69"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2751,19 +2750,19 @@
         <v>162</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="G7" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="M7" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="O7" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -2796,7 +2795,7 @@
       <c r="N10" s="4"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="9" t="s">
         <v>264</v>
       </c>
       <c r="B11" t="s">
@@ -2810,7 +2809,7 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="14" t="s">
         <v>265</v>
       </c>
       <c r="B12" t="s">
@@ -2824,7 +2823,7 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="9" t="s">
         <v>266</v>
       </c>
       <c r="B13" t="s">
@@ -2838,7 +2837,7 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="10" t="s">
         <v>299</v>
       </c>
       <c r="B14" t="s">
@@ -2854,30 +2853,30 @@
       <c r="M14" s="9"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="9" t="s">
         <v>267</v>
       </c>
       <c r="B15" t="s">
         <v>162</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="G15" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="M15" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="N15" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="17" t="s">
         <v>268</v>
       </c>
       <c r="B16" t="s">
@@ -2906,7 +2905,7 @@
       <c r="N18" s="4"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="9" t="s">
         <v>271</v>
       </c>
       <c r="B19" t="s">
@@ -2920,7 +2919,7 @@
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="14" t="s">
         <v>272</v>
       </c>
       <c r="B20" t="s">
@@ -2934,7 +2933,7 @@
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="9" t="s">
         <v>273</v>
       </c>
       <c r="B21" t="s">
@@ -2948,7 +2947,7 @@
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="10" t="s">
         <v>300</v>
       </c>
       <c r="B22" t="s">
@@ -2964,30 +2963,30 @@
       <c r="M22" s="9"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="9" t="s">
         <v>274</v>
       </c>
       <c r="B23" t="s">
         <v>162</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="G23" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="M23" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="N23" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="17" t="s">
         <v>275</v>
       </c>
       <c r="B24" t="s">
@@ -3081,16 +3080,16 @@
         <v>162</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="G31" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="M31" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="N31" t="s">
         <v>317</v>
@@ -3126,7 +3125,7 @@
       <c r="N34" s="4"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="A35" s="9" t="s">
         <v>287</v>
       </c>
       <c r="B35" t="s">
@@ -3140,7 +3139,7 @@
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="16" t="s">
+      <c r="A36" s="14" t="s">
         <v>288</v>
       </c>
       <c r="B36" t="s">
@@ -3154,7 +3153,7 @@
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="A37" s="9" t="s">
         <v>289</v>
       </c>
       <c r="B37" t="s">
@@ -3168,7 +3167,7 @@
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="10" t="s">
         <v>302</v>
       </c>
       <c r="B38" t="s">
@@ -3184,30 +3183,30 @@
       <c r="M38" s="9"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="A39" s="9" t="s">
         <v>290</v>
       </c>
       <c r="B39" t="s">
         <v>162</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="G39" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="K39" s="5" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="M39" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="N39" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" s="18" t="s">
+      <c r="A40" s="17" t="s">
         <v>291</v>
       </c>
       <c r="B40" t="s">
@@ -3236,7 +3235,7 @@
       <c r="N42" s="4"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="A43" s="9" t="s">
         <v>292</v>
       </c>
       <c r="B43" t="s">
@@ -3250,7 +3249,7 @@
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" s="16" t="s">
+      <c r="A44" s="14" t="s">
         <v>293</v>
       </c>
       <c r="B44" t="s">
@@ -3264,7 +3263,7 @@
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="A45" s="9" t="s">
         <v>294</v>
       </c>
       <c r="B45" t="s">
@@ -3278,7 +3277,7 @@
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="10" t="s">
         <v>303</v>
       </c>
       <c r="B46" t="s">
@@ -3294,30 +3293,30 @@
       <c r="M46" s="9"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="A47" s="9" t="s">
         <v>295</v>
       </c>
       <c r="B47" t="s">
         <v>162</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="G47" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="K47" s="5" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="M47" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="N47" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A48" s="18" t="s">
+      <c r="A48" s="17" t="s">
         <v>296</v>
       </c>
       <c r="B48" t="s">
@@ -3346,7 +3345,7 @@
       <c r="N50" s="4"/>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="A51" s="9" t="s">
         <v>310</v>
       </c>
       <c r="B51" t="s">
@@ -3360,7 +3359,7 @@
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A52" s="16" t="s">
+      <c r="A52" s="14" t="s">
         <v>308</v>
       </c>
       <c r="B52" t="s">
@@ -3374,7 +3373,7 @@
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="A53" s="9" t="s">
         <v>306</v>
       </c>
       <c r="B53" t="s">
@@ -3388,7 +3387,7 @@
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+      <c r="A54" s="10" t="s">
         <v>304</v>
       </c>
       <c r="B54" t="s">
@@ -3404,30 +3403,30 @@
       <c r="M54" s="9"/>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="A55" s="9" t="s">
         <v>297</v>
       </c>
       <c r="B55" t="s">
         <v>162</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="G55" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="K55" s="5" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="M55" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="N55" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A56" s="18" t="s">
+      <c r="A56" s="17" t="s">
         <v>312</v>
       </c>
       <c r="B56" t="s">
@@ -3465,7 +3464,7 @@
       <c r="N58" s="4"/>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="A59" s="9" t="s">
         <v>311</v>
       </c>
       <c r="B59" t="s">
@@ -3479,7 +3478,7 @@
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A60" s="16" t="s">
+      <c r="A60" s="14" t="s">
         <v>309</v>
       </c>
       <c r="B60" t="s">
@@ -3493,7 +3492,7 @@
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+      <c r="A61" s="9" t="s">
         <v>307</v>
       </c>
       <c r="B61" t="s">
@@ -3507,7 +3506,7 @@
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+      <c r="A62" s="10" t="s">
         <v>305</v>
       </c>
       <c r="B62" t="s">
@@ -3523,30 +3522,30 @@
       <c r="M62" s="9"/>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+      <c r="A63" s="9" t="s">
         <v>298</v>
       </c>
       <c r="B63" t="s">
         <v>162</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="G63" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="K63" s="5" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="M63" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="N63" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A64" s="18" t="s">
+      <c r="A64" s="17" t="s">
         <v>313</v>
       </c>
       <c r="B64" t="s">
@@ -3613,9 +3612,7 @@
   </sheetPr>
   <dimension ref="A1:R70"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3709,10 +3706,10 @@
         <v>3</v>
       </c>
       <c r="F7" s="5">
-        <v>1809302</v>
+        <v>1652909</v>
       </c>
       <c r="G7" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -3723,10 +3720,10 @@
         <v>3</v>
       </c>
       <c r="F8" s="5">
-        <v>1809302</v>
+        <v>1652909</v>
       </c>
       <c r="G8" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -3827,16 +3824,16 @@
         <v>174</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="G16" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="L16" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -3989,16 +3986,16 @@
         <v>174</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="G29" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="L29" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -4154,22 +4151,22 @@
         <v>174</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="G42" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="K42" s="5" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="L42" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="P42" s="5" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="R42" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
@@ -4322,16 +4319,16 @@
         <v>213</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="G55" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="K55" s="5" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="L55" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="M55" s="5"/>
     </row>
@@ -4444,30 +4441,30 @@
     <hyperlink ref="F32" r:id="rId15" display="http://nz.element14.com/koa/rk73b2attd104j/resistor-0805-100k-ohm-5/dp/1809303"/>
     <hyperlink ref="F19" r:id="rId16" display="http://nz.element14.com/koa/rk73b2attd104j/resistor-0805-100k-ohm-5/dp/1809303"/>
     <hyperlink ref="F9" r:id="rId17" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
-    <hyperlink ref="F7" r:id="rId18" display="http://nz.element14.com/koa/rk73b2attd103j/resistor-0805-10k-ohm-5/dp/1809302"/>
-    <hyperlink ref="F8" r:id="rId19" display="http://nz.element14.com/koa/rk73b2attd103j/resistor-0805-10k-ohm-5/dp/1809302"/>
-    <hyperlink ref="F10" r:id="rId20" display="http://nz.element14.com/texas-instruments/sn74ls86ad/logic-quad-2-in-ex-or-gate-14soic/dp/1740035?Ntt=74ls86"/>
-    <hyperlink ref="F20" r:id="rId21" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
-    <hyperlink ref="F33" r:id="rId22" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
-    <hyperlink ref="F46" r:id="rId23" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
-    <hyperlink ref="F59" r:id="rId24" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
-    <hyperlink ref="F3" r:id="rId25" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
-    <hyperlink ref="F4" r:id="rId26" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
-    <hyperlink ref="F5" r:id="rId27" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
-    <hyperlink ref="F6" r:id="rId28" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
-    <hyperlink ref="F21" r:id="rId29" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
-    <hyperlink ref="F34" r:id="rId30" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
-    <hyperlink ref="F47" r:id="rId31" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
-    <hyperlink ref="F60" r:id="rId32" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
-    <hyperlink ref="F42" r:id="rId33" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
-    <hyperlink ref="P42" r:id="rId34" tooltip="Click to view additional information on this product." display="http://nz.mouser.com/ProductDetail/STMicroelectronics/VNP14NV04-E/?qs=sGAEpiMZZMuCmTIBzycWfOPiiwtMaP0Fv4CVvoRPcP8%3d"/>
-    <hyperlink ref="K42" r:id="rId35" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
-    <hyperlink ref="F29" r:id="rId36" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
-    <hyperlink ref="K29" r:id="rId37" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
-    <hyperlink ref="F16" r:id="rId38" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
-    <hyperlink ref="K16" r:id="rId39" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
-    <hyperlink ref="F55" r:id="rId40" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
-    <hyperlink ref="K55" r:id="rId41" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
+    <hyperlink ref="F10" r:id="rId18" display="http://nz.element14.com/texas-instruments/sn74ls86ad/logic-quad-2-in-ex-or-gate-14soic/dp/1740035?Ntt=74ls86"/>
+    <hyperlink ref="F20" r:id="rId19" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
+    <hyperlink ref="F33" r:id="rId20" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
+    <hyperlink ref="F46" r:id="rId21" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
+    <hyperlink ref="F59" r:id="rId22" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
+    <hyperlink ref="F3" r:id="rId23" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
+    <hyperlink ref="F4" r:id="rId24" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
+    <hyperlink ref="F5" r:id="rId25" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
+    <hyperlink ref="F6" r:id="rId26" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
+    <hyperlink ref="F21" r:id="rId27" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
+    <hyperlink ref="F34" r:id="rId28" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
+    <hyperlink ref="F47" r:id="rId29" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
+    <hyperlink ref="F60" r:id="rId30" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
+    <hyperlink ref="F42" r:id="rId31" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
+    <hyperlink ref="P42" r:id="rId32" tooltip="Click to view additional information on this product." display="http://nz.mouser.com/ProductDetail/STMicroelectronics/VNP14NV04-E/?qs=sGAEpiMZZMuCmTIBzycWfOPiiwtMaP0Fv4CVvoRPcP8%3d"/>
+    <hyperlink ref="K42" r:id="rId33" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
+    <hyperlink ref="F29" r:id="rId34" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
+    <hyperlink ref="K29" r:id="rId35" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
+    <hyperlink ref="F16" r:id="rId36" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
+    <hyperlink ref="K16" r:id="rId37" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
+    <hyperlink ref="F55" r:id="rId38" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
+    <hyperlink ref="K55" r:id="rId39" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
+    <hyperlink ref="F7" r:id="rId40" display="http://nz.element14.com/vishay-draloric/crcw080510k0fkta/thick-film-chip-resistor/dp/1652909"/>
+    <hyperlink ref="F8" r:id="rId41" display="http://nz.element14.com/vishay-draloric/crcw080510k0fkta/thick-film-chip-resistor/dp/1652909"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId42"/>
@@ -4495,9 +4492,7 @@
   </sheetPr>
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4621,7 +4616,7 @@
         <v>1809376</v>
       </c>
       <c r="G9" t="s">
-        <v>187</v>
+        <v>223</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25"/>
@@ -4651,9 +4646,7 @@
   </sheetPr>
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4674,7 +4667,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4" t="s">
-        <v>380</v>
+        <v>388</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -4754,12 +4747,12 @@
         <v>1809376</v>
       </c>
       <c r="G7" t="s">
-        <v>187</v>
+        <v>223</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="B8" t="s">
         <v>98</v>
@@ -4773,7 +4766,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="B9" t="s">
         <v>98</v>
@@ -4787,7 +4780,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="B10" t="s">
         <v>99</v>
@@ -4795,7 +4788,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="B11" t="s">
         <v>99</v>
@@ -4803,7 +4796,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="B12" t="s">
         <v>99</v>
@@ -4812,29 +4805,29 @@
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="15"/>
     </row>
-    <row r="14" spans="1:12" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
-        <v>387</v>
+    <row r="14" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="29">
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="27">
         <v>1457153</v>
       </c>
-      <c r="G15" s="28" t="s">
+      <c r="G15" s="26" t="s">
         <v>197</v>
       </c>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
       <c r="J15" s="8" t="s">
         <v>250</v>
       </c>
@@ -4844,184 +4837,202 @@
       <c r="L15" s="8"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="29">
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="27">
         <v>8820120</v>
       </c>
-      <c r="G16" s="28" t="s">
+      <c r="G16" s="26" t="s">
         <v>232</v>
       </c>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="28"/>
-      <c r="L16" s="28"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="26"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="29">
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="27">
         <v>1759199</v>
       </c>
-      <c r="G17" s="28" t="s">
+      <c r="G17" s="26" t="s">
         <v>236</v>
       </c>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="28"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="26"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="29">
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="27">
         <v>1759172</v>
       </c>
-      <c r="G18" s="28" t="s">
+      <c r="G18" s="26" t="s">
         <v>237</v>
       </c>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="28"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="26"/>
+      <c r="L18" s="26"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="29">
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="27">
         <v>1809376</v>
       </c>
-      <c r="G19" s="28" t="s">
-        <v>187</v>
-      </c>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="28"/>
+      <c r="G19" s="26" t="s">
+        <v>223</v>
+      </c>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="26"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="B20" s="28" t="s">
+      <c r="B20" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="29">
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="27">
         <v>1809596</v>
       </c>
-      <c r="G20" s="28" t="s">
+      <c r="G20" s="26" t="s">
         <v>222</v>
       </c>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="28"/>
-      <c r="L20" s="28"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="26"/>
+      <c r="L20" s="26"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="27" t="s">
+      <c r="A21" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="29">
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="27">
         <v>1809596</v>
       </c>
-      <c r="G21" s="28" t="s">
+      <c r="G21" s="26" t="s">
         <v>222</v>
       </c>
-      <c r="H21" s="28"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="28"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="28"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="26"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="27" t="s">
+      <c r="A22" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="B22" s="28"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="28"/>
-      <c r="K22" s="28"/>
-      <c r="L22" s="28"/>
+      <c r="B22" s="26" t="s">
+        <v>387</v>
+      </c>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="27">
+        <v>9556915</v>
+      </c>
+      <c r="G22" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="H22" s="26"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="26"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="27" t="s">
+      <c r="A23" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="28"/>
-      <c r="K23" s="28"/>
-      <c r="L23" s="28"/>
+      <c r="B23" s="26" t="s">
+        <v>387</v>
+      </c>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="27">
+        <v>9556915</v>
+      </c>
+      <c r="G23" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="H23" s="26"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="26"/>
+      <c r="L23" s="26"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="27" t="s">
-        <v>97</v>
-      </c>
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="28"/>
-      <c r="I24" s="28"/>
-      <c r="J24" s="28"/>
-      <c r="K24" s="28"/>
-      <c r="L24" s="28"/>
+      <c r="A24" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="B24" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="27">
+        <v>8820120</v>
+      </c>
+      <c r="G24" s="26" t="s">
+        <v>232</v>
+      </c>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="26"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="26"/>
     </row>
     <row r="25" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
@@ -5046,6 +5057,9 @@
     <hyperlink ref="F17" r:id="rId14" display="http://nz.element14.com/multicomp/mcca000326/mlcc-0805-np0-50v-47pf/dp/1759199"/>
     <hyperlink ref="F18" r:id="rId15" display="http://nz.element14.com/multicomp/mcca000301/mlcc-0805-x7r-25v-220nf/dp/1759172"/>
     <hyperlink ref="K15" r:id="rId16" tooltip="Click to view additional information on this product." display="http://nz.mouser.com/ProductDetail/Freescale-Semiconductor/MPX4250AP/?qs=sGAEpiMZZMvhQj7WZhFIALpLlyV3lh9LDMe%2fRQPZbUw%3d"/>
+    <hyperlink ref="F22" r:id="rId17" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
+    <hyperlink ref="F23" r:id="rId18" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
+    <hyperlink ref="F24" r:id="rId19" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5058,9 +5072,7 @@
   </sheetPr>
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5071,7 +5083,7 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -5081,7 +5093,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4" t="s">
-        <v>381</v>
+        <v>389</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -5147,7 +5159,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="B7" t="s">
         <v>50</v>
@@ -5156,7 +5168,7 @@
         <v>1809376</v>
       </c>
       <c r="G7" t="s">
-        <v>187</v>
+        <v>223</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -5174,27 +5186,27 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>107</v>
+      <c r="A9" s="9" t="s">
+        <v>94</v>
       </c>
       <c r="B9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="B10" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>109</v>
+      <c r="A11" s="10" t="s">
+        <v>96</v>
       </c>
       <c r="B11" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F11" s="5">
         <v>1809596</v>
@@ -5204,37 +5216,41 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="F12" s="5"/>
+      <c r="A12" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:12" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
-        <v>388</v>
-      </c>
-      <c r="F14" s="26"/>
+    <row r="14" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="s">
+        <v>386</v>
+      </c>
+      <c r="F14" s="24"/>
     </row>
     <row r="15" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="29">
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="27">
         <v>1555602</v>
       </c>
-      <c r="G15" s="28" t="s">
+      <c r="G15" s="26" t="s">
         <v>336</v>
       </c>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
       <c r="J15" s="11">
         <v>1703477</v>
       </c>
@@ -5244,178 +5260,198 @@
       <c r="L15" s="8"/>
     </row>
     <row r="16" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="29">
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="27">
         <v>8820120</v>
       </c>
-      <c r="G16" s="28" t="s">
+      <c r="G16" s="26" t="s">
         <v>232</v>
       </c>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="28"/>
-      <c r="L16" s="28"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="26"/>
     </row>
     <row r="17" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="29">
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="27">
         <v>1759199</v>
       </c>
-      <c r="G17" s="28" t="s">
+      <c r="G17" s="26" t="s">
         <v>236</v>
       </c>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="28"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="26"/>
     </row>
     <row r="18" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="28"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="26"/>
+      <c r="L18" s="26"/>
     </row>
     <row r="19" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="B19" s="28" t="s">
+      <c r="A19" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="B19" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="29">
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="27">
         <v>1809376</v>
       </c>
-      <c r="G19" s="28" t="s">
-        <v>187</v>
-      </c>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="28"/>
+      <c r="G19" s="26" t="s">
+        <v>223</v>
+      </c>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="26"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="B20" s="28" t="s">
+      <c r="B20" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="29">
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="27">
         <v>1759172</v>
       </c>
-      <c r="G20" s="28" t="s">
+      <c r="G20" s="26" t="s">
         <v>237</v>
       </c>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="28"/>
-      <c r="L20" s="28"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="26"/>
+      <c r="L20" s="26"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="27" t="s">
-        <v>107</v>
-      </c>
-      <c r="B21" s="28"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="28"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="28"/>
+      <c r="A21" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="27">
+        <v>1809596</v>
+      </c>
+      <c r="G21" s="26" t="s">
+        <v>222</v>
+      </c>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="26"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="B22" s="28"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="28"/>
-      <c r="K22" s="28"/>
-      <c r="L22" s="28"/>
+      <c r="A22" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="26" t="s">
+        <v>387</v>
+      </c>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="27">
+        <v>9556915</v>
+      </c>
+      <c r="G22" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="H22" s="26"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="26"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="B23" s="28" t="s">
-        <v>98</v>
-      </c>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="29">
-        <v>1809596</v>
-      </c>
-      <c r="G23" s="28" t="s">
-        <v>222</v>
-      </c>
-      <c r="H23" s="28"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="28"/>
-      <c r="K23" s="28"/>
-      <c r="L23" s="28"/>
+      <c r="A23" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23" s="26" t="s">
+        <v>387</v>
+      </c>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="27">
+        <v>9556915</v>
+      </c>
+      <c r="G23" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="H23" s="26"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="26"/>
+      <c r="L23" s="26"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="28"/>
-      <c r="I24" s="28"/>
-      <c r="J24" s="28"/>
-      <c r="K24" s="28"/>
-      <c r="L24" s="28"/>
+      <c r="A24" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="B24" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="27">
+        <v>8820120</v>
+      </c>
+      <c r="G24" s="26" t="s">
+        <v>232</v>
+      </c>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="26"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="26"/>
     </row>
     <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
@@ -5433,14 +5469,17 @@
     <hyperlink ref="J3" r:id="rId7" display="http://nz.element14.com/freescale-semiconductor/mpx4100as/ic-pressure-sensor-6-867e/dp/1703477"/>
     <hyperlink ref="F15" r:id="rId8" display="http://nz.element14.com/freescale-semiconductor/mpx4100a/ic-pressure-sensor/dp/1555602"/>
     <hyperlink ref="F19" r:id="rId9" display="http://nz.element14.com/koa/rk73b2attd471j/resistor-0805-470-ohm-5/dp/1809376"/>
-    <hyperlink ref="F23" r:id="rId10" display="http://nz.element14.com/koa/rk73z2attd/resistor-0805-0-ohm-jumper/dp/1809596"/>
+    <hyperlink ref="F21" r:id="rId10" display="http://nz.element14.com/koa/rk73z2attd/resistor-0805-0-ohm-jumper/dp/1809596"/>
     <hyperlink ref="F16" r:id="rId11" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
     <hyperlink ref="F17" r:id="rId12" display="http://nz.element14.com/multicomp/mcca000326/mlcc-0805-np0-50v-47pf/dp/1759199"/>
     <hyperlink ref="F20" r:id="rId13" display="http://nz.element14.com/multicomp/mcca000301/mlcc-0805-x7r-25v-220nf/dp/1759172"/>
     <hyperlink ref="J15" r:id="rId14" display="http://nz.element14.com/freescale-semiconductor/mpx4100as/ic-pressure-sensor-6-867e/dp/1703477"/>
+    <hyperlink ref="F22" r:id="rId15" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
+    <hyperlink ref="F23" r:id="rId16" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
+    <hyperlink ref="F24" r:id="rId17" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId15"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
 
@@ -5451,9 +5490,7 @@
   </sheetPr>
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5514,10 +5551,10 @@
         <v>3</v>
       </c>
       <c r="F4" s="5">
-        <v>1809302</v>
+        <v>1652909</v>
       </c>
       <c r="G4" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -5633,10 +5670,10 @@
         <v>3</v>
       </c>
       <c r="F12" s="5">
-        <v>1809302</v>
+        <v>1652909</v>
       </c>
       <c r="G12" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -5710,18 +5747,18 @@
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1" display="http://nz.element14.com/maxim-integrated-products/max9924uaub/interface-sensor-vr-1ch-10umax/dp/1845719"/>
     <hyperlink ref="F11" r:id="rId2" display="http://nz.element14.com/maxim-integrated-products/max9924uaub/interface-sensor-vr-1ch-10umax/dp/1845719"/>
-    <hyperlink ref="F4" r:id="rId3" display="http://nz.element14.com/koa/rk73b2attd103j/resistor-0805-10k-ohm-5/dp/1809302"/>
-    <hyperlink ref="F12" r:id="rId4" display="http://nz.element14.com/koa/rk73b2attd103j/resistor-0805-10k-ohm-5/dp/1809302"/>
-    <hyperlink ref="F13" r:id="rId5" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
-    <hyperlink ref="F5" r:id="rId6" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
-    <hyperlink ref="F6" r:id="rId7" display="http://nz.element14.com/kemet/c0805c102k2ractu/capacitor-0805-1nf-200v-x7r/dp/1414659"/>
-    <hyperlink ref="F14" r:id="rId8" display="http://nz.element14.com/kemet/c0805c102k2ractu/capacitor-0805-1nf-200v-x7r/dp/1414659"/>
-    <hyperlink ref="K11" r:id="rId9" tooltip="Click to view additional information on this product." display="http://nz.mouser.com/ProductDetail/Maxim-Integrated-Products/MAX9924UAUB+/?qs=sGAEpiMZZMuuBt6TL7D%2f6J4pe%2fE63Xbw"/>
-    <hyperlink ref="K3" r:id="rId10" tooltip="Click to view additional information on this product." display="http://nz.mouser.com/ProductDetail/Maxim-Integrated-Products/MAX9924UAUB+/?qs=sGAEpiMZZMuuBt6TL7D%2f6J4pe%2fE63Xbw"/>
-    <hyperlink ref="F16" r:id="rId11" display="http://nz.element14.com/panasonic/erjt06j103v/resistor-anti-pulse-0805-10k-5/dp/1618242"/>
-    <hyperlink ref="F15" r:id="rId12" display="http://nz.element14.com/panasonic/erjt06j103v/resistor-anti-pulse-0805-10k-5/dp/1618242"/>
-    <hyperlink ref="F8" r:id="rId13" display="http://nz.element14.com/panasonic/erjt06j103v/resistor-anti-pulse-0805-10k-5/dp/1618242"/>
-    <hyperlink ref="F7" r:id="rId14" display="http://nz.element14.com/panasonic/erjt06j103v/resistor-anti-pulse-0805-10k-5/dp/1618242"/>
+    <hyperlink ref="F13" r:id="rId3" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
+    <hyperlink ref="F5" r:id="rId4" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
+    <hyperlink ref="F6" r:id="rId5" display="http://nz.element14.com/kemet/c0805c102k2ractu/capacitor-0805-1nf-200v-x7r/dp/1414659"/>
+    <hyperlink ref="F14" r:id="rId6" display="http://nz.element14.com/kemet/c0805c102k2ractu/capacitor-0805-1nf-200v-x7r/dp/1414659"/>
+    <hyperlink ref="K11" r:id="rId7" tooltip="Click to view additional information on this product." display="http://nz.mouser.com/ProductDetail/Maxim-Integrated-Products/MAX9924UAUB+/?qs=sGAEpiMZZMuuBt6TL7D%2f6J4pe%2fE63Xbw"/>
+    <hyperlink ref="K3" r:id="rId8" tooltip="Click to view additional information on this product." display="http://nz.mouser.com/ProductDetail/Maxim-Integrated-Products/MAX9924UAUB+/?qs=sGAEpiMZZMuuBt6TL7D%2f6J4pe%2fE63Xbw"/>
+    <hyperlink ref="F16" r:id="rId9" display="http://nz.element14.com/panasonic/erjt06j103v/resistor-anti-pulse-0805-10k-5/dp/1618242"/>
+    <hyperlink ref="F15" r:id="rId10" display="http://nz.element14.com/panasonic/erjt06j103v/resistor-anti-pulse-0805-10k-5/dp/1618242"/>
+    <hyperlink ref="F8" r:id="rId11" display="http://nz.element14.com/panasonic/erjt06j103v/resistor-anti-pulse-0805-10k-5/dp/1618242"/>
+    <hyperlink ref="F7" r:id="rId12" display="http://nz.element14.com/panasonic/erjt06j103v/resistor-anti-pulse-0805-10k-5/dp/1618242"/>
+    <hyperlink ref="F4" r:id="rId13" display="http://nz.element14.com/vishay-draloric/crcw080510k0fkta/thick-film-chip-resistor/dp/1652909"/>
+    <hyperlink ref="F12" r:id="rId14" display="http://nz.element14.com/vishay-draloric/crcw080510k0fkta/thick-film-chip-resistor/dp/1652909"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5734,9 +5771,7 @@
   </sheetPr>
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5882,9 +5917,7 @@
   </sheetPr>
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14:G14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6079,9 +6112,7 @@
   </sheetPr>
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14:G14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6277,9 +6308,7 @@
   </sheetPr>
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14:G14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Updated component in secondary power supply and made minor format changes.
</commit_message>
<xml_diff>
--- a/PumaBom-WithMods-Element14.xlsx
+++ b/PumaBom-WithMods-Element14.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="386">
   <si>
     <t>MCU</t>
   </si>
@@ -247,9 +247,6 @@
     <t>C12</t>
   </si>
   <si>
-    <t>2200uF</t>
-  </si>
-  <si>
     <t>Battery Voltage Reference</t>
   </si>
   <si>
@@ -607,12 +604,6 @@
     <t>Not needed wire jumper</t>
   </si>
   <si>
-    <t>LM2937ET-5.0</t>
-  </si>
-  <si>
-    <t>IC, V REG LDO +5.0V, 2937, TO-220-3</t>
-  </si>
-  <si>
     <t>No Longer Stocked by Element14</t>
   </si>
   <si>
@@ -784,12 +775,6 @@
     <t>SCHOTTKY RECTIFIER, 500mA, 20V, SOD-123</t>
   </si>
   <si>
-    <t>CAPACITOR, 2200UF, 25V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Change to 25v </t>
-  </si>
-  <si>
     <t>1/4watt</t>
   </si>
   <si>
@@ -1196,13 +1181,16 @@
   </si>
   <si>
     <t>Schematic pages: 1, 43, 47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LM2937ET-5.0 IC, V REG LDO +5.0V, 2937, TO-220-3 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1228,6 +1216,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1323,7 +1318,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1358,6 +1353,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1665,7 +1662,7 @@
   </sheetPr>
   <dimension ref="A1:L74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1682,14 +1679,14 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="C2" s="19"/>
       <c r="D2" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="H2" s="29" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="I2" s="29"/>
       <c r="J2" s="29"/>
@@ -1698,10 +1695,10 @@
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C3" s="20"/>
       <c r="D3" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="H3" s="28" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="I3" s="29"/>
       <c r="J3" s="29"/>
@@ -1710,7 +1707,7 @@
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C4" s="21"/>
       <c r="D4" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25"/>
@@ -1723,12 +1720,12 @@
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
@@ -1739,13 +1736,13 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="F7" s="5">
         <v>1380343</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1759,7 +1756,7 @@
         <v>1652909</v>
       </c>
       <c r="G8" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1773,7 +1770,7 @@
         <v>1652909</v>
       </c>
       <c r="G9" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1787,7 +1784,7 @@
         <v>1652909</v>
       </c>
       <c r="G10" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1801,7 +1798,7 @@
         <v>1652909</v>
       </c>
       <c r="G11" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1812,14 +1809,14 @@
         <v>3</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="D12" s="16"/>
       <c r="F12" s="5">
         <v>1652909</v>
       </c>
       <c r="G12" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1833,7 +1830,7 @@
         <v>8820120</v>
       </c>
       <c r="G13" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1847,7 +1844,7 @@
         <v>1650875</v>
       </c>
       <c r="G14" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1861,7 +1858,7 @@
         <v>1702127</v>
       </c>
       <c r="G15" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1875,7 +1872,7 @@
         <v>1887296</v>
       </c>
       <c r="G16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1889,7 +1886,7 @@
         <v>1414676</v>
       </c>
       <c r="G17" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -1900,13 +1897,13 @@
         <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="F18" s="5">
         <v>1174062</v>
       </c>
       <c r="G18" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -1920,7 +1917,7 @@
         <v>1712841</v>
       </c>
       <c r="G19" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -1934,7 +1931,7 @@
         <v>8820120</v>
       </c>
       <c r="G20" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -1948,7 +1945,7 @@
         <v>8820120</v>
       </c>
       <c r="G21" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -1956,16 +1953,16 @@
         <v>23</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="F22" s="5">
         <v>1809300</v>
       </c>
       <c r="G22" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -1979,7 +1976,7 @@
         <v>8820120</v>
       </c>
       <c r="G23" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -1993,7 +1990,7 @@
         <v>8820120</v>
       </c>
       <c r="G24" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -2007,7 +2004,7 @@
         <v>8820120</v>
       </c>
       <c r="G25" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25"/>
@@ -2024,7 +2021,7 @@
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="4" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
@@ -2041,7 +2038,7 @@
         <v>1146032</v>
       </c>
       <c r="G29" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -2055,7 +2052,7 @@
         <v>8820120</v>
       </c>
       <c r="G30" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -2064,7 +2061,7 @@
         <v>38</v>
       </c>
       <c r="C31" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -2078,7 +2075,7 @@
         <v>8820120</v>
       </c>
       <c r="G32" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -2092,7 +2089,7 @@
         <v>9334084</v>
       </c>
       <c r="G33" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -2106,7 +2103,7 @@
         <v>9406352</v>
       </c>
       <c r="G34" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -2114,13 +2111,13 @@
         <v>42</v>
       </c>
       <c r="B35" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F35" s="5">
         <v>1355761</v>
       </c>
       <c r="G35" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -2134,7 +2131,7 @@
         <v>1226390</v>
       </c>
       <c r="G36" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -2148,7 +2145,7 @@
         <v>1465996</v>
       </c>
       <c r="G37" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -2162,7 +2159,7 @@
         <v>1809376</v>
       </c>
       <c r="G38" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -2176,7 +2173,7 @@
         <v>1809376</v>
       </c>
       <c r="G39" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25"/>
@@ -2193,7 +2190,7 @@
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
       <c r="I42" s="4" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
@@ -2210,7 +2207,7 @@
         <v>1556741</v>
       </c>
       <c r="G43" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
@@ -2224,7 +2221,7 @@
         <v>9229272</v>
       </c>
       <c r="G44" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
@@ -2238,7 +2235,7 @@
         <v>8820120</v>
       </c>
       <c r="G45" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
@@ -2246,13 +2243,13 @@
         <v>33</v>
       </c>
       <c r="B46" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F46" s="5">
         <v>9556915</v>
       </c>
       <c r="G46" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
@@ -2266,7 +2263,7 @@
         <v>1617365</v>
       </c>
       <c r="G47" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
@@ -2280,7 +2277,7 @@
         <v>8820120</v>
       </c>
       <c r="G48" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -2291,7 +2288,7 @@
         <v>57</v>
       </c>
       <c r="C49" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25"/>
@@ -2308,177 +2305,166 @@
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
       <c r="I52" s="4" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B53" s="1" t="s">
+      <c r="A53" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B53" t="s">
+        <v>62</v>
+      </c>
+      <c r="F53" s="5">
+        <v>9486038</v>
+      </c>
+      <c r="G53" s="7" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B54" t="s">
         <v>57</v>
       </c>
-      <c r="C53" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>316</v>
+      <c r="F54" s="5">
+        <v>1324152</v>
+      </c>
+      <c r="G54" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B55" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="F55" s="5">
-        <v>9486038</v>
-      </c>
-      <c r="G55" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="H55" t="s">
-        <v>194</v>
+        <v>1617365</v>
+      </c>
+      <c r="G55" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="10" t="s">
+      <c r="A56" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B56" t="s">
+        <v>22</v>
+      </c>
+      <c r="F56" s="5">
+        <v>8820120</v>
+      </c>
+      <c r="G56" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B57" t="s">
+        <v>31</v>
+      </c>
+      <c r="F57" s="5">
+        <v>9229272</v>
+      </c>
+      <c r="G57" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="B58" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="F58" s="5">
+        <v>1617365</v>
+      </c>
+      <c r="G58" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B59" t="s">
+        <v>22</v>
+      </c>
+      <c r="F59" s="5">
+        <v>8820120</v>
+      </c>
+      <c r="G59" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="10" t="s">
+      <c r="B60" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="10" t="s">
+      <c r="B61" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="F58" s="5"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="10" t="s">
+      <c r="B62" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="F59" s="5"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B60" t="s">
-        <v>53</v>
-      </c>
-      <c r="F60" s="5">
-        <v>1617365</v>
-      </c>
-      <c r="G60" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="B61" t="s">
-        <v>22</v>
-      </c>
-      <c r="F61" s="5">
-        <v>8820120</v>
-      </c>
-      <c r="G61" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="B62" t="s">
+      <c r="B63" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F62" s="5">
-        <v>1324152</v>
-      </c>
-      <c r="G62" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="B63" t="s">
-        <v>31</v>
-      </c>
-      <c r="D63" t="s">
-        <v>253</v>
-      </c>
-      <c r="F63" s="5">
-        <v>9229272</v>
-      </c>
-      <c r="G63" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="B64" t="s">
-        <v>73</v>
-      </c>
-      <c r="F64" s="5">
-        <v>8812519</v>
-      </c>
-      <c r="G64" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="B65" t="s">
-        <v>22</v>
-      </c>
-      <c r="F65" s="5">
-        <v>8820120</v>
-      </c>
-      <c r="G65" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25"/>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F67" s="5"/>
     </row>
-    <row r="68" spans="1:7" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="1:6" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="H3:K3"/>
@@ -2493,11 +2479,11 @@
     <hyperlink ref="F38" r:id="rId6" display="http://nz.element14.com/koa/rk73b2attd471j/resistor-0805-470-ohm-5/dp/1809376"/>
     <hyperlink ref="F39" r:id="rId7" display="http://nz.element14.com/koa/rk73b2attd471j/resistor-0805-470-ohm-5/dp/1809376"/>
     <hyperlink ref="F35" r:id="rId8" display="http://nz.element14.com/molex/678038020/socket-mini-usb-otg/dp/1355761"/>
-    <hyperlink ref="F55" r:id="rId9" display="http://nz.element14.com/national-semiconductor/lm2937-5-0/ic-v-reg-ldo-5-0v-2937-to-220-3/dp/9486038"/>
+    <hyperlink ref="F53" r:id="rId9" display="http://nz.element14.com/national-semiconductor/lm2937-5-0/ic-v-reg-ldo-5-0v-2937-to-220-3/dp/9486038"/>
     <hyperlink ref="F16" r:id="rId10" display="http://nz.element14.com/multicomp/mcpwr05ftew3901/resistor-0805-3-9k-1-0-125w/dp/1887296"/>
     <hyperlink ref="F43" r:id="rId11" display="http://nz.element14.com/micrel-semiconductor/mic2954-02ws/ic-reg-ldo-250ma-5v-0-5/dp/1556741"/>
-    <hyperlink ref="F61" r:id="rId12" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
-    <hyperlink ref="F65" r:id="rId13" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
+    <hyperlink ref="F56" r:id="rId12" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
+    <hyperlink ref="F59" r:id="rId13" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
     <hyperlink ref="F48" r:id="rId14" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
     <hyperlink ref="F45" r:id="rId15" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
     <hyperlink ref="F30" r:id="rId16" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
@@ -2513,21 +2499,21 @@
     <hyperlink ref="F15" r:id="rId26" display="http://nz.element14.com/kemet/c0805c332kcractu/capacitor-0805-3-3nf-500v-x7r/dp/1702127"/>
     <hyperlink ref="F17" r:id="rId27" display="http://nz.element14.com/kemet/c0805c220j1gactu/capacitor-0805-22pf-100v-np0/dp/1414676"/>
     <hyperlink ref="F47" r:id="rId28" display="http://nz.element14.com/vishay-sprague/199d106x9035d1v1e3/capacitor-tant-10uf-35v-radial/dp/1617365"/>
-    <hyperlink ref="F60" r:id="rId29" display="http://nz.element14.com/vishay-sprague/199d106x9035d1v1e3/capacitor-tant-10uf-35v-radial/dp/1617365"/>
-    <hyperlink ref="F63" r:id="rId30" display="http://nz.element14.com/kemet/t495d226k035ate300/capacitor-22uf-35v/dp/9229272"/>
+    <hyperlink ref="F55" r:id="rId29" display="http://nz.element14.com/vishay-sprague/199d106x9035d1v1e3/capacitor-tant-10uf-35v-radial/dp/1617365"/>
+    <hyperlink ref="F57" r:id="rId30" display="http://nz.element14.com/kemet/t495d226k035ate300/capacitor-22uf-35v/dp/9229272"/>
     <hyperlink ref="F44" r:id="rId31" display="http://nz.element14.com/kemet/t495d226k035ate300/capacitor-22uf-35v/dp/9229272"/>
-    <hyperlink ref="F62" r:id="rId32" display="http://nz.element14.com/fairchild-semiconductor/1n4007/bridge-rectifier-rohs-compliant/dp/9109625"/>
-    <hyperlink ref="F64" r:id="rId33" display="http://nz.element14.com/nichicon/upm1e222mhd/capacitor-2200uf-25v/dp/8812519"/>
-    <hyperlink ref="F18" r:id="rId34" display="http://nz.element14.com/te-connectivity-cgs/rh73u2a10mjtd/resistor-0805-10m/dp/1174062"/>
-    <hyperlink ref="F22" r:id="rId35" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
-    <hyperlink ref="F34" r:id="rId36" display="http://nz.element14.com/multicomp/u0805r103kct/capacitor-0805-10nf-50v/dp/9406352"/>
-    <hyperlink ref="H3" r:id="rId37"/>
-    <hyperlink ref="F46" r:id="rId38" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
-    <hyperlink ref="F8" r:id="rId39" display="http://nz.element14.com/vishay-draloric/crcw080510k0fkta/thick-film-chip-resistor/dp/1652909"/>
-    <hyperlink ref="F9" r:id="rId40" display="http://nz.element14.com/vishay-draloric/crcw080510k0fkta/thick-film-chip-resistor/dp/1652909"/>
-    <hyperlink ref="F10" r:id="rId41" display="http://nz.element14.com/vishay-draloric/crcw080510k0fkta/thick-film-chip-resistor/dp/1652909"/>
-    <hyperlink ref="F11" r:id="rId42" display="http://nz.element14.com/vishay-draloric/crcw080510k0fkta/thick-film-chip-resistor/dp/1652909"/>
-    <hyperlink ref="F12" r:id="rId43" display="http://nz.element14.com/vishay-draloric/crcw080510k0fkta/thick-film-chip-resistor/dp/1652909"/>
+    <hyperlink ref="F54" r:id="rId32" display="http://nz.element14.com/fairchild-semiconductor/1n4007/bridge-rectifier-rohs-compliant/dp/9109625"/>
+    <hyperlink ref="F18" r:id="rId33" display="http://nz.element14.com/te-connectivity-cgs/rh73u2a10mjtd/resistor-0805-10m/dp/1174062"/>
+    <hyperlink ref="F22" r:id="rId34" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
+    <hyperlink ref="F34" r:id="rId35" display="http://nz.element14.com/multicomp/u0805r103kct/capacitor-0805-10nf-50v/dp/9406352"/>
+    <hyperlink ref="H3" r:id="rId36"/>
+    <hyperlink ref="F46" r:id="rId37" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
+    <hyperlink ref="F8" r:id="rId38" display="http://nz.element14.com/vishay-draloric/crcw080510k0fkta/thick-film-chip-resistor/dp/1652909"/>
+    <hyperlink ref="F9" r:id="rId39" display="http://nz.element14.com/vishay-draloric/crcw080510k0fkta/thick-film-chip-resistor/dp/1652909"/>
+    <hyperlink ref="F10" r:id="rId40" display="http://nz.element14.com/vishay-draloric/crcw080510k0fkta/thick-film-chip-resistor/dp/1652909"/>
+    <hyperlink ref="F11" r:id="rId41" display="http://nz.element14.com/vishay-draloric/crcw080510k0fkta/thick-film-chip-resistor/dp/1652909"/>
+    <hyperlink ref="F12" r:id="rId42" display="http://nz.element14.com/vishay-draloric/crcw080510k0fkta/thick-film-chip-resistor/dp/1652909"/>
+    <hyperlink ref="F58" r:id="rId43" display="http://nz.element14.com/vishay-sprague/199d106x9035d1v1e3/capacitor-tant-10uf-35v-radial/dp/1617365"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId44"/>
@@ -2554,7 +2540,7 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -2564,7 +2550,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -2572,7 +2558,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B3" t="s">
         <v>50</v>
@@ -2581,12 +2567,12 @@
         <v>1809376</v>
       </c>
       <c r="G3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B4" t="s">
         <v>22</v>
@@ -2595,35 +2581,35 @@
         <v>8820120</v>
       </c>
       <c r="G4" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F5" s="5">
         <v>9556915</v>
       </c>
       <c r="G5" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F6" s="5">
         <v>9556915</v>
       </c>
       <c r="G6" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25"/>
@@ -2666,7 +2652,7 @@
     <row r="1" spans="1:15" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -2676,7 +2662,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -2686,97 +2672,97 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F3" s="5">
         <v>1809300</v>
       </c>
       <c r="G3" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F4" s="5">
         <v>1809376</v>
       </c>
       <c r="G4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F5" s="5">
         <v>1465996</v>
       </c>
       <c r="G5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="B6" t="s">
         <v>159</v>
       </c>
-      <c r="B6" t="s">
-        <v>160</v>
-      </c>
       <c r="F6" s="9" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="B7" t="s">
         <v>161</v>
       </c>
-      <c r="B7" t="s">
-        <v>162</v>
-      </c>
       <c r="F7" s="5" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="G7" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="M7" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="O7" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B8" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -2786,7 +2772,7 @@
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
@@ -2796,97 +2782,97 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="B11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F11" s="5">
         <v>1809300</v>
       </c>
       <c r="G11" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="B12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F12" s="5">
         <v>1809376</v>
       </c>
       <c r="G12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="B13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F13" s="5">
         <v>1465996</v>
       </c>
       <c r="G13" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="B14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="L14" s="9"/>
       <c r="M14" s="9"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="B15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="G15" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="M15" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="N15" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="B16" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25"/>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -2896,7 +2882,7 @@
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
@@ -2906,97 +2892,97 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="B19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F19" s="5">
         <v>1809300</v>
       </c>
       <c r="G19" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F20" s="5">
         <v>1809376</v>
       </c>
       <c r="G20" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B21" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F21" s="5">
         <v>1465996</v>
       </c>
       <c r="G21" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="B22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="K22" s="9" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="L22" s="9"/>
       <c r="M22" s="9"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="B23" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="G23" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="M23" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="N23" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B24" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -3006,7 +2992,7 @@
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
       <c r="I26" s="4" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
@@ -3016,97 +3002,97 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="B27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F27" s="5">
         <v>1809300</v>
       </c>
       <c r="G27" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="B28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F28" s="5">
         <v>1809376</v>
       </c>
       <c r="G28" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="B29" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F29" s="5">
         <v>1465996</v>
       </c>
       <c r="G29" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="B30" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="K30" s="9" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="L30" s="9"/>
       <c r="M30" s="9"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="B31" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="G31" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="M31" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="N31" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="B32" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25"/>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -3116,7 +3102,7 @@
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
       <c r="I34" s="4" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
@@ -3126,97 +3112,97 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="B35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F35" s="5">
         <v>1809300</v>
       </c>
       <c r="G35" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="B36" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F36" s="5">
         <v>1809376</v>
       </c>
       <c r="G36" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="B37" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F37" s="5">
         <v>1465996</v>
       </c>
       <c r="G37" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="B38" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="K38" s="9" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="L38" s="9"/>
       <c r="M38" s="9"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="B39" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="G39" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="K39" s="5" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="M39" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="N39" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="B40" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25"/>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -3226,7 +3212,7 @@
       <c r="G42" s="4"/>
       <c r="H42" s="4"/>
       <c r="I42" s="4" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
@@ -3236,97 +3222,97 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="B43" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F43" s="5">
         <v>1809300</v>
       </c>
       <c r="G43" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="B44" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F44" s="5">
         <v>1809376</v>
       </c>
       <c r="G44" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="B45" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F45" s="5">
         <v>1465996</v>
       </c>
       <c r="G45" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="B46" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="K46" s="9" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="L46" s="9"/>
       <c r="M46" s="9"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="B47" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="G47" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="K47" s="5" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="M47" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="N47" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="17" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="B48" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25"/>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -3336,7 +3322,7 @@
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
       <c r="I50" s="4" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
@@ -3346,91 +3332,91 @@
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="B51" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F51" s="5">
         <v>1809300</v>
       </c>
       <c r="G51" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="B52" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F52" s="5">
         <v>1809376</v>
       </c>
       <c r="G52" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="B53" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F53" s="5">
         <v>1465996</v>
       </c>
       <c r="G53" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="B54" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F54" s="9" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="K54" s="9" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="L54" s="9"/>
       <c r="M54" s="9"/>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="B55" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="G55" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="K55" s="5" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="M55" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="N55" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="17" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="B56" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
@@ -3445,7 +3431,7 @@
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -3455,7 +3441,7 @@
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
       <c r="I58" s="4" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
@@ -3465,91 +3451,91 @@
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="B59" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F59" s="5">
         <v>1809300</v>
       </c>
       <c r="G59" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="14" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="B60" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F60" s="5">
         <v>1809376</v>
       </c>
       <c r="G60" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="B61" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F61" s="5">
         <v>1465996</v>
       </c>
       <c r="G61" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="10" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="B62" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F62" s="9" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="K62" s="9" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="L62" s="9"/>
       <c r="M62" s="9"/>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="B63" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="G63" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="K63" s="5" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="M63" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="N63" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="17" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="B64" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
     </row>
     <row r="65" x14ac:dyDescent="0.25"/>
@@ -3624,7 +3610,7 @@
     <row r="1" spans="1:14" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -3634,7 +3620,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -3644,63 +3630,63 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F3" s="5">
         <v>1809300</v>
       </c>
       <c r="G3" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F4" s="5">
         <v>1809300</v>
       </c>
       <c r="G4" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F5" s="5">
         <v>1809300</v>
       </c>
       <c r="G5" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="B6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F6" s="5">
         <v>1809300</v>
       </c>
       <c r="G6" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
@@ -3709,12 +3695,12 @@
         <v>1652909</v>
       </c>
       <c r="G7" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
@@ -3723,12 +3709,12 @@
         <v>1652909</v>
       </c>
       <c r="G8" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="B9" t="s">
         <v>22</v>
@@ -3737,27 +3723,27 @@
         <v>8820120</v>
       </c>
       <c r="G9" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="B10" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="F10" s="5">
         <v>1740035</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -3767,7 +3753,7 @@
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
@@ -3777,149 +3763,149 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B13" t="s">
         <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="F13" s="5">
         <v>9334084</v>
       </c>
       <c r="G13" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F14" s="5">
         <v>1686068</v>
       </c>
       <c r="G14" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="F15" s="9" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="L15" s="9"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="B16" t="s">
         <v>173</v>
       </c>
-      <c r="B16" t="s">
-        <v>174</v>
-      </c>
       <c r="F16" s="5" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="G16" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="L16" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B17" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F18" s="5">
         <v>1809596</v>
       </c>
       <c r="G18" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F19" s="5">
         <v>1809303</v>
       </c>
       <c r="G19" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F20" s="5">
         <v>1809300</v>
       </c>
       <c r="G20" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F21" s="5">
         <v>9556915</v>
       </c>
       <c r="G21" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B22" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B23" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -3929,7 +3915,7 @@
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
       <c r="I25" s="4" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
@@ -3939,151 +3925,151 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B26" t="s">
         <v>40</v>
       </c>
       <c r="C26" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="F26" s="5">
         <v>9334084</v>
       </c>
       <c r="G26" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B27" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F27" s="5">
         <v>1686068</v>
       </c>
       <c r="G27" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
       <c r="F28" s="9" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="K28" s="9" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="L28" s="9"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B29" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="G29" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="L29" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B30" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F31" s="5">
         <v>1809596</v>
       </c>
       <c r="G31" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B32" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F32" s="5">
         <v>1809303</v>
       </c>
       <c r="G32" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F33" s="5">
         <v>1809300</v>
       </c>
       <c r="G33" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B34" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F34" s="5">
         <v>9556915</v>
       </c>
       <c r="G34" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B35" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="F35" s="5"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B36" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="F36" s="5"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25"/>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -4093,7 +4079,7 @@
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
       <c r="I38" s="4" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
@@ -4103,158 +4089,158 @@
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B39" t="s">
         <v>40</v>
       </c>
       <c r="C39" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="F39" s="5">
         <v>9334084</v>
       </c>
       <c r="G39" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B40" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F40" s="5">
         <v>1686068</v>
       </c>
       <c r="G40" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="9"/>
       <c r="F41" s="9" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="K41" s="9" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="L41" s="9"/>
       <c r="M41" s="9"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B42" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="G42" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="K42" s="5" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="L42" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="P42" s="5" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="R42" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B43" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B44" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F44" s="5">
         <v>1809596</v>
       </c>
       <c r="G44" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B45" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F45" s="5">
         <v>1809303</v>
       </c>
       <c r="G45" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F46" s="5">
         <v>1809300</v>
       </c>
       <c r="G46" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B47" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F47" s="5">
         <v>9556915</v>
       </c>
       <c r="G47" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B48" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="F48" s="5"/>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B49" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="F49" s="5"/>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25"/>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -4264,7 +4250,7 @@
       <c r="G51" s="4"/>
       <c r="H51" s="4"/>
       <c r="I51" s="4" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
@@ -4274,143 +4260,143 @@
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B52" t="s">
         <v>40</v>
       </c>
       <c r="C52" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="F52" s="5">
         <v>9334084</v>
       </c>
       <c r="G52" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B53" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F53" s="5">
         <v>1686068</v>
       </c>
       <c r="G53" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="9"/>
       <c r="F54" s="9" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="K54" s="9" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="L54" s="9"/>
       <c r="M54" s="9"/>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="G55" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="K55" s="5" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="L55" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="M55" s="5"/>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="B56" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B57" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F57" s="5">
         <v>1809596</v>
       </c>
       <c r="G57" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="14" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F58" s="5">
         <v>1809303</v>
       </c>
       <c r="G58" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="14" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F59" s="5">
         <v>1809300</v>
       </c>
       <c r="G59" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B60" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F60" s="5">
         <v>9556915</v>
       </c>
       <c r="G60" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B61" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="F61" s="5"/>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="10" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B62" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="F62" s="5"/>
     </row>
@@ -4503,7 +4489,7 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -4513,7 +4499,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -4521,7 +4507,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
@@ -4530,40 +4516,40 @@
         <v>1887296</v>
       </c>
       <c r="G3" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" t="s">
         <v>76</v>
-      </c>
-      <c r="B4" t="s">
-        <v>77</v>
       </c>
       <c r="F4" s="5">
         <v>1506077</v>
       </c>
       <c r="G4" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" t="s">
         <v>78</v>
-      </c>
-      <c r="B5" t="s">
-        <v>79</v>
       </c>
       <c r="F5" s="5">
         <v>1809596</v>
       </c>
       <c r="G5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B6" t="s">
         <v>22</v>
@@ -4572,41 +4558,41 @@
         <v>8820120</v>
       </c>
       <c r="G6" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="I6" s="5"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F7" s="5">
         <v>9556915</v>
       </c>
       <c r="G7" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" t="s">
         <v>82</v>
-      </c>
-      <c r="B8" t="s">
-        <v>83</v>
       </c>
       <c r="F8" s="5">
         <v>9556915</v>
       </c>
       <c r="G8" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B9" t="s">
         <v>50</v>
@@ -4616,7 +4602,7 @@
         <v>1809376</v>
       </c>
       <c r="G9" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25"/>
@@ -4657,7 +4643,7 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -4667,7 +4653,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -4675,28 +4661,28 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" t="s">
         <v>85</v>
-      </c>
-      <c r="B3" t="s">
-        <v>86</v>
       </c>
       <c r="F3" s="5">
         <v>1457153</v>
       </c>
       <c r="G3" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="L3" s="8"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B4" t="s">
         <v>22</v>
@@ -4705,40 +4691,40 @@
         <v>8820120</v>
       </c>
       <c r="G4" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F5" s="5">
         <v>1759199</v>
       </c>
       <c r="G5" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F6" s="5">
         <v>1759172</v>
       </c>
       <c r="G6" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B7" t="s">
         <v>50</v>
@@ -4747,59 +4733,59 @@
         <v>1809376</v>
       </c>
       <c r="G7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F8" s="5">
         <v>1809596</v>
       </c>
       <c r="G8" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F9" s="5">
         <v>1809596</v>
       </c>
       <c r="G9" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -4807,15 +4793,15 @@
     </row>
     <row r="14" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" s="26" t="s">
         <v>85</v>
-      </c>
-      <c r="B15" s="26" t="s">
-        <v>86</v>
       </c>
       <c r="C15" s="26"/>
       <c r="D15" s="26"/>
@@ -4824,21 +4810,21 @@
         <v>1457153</v>
       </c>
       <c r="G15" s="26" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H15" s="26"/>
       <c r="I15" s="26"/>
       <c r="J15" s="8" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="K15" s="11" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="L15" s="8"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B16" s="26" t="s">
         <v>22</v>
@@ -4850,7 +4836,7 @@
         <v>8820120</v>
       </c>
       <c r="G16" s="26" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="H16" s="26"/>
       <c r="I16" s="26"/>
@@ -4860,10 +4846,10 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C17" s="26"/>
       <c r="D17" s="26"/>
@@ -4872,7 +4858,7 @@
         <v>1759199</v>
       </c>
       <c r="G17" s="26" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="H17" s="26"/>
       <c r="I17" s="26"/>
@@ -4882,10 +4868,10 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C18" s="26"/>
       <c r="D18" s="26"/>
@@ -4894,7 +4880,7 @@
         <v>1759172</v>
       </c>
       <c r="G18" s="26" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="H18" s="26"/>
       <c r="I18" s="26"/>
@@ -4904,7 +4890,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B19" s="26" t="s">
         <v>50</v>
@@ -4916,7 +4902,7 @@
         <v>1809376</v>
       </c>
       <c r="G19" s="26" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="H19" s="26"/>
       <c r="I19" s="26"/>
@@ -4926,10 +4912,10 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C20" s="26"/>
       <c r="D20" s="26"/>
@@ -4938,7 +4924,7 @@
         <v>1809596</v>
       </c>
       <c r="G20" s="26" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="H20" s="26"/>
       <c r="I20" s="26"/>
@@ -4948,10 +4934,10 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C21" s="26"/>
       <c r="D21" s="26"/>
@@ -4960,7 +4946,7 @@
         <v>1809596</v>
       </c>
       <c r="G21" s="26" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="H21" s="26"/>
       <c r="I21" s="26"/>
@@ -4970,10 +4956,10 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="C22" s="26"/>
       <c r="D22" s="26"/>
@@ -4982,7 +4968,7 @@
         <v>9556915</v>
       </c>
       <c r="G22" s="26" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="H22" s="26"/>
       <c r="I22" s="26"/>
@@ -4992,10 +4978,10 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="C23" s="26"/>
       <c r="D23" s="26"/>
@@ -5004,7 +4990,7 @@
         <v>9556915</v>
       </c>
       <c r="G23" s="26" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="H23" s="26"/>
       <c r="I23" s="26"/>
@@ -5014,7 +5000,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B24" s="26" t="s">
         <v>22</v>
@@ -5026,7 +5012,7 @@
         <v>8820120</v>
       </c>
       <c r="G24" s="26" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="H24" s="26"/>
       <c r="I24" s="26"/>
@@ -5083,7 +5069,7 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -5093,7 +5079,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -5101,28 +5087,28 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F3" s="5">
         <v>1555602</v>
       </c>
       <c r="G3" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="J3" s="11">
         <v>1703477</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="L3" s="8"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B4" t="s">
         <v>22</v>
@@ -5131,35 +5117,35 @@
         <v>8820120</v>
       </c>
       <c r="G4" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F5" s="5">
         <v>1759199</v>
       </c>
       <c r="G5" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B7" t="s">
         <v>50</v>
@@ -5168,59 +5154,59 @@
         <v>1809376</v>
       </c>
       <c r="G7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F8" s="5">
         <v>1759172</v>
       </c>
       <c r="G8" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F11" s="5">
         <v>1809596</v>
       </c>
       <c r="G11" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -5229,16 +5215,16 @@
     </row>
     <row r="14" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="F14" s="24"/>
     </row>
     <row r="15" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C15" s="26"/>
       <c r="D15" s="26"/>
@@ -5247,7 +5233,7 @@
         <v>1555602</v>
       </c>
       <c r="G15" s="26" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="H15" s="26"/>
       <c r="I15" s="26"/>
@@ -5255,13 +5241,13 @@
         <v>1703477</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="L15" s="8"/>
     </row>
     <row r="16" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B16" s="26" t="s">
         <v>22</v>
@@ -5273,7 +5259,7 @@
         <v>8820120</v>
       </c>
       <c r="G16" s="26" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="H16" s="26"/>
       <c r="I16" s="26"/>
@@ -5283,10 +5269,10 @@
     </row>
     <row r="17" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C17" s="26"/>
       <c r="D17" s="26"/>
@@ -5295,7 +5281,7 @@
         <v>1759199</v>
       </c>
       <c r="G17" s="26" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="H17" s="26"/>
       <c r="I17" s="26"/>
@@ -5305,10 +5291,10 @@
     </row>
     <row r="18" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C18" s="26"/>
       <c r="D18" s="26"/>
@@ -5323,7 +5309,7 @@
     </row>
     <row r="19" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B19" s="26" t="s">
         <v>50</v>
@@ -5335,7 +5321,7 @@
         <v>1809376</v>
       </c>
       <c r="G19" s="26" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="H19" s="26"/>
       <c r="I19" s="26"/>
@@ -5345,10 +5331,10 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C20" s="26"/>
       <c r="D20" s="26"/>
@@ -5357,7 +5343,7 @@
         <v>1759172</v>
       </c>
       <c r="G20" s="26" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="H20" s="26"/>
       <c r="I20" s="26"/>
@@ -5367,10 +5353,10 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C21" s="26"/>
       <c r="D21" s="26"/>
@@ -5379,7 +5365,7 @@
         <v>1809596</v>
       </c>
       <c r="G21" s="26" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="H21" s="26"/>
       <c r="I21" s="26"/>
@@ -5389,10 +5375,10 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="C22" s="26"/>
       <c r="D22" s="26"/>
@@ -5401,7 +5387,7 @@
         <v>9556915</v>
       </c>
       <c r="G22" s="26" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="H22" s="26"/>
       <c r="I22" s="26"/>
@@ -5411,10 +5397,10 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="C23" s="26"/>
       <c r="D23" s="26"/>
@@ -5423,7 +5409,7 @@
         <v>9556915</v>
       </c>
       <c r="G23" s="26" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="H23" s="26"/>
       <c r="I23" s="26"/>
@@ -5433,7 +5419,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B24" s="26" t="s">
         <v>22</v>
@@ -5445,7 +5431,7 @@
         <v>8820120</v>
       </c>
       <c r="G24" s="26" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="H24" s="26"/>
       <c r="I24" s="26"/>
@@ -5503,7 +5489,7 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -5513,7 +5499,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -5521,31 +5507,31 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="12">
         <v>1845719</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="8" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="L3" s="8"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -5554,12 +5540,12 @@
         <v>1652909</v>
       </c>
       <c r="G4" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B5" t="s">
         <v>22</v>
@@ -5568,61 +5554,61 @@
         <v>8820120</v>
       </c>
       <c r="G5" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F6" s="5">
         <v>1414659</v>
       </c>
       <c r="G6" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="F7" s="5">
         <v>1618242</v>
       </c>
       <c r="G7" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="F8" s="5">
         <v>1618242</v>
       </c>
       <c r="G8" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -5632,7 +5618,7 @@
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
@@ -5640,31 +5626,31 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="12">
         <v>1845719</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="8" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="L11" s="8"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
@@ -5673,12 +5659,12 @@
         <v>1652909</v>
       </c>
       <c r="G12" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B13" t="s">
         <v>22</v>
@@ -5687,55 +5673,55 @@
         <v>8820120</v>
       </c>
       <c r="G13" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F14" s="5">
         <v>1414659</v>
       </c>
       <c r="G14" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B15" t="s">
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="F15" s="5">
         <v>1618242</v>
       </c>
       <c r="G15" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B16" t="s">
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="F16" s="5">
         <v>1618242</v>
       </c>
       <c r="G16" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="17" x14ac:dyDescent="0.25"/>
@@ -5782,7 +5768,7 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -5798,95 +5784,95 @@
     </row>
     <row r="3" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="B3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C3"/>
       <c r="F3" s="5">
         <v>1017798</v>
       </c>
       <c r="G3" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F4" s="5">
         <v>1465996</v>
       </c>
       <c r="G4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F5" s="5">
         <v>1809376</v>
       </c>
       <c r="G5" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F6" s="5">
         <v>1809303</v>
       </c>
       <c r="G6" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F7" s="5">
         <v>1809300</v>
       </c>
       <c r="G7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25"/>
@@ -5928,7 +5914,7 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -5938,7 +5924,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -5946,7 +5932,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B3" t="s">
         <v>22</v>
@@ -5955,12 +5941,12 @@
         <v>8820120</v>
       </c>
       <c r="G3" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B4" t="s">
         <v>50</v>
@@ -5969,12 +5955,12 @@
         <v>1809376</v>
       </c>
       <c r="G4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B5" t="s">
         <v>22</v>
@@ -5983,101 +5969,101 @@
         <v>8820120</v>
       </c>
       <c r="G5" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="B6" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="F6" s="5">
         <v>1809596</v>
       </c>
       <c r="G6" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="B7" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="F7" s="5">
         <v>1809596</v>
       </c>
       <c r="G7" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="B8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F8" s="5">
         <v>9556915</v>
       </c>
       <c r="G8" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="B9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F9" s="5">
         <v>9556915</v>
       </c>
       <c r="G9" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F10" s="5">
         <v>1887290</v>
       </c>
       <c r="G10" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="B12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -6123,7 +6109,7 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -6133,7 +6119,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -6141,7 +6127,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B3" t="s">
         <v>22</v>
@@ -6150,12 +6136,12 @@
         <v>8820120</v>
       </c>
       <c r="G3" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B4" t="s">
         <v>50</v>
@@ -6164,12 +6150,12 @@
         <v>1809376</v>
       </c>
       <c r="G4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B5" t="s">
         <v>22</v>
@@ -6178,101 +6164,101 @@
         <v>8820120</v>
       </c>
       <c r="G5" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
+        <v>345</v>
+      </c>
+      <c r="B6" t="s">
         <v>350</v>
-      </c>
-      <c r="B6" t="s">
-        <v>355</v>
       </c>
       <c r="F6" s="5">
         <v>1809596</v>
       </c>
       <c r="G6" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="B7" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="F7" s="5">
         <v>1809596</v>
       </c>
       <c r="G7" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="B8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F8" s="5">
         <v>9556915</v>
       </c>
       <c r="G8" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="B9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F9" s="5">
         <v>9556915</v>
       </c>
       <c r="G9" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F10" s="5">
         <v>1887290</v>
       </c>
       <c r="G10" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="B13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -6319,7 +6305,7 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -6329,7 +6315,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -6337,7 +6323,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B3" t="s">
         <v>22</v>
@@ -6346,12 +6332,12 @@
         <v>8820120</v>
       </c>
       <c r="G3" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B4" t="s">
         <v>50</v>
@@ -6360,12 +6346,12 @@
         <v>1809376</v>
       </c>
       <c r="G4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B5" t="s">
         <v>22</v>
@@ -6374,101 +6360,101 @@
         <v>8820120</v>
       </c>
       <c r="G5" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="B6" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="F6" s="5">
         <v>1809596</v>
       </c>
       <c r="G6" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B7" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="F7" s="5">
         <v>1809596</v>
       </c>
       <c r="G7" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="B8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F8" s="5">
         <v>9556915</v>
       </c>
       <c r="G8" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="B9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F9" s="5">
         <v>9556915</v>
       </c>
       <c r="G9" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F10" s="5">
         <v>1887290</v>
       </c>
       <c r="G10" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="B13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added XOR pulldown mod components and tidied layout on multiple tabs.
</commit_message>
<xml_diff>
--- a/PumaBom-WithMods-Element14.xlsx
+++ b/PumaBom-WithMods-Element14.xlsx
@@ -25,8 +25,360 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>el_presto</author>
+  </authors>
+  <commentList>
+    <comment ref="A31" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>el_presto:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Modification to be documented</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A34" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>el_presto:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Modification to be documented</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>el_presto</author>
+  </authors>
+  <commentList>
+    <comment ref="A4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>el_presto:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Modification to be documented / optional</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>el_presto:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Modification to be documented / optional</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>el_presto</author>
+  </authors>
+  <commentList>
+    <comment ref="A8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>el_presto:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Modification to be documented</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A16" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>el_presto:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Modification to be documented</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A24" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>el_presto:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Modification to be documented</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A32" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>el_presto:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Modification to be documented</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A40" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>el_presto:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Modification to be documented</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A48" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>el_presto:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Modification to be documented</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A56" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>el_presto:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Modification to be documented</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A64" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>el_presto:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Modification to be documented</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>el_presto</author>
+  </authors>
+  <commentList>
+    <comment ref="A12" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>el_presto:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+to be documented in how to.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="389">
   <si>
     <t>MCU</t>
   </si>
@@ -1184,13 +1536,22 @@
   </si>
   <si>
     <t xml:space="preserve">LM2937ET-5.0 IC, V REG LDO +5.0V, 2937, TO-220-3 </t>
+  </si>
+  <si>
+    <t>R Mod 100k pulldown</t>
+  </si>
+  <si>
+    <t>1% Resistor, MF12 Package &lt;-- will fit through via's</t>
+  </si>
+  <si>
+    <t>12 x</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1226,6 +1587,27 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="11">
@@ -1318,7 +1700,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1355,6 +1737,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1656,7 +2039,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
@@ -2517,6 +2900,7 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId44"/>
+  <legacyDrawing r:id="rId45"/>
 </worksheet>
 </file>
 
@@ -2528,7 +2912,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -2613,8 +2997,8 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
@@ -2634,7 +3018,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
@@ -3588,22 +3972,23 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId41"/>
+  <legacyDrawing r:id="rId42"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:R70"/>
+  <dimension ref="A1:R73"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="13" width="9.140625" customWidth="1"/>
-    <col min="14" max="14" width="27.28515625" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" customWidth="1"/>
     <col min="15" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
@@ -3740,720 +4125,745 @@
         <v>325</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>386</v>
+      </c>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="32" t="s">
+        <v>388</v>
+      </c>
+      <c r="F12" s="5">
+        <v>9342427</v>
+      </c>
+      <c r="G12" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4" t="s">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4" t="s">
         <v>371</v>
       </c>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B15" t="s">
         <v>40</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C15" t="s">
         <v>231</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F15" s="5">
         <v>9334084</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G15" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="B14" t="s">
-        <v>125</v>
-      </c>
-      <c r="F14" s="5">
-        <v>1686068</v>
-      </c>
-      <c r="G14" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="F15" s="9" t="s">
-        <v>314</v>
-      </c>
-      <c r="K15" s="9" t="s">
-        <v>313</v>
-      </c>
-      <c r="L15" s="9"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B16" t="s">
-        <v>173</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>378</v>
+        <v>125</v>
+      </c>
+      <c r="F16" s="5">
+        <v>1686068</v>
       </c>
       <c r="G16" t="s">
-        <v>379</v>
-      </c>
-      <c r="K16" s="5" t="s">
-        <v>378</v>
-      </c>
-      <c r="L16" t="s">
-        <v>379</v>
+        <v>239</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
-        <v>174</v>
-      </c>
-      <c r="B17" t="s">
-        <v>328</v>
-      </c>
+      <c r="A17" s="9"/>
+      <c r="F17" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="L17" s="9"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="B18" t="s">
+        <v>173</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="G18" t="s">
+        <v>379</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="L18" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>97</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F19" s="5">
         <v>1809596</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G19" t="s">
         <v>219</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="F19" s="5">
-        <v>1809303</v>
-      </c>
-      <c r="G19" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>199</v>
+        <v>176</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>76</v>
+        <v>129</v>
       </c>
       <c r="F20" s="5">
-        <v>1809300</v>
+        <v>1809303</v>
       </c>
       <c r="G20" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F21" s="5">
+        <v>1809300</v>
+      </c>
+      <c r="G21" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>82</v>
       </c>
-      <c r="F21" s="5">
+      <c r="F22" s="5">
         <v>9556915</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G22" t="s">
         <v>248</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="B22" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="B23" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B24" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B25" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4" t="s">
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4" t="s">
         <v>372</v>
       </c>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="4"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B28" t="s">
         <v>40</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C28" t="s">
         <v>231</v>
       </c>
-      <c r="F26" s="5">
+      <c r="F28" s="5">
         <v>9334084</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G28" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="B27" t="s">
-        <v>125</v>
-      </c>
-      <c r="F27" s="5">
-        <v>1686068</v>
-      </c>
-      <c r="G27" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="9"/>
-      <c r="F28" s="9" t="s">
-        <v>314</v>
-      </c>
-      <c r="K28" s="9" t="s">
-        <v>313</v>
-      </c>
-      <c r="L28" s="9"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B29" t="s">
-        <v>173</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>378</v>
+        <v>125</v>
+      </c>
+      <c r="F29" s="5">
+        <v>1686068</v>
       </c>
       <c r="G29" t="s">
-        <v>379</v>
-      </c>
-      <c r="K29" s="5" t="s">
-        <v>378</v>
-      </c>
-      <c r="L29" t="s">
-        <v>379</v>
+        <v>239</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="B30" t="s">
-        <v>328</v>
-      </c>
+      <c r="A30" s="9"/>
+      <c r="F30" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="K30" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="L30" s="9"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="B31" t="s">
+        <v>173</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="G31" t="s">
+        <v>379</v>
+      </c>
+      <c r="K31" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="L31" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>97</v>
       </c>
-      <c r="F31" s="5">
+      <c r="F32" s="5">
         <v>1809596</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G32" t="s">
         <v>219</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
-        <v>200</v>
-      </c>
-      <c r="B32" t="s">
-        <v>129</v>
-      </c>
-      <c r="F32" s="5">
-        <v>1809303</v>
-      </c>
-      <c r="G32" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
-        <v>201</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>76</v>
+        <v>200</v>
+      </c>
+      <c r="B33" t="s">
+        <v>129</v>
       </c>
       <c r="F33" s="5">
-        <v>1809300</v>
+        <v>1809303</v>
       </c>
       <c r="G33" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
+      <c r="A34" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F34" s="5">
+        <v>1809300</v>
+      </c>
+      <c r="G34" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>82</v>
       </c>
-      <c r="F34" s="5">
+      <c r="F35" s="5">
         <v>9556915</v>
       </c>
-      <c r="G34" t="s">
+      <c r="G35" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A35" s="10" t="s">
-        <v>217</v>
-      </c>
-      <c r="B35" t="s">
-        <v>329</v>
-      </c>
-      <c r="F35" s="5"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="B36" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="B37" t="s">
+        <v>329</v>
+      </c>
+      <c r="F37" s="5"/>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B38" t="s">
         <v>329</v>
       </c>
-      <c r="F36" s="5"/>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
+      <c r="F38" s="5"/>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
-      <c r="I38" s="4" t="s">
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4" t="s">
         <v>373</v>
       </c>
-      <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
-      <c r="L38" s="4"/>
-      <c r="M38" s="4"/>
-      <c r="N38" s="4"/>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A39" s="9" t="s">
+      <c r="J40" s="4"/>
+      <c r="K40" s="4"/>
+      <c r="L40" s="4"/>
+      <c r="M40" s="4"/>
+      <c r="N40" s="4"/>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B41" t="s">
         <v>40</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C41" t="s">
         <v>231</v>
       </c>
-      <c r="F39" s="5">
+      <c r="F41" s="5">
         <v>9334084</v>
       </c>
-      <c r="G39" t="s">
+      <c r="G41" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A40" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="B40" t="s">
-        <v>125</v>
-      </c>
-      <c r="F40" s="5">
-        <v>1686068</v>
-      </c>
-      <c r="G40" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A41" s="9"/>
-      <c r="F41" s="9" t="s">
-        <v>314</v>
-      </c>
-      <c r="K41" s="9" t="s">
-        <v>313</v>
-      </c>
-      <c r="L41" s="9"/>
-      <c r="M41" s="9"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B42" t="s">
-        <v>173</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>378</v>
+        <v>125</v>
+      </c>
+      <c r="F42" s="5">
+        <v>1686068</v>
       </c>
       <c r="G42" t="s">
-        <v>379</v>
-      </c>
-      <c r="K42" s="5" t="s">
-        <v>378</v>
-      </c>
-      <c r="L42" t="s">
-        <v>379</v>
-      </c>
-      <c r="P42" s="5" t="s">
-        <v>376</v>
-      </c>
-      <c r="R42" t="s">
-        <v>377</v>
+        <v>239</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A43" s="10" t="s">
-        <v>205</v>
-      </c>
-      <c r="B43" t="s">
-        <v>328</v>
-      </c>
+      <c r="A43" s="9"/>
+      <c r="F43" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="K43" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="L43" s="9"/>
+      <c r="M43" s="9"/>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="B44" t="s">
+        <v>173</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="G44" t="s">
+        <v>379</v>
+      </c>
+      <c r="K44" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="L44" t="s">
+        <v>379</v>
+      </c>
+      <c r="P44" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="R44" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A45" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>97</v>
       </c>
-      <c r="F44" s="5">
+      <c r="F45" s="5">
         <v>1809596</v>
       </c>
-      <c r="G44" t="s">
+      <c r="G45" t="s">
         <v>219</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A45" s="14" t="s">
-        <v>206</v>
-      </c>
-      <c r="B45" t="s">
-        <v>129</v>
-      </c>
-      <c r="F45" s="5">
-        <v>1809303</v>
-      </c>
-      <c r="G45" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
-        <v>207</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>76</v>
+        <v>206</v>
+      </c>
+      <c r="B46" t="s">
+        <v>129</v>
       </c>
       <c r="F46" s="5">
-        <v>1809300</v>
+        <v>1809303</v>
       </c>
       <c r="G46" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A47" s="9" t="s">
+      <c r="A47" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F47" s="5">
+        <v>1809300</v>
+      </c>
+      <c r="G47" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A48" s="9" t="s">
         <v>216</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>82</v>
       </c>
-      <c r="F47" s="5">
+      <c r="F48" s="5">
         <v>9556915</v>
       </c>
-      <c r="G47" t="s">
+      <c r="G48" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A48" s="10" t="s">
-        <v>215</v>
-      </c>
-      <c r="B48" t="s">
-        <v>329</v>
-      </c>
-      <c r="F48" s="5"/>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B49" t="s">
         <v>329</v>
       </c>
-      <c r="F49" s="5"/>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A50" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="B50" t="s">
+        <v>329</v>
+      </c>
+      <c r="F50" s="5"/>
+    </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
+      <c r="A51" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="B51" t="s">
+        <v>328</v>
+      </c>
+      <c r="F51" s="5"/>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="B51" s="4"/>
-      <c r="C51" s="4"/>
-      <c r="D51" s="4"/>
-      <c r="E51" s="4"/>
-      <c r="F51" s="4"/>
-      <c r="G51" s="4"/>
-      <c r="H51" s="4"/>
-      <c r="I51" s="4" t="s">
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="4" t="s">
         <v>374</v>
       </c>
-      <c r="J51" s="4"/>
-      <c r="K51" s="4"/>
-      <c r="L51" s="4"/>
-      <c r="M51" s="4"/>
-      <c r="N51" s="4"/>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A52" s="9" t="s">
+      <c r="J53" s="4"/>
+      <c r="K53" s="4"/>
+      <c r="L53" s="4"/>
+      <c r="M53" s="4"/>
+      <c r="N53" s="4"/>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A54" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B54" t="s">
         <v>40</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C54" t="s">
         <v>231</v>
       </c>
-      <c r="F52" s="5">
+      <c r="F54" s="5">
         <v>9334084</v>
       </c>
-      <c r="G52" t="s">
+      <c r="G54" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A53" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="B53" t="s">
-        <v>125</v>
-      </c>
-      <c r="F53" s="5">
-        <v>1686068</v>
-      </c>
-      <c r="G53" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A54" s="9"/>
-      <c r="F54" s="9" t="s">
-        <v>314</v>
-      </c>
-      <c r="K54" s="9" t="s">
-        <v>313</v>
-      </c>
-      <c r="L54" s="9"/>
-      <c r="M54" s="9"/>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>378</v>
+        <v>209</v>
+      </c>
+      <c r="B55" t="s">
+        <v>125</v>
+      </c>
+      <c r="F55" s="5">
+        <v>1686068</v>
       </c>
       <c r="G55" t="s">
-        <v>379</v>
-      </c>
-      <c r="K55" s="5" t="s">
-        <v>378</v>
-      </c>
-      <c r="L55" t="s">
-        <v>379</v>
-      </c>
-      <c r="M55" s="5"/>
+        <v>239</v>
+      </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A56" s="10" t="s">
-        <v>309</v>
-      </c>
-      <c r="B56" t="s">
-        <v>328</v>
-      </c>
+      <c r="A56" s="9"/>
+      <c r="F56" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="K56" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="L56" s="9"/>
+      <c r="M56" s="9"/>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="G57" t="s">
+        <v>379</v>
+      </c>
+      <c r="K57" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="L57" t="s">
+        <v>379</v>
+      </c>
+      <c r="M57" s="5"/>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A58" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B58" t="s">
         <v>97</v>
       </c>
-      <c r="F57" s="5">
+      <c r="F58" s="5">
         <v>1809596</v>
       </c>
-      <c r="G57" t="s">
+      <c r="G58" t="s">
         <v>219</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A58" s="14" t="s">
-        <v>211</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="F58" s="5">
-        <v>1809303</v>
-      </c>
-      <c r="G58" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="14" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>76</v>
+        <v>129</v>
       </c>
       <c r="F59" s="5">
-        <v>1809300</v>
+        <v>1809303</v>
       </c>
       <c r="G59" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A60" s="9" t="s">
+      <c r="A60" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F60" s="5">
+        <v>1809300</v>
+      </c>
+      <c r="G60" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A61" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B61" t="s">
         <v>82</v>
       </c>
-      <c r="F60" s="5">
+      <c r="F61" s="5">
         <v>9556915</v>
       </c>
-      <c r="G60" t="s">
+      <c r="G61" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A61" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="B61" t="s">
-        <v>329</v>
-      </c>
-      <c r="F61" s="5"/>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B62" t="s">
         <v>329</v>
       </c>
-      <c r="F62" s="5"/>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="1:14" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="65" hidden="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A63" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="B63" t="s">
+        <v>329</v>
+      </c>
+      <c r="F63" s="5"/>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A64" s="10" t="s">
+        <v>309</v>
+      </c>
+      <c r="B64" t="s">
+        <v>328</v>
+      </c>
+      <c r="F64" s="5"/>
+    </row>
+    <row r="65" x14ac:dyDescent="0.25"/>
     <row r="66" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="67" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="68" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="69" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="70" x14ac:dyDescent="0.25"/>
+    <row r="70" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="71" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="72" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="73" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F18" r:id="rId1" display="http://nz.element14.com/koa/rk73z2attd/resistor-0805-0-ohm-jumper/dp/1809596"/>
-    <hyperlink ref="F31" r:id="rId2" display="http://nz.element14.com/koa/rk73z2attd/resistor-0805-0-ohm-jumper/dp/1809596"/>
-    <hyperlink ref="F44" r:id="rId3" display="http://nz.element14.com/koa/rk73z2attd/resistor-0805-0-ohm-jumper/dp/1809596"/>
-    <hyperlink ref="F57" r:id="rId4" display="http://nz.element14.com/koa/rk73z2attd/resistor-0805-0-ohm-jumper/dp/1809596"/>
-    <hyperlink ref="F52" r:id="rId5" display="http://nz.element14.com/multicomp/mc-0-1w-0805-5-2k/resistor-0805-2k/dp/9334084"/>
-    <hyperlink ref="F39" r:id="rId6" display="http://nz.element14.com/multicomp/mc-0-1w-0805-5-2k/resistor-0805-2k/dp/9334084"/>
-    <hyperlink ref="F26" r:id="rId7" display="http://nz.element14.com/multicomp/mc-0-1w-0805-5-2k/resistor-0805-2k/dp/9334084"/>
-    <hyperlink ref="F13" r:id="rId8" display="http://nz.element14.com/multicomp/mc-0-1w-0805-5-2k/resistor-0805-2k/dp/9334084"/>
-    <hyperlink ref="F14" r:id="rId9" display="http://nz.element14.com/kingbright/kphcm-2012seck/led-smd-0805-orange/dp/1686068"/>
-    <hyperlink ref="F27" r:id="rId10" display="http://nz.element14.com/kingbright/kphcm-2012seck/led-smd-0805-orange/dp/1686068"/>
-    <hyperlink ref="F40" r:id="rId11" display="http://nz.element14.com/kingbright/kphcm-2012seck/led-smd-0805-orange/dp/1686068"/>
-    <hyperlink ref="F53" r:id="rId12" display="http://nz.element14.com/kingbright/kphcm-2012seck/led-smd-0805-orange/dp/1686068"/>
-    <hyperlink ref="F58" r:id="rId13" display="http://nz.element14.com/koa/rk73b2attd104j/resistor-0805-100k-ohm-5/dp/1809303"/>
-    <hyperlink ref="F45" r:id="rId14" display="http://nz.element14.com/koa/rk73b2attd104j/resistor-0805-100k-ohm-5/dp/1809303"/>
-    <hyperlink ref="F32" r:id="rId15" display="http://nz.element14.com/koa/rk73b2attd104j/resistor-0805-100k-ohm-5/dp/1809303"/>
-    <hyperlink ref="F19" r:id="rId16" display="http://nz.element14.com/koa/rk73b2attd104j/resistor-0805-100k-ohm-5/dp/1809303"/>
+    <hyperlink ref="F19" r:id="rId1" display="http://nz.element14.com/koa/rk73z2attd/resistor-0805-0-ohm-jumper/dp/1809596"/>
+    <hyperlink ref="F32" r:id="rId2" display="http://nz.element14.com/koa/rk73z2attd/resistor-0805-0-ohm-jumper/dp/1809596"/>
+    <hyperlink ref="F45" r:id="rId3" display="http://nz.element14.com/koa/rk73z2attd/resistor-0805-0-ohm-jumper/dp/1809596"/>
+    <hyperlink ref="F58" r:id="rId4" display="http://nz.element14.com/koa/rk73z2attd/resistor-0805-0-ohm-jumper/dp/1809596"/>
+    <hyperlink ref="F54" r:id="rId5" display="http://nz.element14.com/multicomp/mc-0-1w-0805-5-2k/resistor-0805-2k/dp/9334084"/>
+    <hyperlink ref="F41" r:id="rId6" display="http://nz.element14.com/multicomp/mc-0-1w-0805-5-2k/resistor-0805-2k/dp/9334084"/>
+    <hyperlink ref="F28" r:id="rId7" display="http://nz.element14.com/multicomp/mc-0-1w-0805-5-2k/resistor-0805-2k/dp/9334084"/>
+    <hyperlink ref="F15" r:id="rId8" display="http://nz.element14.com/multicomp/mc-0-1w-0805-5-2k/resistor-0805-2k/dp/9334084"/>
+    <hyperlink ref="F16" r:id="rId9" display="http://nz.element14.com/kingbright/kphcm-2012seck/led-smd-0805-orange/dp/1686068"/>
+    <hyperlink ref="F29" r:id="rId10" display="http://nz.element14.com/kingbright/kphcm-2012seck/led-smd-0805-orange/dp/1686068"/>
+    <hyperlink ref="F42" r:id="rId11" display="http://nz.element14.com/kingbright/kphcm-2012seck/led-smd-0805-orange/dp/1686068"/>
+    <hyperlink ref="F55" r:id="rId12" display="http://nz.element14.com/kingbright/kphcm-2012seck/led-smd-0805-orange/dp/1686068"/>
+    <hyperlink ref="F59" r:id="rId13" display="http://nz.element14.com/koa/rk73b2attd104j/resistor-0805-100k-ohm-5/dp/1809303"/>
+    <hyperlink ref="F46" r:id="rId14" display="http://nz.element14.com/koa/rk73b2attd104j/resistor-0805-100k-ohm-5/dp/1809303"/>
+    <hyperlink ref="F33" r:id="rId15" display="http://nz.element14.com/koa/rk73b2attd104j/resistor-0805-100k-ohm-5/dp/1809303"/>
+    <hyperlink ref="F20" r:id="rId16" display="http://nz.element14.com/koa/rk73b2attd104j/resistor-0805-100k-ohm-5/dp/1809303"/>
     <hyperlink ref="F9" r:id="rId17" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
     <hyperlink ref="F10" r:id="rId18" display="http://nz.element14.com/texas-instruments/sn74ls86ad/logic-quad-2-in-ex-or-gate-14soic/dp/1740035?Ntt=74ls86"/>
-    <hyperlink ref="F20" r:id="rId19" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
-    <hyperlink ref="F33" r:id="rId20" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
-    <hyperlink ref="F46" r:id="rId21" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
-    <hyperlink ref="F59" r:id="rId22" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
+    <hyperlink ref="F21" r:id="rId19" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
+    <hyperlink ref="F34" r:id="rId20" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
+    <hyperlink ref="F47" r:id="rId21" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
+    <hyperlink ref="F60" r:id="rId22" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
     <hyperlink ref="F3" r:id="rId23" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
     <hyperlink ref="F4" r:id="rId24" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
     <hyperlink ref="F5" r:id="rId25" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
     <hyperlink ref="F6" r:id="rId26" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
-    <hyperlink ref="F21" r:id="rId27" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
-    <hyperlink ref="F34" r:id="rId28" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
-    <hyperlink ref="F47" r:id="rId29" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
-    <hyperlink ref="F60" r:id="rId30" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
-    <hyperlink ref="F42" r:id="rId31" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
-    <hyperlink ref="P42" r:id="rId32" tooltip="Click to view additional information on this product." display="http://nz.mouser.com/ProductDetail/STMicroelectronics/VNP14NV04-E/?qs=sGAEpiMZZMuCmTIBzycWfOPiiwtMaP0Fv4CVvoRPcP8%3d"/>
-    <hyperlink ref="K42" r:id="rId33" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
-    <hyperlink ref="F29" r:id="rId34" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
-    <hyperlink ref="K29" r:id="rId35" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
-    <hyperlink ref="F16" r:id="rId36" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
-    <hyperlink ref="K16" r:id="rId37" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
-    <hyperlink ref="F55" r:id="rId38" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
-    <hyperlink ref="K55" r:id="rId39" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
+    <hyperlink ref="F22" r:id="rId27" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
+    <hyperlink ref="F35" r:id="rId28" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
+    <hyperlink ref="F48" r:id="rId29" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
+    <hyperlink ref="F61" r:id="rId30" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
+    <hyperlink ref="F44" r:id="rId31" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
+    <hyperlink ref="P44" r:id="rId32" tooltip="Click to view additional information on this product." display="http://nz.mouser.com/ProductDetail/STMicroelectronics/VNP14NV04-E/?qs=sGAEpiMZZMuCmTIBzycWfOPiiwtMaP0Fv4CVvoRPcP8%3d"/>
+    <hyperlink ref="K44" r:id="rId33" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
+    <hyperlink ref="F31" r:id="rId34" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
+    <hyperlink ref="K31" r:id="rId35" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
+    <hyperlink ref="F18" r:id="rId36" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
+    <hyperlink ref="K18" r:id="rId37" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
+    <hyperlink ref="F57" r:id="rId38" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
+    <hyperlink ref="K57" r:id="rId39" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
     <hyperlink ref="F7" r:id="rId40" display="http://nz.element14.com/vishay-draloric/crcw080510k0fkta/thick-film-chip-resistor/dp/1652909"/>
     <hyperlink ref="F8" r:id="rId41" display="http://nz.element14.com/vishay-draloric/crcw080510k0fkta/thick-film-chip-resistor/dp/1652909"/>
+    <hyperlink ref="F12" r:id="rId42" display="http://nz.element14.com/multicomp/mf12-100k/resistor-0-125w-1-100k/dp/9342427"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId42"/>
+  <pageSetup orientation="portrait" r:id="rId43"/>
+  <legacyDrawing r:id="rId44"/>
 </worksheet>
 </file>
 
@@ -5751,7 +6161,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
@@ -5893,6 +6303,7 @@
     <hyperlink ref="F3" r:id="rId5" display="http://nz.element14.com/fairchild-semiconductor/rfp30n06le/mosfet-n-logic-to-220/dp/1017798"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId6"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Fixed viewing issues on Primary parts, AAP and RPM pages. Added permanent link to Puma-HowTo
</commit_message>
<xml_diff>
--- a/PumaBom-WithMods-Element14.xlsx
+++ b/PumaBom-WithMods-Element14.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="423">
   <si>
     <t>MCU</t>
   </si>
@@ -907,9 +907,6 @@
     <t>Shutdown circuit design flawed do not use</t>
   </si>
   <si>
-    <t xml:space="preserve"> Not needed wire jumper too U4</t>
-  </si>
-  <si>
     <t>MOSFET, N, LOGIC, TO-220</t>
   </si>
   <si>
@@ -920,9 +917,6 @@
   </si>
   <si>
     <t>Link to Assembly / Mod guide</t>
-  </si>
-  <si>
-    <t>http://stuff.fredcooke.com/spin1howto/spin1.html</t>
   </si>
   <si>
     <t>R230</t>
@@ -1263,22 +1257,6 @@
     <t>USB Bus Powered Hack</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">10K SM pullup mod                                                </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1 x</t>
-    </r>
-  </si>
-  <si>
     <t>On Board Manifold Air Pressure (Added these components if you plan on having an ON board MAP sensor)</t>
   </si>
   <si>
@@ -1334,6 +1312,15 @@
   </si>
   <si>
     <t>1 x</t>
+  </si>
+  <si>
+    <t>10K SM pullup mod</t>
+  </si>
+  <si>
+    <t>Not needed wire jumper too U4</t>
+  </si>
+  <si>
+    <t>http://puma.freeems.org/how.to.guide/spin1/</t>
   </si>
 </sst>
 </file>
@@ -1736,7 +1723,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1833,10 +1820,32 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
@@ -1854,6 +1863,21 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1869,52 +1893,19 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2355,54 +2346,54 @@
         <v>238</v>
       </c>
       <c r="C2" s="17"/>
-      <c r="D2" s="91" t="s">
-        <v>388</v>
-      </c>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="72" t="s">
-        <v>296</v>
-      </c>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
-      <c r="K2" s="72"/>
+      <c r="D2" s="72" t="s">
+        <v>386</v>
+      </c>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="97" t="s">
+        <v>295</v>
+      </c>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
       <c r="L2" s="47"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="47"/>
       <c r="B3" s="47"/>
       <c r="C3" s="18"/>
-      <c r="D3" s="92" t="s">
-        <v>389</v>
-      </c>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="70" t="s">
-        <v>297</v>
-      </c>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
+      <c r="D3" s="76" t="s">
+        <v>387</v>
+      </c>
+      <c r="E3" s="77"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="80" t="s">
+        <v>422</v>
+      </c>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
       <c r="L3" s="47"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="47"/>
       <c r="B4" s="47"/>
       <c r="C4" s="19"/>
-      <c r="D4" s="91" t="s">
-        <v>390</v>
-      </c>
-      <c r="E4" s="68"/>
-      <c r="F4" s="68"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="71" t="s">
-        <v>387</v>
-      </c>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
-      <c r="K4" s="71"/>
+      <c r="D4" s="72" t="s">
+        <v>388</v>
+      </c>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="99" t="s">
+        <v>385</v>
+      </c>
+      <c r="I4" s="99"/>
+      <c r="J4" s="99"/>
+      <c r="K4" s="99"/>
       <c r="L4" s="47"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -2413,13 +2404,13 @@
       <c r="E5" s="47"/>
       <c r="F5" s="56"/>
       <c r="G5" s="47"/>
-      <c r="H5" s="73" t="s">
-        <v>386</v>
-      </c>
-      <c r="I5" s="73"/>
-      <c r="J5" s="73"/>
-      <c r="K5" s="73"/>
-      <c r="L5" s="73"/>
+      <c r="H5" s="83" t="s">
+        <v>384</v>
+      </c>
+      <c r="I5" s="83"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="83"/>
+      <c r="L5" s="83"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="47"/>
@@ -2436,22 +2427,22 @@
       <c r="L6" s="47"/>
     </row>
     <row r="7" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="83" t="s">
+      <c r="A7" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="83"/>
-      <c r="C7" s="83"/>
-      <c r="D7" s="83"/>
-      <c r="E7" s="83"/>
-      <c r="F7" s="83" t="s">
+      <c r="B7" s="85"/>
+      <c r="C7" s="85"/>
+      <c r="D7" s="85"/>
+      <c r="E7" s="85"/>
+      <c r="F7" s="85" t="s">
         <v>175</v>
       </c>
-      <c r="G7" s="83"/>
+      <c r="G7" s="85"/>
       <c r="H7" s="4"/>
-      <c r="I7" s="82" t="s">
-        <v>332</v>
-      </c>
-      <c r="J7" s="82"/>
+      <c r="I7" s="86" t="s">
+        <v>330</v>
+      </c>
+      <c r="J7" s="86"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
     </row>
@@ -2459,10 +2450,10 @@
       <c r="A8" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="68" t="s">
+      <c r="B8" s="73" t="s">
         <v>227</v>
       </c>
-      <c r="C8" s="68"/>
+      <c r="C8" s="73"/>
       <c r="F8" s="59">
         <v>1380343</v>
       </c>
@@ -2543,118 +2534,118 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="94" t="s">
+      <c r="A14" s="68" t="s">
         <v>7</v>
       </c>
       <c r="B14" s="42" t="s">
         <v>87</v>
       </c>
       <c r="C14" s="46" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="F14" s="59">
         <v>1740667</v>
       </c>
       <c r="G14" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="95" t="s">
+      <c r="A15" s="69" t="s">
         <v>9</v>
       </c>
       <c r="B15" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="F15" s="59">
         <v>1414699</v>
       </c>
       <c r="G15" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="95" t="s">
+      <c r="A16" s="69" t="s">
         <v>10</v>
       </c>
       <c r="B16" s="43" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="F16" s="59">
         <v>8820066</v>
       </c>
-      <c r="G16" s="68" t="s">
-        <v>383</v>
-      </c>
-      <c r="H16" s="68"/>
+      <c r="G16" s="73" t="s">
+        <v>381</v>
+      </c>
+      <c r="H16" s="73"/>
     </row>
     <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="96" t="s">
+      <c r="A17" s="70" t="s">
         <v>11</v>
       </c>
       <c r="B17" s="44" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C17" s="45"/>
       <c r="F17" s="59">
         <v>1887293</v>
       </c>
-      <c r="G17" s="68" t="s">
-        <v>384</v>
-      </c>
-      <c r="H17" s="68"/>
+      <c r="G17" s="73" t="s">
+        <v>382</v>
+      </c>
+      <c r="H17" s="73"/>
     </row>
     <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="97" t="s">
-        <v>368</v>
+      <c r="A18" s="71" t="s">
+        <v>366</v>
       </c>
       <c r="B18" s="35" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="39" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="F18" s="59">
         <v>1414676</v>
       </c>
-      <c r="G18" s="68" t="s">
+      <c r="G18" s="73" t="s">
         <v>224</v>
       </c>
-      <c r="H18" s="68"/>
-      <c r="I18" s="68"/>
+      <c r="H18" s="73"/>
+      <c r="I18" s="73"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="34"/>
       <c r="B19" s="37" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C19" s="36"/>
       <c r="F19" s="59">
         <v>1414668</v>
       </c>
-      <c r="G19" s="68" t="s">
-        <v>370</v>
-      </c>
-      <c r="H19" s="68"/>
-      <c r="I19" s="68"/>
+      <c r="G19" s="73" t="s">
+        <v>368</v>
+      </c>
+      <c r="H19" s="73"/>
+      <c r="I19" s="73"/>
     </row>
     <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="30"/>
       <c r="B20" s="38" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C20" s="36"/>
       <c r="F20" s="59">
         <v>1414685</v>
       </c>
-      <c r="G20" s="68" t="s">
-        <v>371</v>
-      </c>
-      <c r="H20" s="68"/>
-      <c r="I20" s="68"/>
+      <c r="G20" s="73" t="s">
+        <v>369</v>
+      </c>
+      <c r="H20" s="73"/>
+      <c r="I20" s="73"/>
     </row>
     <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="97" t="s">
+      <c r="A21" s="71" t="s">
         <v>13</v>
       </c>
       <c r="B21" s="35" t="s">
@@ -2664,39 +2655,39 @@
       <c r="F21" s="59">
         <v>1414676</v>
       </c>
-      <c r="G21" s="68" t="s">
+      <c r="G21" s="73" t="s">
         <v>224</v>
       </c>
-      <c r="H21" s="68"/>
-      <c r="I21" s="68"/>
+      <c r="H21" s="73"/>
+      <c r="I21" s="73"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="32"/>
       <c r="B22" s="29" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="F22" s="59">
         <v>1414668</v>
       </c>
-      <c r="G22" s="68" t="s">
-        <v>370</v>
-      </c>
-      <c r="H22" s="68"/>
-      <c r="I22" s="68"/>
+      <c r="G22" s="73" t="s">
+        <v>368</v>
+      </c>
+      <c r="H22" s="73"/>
+      <c r="I22" s="73"/>
     </row>
     <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="33"/>
       <c r="B23" s="31" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="F23" s="59">
         <v>1414685</v>
       </c>
-      <c r="G23" s="68" t="s">
-        <v>371</v>
-      </c>
-      <c r="H23" s="68"/>
-      <c r="I23" s="68"/>
+      <c r="G23" s="73" t="s">
+        <v>369</v>
+      </c>
+      <c r="H23" s="73"/>
+      <c r="I23" s="73"/>
     </row>
     <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="26" t="s">
@@ -2705,11 +2696,11 @@
       <c r="B24" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="89" t="s">
-        <v>393</v>
-      </c>
-      <c r="D24" s="68"/>
-      <c r="E24" s="68"/>
+      <c r="C24" s="74" t="s">
+        <v>391</v>
+      </c>
+      <c r="D24" s="73"/>
+      <c r="E24" s="73"/>
       <c r="F24" s="59">
         <v>1469858</v>
       </c>
@@ -2720,13 +2711,13 @@
     <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="13"/>
       <c r="B25" s="27" t="s">
-        <v>365</v>
-      </c>
-      <c r="C25" s="89" t="s">
-        <v>393</v>
-      </c>
-      <c r="D25" s="90"/>
-      <c r="E25" s="90"/>
+        <v>363</v>
+      </c>
+      <c r="C25" s="74" t="s">
+        <v>391</v>
+      </c>
+      <c r="D25" s="75"/>
+      <c r="E25" s="75"/>
       <c r="F25" s="59">
         <v>9332413</v>
       </c>
@@ -2744,11 +2735,11 @@
       <c r="F26" s="59">
         <v>1712841</v>
       </c>
-      <c r="G26" s="68" t="s">
+      <c r="G26" s="73" t="s">
         <v>219</v>
       </c>
-      <c r="H26" s="68"/>
-      <c r="I26" s="68"/>
+      <c r="H26" s="73"/>
+      <c r="I26" s="73"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
@@ -2760,14 +2751,14 @@
       <c r="F27" s="59">
         <v>1740667</v>
       </c>
-      <c r="G27" s="68" t="s">
-        <v>381</v>
-      </c>
-      <c r="H27" s="68"/>
+      <c r="G27" s="73" t="s">
+        <v>379</v>
+      </c>
+      <c r="H27" s="73"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B28" s="14" t="s">
         <v>87</v>
@@ -2775,10 +2766,10 @@
       <c r="F28" s="59">
         <v>1740667</v>
       </c>
-      <c r="G28" s="68" t="s">
-        <v>381</v>
-      </c>
-      <c r="H28" s="68"/>
+      <c r="G28" s="73" t="s">
+        <v>379</v>
+      </c>
+      <c r="H28" s="73"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
@@ -2787,10 +2778,10 @@
       <c r="B29" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="C29" s="86" t="s">
-        <v>380</v>
-      </c>
-      <c r="D29" s="86"/>
+      <c r="C29" s="78" t="s">
+        <v>378</v>
+      </c>
+      <c r="D29" s="78"/>
       <c r="F29" s="59">
         <v>1809300</v>
       </c>
@@ -2808,10 +2799,10 @@
       <c r="F30" s="59">
         <v>1740667</v>
       </c>
-      <c r="G30" s="68" t="s">
-        <v>381</v>
-      </c>
-      <c r="H30" s="68"/>
+      <c r="G30" s="73" t="s">
+        <v>379</v>
+      </c>
+      <c r="H30" s="73"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
@@ -2823,10 +2814,10 @@
       <c r="F31" s="59">
         <v>1740667</v>
       </c>
-      <c r="G31" s="68" t="s">
-        <v>381</v>
-      </c>
-      <c r="H31" s="68"/>
+      <c r="G31" s="73" t="s">
+        <v>379</v>
+      </c>
+      <c r="H31" s="73"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
@@ -2838,10 +2829,10 @@
       <c r="F32" s="59">
         <v>1740667</v>
       </c>
-      <c r="G32" s="68" t="s">
-        <v>381</v>
-      </c>
-      <c r="H32" s="68"/>
+      <c r="G32" s="73" t="s">
+        <v>379</v>
+      </c>
+      <c r="H32" s="73"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
@@ -2849,36 +2840,38 @@
       <c r="F33" s="59"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="69" t="s">
-        <v>403</v>
-      </c>
-      <c r="B34" s="69"/>
-      <c r="C34" s="69"/>
-      <c r="D34" s="69"/>
-      <c r="E34" s="69"/>
+      <c r="A34" s="88" t="s">
+        <v>420</v>
+      </c>
+      <c r="B34" s="88"/>
+      <c r="C34" s="88"/>
+      <c r="D34" s="88"/>
+      <c r="E34" s="98" t="s">
+        <v>419</v>
+      </c>
       <c r="F34" s="59">
         <v>1833277</v>
       </c>
       <c r="G34" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="74" t="s">
+      <c r="A36" s="84" t="s">
         <v>25</v>
       </c>
-      <c r="B36" s="74"/>
-      <c r="C36" s="74"/>
-      <c r="D36" s="74"/>
-      <c r="E36" s="74"/>
-      <c r="F36" s="74"/>
+      <c r="B36" s="84"/>
+      <c r="C36" s="84"/>
+      <c r="D36" s="84"/>
+      <c r="E36" s="84"/>
+      <c r="F36" s="84"/>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
-      <c r="I36" s="82" t="s">
-        <v>333</v>
-      </c>
-      <c r="J36" s="82"/>
+      <c r="I36" s="86" t="s">
+        <v>331</v>
+      </c>
+      <c r="J36" s="86"/>
       <c r="K36" s="4"/>
       <c r="L36" s="4"/>
     </row>
@@ -2906,28 +2899,28 @@
       <c r="F38" s="59">
         <v>8820120</v>
       </c>
-      <c r="G38" s="68" t="s">
+      <c r="G38" s="73" t="s">
         <v>218</v>
       </c>
-      <c r="H38" s="68"/>
+      <c r="H38" s="73"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="50"/>
       <c r="B39" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="C39" s="88" t="s">
+      <c r="C39" s="87" t="s">
         <v>217</v>
       </c>
-      <c r="D39" s="68"/>
-      <c r="E39" s="68"/>
+      <c r="D39" s="73"/>
+      <c r="E39" s="73"/>
       <c r="F39" s="59">
         <v>1853520</v>
       </c>
-      <c r="G39" s="68" t="s">
-        <v>385</v>
-      </c>
-      <c r="H39" s="68"/>
+      <c r="G39" s="73" t="s">
+        <v>383</v>
+      </c>
+      <c r="H39" s="73"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
@@ -2939,10 +2932,10 @@
       <c r="F40" s="59">
         <v>8820120</v>
       </c>
-      <c r="G40" s="68" t="s">
+      <c r="G40" s="73" t="s">
         <v>218</v>
       </c>
-      <c r="H40" s="68"/>
+      <c r="H40" s="73"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
@@ -2963,28 +2956,28 @@
       <c r="A42" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B42" s="68" t="s">
+      <c r="B42" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="C42" s="68"/>
-      <c r="D42" s="68"/>
+      <c r="C42" s="73"/>
+      <c r="D42" s="73"/>
       <c r="F42" s="59">
         <v>9406352</v>
       </c>
-      <c r="G42" s="68" t="s">
+      <c r="G42" s="73" t="s">
         <v>239</v>
       </c>
-      <c r="H42" s="68"/>
+      <c r="H42" s="73"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B43" s="68" t="s">
+      <c r="B43" s="73" t="s">
         <v>169</v>
       </c>
-      <c r="C43" s="68"/>
-      <c r="D43" s="68"/>
+      <c r="C43" s="73"/>
+      <c r="D43" s="73"/>
       <c r="F43" s="59">
         <v>1355761</v>
       </c>
@@ -3053,40 +3046,40 @@
       <c r="F48" s="59"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A49" s="69" t="s">
-        <v>402</v>
-      </c>
-      <c r="B49" s="69"/>
-      <c r="C49" s="69"/>
+      <c r="A49" s="88" t="s">
+        <v>400</v>
+      </c>
+      <c r="B49" s="88"/>
+      <c r="C49" s="88"/>
       <c r="D49" s="1"/>
       <c r="E49" s="10" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="F49" s="59">
         <v>9558527</v>
       </c>
-      <c r="G49" s="68" t="s">
-        <v>401</v>
-      </c>
-      <c r="H49" s="68"/>
-      <c r="I49" s="68"/>
+      <c r="G49" s="73" t="s">
+        <v>399</v>
+      </c>
+      <c r="H49" s="73"/>
+      <c r="I49" s="73"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" s="74" t="s">
+      <c r="A51" s="84" t="s">
         <v>49</v>
       </c>
-      <c r="B51" s="74"/>
-      <c r="C51" s="74"/>
-      <c r="D51" s="74"/>
-      <c r="E51" s="74"/>
-      <c r="F51" s="74"/>
+      <c r="B51" s="84"/>
+      <c r="C51" s="84"/>
+      <c r="D51" s="84"/>
+      <c r="E51" s="84"/>
+      <c r="F51" s="84"/>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
-      <c r="I51" s="82" t="s">
-        <v>334</v>
-      </c>
-      <c r="J51" s="82"/>
+      <c r="I51" s="86" t="s">
+        <v>332</v>
+      </c>
+      <c r="J51" s="86"/>
       <c r="K51" s="4"/>
       <c r="L51" s="4"/>
     </row>
@@ -3100,12 +3093,12 @@
       <c r="F52" s="59">
         <v>1556741</v>
       </c>
-      <c r="G52" s="68" t="s">
+      <c r="G52" s="73" t="s">
         <v>182</v>
       </c>
-      <c r="H52" s="68"/>
-      <c r="I52" s="68"/>
-      <c r="J52" s="68"/>
+      <c r="H52" s="73"/>
+      <c r="I52" s="73"/>
+      <c r="J52" s="73"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
@@ -3117,12 +3110,12 @@
       <c r="F53" s="59">
         <v>9229272</v>
       </c>
-      <c r="G53" s="68" t="s">
+      <c r="G53" s="73" t="s">
         <v>229</v>
       </c>
-      <c r="H53" s="68"/>
-      <c r="I53" s="68"/>
-      <c r="J53" s="68"/>
+      <c r="H53" s="73"/>
+      <c r="I53" s="73"/>
+      <c r="J53" s="73"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
@@ -3134,12 +3127,12 @@
       <c r="F54" s="59">
         <v>8820120</v>
       </c>
-      <c r="G54" s="68" t="s">
+      <c r="G54" s="73" t="s">
         <v>218</v>
       </c>
-      <c r="H54" s="68"/>
-      <c r="I54" s="68"/>
-      <c r="J54" s="68"/>
+      <c r="H54" s="73"/>
+      <c r="I54" s="73"/>
+      <c r="J54" s="73"/>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
@@ -3151,12 +3144,12 @@
       <c r="F55" s="59">
         <v>9556915</v>
       </c>
-      <c r="G55" s="68" t="s">
+      <c r="G55" s="73" t="s">
         <v>235</v>
       </c>
-      <c r="H55" s="68"/>
-      <c r="I55" s="68"/>
-      <c r="J55" s="68"/>
+      <c r="H55" s="73"/>
+      <c r="I55" s="73"/>
+      <c r="J55" s="73"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
@@ -3168,12 +3161,12 @@
       <c r="F56" s="59">
         <v>1617365</v>
       </c>
-      <c r="G56" s="68" t="s">
+      <c r="G56" s="73" t="s">
         <v>228</v>
       </c>
-      <c r="H56" s="68"/>
-      <c r="I56" s="68"/>
-      <c r="J56" s="68"/>
+      <c r="H56" s="73"/>
+      <c r="I56" s="73"/>
+      <c r="J56" s="73"/>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
@@ -3185,12 +3178,12 @@
       <c r="F57" s="59">
         <v>8820120</v>
       </c>
-      <c r="G57" s="68" t="s">
+      <c r="G57" s="73" t="s">
         <v>218</v>
       </c>
-      <c r="H57" s="68"/>
-      <c r="I57" s="68"/>
-      <c r="J57" s="68"/>
+      <c r="H57" s="73"/>
+      <c r="I57" s="73"/>
+      <c r="J57" s="73"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
@@ -3199,29 +3192,29 @@
       <c r="B58" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C58" s="68" t="s">
-        <v>394</v>
-      </c>
-      <c r="D58" s="68"/>
-      <c r="E58" s="68"/>
+      <c r="C58" s="73" t="s">
+        <v>392</v>
+      </c>
+      <c r="D58" s="73"/>
+      <c r="E58" s="73"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="61" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="74" t="s">
+      <c r="A61" s="84" t="s">
         <v>56</v>
       </c>
-      <c r="B61" s="74"/>
-      <c r="C61" s="74"/>
-      <c r="D61" s="74"/>
-      <c r="E61" s="74"/>
+      <c r="B61" s="84"/>
+      <c r="C61" s="84"/>
+      <c r="D61" s="84"/>
+      <c r="E61" s="84"/>
       <c r="F61" s="60"/>
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
-      <c r="I61" s="82" t="s">
-        <v>335</v>
-      </c>
-      <c r="J61" s="82"/>
+      <c r="I61" s="86" t="s">
+        <v>333</v>
+      </c>
+      <c r="J61" s="86"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
@@ -3233,12 +3226,12 @@
       <c r="F62" s="59">
         <v>9486038</v>
       </c>
-      <c r="G62" s="87" t="s">
-        <v>358</v>
-      </c>
-      <c r="H62" s="87"/>
-      <c r="I62" s="87"/>
-      <c r="J62" s="87"/>
+      <c r="G62" s="79" t="s">
+        <v>356</v>
+      </c>
+      <c r="H62" s="79"/>
+      <c r="I62" s="79"/>
+      <c r="J62" s="79"/>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
@@ -3250,11 +3243,11 @@
       <c r="F63" s="59">
         <v>1324152</v>
       </c>
-      <c r="G63" s="68" t="s">
+      <c r="G63" s="73" t="s">
         <v>230</v>
       </c>
-      <c r="H63" s="68"/>
-      <c r="I63" s="68"/>
+      <c r="H63" s="73"/>
+      <c r="I63" s="73"/>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
@@ -3266,11 +3259,11 @@
       <c r="F64" s="59">
         <v>1617365</v>
       </c>
-      <c r="G64" s="68" t="s">
+      <c r="G64" s="73" t="s">
         <v>228</v>
       </c>
-      <c r="H64" s="68"/>
-      <c r="I64" s="68"/>
+      <c r="H64" s="73"/>
+      <c r="I64" s="73"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
@@ -3282,11 +3275,11 @@
       <c r="F65" s="59">
         <v>8820120</v>
       </c>
-      <c r="G65" s="68" t="s">
+      <c r="G65" s="73" t="s">
         <v>218</v>
       </c>
-      <c r="H65" s="68"/>
-      <c r="I65" s="68"/>
+      <c r="H65" s="73"/>
+      <c r="I65" s="73"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
@@ -3298,11 +3291,11 @@
       <c r="F66" s="59">
         <v>9229272</v>
       </c>
-      <c r="G66" s="68" t="s">
+      <c r="G66" s="73" t="s">
         <v>229</v>
       </c>
-      <c r="H66" s="68"/>
-      <c r="I66" s="68"/>
+      <c r="H66" s="73"/>
+      <c r="I66" s="73"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="23" t="s">
@@ -3314,11 +3307,11 @@
       <c r="F67" s="59">
         <v>1617365</v>
       </c>
-      <c r="G67" s="68" t="s">
+      <c r="G67" s="73" t="s">
         <v>228</v>
       </c>
-      <c r="H67" s="68"/>
-      <c r="I67" s="68"/>
+      <c r="H67" s="73"/>
+      <c r="I67" s="73"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
@@ -3330,11 +3323,11 @@
       <c r="F68" s="59">
         <v>8820120</v>
       </c>
-      <c r="G68" s="68" t="s">
+      <c r="G68" s="73" t="s">
         <v>218</v>
       </c>
-      <c r="H68" s="68"/>
-      <c r="I68" s="68"/>
+      <c r="H68" s="73"/>
+      <c r="I68" s="73"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="9"/>
@@ -3344,49 +3337,49 @@
       <c r="A70" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B70" s="69" t="s">
+      <c r="B70" s="88" t="s">
         <v>291</v>
       </c>
-      <c r="C70" s="69"/>
-      <c r="D70" s="69"/>
-      <c r="E70" s="69"/>
-      <c r="F70" s="69"/>
+      <c r="C70" s="88"/>
+      <c r="D70" s="88"/>
+      <c r="E70" s="88"/>
+      <c r="F70" s="88"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B71" s="69" t="s">
+      <c r="B71" s="88" t="s">
         <v>291</v>
       </c>
-      <c r="C71" s="69"/>
-      <c r="D71" s="69"/>
-      <c r="E71" s="69"/>
-      <c r="F71" s="69"/>
+      <c r="C71" s="88"/>
+      <c r="D71" s="88"/>
+      <c r="E71" s="88"/>
+      <c r="F71" s="88"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B72" s="69" t="s">
+      <c r="B72" s="88" t="s">
         <v>291</v>
       </c>
-      <c r="C72" s="69"/>
-      <c r="D72" s="69"/>
-      <c r="E72" s="69"/>
-      <c r="F72" s="69"/>
+      <c r="C72" s="88"/>
+      <c r="D72" s="88"/>
+      <c r="E72" s="88"/>
+      <c r="F72" s="88"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B73" s="69" t="s">
+      <c r="B73" s="88" t="s">
         <v>291</v>
       </c>
-      <c r="C73" s="69"/>
-      <c r="D73" s="69"/>
-      <c r="E73" s="69"/>
-      <c r="F73" s="69"/>
+      <c r="C73" s="88"/>
+      <c r="D73" s="88"/>
+      <c r="E73" s="88"/>
+      <c r="F73" s="88"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="10" t="s">
@@ -3400,12 +3393,12 @@
       <c r="A75" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B75" s="69" t="s">
-        <v>292</v>
-      </c>
-      <c r="C75" s="69"/>
-      <c r="D75" s="69"/>
-      <c r="E75" s="69"/>
+      <c r="B75" s="88" t="s">
+        <v>421</v>
+      </c>
+      <c r="C75" s="88"/>
+      <c r="D75" s="88"/>
+      <c r="E75" s="88"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25"/>
     <row r="77" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
@@ -3423,55 +3416,7 @@
     <row r="87" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G56:J56"/>
-    <mergeCell ref="G55:J55"/>
-    <mergeCell ref="G54:J54"/>
-    <mergeCell ref="G53:J53"/>
-    <mergeCell ref="G52:J52"/>
-    <mergeCell ref="G65:I65"/>
-    <mergeCell ref="G64:I64"/>
-    <mergeCell ref="G63:I63"/>
-    <mergeCell ref="G62:J62"/>
-    <mergeCell ref="G57:J57"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="H5:L5"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="A36:F36"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="C39:E39"/>
     <mergeCell ref="C58:E58"/>
-    <mergeCell ref="A34:E34"/>
     <mergeCell ref="G49:I49"/>
     <mergeCell ref="A49:C49"/>
     <mergeCell ref="B75:E75"/>
@@ -3486,6 +3431,54 @@
     <mergeCell ref="G68:I68"/>
     <mergeCell ref="G67:I67"/>
     <mergeCell ref="G66:I66"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="G65:I65"/>
+    <mergeCell ref="G64:I64"/>
+    <mergeCell ref="G63:I63"/>
+    <mergeCell ref="G62:J62"/>
+    <mergeCell ref="G57:J57"/>
+    <mergeCell ref="G56:J56"/>
+    <mergeCell ref="G55:J55"/>
+    <mergeCell ref="G54:J54"/>
+    <mergeCell ref="G53:J53"/>
+    <mergeCell ref="G52:J52"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="H5:L5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F8" r:id="rId1" display="http://nz.element14.com/freescale-semiconductor/mc9s12xdp512mal/ic-16bit-microcontroller/dp/1380343"/>
@@ -3513,34 +3506,34 @@
     <hyperlink ref="F63" r:id="rId23" display="http://nz.element14.com/fairchild-semiconductor/1n4007/bridge-rectifier-rohs-compliant/dp/9109625"/>
     <hyperlink ref="F29" r:id="rId24" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
     <hyperlink ref="F42" r:id="rId25" display="http://nz.element14.com/multicomp/u0805r103kct/capacitor-0805-10nf-50v/dp/9406352"/>
-    <hyperlink ref="H3" r:id="rId26"/>
-    <hyperlink ref="F55" r:id="rId27" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
-    <hyperlink ref="F9" r:id="rId28" display="http://nz.element14.com/vishay-draloric/crcw080510k0fkta/thick-film-chip-resistor/dp/1652909"/>
-    <hyperlink ref="F10" r:id="rId29" display="http://nz.element14.com/vishay-draloric/crcw080510k0fkta/thick-film-chip-resistor/dp/1652909"/>
-    <hyperlink ref="F11" r:id="rId30" display="http://nz.element14.com/vishay-draloric/crcw080510k0fkta/thick-film-chip-resistor/dp/1652909"/>
-    <hyperlink ref="F12" r:id="rId31" display="http://nz.element14.com/vishay-draloric/crcw080510k0fkta/thick-film-chip-resistor/dp/1652909"/>
-    <hyperlink ref="F13" r:id="rId32" display="http://nz.element14.com/vishay-draloric/crcw080510k0fkta/thick-film-chip-resistor/dp/1652909"/>
-    <hyperlink ref="F67" r:id="rId33" display="http://nz.element14.com/vishay-sprague/199d106x9035d1v1e3/capacitor-tant-10uf-35v-radial/dp/1617365"/>
-    <hyperlink ref="F21" r:id="rId34" display="http://nz.element14.com/kemet/c0805c220j1gactu/capacitor-0805-22pf-100v-np0/dp/1414676"/>
-    <hyperlink ref="F19" r:id="rId35" display="http://nz.element14.com/kemet/c0805c150j5gactu/capacitor-0805-15pf-50v-np0/dp/1414668"/>
-    <hyperlink ref="F22" r:id="rId36" display="http://nz.element14.com/kemet/c0805c150j5gactu/capacitor-0805-15pf-50v-np0/dp/1414668"/>
-    <hyperlink ref="F20" r:id="rId37" display="http://nz.element14.com/kemet/c0805c330j5gactu/capacitor-0805-33pf-50v-np0/dp/1414685"/>
-    <hyperlink ref="F23" r:id="rId38" display="http://nz.element14.com/kemet/c0805c330j5gactu/capacitor-0805-33pf-50v-np0/dp/1414685"/>
-    <hyperlink ref="F14" r:id="rId39" display="http://nz.element14.com/avx/08053c224jat2a/capacitor-mlcc-0805-25v-220nf/dp/1740667"/>
-    <hyperlink ref="F27" r:id="rId40" display="http://nz.element14.com/avx/08053c224jat2a/capacitor-mlcc-0805-25v-220nf/dp/1740667"/>
-    <hyperlink ref="F28" r:id="rId41" display="http://nz.element14.com/avx/08053c224jat2a/capacitor-mlcc-0805-25v-220nf/dp/1740667"/>
-    <hyperlink ref="F30" r:id="rId42" display="http://nz.element14.com/avx/08053c224jat2a/capacitor-mlcc-0805-25v-220nf/dp/1740667"/>
-    <hyperlink ref="F31" r:id="rId43" display="http://nz.element14.com/avx/08053c224jat2a/capacitor-mlcc-0805-25v-220nf/dp/1740667"/>
-    <hyperlink ref="F32" r:id="rId44" display="http://nz.element14.com/avx/08053c224jat2a/capacitor-mlcc-0805-25v-220nf/dp/1740667"/>
-    <hyperlink ref="F15" r:id="rId45" display="http://nz.element14.com/kemet"/>
-    <hyperlink ref="F16" r:id="rId46" display="http://nz.element14.com/murata/grm2195c1h682ja01d/capacitor-0805-6-8nf-50v/dp/8820066"/>
-    <hyperlink ref="F17" r:id="rId47" display="http://nz.element14.com/multicomp/mcpwr05ftew3301/resistor-0805-3-3k-1-0-125w/dp/1887293"/>
-    <hyperlink ref="F24" r:id="rId48" display="http://nz.element14.com/yageo-phycomp/rc0805fr-0710ml/resistor-rc12h-0805-10m/dp/9238115"/>
-    <hyperlink ref="F25" r:id="rId49" display="http://nz.element14.com/multicomp/mc-0-1w-0805-1-1m/resistor-1mohm-0-1w-1/dp/9332413"/>
-    <hyperlink ref="F39" r:id="rId50" display="http://nz.element14.com/taiyo-yuden/emk212b7475kg-t/capacitor-ceramic-4-7uf-16v-x7r/dp/1853520"/>
-    <hyperlink ref="H5" r:id="rId51"/>
-    <hyperlink ref="F34" r:id="rId52" display="http://nz.element14.com/welwyn/mfr3-10kfc/resistor-metal-film-10kohm-400mw/dp/1833277"/>
-    <hyperlink ref="F49" r:id="rId53" display="http://nz.element14.com/on-semiconductor/bc557bzl1g/transistor-pnp-45v-0-1a-to-92/dp/9558527"/>
+    <hyperlink ref="F55" r:id="rId26" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
+    <hyperlink ref="F9" r:id="rId27" display="http://nz.element14.com/vishay-draloric/crcw080510k0fkta/thick-film-chip-resistor/dp/1652909"/>
+    <hyperlink ref="F10" r:id="rId28" display="http://nz.element14.com/vishay-draloric/crcw080510k0fkta/thick-film-chip-resistor/dp/1652909"/>
+    <hyperlink ref="F11" r:id="rId29" display="http://nz.element14.com/vishay-draloric/crcw080510k0fkta/thick-film-chip-resistor/dp/1652909"/>
+    <hyperlink ref="F12" r:id="rId30" display="http://nz.element14.com/vishay-draloric/crcw080510k0fkta/thick-film-chip-resistor/dp/1652909"/>
+    <hyperlink ref="F13" r:id="rId31" display="http://nz.element14.com/vishay-draloric/crcw080510k0fkta/thick-film-chip-resistor/dp/1652909"/>
+    <hyperlink ref="F67" r:id="rId32" display="http://nz.element14.com/vishay-sprague/199d106x9035d1v1e3/capacitor-tant-10uf-35v-radial/dp/1617365"/>
+    <hyperlink ref="F21" r:id="rId33" display="http://nz.element14.com/kemet/c0805c220j1gactu/capacitor-0805-22pf-100v-np0/dp/1414676"/>
+    <hyperlink ref="F19" r:id="rId34" display="http://nz.element14.com/kemet/c0805c150j5gactu/capacitor-0805-15pf-50v-np0/dp/1414668"/>
+    <hyperlink ref="F22" r:id="rId35" display="http://nz.element14.com/kemet/c0805c150j5gactu/capacitor-0805-15pf-50v-np0/dp/1414668"/>
+    <hyperlink ref="F20" r:id="rId36" display="http://nz.element14.com/kemet/c0805c330j5gactu/capacitor-0805-33pf-50v-np0/dp/1414685"/>
+    <hyperlink ref="F23" r:id="rId37" display="http://nz.element14.com/kemet/c0805c330j5gactu/capacitor-0805-33pf-50v-np0/dp/1414685"/>
+    <hyperlink ref="F14" r:id="rId38" display="http://nz.element14.com/avx/08053c224jat2a/capacitor-mlcc-0805-25v-220nf/dp/1740667"/>
+    <hyperlink ref="F27" r:id="rId39" display="http://nz.element14.com/avx/08053c224jat2a/capacitor-mlcc-0805-25v-220nf/dp/1740667"/>
+    <hyperlink ref="F28" r:id="rId40" display="http://nz.element14.com/avx/08053c224jat2a/capacitor-mlcc-0805-25v-220nf/dp/1740667"/>
+    <hyperlink ref="F30" r:id="rId41" display="http://nz.element14.com/avx/08053c224jat2a/capacitor-mlcc-0805-25v-220nf/dp/1740667"/>
+    <hyperlink ref="F31" r:id="rId42" display="http://nz.element14.com/avx/08053c224jat2a/capacitor-mlcc-0805-25v-220nf/dp/1740667"/>
+    <hyperlink ref="F32" r:id="rId43" display="http://nz.element14.com/avx/08053c224jat2a/capacitor-mlcc-0805-25v-220nf/dp/1740667"/>
+    <hyperlink ref="F15" r:id="rId44" display="http://nz.element14.com/kemet"/>
+    <hyperlink ref="F16" r:id="rId45" display="http://nz.element14.com/murata/grm2195c1h682ja01d/capacitor-0805-6-8nf-50v/dp/8820066"/>
+    <hyperlink ref="F17" r:id="rId46" display="http://nz.element14.com/multicomp/mcpwr05ftew3301/resistor-0805-3-3k-1-0-125w/dp/1887293"/>
+    <hyperlink ref="F24" r:id="rId47" display="http://nz.element14.com/yageo-phycomp/rc0805fr-0710ml/resistor-rc12h-0805-10m/dp/9238115"/>
+    <hyperlink ref="F25" r:id="rId48" display="http://nz.element14.com/multicomp/mc-0-1w-0805-1-1m/resistor-1mohm-0-1w-1/dp/9332413"/>
+    <hyperlink ref="F39" r:id="rId49" display="http://nz.element14.com/taiyo-yuden/emk212b7475kg-t/capacitor-ceramic-4-7uf-16v-x7r/dp/1853520"/>
+    <hyperlink ref="H5" r:id="rId50"/>
+    <hyperlink ref="F34" r:id="rId51" display="http://nz.element14.com/welwyn/mfr3-10kfc/resistor-metal-film-10kohm-400mw/dp/1833277"/>
+    <hyperlink ref="F49" r:id="rId52" display="http://nz.element14.com/on-semiconductor/bc557bzl1g/transistor-pnp-45v-0-1a-to-92/dp/9558527"/>
+    <hyperlink ref="H3" r:id="rId53"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" orientation="landscape" r:id="rId54"/>
@@ -3567,26 +3560,26 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="85" t="s">
         <v>144</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="58"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="82" t="s">
-        <v>375</v>
-      </c>
-      <c r="J2" s="82"/>
-      <c r="K2" s="82"/>
+      <c r="I2" s="86" t="s">
+        <v>373</v>
+      </c>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
       <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B3" t="s">
         <v>48</v>
@@ -3600,7 +3593,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
@@ -3614,7 +3607,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B5" t="s">
         <v>79</v>
@@ -3628,7 +3621,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B6" t="s">
         <v>79</v>
@@ -3642,7 +3635,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>94</v>
@@ -3702,21 +3695,21 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="85" t="s">
         <v>145</v>
       </c>
-      <c r="B2" s="83"/>
+      <c r="B2" s="85"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="58"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="82" t="s">
-        <v>337</v>
-      </c>
-      <c r="J2" s="82"/>
-      <c r="K2" s="82"/>
+      <c r="I2" s="86" t="s">
+        <v>335</v>
+      </c>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
@@ -3771,10 +3764,10 @@
         <v>150</v>
       </c>
       <c r="F6" s="64" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
@@ -3787,16 +3780,16 @@
         <v>152</v>
       </c>
       <c r="F7" s="59" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="G7" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="M7" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -3809,21 +3802,21 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="83" t="s">
+      <c r="A10" s="85" t="s">
         <v>154</v>
       </c>
-      <c r="B10" s="83"/>
+      <c r="B10" s="85"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="58"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
-      <c r="I10" s="82" t="s">
-        <v>338</v>
-      </c>
-      <c r="J10" s="82"/>
-      <c r="K10" s="82"/>
+      <c r="I10" s="86" t="s">
+        <v>336</v>
+      </c>
+      <c r="J10" s="86"/>
+      <c r="K10" s="86"/>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
@@ -3878,10 +3871,10 @@
         <v>150</v>
       </c>
       <c r="F14" s="64" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="L14" s="9"/>
       <c r="M14" s="9"/>
@@ -3894,19 +3887,19 @@
         <v>152</v>
       </c>
       <c r="F15" s="59" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="G15" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="M15" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="N15" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -3919,21 +3912,21 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25"/>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="83" t="s">
+      <c r="A18" s="85" t="s">
         <v>155</v>
       </c>
-      <c r="B18" s="83"/>
+      <c r="B18" s="85"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="58"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
-      <c r="I18" s="82" t="s">
-        <v>339</v>
-      </c>
-      <c r="J18" s="82"/>
-      <c r="K18" s="82"/>
+      <c r="I18" s="86" t="s">
+        <v>337</v>
+      </c>
+      <c r="J18" s="86"/>
+      <c r="K18" s="86"/>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
@@ -3988,10 +3981,10 @@
         <v>150</v>
       </c>
       <c r="F22" s="64" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K22" s="9" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="L22" s="9"/>
       <c r="M22" s="9"/>
@@ -4004,19 +3997,19 @@
         <v>152</v>
       </c>
       <c r="F23" s="59" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="G23" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="M23" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="N23" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -4029,21 +4022,21 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="83" t="s">
+      <c r="A26" s="85" t="s">
         <v>156</v>
       </c>
-      <c r="B26" s="83"/>
+      <c r="B26" s="85"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="58"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
-      <c r="I26" s="82" t="s">
-        <v>340</v>
-      </c>
-      <c r="J26" s="82"/>
-      <c r="K26" s="82"/>
+      <c r="I26" s="86" t="s">
+        <v>338</v>
+      </c>
+      <c r="J26" s="86"/>
+      <c r="K26" s="86"/>
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
       <c r="N26" s="4"/>
@@ -4098,10 +4091,10 @@
         <v>150</v>
       </c>
       <c r="F30" s="64" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K30" s="9" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="L30" s="9"/>
       <c r="M30" s="9"/>
@@ -4114,19 +4107,19 @@
         <v>152</v>
       </c>
       <c r="F31" s="59" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="G31" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="M31" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="N31" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
@@ -4139,21 +4132,21 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25"/>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="83" t="s">
+      <c r="A34" s="85" t="s">
         <v>157</v>
       </c>
-      <c r="B34" s="83"/>
+      <c r="B34" s="85"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="58"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
-      <c r="I34" s="82" t="s">
-        <v>341</v>
-      </c>
-      <c r="J34" s="82"/>
-      <c r="K34" s="82"/>
+      <c r="I34" s="86" t="s">
+        <v>339</v>
+      </c>
+      <c r="J34" s="86"/>
+      <c r="K34" s="86"/>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
@@ -4208,10 +4201,10 @@
         <v>150</v>
       </c>
       <c r="F38" s="64" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K38" s="9" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="L38" s="9"/>
       <c r="M38" s="9"/>
@@ -4224,19 +4217,19 @@
         <v>152</v>
       </c>
       <c r="F39" s="59" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="G39" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="K39" s="5" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="M39" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="N39" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
@@ -4249,21 +4242,21 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25"/>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" s="83" t="s">
+      <c r="A42" s="85" t="s">
         <v>158</v>
       </c>
-      <c r="B42" s="83"/>
+      <c r="B42" s="85"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
       <c r="F42" s="58"/>
       <c r="G42" s="4"/>
       <c r="H42" s="4"/>
-      <c r="I42" s="82" t="s">
-        <v>342</v>
-      </c>
-      <c r="J42" s="82"/>
-      <c r="K42" s="82"/>
+      <c r="I42" s="86" t="s">
+        <v>340</v>
+      </c>
+      <c r="J42" s="86"/>
+      <c r="K42" s="86"/>
       <c r="L42" s="4"/>
       <c r="M42" s="4"/>
       <c r="N42" s="4"/>
@@ -4318,10 +4311,10 @@
         <v>150</v>
       </c>
       <c r="F46" s="64" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K46" s="9" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="L46" s="9"/>
       <c r="M46" s="9"/>
@@ -4334,19 +4327,19 @@
         <v>152</v>
       </c>
       <c r="F47" s="59" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="G47" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="K47" s="5" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="M47" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="N47" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
@@ -4359,21 +4352,21 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25"/>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A50" s="83" t="s">
+      <c r="A50" s="85" t="s">
         <v>159</v>
       </c>
-      <c r="B50" s="83"/>
+      <c r="B50" s="85"/>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
       <c r="F50" s="58"/>
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
-      <c r="I50" s="82" t="s">
-        <v>343</v>
-      </c>
-      <c r="J50" s="82"/>
-      <c r="K50" s="82"/>
+      <c r="I50" s="86" t="s">
+        <v>341</v>
+      </c>
+      <c r="J50" s="86"/>
+      <c r="K50" s="86"/>
       <c r="L50" s="4"/>
       <c r="M50" s="4"/>
       <c r="N50" s="4"/>
@@ -4428,10 +4421,10 @@
         <v>150</v>
       </c>
       <c r="F54" s="64" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K54" s="9" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="L54" s="9"/>
       <c r="M54" s="9"/>
@@ -4444,19 +4437,19 @@
         <v>152</v>
       </c>
       <c r="F55" s="59" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="G55" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="K55" s="5" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="M55" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="N55" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
@@ -4478,21 +4471,21 @@
       <c r="N57" s="2"/>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A58" s="83" t="s">
+      <c r="A58" s="85" t="s">
         <v>160</v>
       </c>
-      <c r="B58" s="83"/>
+      <c r="B58" s="85"/>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
       <c r="E58" s="4"/>
       <c r="F58" s="58"/>
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
-      <c r="I58" s="82" t="s">
-        <v>344</v>
-      </c>
-      <c r="J58" s="82"/>
-      <c r="K58" s="82"/>
+      <c r="I58" s="86" t="s">
+        <v>342</v>
+      </c>
+      <c r="J58" s="86"/>
+      <c r="K58" s="86"/>
       <c r="L58" s="4"/>
       <c r="M58" s="4"/>
       <c r="N58" s="4"/>
@@ -4547,10 +4540,10 @@
         <v>150</v>
       </c>
       <c r="F62" s="64" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K62" s="9" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="L62" s="9"/>
       <c r="M62" s="9"/>
@@ -4563,19 +4556,19 @@
         <v>152</v>
       </c>
       <c r="F63" s="59" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="G63" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="K63" s="5" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="M63" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="N63" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
@@ -4593,6 +4586,14 @@
     <row r="69" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A18:B18"/>
     <mergeCell ref="I50:K50"/>
     <mergeCell ref="I58:K58"/>
     <mergeCell ref="I2:K2"/>
@@ -4601,14 +4602,6 @@
     <mergeCell ref="I26:K26"/>
     <mergeCell ref="I34:K34"/>
     <mergeCell ref="I42:K42"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A18:B18"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F4" r:id="rId1" display="http://nz.element14.com/koa/rk73b2attd471j/resistor-0805-470-ohm-5/dp/1809376"/>
@@ -4680,7 +4673,7 @@
     <row r="1" spans="1:14" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -4689,18 +4682,18 @@
       <c r="F2" s="58"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="82" t="s">
-        <v>345</v>
-      </c>
-      <c r="J2" s="82"/>
-      <c r="K2" s="82"/>
+      <c r="I2" s="86" t="s">
+        <v>343</v>
+      </c>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B3" t="s">
         <v>73</v>
@@ -4714,7 +4707,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B4" t="s">
         <v>73</v>
@@ -4728,7 +4721,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B5" t="s">
         <v>73</v>
@@ -4742,7 +4735,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B6" t="s">
         <v>73</v>
@@ -4756,7 +4749,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
@@ -4770,7 +4763,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
@@ -4784,7 +4777,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B9" t="s">
         <v>20</v>
@@ -4798,16 +4791,16 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B10" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F10" s="59">
         <v>1740035</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -4816,42 +4809,42 @@
       <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="80" t="s">
-        <v>396</v>
-      </c>
-      <c r="B12" s="80"/>
-      <c r="C12" s="80"/>
+      <c r="A12" s="96" t="s">
+        <v>394</v>
+      </c>
+      <c r="B12" s="96"/>
+      <c r="C12" s="96"/>
       <c r="D12" s="16"/>
       <c r="E12" s="25" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="F12" s="59">
         <v>9342427</v>
       </c>
       <c r="G12" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="80" t="s">
-        <v>398</v>
-      </c>
-      <c r="B13" s="80"/>
-      <c r="C13" s="80"/>
+      <c r="A13" s="96" t="s">
+        <v>396</v>
+      </c>
+      <c r="B13" s="96"/>
+      <c r="C13" s="96"/>
       <c r="D13" s="16"/>
       <c r="E13" s="25" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="F13" s="59">
         <v>5402608</v>
       </c>
-      <c r="G13" s="68" t="s">
-        <v>399</v>
-      </c>
-      <c r="H13" s="68"/>
-      <c r="I13" s="68"/>
-      <c r="J13" s="68"/>
-      <c r="K13" s="68"/>
+      <c r="G13" s="73" t="s">
+        <v>397</v>
+      </c>
+      <c r="H13" s="73"/>
+      <c r="I13" s="73"/>
+      <c r="J13" s="73"/>
+      <c r="K13" s="73"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -4865,11 +4858,11 @@
       <c r="F15" s="58"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
-      <c r="I15" s="82" t="s">
-        <v>346</v>
-      </c>
-      <c r="J15" s="82"/>
-      <c r="K15" s="82"/>
+      <c r="I15" s="86" t="s">
+        <v>344</v>
+      </c>
+      <c r="J15" s="86"/>
+      <c r="K15" s="86"/>
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
@@ -4887,12 +4880,12 @@
       <c r="G16" t="s">
         <v>209</v>
       </c>
-      <c r="I16" s="72" t="s">
+      <c r="I16" s="82" t="s">
         <v>220</v>
       </c>
-      <c r="J16" s="72"/>
-      <c r="K16" s="72"/>
-      <c r="L16" s="72"/>
+      <c r="J16" s="82"/>
+      <c r="K16" s="82"/>
+      <c r="L16" s="82"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
@@ -4911,10 +4904,10 @@
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="F18" s="64" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="L18" s="9"/>
     </row>
@@ -4926,16 +4919,16 @@
         <v>164</v>
       </c>
       <c r="F19" s="59" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="G19" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="L19" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -4999,7 +4992,7 @@
         <v>165</v>
       </c>
       <c r="B24" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
@@ -5007,7 +5000,7 @@
         <v>166</v>
       </c>
       <c r="B25" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -5015,7 +5008,7 @@
         <v>168</v>
       </c>
       <c r="B26" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25"/>
@@ -5030,11 +5023,11 @@
       <c r="F28" s="58"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
-      <c r="I28" s="82" t="s">
-        <v>347</v>
-      </c>
-      <c r="J28" s="82"/>
-      <c r="K28" s="82"/>
+      <c r="I28" s="86" t="s">
+        <v>345</v>
+      </c>
+      <c r="J28" s="86"/>
+      <c r="K28" s="86"/>
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
@@ -5052,12 +5045,12 @@
       <c r="G29" t="s">
         <v>209</v>
       </c>
-      <c r="I29" s="72" t="s">
+      <c r="I29" s="82" t="s">
         <v>220</v>
       </c>
-      <c r="J29" s="72"/>
-      <c r="K29" s="72"/>
-      <c r="L29" s="72"/>
+      <c r="J29" s="82"/>
+      <c r="K29" s="82"/>
+      <c r="L29" s="82"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
@@ -5076,10 +5069,10 @@
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="9"/>
       <c r="F31" s="64" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K31" s="9" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="L31" s="9"/>
     </row>
@@ -5091,16 +5084,16 @@
         <v>164</v>
       </c>
       <c r="F32" s="59" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="G32" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="K32" s="5" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="L32" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
@@ -5164,7 +5157,7 @@
         <v>187</v>
       </c>
       <c r="B37" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
@@ -5172,7 +5165,7 @@
         <v>206</v>
       </c>
       <c r="B38" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="F38" s="59"/>
     </row>
@@ -5181,7 +5174,7 @@
         <v>207</v>
       </c>
       <c r="B39" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="F39" s="59"/>
     </row>
@@ -5197,11 +5190,11 @@
       <c r="F41" s="58"/>
       <c r="G41" s="4"/>
       <c r="H41" s="4"/>
-      <c r="I41" s="82" t="s">
-        <v>348</v>
-      </c>
-      <c r="J41" s="82"/>
-      <c r="K41" s="82"/>
+      <c r="I41" s="86" t="s">
+        <v>346</v>
+      </c>
+      <c r="J41" s="86"/>
+      <c r="K41" s="86"/>
       <c r="L41" s="4"/>
       <c r="M41" s="4"/>
       <c r="N41" s="4"/>
@@ -5219,12 +5212,12 @@
       <c r="G42" t="s">
         <v>209</v>
       </c>
-      <c r="I42" s="72" t="s">
+      <c r="I42" s="82" t="s">
         <v>220</v>
       </c>
-      <c r="J42" s="72"/>
-      <c r="K42" s="72"/>
-      <c r="L42" s="72"/>
+      <c r="J42" s="82"/>
+      <c r="K42" s="82"/>
+      <c r="L42" s="82"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
@@ -5243,10 +5236,10 @@
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="9"/>
       <c r="F44" s="64" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K44" s="9" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="L44" s="9"/>
       <c r="M44" s="9"/>
@@ -5259,16 +5252,16 @@
         <v>164</v>
       </c>
       <c r="F45" s="59" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="G45" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="K45" s="5" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="L45" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="P45" s="5"/>
     </row>
@@ -5334,7 +5327,7 @@
         <v>204</v>
       </c>
       <c r="B50" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
@@ -5342,7 +5335,7 @@
         <v>205</v>
       </c>
       <c r="B51" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="F51" s="59"/>
     </row>
@@ -5351,7 +5344,7 @@
         <v>194</v>
       </c>
       <c r="B52" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F52" s="59"/>
     </row>
@@ -5367,11 +5360,11 @@
       <c r="F54" s="58"/>
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
-      <c r="I54" s="82" t="s">
-        <v>349</v>
-      </c>
-      <c r="J54" s="82"/>
-      <c r="K54" s="82"/>
+      <c r="I54" s="86" t="s">
+        <v>347</v>
+      </c>
+      <c r="J54" s="86"/>
+      <c r="K54" s="86"/>
       <c r="L54" s="4"/>
       <c r="M54" s="4"/>
       <c r="N54" s="4"/>
@@ -5389,12 +5382,12 @@
       <c r="G55" t="s">
         <v>209</v>
       </c>
-      <c r="I55" s="72" t="s">
+      <c r="I55" s="82" t="s">
         <v>220</v>
       </c>
-      <c r="J55" s="72"/>
-      <c r="K55" s="72"/>
-      <c r="L55" s="72"/>
+      <c r="J55" s="82"/>
+      <c r="K55" s="82"/>
+      <c r="L55" s="82"/>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
@@ -5413,10 +5406,10 @@
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="9"/>
       <c r="F57" s="64" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K57" s="9" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="L57" s="9"/>
       <c r="M57" s="9"/>
@@ -5426,16 +5419,16 @@
         <v>199</v>
       </c>
       <c r="F58" s="59" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="G58" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="K58" s="5" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="L58" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="M58" s="5"/>
     </row>
@@ -5500,7 +5493,7 @@
         <v>202</v>
       </c>
       <c r="B63" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
@@ -5508,7 +5501,7 @@
         <v>203</v>
       </c>
       <c r="B64" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="F64" s="59"/>
     </row>
@@ -5517,7 +5510,7 @@
         <v>290</v>
       </c>
       <c r="B65" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F65" s="59"/>
     </row>
@@ -5532,6 +5525,10 @@
     <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="G13:K13"/>
+    <mergeCell ref="I54:K54"/>
+    <mergeCell ref="A13:C13"/>
     <mergeCell ref="I15:K15"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="I28:K28"/>
@@ -5540,10 +5537,6 @@
     <mergeCell ref="I42:L42"/>
     <mergeCell ref="I29:L29"/>
     <mergeCell ref="I16:L16"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="G13:K13"/>
-    <mergeCell ref="I54:K54"/>
-    <mergeCell ref="A13:C13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F20" r:id="rId1" display="http://nz.element14.com/koa/rk73z2attd/resistor-0805-0-ohm-jumper/dp/1809596"/>
@@ -5605,13 +5598,13 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="81" t="s">
-        <v>395</v>
-      </c>
-      <c r="C7" s="81"/>
-      <c r="D7" s="81"/>
-      <c r="E7" s="81"/>
-      <c r="F7" s="81"/>
+      <c r="B7" s="97" t="s">
+        <v>393</v>
+      </c>
+      <c r="C7" s="97"/>
+      <c r="D7" s="97"/>
+      <c r="E7" s="97"/>
+      <c r="F7" s="97"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5641,20 +5634,20 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="74" t="s">
-        <v>397</v>
-      </c>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
+      <c r="A2" s="84" t="s">
+        <v>395</v>
+      </c>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="60"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="82" t="s">
-        <v>331</v>
-      </c>
-      <c r="J2" s="82"/>
+      <c r="I2" s="86" t="s">
+        <v>329</v>
+      </c>
+      <c r="J2" s="86"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
     </row>
@@ -5668,10 +5661,10 @@
       <c r="F3" s="59">
         <v>1887296</v>
       </c>
-      <c r="G3" s="68" t="s">
+      <c r="G3" s="73" t="s">
         <v>216</v>
       </c>
-      <c r="H3" s="68"/>
+      <c r="H3" s="73"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
@@ -5683,27 +5676,27 @@
       <c r="F4" s="59">
         <v>1506077</v>
       </c>
-      <c r="G4" s="68" t="s">
+      <c r="G4" s="73" t="s">
         <v>221</v>
       </c>
-      <c r="H4" s="68"/>
+      <c r="H4" s="73"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="73" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
       <c r="F5" s="59">
         <v>1809596</v>
       </c>
-      <c r="G5" s="68" t="s">
+      <c r="G5" s="73" t="s">
         <v>208</v>
       </c>
-      <c r="H5" s="68"/>
+      <c r="H5" s="73"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
@@ -5715,11 +5708,11 @@
       <c r="F6" s="59">
         <v>1759172</v>
       </c>
-      <c r="G6" s="68" t="s">
+      <c r="G6" s="73" t="s">
         <v>223</v>
       </c>
-      <c r="H6" s="68"/>
-      <c r="I6" s="68"/>
+      <c r="H6" s="73"/>
+      <c r="I6" s="73"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
@@ -5731,13 +5724,13 @@
       <c r="F7" s="59">
         <v>9556915</v>
       </c>
-      <c r="G7" s="68" t="s">
+      <c r="G7" s="73" t="s">
         <v>235</v>
       </c>
-      <c r="H7" s="68"/>
-      <c r="I7" s="68"/>
-      <c r="J7" s="68"/>
-      <c r="K7" s="68"/>
+      <c r="H7" s="73"/>
+      <c r="I7" s="73"/>
+      <c r="J7" s="73"/>
+      <c r="K7" s="73"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
@@ -5749,13 +5742,13 @@
       <c r="F8" s="59">
         <v>9556915</v>
       </c>
-      <c r="G8" s="68" t="s">
+      <c r="G8" s="73" t="s">
         <v>235</v>
       </c>
-      <c r="H8" s="68"/>
-      <c r="I8" s="68"/>
-      <c r="J8" s="68"/>
-      <c r="K8" s="68"/>
+      <c r="H8" s="73"/>
+      <c r="I8" s="73"/>
+      <c r="J8" s="73"/>
+      <c r="K8" s="73"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
@@ -5768,10 +5761,10 @@
       <c r="F9" s="59">
         <v>1809376</v>
       </c>
-      <c r="G9" s="68" t="s">
+      <c r="G9" s="73" t="s">
         <v>209</v>
       </c>
-      <c r="H9" s="68"/>
+      <c r="H9" s="73"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
@@ -5779,16 +5772,16 @@
     <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
     <mergeCell ref="G6:I6"/>
     <mergeCell ref="G7:K7"/>
     <mergeCell ref="G8:K8"/>
     <mergeCell ref="G9:H9"/>
     <mergeCell ref="B5:D5"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F9" r:id="rId1" display="http://nz.element14.com/koa/rk73b2attd471j/resistor-0805-470-ohm-5/dp/1809376"/>
@@ -5823,30 +5816,30 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="74" t="s">
-        <v>360</v>
-      </c>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
+      <c r="A2" s="84" t="s">
+        <v>358</v>
+      </c>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
       <c r="E2" s="3"/>
       <c r="F2" s="60"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="82" t="s">
-        <v>356</v>
-      </c>
-      <c r="J2" s="82"/>
-      <c r="K2" s="82"/>
+      <c r="I2" s="86" t="s">
+        <v>354</v>
+      </c>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
       <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="84" t="s">
-        <v>409</v>
-      </c>
-      <c r="B3" s="84"/>
-      <c r="C3" s="84"/>
-      <c r="D3" s="84"/>
+      <c r="A3" s="89" t="s">
+        <v>406</v>
+      </c>
+      <c r="B3" s="89"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
       <c r="E3" s="3"/>
       <c r="F3" s="60"/>
       <c r="G3" s="4"/>
@@ -5866,11 +5859,11 @@
       <c r="F4" s="59">
         <v>8820120</v>
       </c>
-      <c r="G4" s="68" t="s">
+      <c r="G4" s="73" t="s">
         <v>218</v>
       </c>
-      <c r="H4" s="68"/>
-      <c r="I4" s="68"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
@@ -5882,11 +5875,11 @@
       <c r="F5" s="59">
         <v>1759199</v>
       </c>
-      <c r="G5" s="68" t="s">
+      <c r="G5" s="73" t="s">
         <v>222</v>
       </c>
-      <c r="H5" s="68"/>
-      <c r="I5" s="68"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
@@ -5898,11 +5891,11 @@
       <c r="F6" s="59">
         <v>1759172</v>
       </c>
-      <c r="G6" s="68" t="s">
+      <c r="G6" s="73" t="s">
         <v>223</v>
       </c>
-      <c r="H6" s="68"/>
-      <c r="I6" s="68"/>
+      <c r="H6" s="73"/>
+      <c r="I6" s="73"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
@@ -5914,10 +5907,10 @@
       <c r="F7" s="59">
         <v>1809376</v>
       </c>
-      <c r="G7" s="68" t="s">
+      <c r="G7" s="73" t="s">
         <v>209</v>
       </c>
-      <c r="H7" s="68"/>
+      <c r="H7" s="73"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
@@ -5929,10 +5922,10 @@
       <c r="F8" s="59">
         <v>1809596</v>
       </c>
-      <c r="G8" s="68" t="s">
+      <c r="G8" s="73" t="s">
         <v>208</v>
       </c>
-      <c r="H8" s="68"/>
+      <c r="H8" s="73"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
@@ -5944,20 +5937,20 @@
       <c r="F9" s="59">
         <v>1809596</v>
       </c>
-      <c r="G9" s="68" t="s">
+      <c r="G9" s="73" t="s">
         <v>208</v>
       </c>
-      <c r="H9" s="68"/>
+      <c r="H9" s="73"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>373</v>
-      </c>
-      <c r="B10" s="68" t="s">
+        <v>371</v>
+      </c>
+      <c r="B10" s="73" t="s">
         <v>95</v>
       </c>
-      <c r="C10" s="68"/>
-      <c r="D10" s="68"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="73"/>
       <c r="F10" s="59"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -5965,100 +5958,100 @@
       <c r="F11" s="59"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="75" t="s">
-        <v>404</v>
-      </c>
-      <c r="B12" s="75"/>
-      <c r="C12" s="75"/>
-      <c r="D12" s="75"/>
-      <c r="E12" s="75"/>
-      <c r="F12" s="75"/>
-      <c r="G12" s="75"/>
-      <c r="H12" s="75"/>
-      <c r="I12" s="75"/>
-      <c r="J12" s="75"/>
-      <c r="K12" s="75"/>
-      <c r="L12" s="75"/>
+      <c r="A12" s="90" t="s">
+        <v>401</v>
+      </c>
+      <c r="B12" s="90"/>
+      <c r="C12" s="90"/>
+      <c r="D12" s="90"/>
+      <c r="E12" s="90"/>
+      <c r="F12" s="90"/>
+      <c r="G12" s="90"/>
+      <c r="H12" s="90"/>
+      <c r="I12" s="90"/>
+      <c r="J12" s="90"/>
+      <c r="K12" s="90"/>
+      <c r="L12" s="90"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="B13" s="68" t="s">
+      <c r="B13" s="73" t="s">
         <v>82</v>
       </c>
-      <c r="C13" s="68"/>
+      <c r="C13" s="73"/>
       <c r="F13" s="59">
         <v>1457153</v>
       </c>
-      <c r="G13" s="68" t="s">
+      <c r="G13" s="73" t="s">
         <v>183</v>
       </c>
-      <c r="H13" s="68"/>
-      <c r="I13" s="68"/>
+      <c r="H13" s="73"/>
+      <c r="I13" s="73"/>
       <c r="J13" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="K13" s="76" t="s">
+      <c r="K13" s="91" t="s">
         <v>233</v>
       </c>
-      <c r="L13" s="76"/>
+      <c r="L13" s="91"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="B14" s="68" t="s">
+      <c r="B14" s="73" t="s">
         <v>95</v>
       </c>
-      <c r="C14" s="68"/>
-      <c r="D14" s="68"/>
+      <c r="C14" s="73"/>
+      <c r="D14" s="73"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="B15" s="68" t="s">
+      <c r="B15" s="73" t="s">
         <v>95</v>
       </c>
-      <c r="C15" s="68"/>
-      <c r="D15" s="68"/>
+      <c r="C15" s="73"/>
+      <c r="D15" s="73"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="B16" s="68" t="s">
+      <c r="B16" s="73" t="s">
         <v>95</v>
       </c>
-      <c r="C16" s="68"/>
-      <c r="D16" s="68"/>
+      <c r="C16" s="73"/>
+      <c r="D16" s="73"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
     </row>
     <row r="18" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="77" t="s">
-        <v>405</v>
-      </c>
-      <c r="B18" s="77"/>
-      <c r="C18" s="77"/>
-      <c r="D18" s="77"/>
-      <c r="E18" s="77"/>
-      <c r="F18" s="77"/>
-      <c r="G18" s="77"/>
-      <c r="H18" s="77"/>
-      <c r="I18" s="77"/>
-      <c r="J18" s="77"/>
-      <c r="K18" s="77"/>
-      <c r="L18" s="77"/>
+      <c r="A18" s="92" t="s">
+        <v>402</v>
+      </c>
+      <c r="B18" s="92"/>
+      <c r="C18" s="92"/>
+      <c r="D18" s="92"/>
+      <c r="E18" s="92"/>
+      <c r="F18" s="92"/>
+      <c r="G18" s="92"/>
+      <c r="H18" s="92"/>
+      <c r="I18" s="92"/>
+      <c r="J18" s="92"/>
+      <c r="K18" s="92"/>
+      <c r="L18" s="92"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
         <v>103</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C19" s="22"/>
       <c r="D19" s="22"/>
@@ -6066,13 +6059,13 @@
       <c r="F19" s="61">
         <v>9556915</v>
       </c>
-      <c r="G19" s="78" t="s">
+      <c r="G19" s="93" t="s">
         <v>235</v>
       </c>
-      <c r="H19" s="78"/>
-      <c r="I19" s="78"/>
-      <c r="J19" s="78"/>
-      <c r="K19" s="78"/>
+      <c r="H19" s="93"/>
+      <c r="I19" s="93"/>
+      <c r="J19" s="93"/>
+      <c r="K19" s="93"/>
       <c r="L19" s="22"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -6080,7 +6073,7 @@
         <v>104</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C20" s="22"/>
       <c r="D20" s="22"/>
@@ -6088,13 +6081,13 @@
       <c r="F20" s="61">
         <v>9556915</v>
       </c>
-      <c r="G20" s="78" t="s">
+      <c r="G20" s="93" t="s">
         <v>235</v>
       </c>
-      <c r="H20" s="78"/>
-      <c r="I20" s="78"/>
-      <c r="J20" s="78"/>
-      <c r="K20" s="78"/>
+      <c r="H20" s="93"/>
+      <c r="I20" s="93"/>
+      <c r="J20" s="93"/>
+      <c r="K20" s="93"/>
       <c r="L20" s="22"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -6110,11 +6103,11 @@
       <c r="F21" s="61">
         <v>8820120</v>
       </c>
-      <c r="G21" s="78" t="s">
+      <c r="G21" s="93" t="s">
         <v>218</v>
       </c>
-      <c r="H21" s="78"/>
-      <c r="I21" s="78"/>
+      <c r="H21" s="93"/>
+      <c r="I21" s="93"/>
       <c r="J21" s="22"/>
       <c r="K21" s="22"/>
       <c r="L21" s="22"/>
@@ -6135,6 +6128,11 @@
     <row r="35" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A18:L18"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="G20:K20"/>
+    <mergeCell ref="G19:K19"/>
+    <mergeCell ref="B16:D16"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="I2:K2"/>
@@ -6151,11 +6149,6 @@
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="A12:L12"/>
     <mergeCell ref="K13:L13"/>
-    <mergeCell ref="A18:L18"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="G20:K20"/>
-    <mergeCell ref="G19:K19"/>
-    <mergeCell ref="B16:D16"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F13" r:id="rId1" display="http://nz.element14.com/freescale-semiconductor/mpx4250ap/ic-sensor-abs-press-36-3-psi/dp/1457153"/>
@@ -6190,35 +6183,36 @@
     <col min="6" max="6" width="9.140625" style="57" customWidth="1"/>
     <col min="7" max="8" width="9.140625" customWidth="1"/>
     <col min="9" max="9" width="12.5703125" customWidth="1"/>
-    <col min="10" max="12" width="9.140625" customWidth="1"/>
+    <col min="10" max="11" width="9.140625" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="74" t="s">
-        <v>350</v>
-      </c>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
+      <c r="A2" s="84" t="s">
+        <v>348</v>
+      </c>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
       <c r="E2" s="3"/>
       <c r="F2" s="60"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="82" t="s">
-        <v>357</v>
-      </c>
-      <c r="J2" s="82"/>
-      <c r="K2" s="82"/>
+      <c r="I2" s="86" t="s">
+        <v>355</v>
+      </c>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
       <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="79" t="s">
-        <v>408</v>
-      </c>
-      <c r="B3" s="79"/>
-      <c r="C3" s="79"/>
+      <c r="A3" s="94" t="s">
+        <v>405</v>
+      </c>
+      <c r="B3" s="94"/>
+      <c r="C3" s="94"/>
       <c r="F3" s="58"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -6231,21 +6225,21 @@
       <c r="F4" s="59">
         <v>8820120</v>
       </c>
-      <c r="G4" s="68" t="s">
+      <c r="G4" s="73" t="s">
         <v>218</v>
       </c>
-      <c r="H4" s="68"/>
-      <c r="I4" s="68"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="73" t="s">
         <v>95</v>
       </c>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
       <c r="F5" s="59"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -6258,11 +6252,11 @@
       <c r="F6" s="59">
         <v>1759199</v>
       </c>
-      <c r="G6" s="68" t="s">
+      <c r="G6" s="73" t="s">
         <v>222</v>
       </c>
-      <c r="H6" s="68"/>
-      <c r="I6" s="68"/>
+      <c r="H6" s="73"/>
+      <c r="I6" s="73"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
@@ -6274,11 +6268,11 @@
       <c r="F7" s="59">
         <v>1759172</v>
       </c>
-      <c r="G7" s="68" t="s">
+      <c r="G7" s="73" t="s">
         <v>223</v>
       </c>
-      <c r="H7" s="68"/>
-      <c r="I7" s="68"/>
+      <c r="H7" s="73"/>
+      <c r="I7" s="73"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
@@ -6290,10 +6284,10 @@
       <c r="F8" s="59">
         <v>1809376</v>
       </c>
-      <c r="G8" s="68" t="s">
+      <c r="G8" s="73" t="s">
         <v>209</v>
       </c>
-      <c r="H8" s="68"/>
+      <c r="H8" s="73"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
@@ -6305,93 +6299,93 @@
       <c r="F9" s="59">
         <v>1809596</v>
       </c>
-      <c r="G9" s="68" t="s">
+      <c r="G9" s="73" t="s">
         <v>208</v>
       </c>
-      <c r="H9" s="68"/>
+      <c r="H9" s="73"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
       <c r="F10" s="59"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="75" t="s">
-        <v>406</v>
-      </c>
-      <c r="B11" s="75"/>
-      <c r="C11" s="75"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="75"/>
-      <c r="G11" s="75"/>
-      <c r="H11" s="75"/>
-      <c r="I11" s="75"/>
-      <c r="J11" s="75"/>
-      <c r="K11" s="75"/>
-      <c r="L11" s="75"/>
+      <c r="A11" s="90" t="s">
+        <v>403</v>
+      </c>
+      <c r="B11" s="90"/>
+      <c r="C11" s="90"/>
+      <c r="D11" s="90"/>
+      <c r="E11" s="90"/>
+      <c r="F11" s="90"/>
+      <c r="G11" s="90"/>
+      <c r="H11" s="90"/>
+      <c r="I11" s="90"/>
+      <c r="J11" s="90"/>
+      <c r="K11" s="90"/>
+      <c r="L11" s="90"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="B12" s="68" t="s">
+      <c r="B12" s="73" t="s">
         <v>96</v>
       </c>
-      <c r="C12" s="68"/>
+      <c r="C12" s="73"/>
       <c r="F12" s="67">
         <v>1703477</v>
       </c>
-      <c r="G12" s="68" t="s">
-        <v>410</v>
-      </c>
-      <c r="H12" s="68"/>
-      <c r="I12" s="68"/>
+      <c r="G12" s="73" t="s">
+        <v>407</v>
+      </c>
+      <c r="H12" s="73"/>
+      <c r="I12" s="73"/>
       <c r="J12" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="K12" s="76" t="s">
-        <v>411</v>
-      </c>
-      <c r="L12" s="76"/>
+      <c r="K12" s="91" t="s">
+        <v>408</v>
+      </c>
+      <c r="L12" s="91"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="B13" s="68" t="s">
+      <c r="B13" s="73" t="s">
         <v>95</v>
       </c>
-      <c r="C13" s="68"/>
-      <c r="D13" s="68"/>
+      <c r="C13" s="73"/>
+      <c r="D13" s="73"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="B14" s="68" t="s">
+      <c r="B14" s="73" t="s">
         <v>95</v>
       </c>
-      <c r="C14" s="68"/>
-      <c r="D14" s="68"/>
+      <c r="C14" s="73"/>
+      <c r="D14" s="73"/>
       <c r="F14" s="59"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="B15" s="86" t="s">
+      <c r="B15" s="78" t="s">
         <v>95</v>
       </c>
-      <c r="C15" s="86"/>
-      <c r="D15" s="86"/>
+      <c r="C15" s="78"/>
+      <c r="D15" s="78"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
       <c r="F16" s="59"/>
     </row>
-    <row r="17" spans="1:12" s="77" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="77" t="s">
-        <v>407</v>
+    <row r="17" spans="1:12" s="92" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="92" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -6399,7 +6393,7 @@
         <v>91</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C18" s="22"/>
       <c r="D18" s="22"/>
@@ -6407,12 +6401,12 @@
       <c r="F18" s="61">
         <v>9556915</v>
       </c>
-      <c r="G18" s="78" t="s">
+      <c r="G18" s="93" t="s">
         <v>235</v>
       </c>
-      <c r="H18" s="78"/>
-      <c r="I18" s="78"/>
-      <c r="J18" s="78"/>
+      <c r="H18" s="93"/>
+      <c r="I18" s="93"/>
+      <c r="J18" s="93"/>
       <c r="K18" s="22"/>
       <c r="L18" s="22"/>
     </row>
@@ -6421,7 +6415,7 @@
         <v>92</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C19" s="22"/>
       <c r="D19" s="22"/>
@@ -6429,12 +6423,12 @@
       <c r="F19" s="61">
         <v>9556915</v>
       </c>
-      <c r="G19" s="78" t="s">
+      <c r="G19" s="93" t="s">
         <v>235</v>
       </c>
-      <c r="H19" s="78"/>
-      <c r="I19" s="78"/>
-      <c r="J19" s="78"/>
+      <c r="H19" s="93"/>
+      <c r="I19" s="93"/>
+      <c r="J19" s="93"/>
       <c r="K19" s="22"/>
       <c r="L19" s="22"/>
     </row>
@@ -6451,11 +6445,11 @@
       <c r="F20" s="61">
         <v>8820120</v>
       </c>
-      <c r="G20" s="78" t="s">
+      <c r="G20" s="93" t="s">
         <v>218</v>
       </c>
-      <c r="H20" s="78"/>
-      <c r="I20" s="78"/>
+      <c r="H20" s="93"/>
+      <c r="I20" s="93"/>
       <c r="J20" s="62"/>
       <c r="K20" s="22"/>
       <c r="L20" s="22"/>
@@ -6476,6 +6470,19 @@
     <row r="34" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="G18:J18"/>
+    <mergeCell ref="G19:J19"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="A11:L11"/>
+    <mergeCell ref="A17:XFD17"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="B15:D15"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="G4:I4"/>
@@ -6483,19 +6490,6 @@
     <mergeCell ref="G7:I7"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="A3:C3"/>
-    <mergeCell ref="G18:J18"/>
-    <mergeCell ref="G19:J19"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="A11:L11"/>
-    <mergeCell ref="A17:XFD17"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F8" r:id="rId1" display="http://nz.element14.com/koa/rk73b2attd471j/resistor-0805-470-ohm-5/dp/1809376"/>
@@ -6521,36 +6515,39 @@
   </sheetPr>
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19:I19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="9.140625" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="57" customWidth="1"/>
     <col min="7" max="8" width="9.140625" customWidth="1"/>
-    <col min="9" max="9" width="13" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" customWidth="1"/>
     <col min="10" max="10" width="11.42578125" customWidth="1"/>
-    <col min="11" max="12" width="9.140625" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="84" t="s">
         <v>118</v>
       </c>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
       <c r="D2" s="3"/>
       <c r="E2" s="4"/>
       <c r="F2" s="58"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="82" t="s">
-        <v>420</v>
-      </c>
-      <c r="J2" s="82"/>
-      <c r="K2" s="82"/>
+      <c r="I2" s="86" t="s">
+        <v>417</v>
+      </c>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
       <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -6564,18 +6561,18 @@
       <c r="F3" s="63">
         <v>1845719</v>
       </c>
-      <c r="G3" s="85" t="s">
+      <c r="G3" s="95" t="s">
         <v>181</v>
       </c>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="95"/>
       <c r="J3" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="K3" s="76" t="s">
+      <c r="K3" s="91" t="s">
         <v>231</v>
       </c>
-      <c r="L3" s="76"/>
+      <c r="L3" s="91"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
@@ -6587,10 +6584,10 @@
       <c r="F4" s="59">
         <v>1652909</v>
       </c>
-      <c r="G4" s="68" t="s">
+      <c r="G4" s="73" t="s">
         <v>216</v>
       </c>
-      <c r="H4" s="68"/>
+      <c r="H4" s="73"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
@@ -6602,12 +6599,12 @@
       <c r="F5" s="59">
         <v>8820120</v>
       </c>
-      <c r="G5" s="68" t="s">
+      <c r="G5" s="73" t="s">
         <v>218</v>
       </c>
-      <c r="H5" s="68"/>
-      <c r="I5" s="68"/>
-      <c r="J5" s="68"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
+      <c r="J5" s="73"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
@@ -6619,12 +6616,12 @@
       <c r="F6" s="59">
         <v>1414659</v>
       </c>
-      <c r="G6" s="68" t="s">
+      <c r="G6" s="73" t="s">
         <v>225</v>
       </c>
-      <c r="H6" s="68"/>
-      <c r="I6" s="68"/>
-      <c r="J6" s="68"/>
+      <c r="H6" s="73"/>
+      <c r="I6" s="73"/>
+      <c r="J6" s="73"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
@@ -6639,11 +6636,11 @@
       <c r="F7" s="59">
         <v>1618242</v>
       </c>
-      <c r="G7" s="68" t="s">
+      <c r="G7" s="73" t="s">
         <v>237</v>
       </c>
-      <c r="H7" s="68"/>
-      <c r="I7" s="68"/>
+      <c r="H7" s="73"/>
+      <c r="I7" s="73"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
@@ -6658,15 +6655,15 @@
       <c r="F8" s="59">
         <v>1618242</v>
       </c>
-      <c r="G8" s="68" t="s">
+      <c r="G8" s="73" t="s">
         <v>237</v>
       </c>
-      <c r="H8" s="68"/>
-      <c r="I8" s="68"/>
+      <c r="H8" s="73"/>
+      <c r="I8" s="73"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="B9" t="s">
         <v>73</v>
@@ -6674,14 +6671,14 @@
       <c r="F9" s="59">
         <v>1809300</v>
       </c>
-      <c r="G9" s="68" t="s">
+      <c r="G9" s="73" t="s">
         <v>209</v>
       </c>
-      <c r="H9" s="68"/>
+      <c r="H9" s="73"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B10" t="s">
         <v>94</v>
@@ -6689,38 +6686,38 @@
       <c r="F10" s="65">
         <v>1809596</v>
       </c>
-      <c r="G10" s="68" t="s">
+      <c r="G10" s="73" t="s">
         <v>208</v>
       </c>
-      <c r="H10" s="68"/>
+      <c r="H10" s="73"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>414</v>
-      </c>
-      <c r="B11" s="68" t="s">
-        <v>415</v>
-      </c>
-      <c r="C11" s="68"/>
+        <v>411</v>
+      </c>
+      <c r="B11" s="73" t="s">
+        <v>412</v>
+      </c>
+      <c r="C11" s="73"/>
       <c r="F11" s="59"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="74" t="s">
+      <c r="A13" s="84" t="s">
         <v>119</v>
       </c>
-      <c r="B13" s="74"/>
-      <c r="C13" s="74"/>
+      <c r="B13" s="84"/>
+      <c r="C13" s="84"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="58"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
-      <c r="I13" s="82" t="s">
-        <v>421</v>
-      </c>
-      <c r="J13" s="82"/>
-      <c r="K13" s="82"/>
+      <c r="I13" s="86" t="s">
+        <v>418</v>
+      </c>
+      <c r="J13" s="86"/>
+      <c r="K13" s="86"/>
       <c r="L13" s="4"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -6734,18 +6731,18 @@
       <c r="F14" s="63">
         <v>1845719</v>
       </c>
-      <c r="G14" s="85" t="s">
+      <c r="G14" s="95" t="s">
         <v>181</v>
       </c>
-      <c r="H14" s="85"/>
-      <c r="I14" s="85"/>
+      <c r="H14" s="95"/>
+      <c r="I14" s="95"/>
       <c r="J14" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="K14" s="76" t="s">
+      <c r="K14" s="91" t="s">
         <v>231</v>
       </c>
-      <c r="L14" s="76"/>
+      <c r="L14" s="91"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
@@ -6757,10 +6754,10 @@
       <c r="F15" s="59">
         <v>1652909</v>
       </c>
-      <c r="G15" s="68" t="s">
+      <c r="G15" s="73" t="s">
         <v>216</v>
       </c>
-      <c r="H15" s="68"/>
+      <c r="H15" s="73"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
@@ -6772,11 +6769,11 @@
       <c r="F16" s="59">
         <v>8820120</v>
       </c>
-      <c r="G16" s="68" t="s">
+      <c r="G16" s="73" t="s">
         <v>218</v>
       </c>
-      <c r="H16" s="68"/>
-      <c r="I16" s="68"/>
+      <c r="H16" s="73"/>
+      <c r="I16" s="73"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
@@ -6788,12 +6785,12 @@
       <c r="F17" s="59">
         <v>1414659</v>
       </c>
-      <c r="G17" s="68" t="s">
+      <c r="G17" s="73" t="s">
         <v>225</v>
       </c>
-      <c r="H17" s="68"/>
-      <c r="I17" s="68"/>
-      <c r="J17" s="68"/>
+      <c r="H17" s="73"/>
+      <c r="I17" s="73"/>
+      <c r="J17" s="73"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
@@ -6808,11 +6805,11 @@
       <c r="F18" s="59">
         <v>1618242</v>
       </c>
-      <c r="G18" s="68" t="s">
+      <c r="G18" s="73" t="s">
         <v>237</v>
       </c>
-      <c r="H18" s="68"/>
-      <c r="I18" s="68"/>
+      <c r="H18" s="73"/>
+      <c r="I18" s="73"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
@@ -6827,15 +6824,15 @@
       <c r="F19" s="59">
         <v>1618242</v>
       </c>
-      <c r="G19" s="68" t="s">
+      <c r="G19" s="73" t="s">
         <v>237</v>
       </c>
-      <c r="H19" s="68"/>
-      <c r="I19" s="68"/>
+      <c r="H19" s="73"/>
+      <c r="I19" s="73"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="B20" t="s">
         <v>73</v>
@@ -6843,14 +6840,14 @@
       <c r="F20" s="59">
         <v>1809300</v>
       </c>
-      <c r="G20" s="68" t="s">
+      <c r="G20" s="73" t="s">
         <v>209</v>
       </c>
-      <c r="H20" s="68"/>
+      <c r="H20" s="73"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="B21" t="s">
         <v>94</v>
@@ -6858,19 +6855,19 @@
       <c r="F21" s="65">
         <v>1809596</v>
       </c>
-      <c r="G21" s="68" t="s">
+      <c r="G21" s="73" t="s">
         <v>208</v>
       </c>
-      <c r="H21" s="68"/>
+      <c r="H21" s="73"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>418</v>
-      </c>
-      <c r="B22" s="68" t="s">
         <v>415</v>
       </c>
-      <c r="C22" s="68"/>
+      <c r="B22" s="73" t="s">
+        <v>412</v>
+      </c>
+      <c r="C22" s="73"/>
       <c r="F22" s="59"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25"/>
@@ -6880,12 +6877,8 @@
     <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="I13:K13"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="G19:I19"/>
     <mergeCell ref="K14:L14"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="B11:C11"/>
@@ -6902,8 +6895,12 @@
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="G16:I16"/>
     <mergeCell ref="G17:J17"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="G10:H10"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1" display="http://nz.element14.com/maxim-integrated-products/max9924uaub/interface-sensor-vr-1ch-10umax/dp/1845719"/>
@@ -6949,24 +6946,24 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="74" t="s">
-        <v>312</v>
-      </c>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="74"/>
+      <c r="A2" s="84" t="s">
+        <v>310</v>
+      </c>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B3" t="s">
         <v>164</v>
@@ -6976,7 +6973,7 @@
         <v>1017798</v>
       </c>
       <c r="G3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -7095,21 +7092,21 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="74" t="s">
-        <v>361</v>
-      </c>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
+      <c r="A2" s="84" t="s">
+        <v>359</v>
+      </c>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
       <c r="E2" s="3"/>
       <c r="F2" s="58"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="82" t="s">
-        <v>329</v>
-      </c>
-      <c r="J2" s="82"/>
-      <c r="K2" s="82"/>
+      <c r="I2" s="86" t="s">
+        <v>327</v>
+      </c>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
       <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -7156,10 +7153,10 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B6" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="F6" s="59">
         <v>1809596</v>
@@ -7170,10 +7167,10 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B7" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="F7" s="59">
         <v>1809596</v>
@@ -7184,7 +7181,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B8" t="s">
         <v>79</v>
@@ -7198,7 +7195,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B9" t="s">
         <v>79</v>
@@ -7234,7 +7231,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B12" t="s">
         <v>95</v>
@@ -7297,21 +7294,21 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="84" t="s">
         <v>131</v>
       </c>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
       <c r="E2" s="3"/>
       <c r="F2" s="60"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="82" t="s">
-        <v>336</v>
-      </c>
-      <c r="J2" s="82"/>
-      <c r="K2" s="82"/>
+      <c r="I2" s="86" t="s">
+        <v>334</v>
+      </c>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
       <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -7358,10 +7355,10 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B6" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="F6" s="59">
         <v>1809596</v>
@@ -7372,10 +7369,10 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B7" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="F7" s="59">
         <v>1809596</v>
@@ -7386,7 +7383,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B8" t="s">
         <v>79</v>
@@ -7400,7 +7397,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B9" t="s">
         <v>79</v>
@@ -7444,7 +7441,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B13" t="s">
         <v>95</v>
@@ -7500,21 +7497,21 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="85" t="s">
         <v>137</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="58"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="82" t="s">
-        <v>330</v>
-      </c>
-      <c r="J2" s="82"/>
-      <c r="K2" s="82"/>
+      <c r="I2" s="86" t="s">
+        <v>328</v>
+      </c>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
       <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -7561,10 +7558,10 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B6" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="F6" s="59">
         <v>1809596</v>
@@ -7575,10 +7572,10 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B7" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="F7" s="59">
         <v>1809596</v>
@@ -7589,7 +7586,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B8" t="s">
         <v>79</v>
@@ -7603,7 +7600,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B9" t="s">
         <v>79</v>
@@ -7647,7 +7644,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B13" t="s">
         <v>95</v>

</xml_diff>

<commit_message>
Added excel download link, corrected omnifet option B in ignition page.
</commit_message>
<xml_diff>
--- a/PumaBom-WithMods-Element14.xlsx
+++ b/PumaBom-WithMods-Element14.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="0" windowWidth="15600" windowHeight="5160" tabRatio="710"/>
+    <workbookView xWindow="-75" yWindow="3105" windowWidth="15600" windowHeight="5160" tabRatio="710"/>
   </bookViews>
   <sheets>
     <sheet name="Primary Parts" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="425">
   <si>
     <t>MCU</t>
   </si>
@@ -1321,6 +1321,12 @@
   </si>
   <si>
     <t>http://puma.freeems.org/how.to.guide/spin1/</t>
+  </si>
+  <si>
+    <t>BOM in Excel format found here</t>
+  </si>
+  <si>
+    <t>http://puma.freeems.org/preston.bom/PumaBom-WithMods-Element14.xlsx</t>
   </si>
 </sst>
 </file>
@@ -1723,7 +1729,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1820,6 +1826,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1906,6 +1915,15 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1927,13 +1945,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>212912</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>11206</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>224118</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>179295</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1974,13 +1992,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>208429</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>186018</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>212911</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>168088</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2310,7 +2328,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:L87"/>
+  <dimension ref="A1:L89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
@@ -2346,54 +2364,54 @@
         <v>238</v>
       </c>
       <c r="C2" s="17"/>
-      <c r="D2" s="72" t="s">
+      <c r="D2" s="73" t="s">
         <v>386</v>
       </c>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="97" t="s">
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="100" t="s">
         <v>295</v>
       </c>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
+      <c r="I2" s="100"/>
+      <c r="J2" s="100"/>
+      <c r="K2" s="100"/>
       <c r="L2" s="47"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="47"/>
       <c r="B3" s="47"/>
       <c r="C3" s="18"/>
-      <c r="D3" s="76" t="s">
+      <c r="D3" s="77" t="s">
         <v>387</v>
       </c>
-      <c r="E3" s="77"/>
-      <c r="F3" s="77"/>
-      <c r="G3" s="77"/>
-      <c r="H3" s="80" t="s">
+      <c r="E3" s="78"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="81" t="s">
         <v>422</v>
       </c>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="82"/>
       <c r="L3" s="47"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="47"/>
       <c r="B4" s="47"/>
       <c r="C4" s="19"/>
-      <c r="D4" s="72" t="s">
+      <c r="D4" s="73" t="s">
         <v>388</v>
       </c>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
-      <c r="H4" s="99" t="s">
+      <c r="E4" s="74"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="100" t="s">
         <v>385</v>
       </c>
-      <c r="I4" s="99"/>
-      <c r="J4" s="99"/>
-      <c r="K4" s="99"/>
+      <c r="I4" s="100"/>
+      <c r="J4" s="100"/>
+      <c r="K4" s="100"/>
       <c r="L4" s="47"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -2404,94 +2422,98 @@
       <c r="E5" s="47"/>
       <c r="F5" s="56"/>
       <c r="G5" s="47"/>
-      <c r="H5" s="83" t="s">
+      <c r="H5" s="103" t="s">
         <v>384</v>
       </c>
-      <c r="I5" s="83"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="83"/>
-      <c r="L5" s="83"/>
+      <c r="I5" s="103"/>
+      <c r="J5" s="103"/>
+      <c r="K5" s="103"/>
+      <c r="L5" s="103"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="47"/>
       <c r="B6" s="47"/>
-      <c r="C6" s="47"/>
+      <c r="C6" s="53"/>
       <c r="D6" s="47"/>
       <c r="E6" s="47"/>
-      <c r="F6" s="56"/>
+      <c r="F6" s="68"/>
       <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="47"/>
-      <c r="J6" s="47"/>
-      <c r="K6" s="47"/>
-      <c r="L6" s="47"/>
-    </row>
-    <row r="7" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="85" t="s">
+      <c r="H6" s="100" t="s">
+        <v>423</v>
+      </c>
+      <c r="I6" s="100"/>
+      <c r="J6" s="100"/>
+      <c r="K6" s="100"/>
+      <c r="L6" s="102"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="47"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="101" t="s">
+        <v>424</v>
+      </c>
+      <c r="H7" s="101"/>
+      <c r="I7" s="101"/>
+      <c r="J7" s="101"/>
+      <c r="K7" s="101"/>
+      <c r="L7" s="101"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="47"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="56"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="47"/>
+      <c r="L8" s="47"/>
+    </row>
+    <row r="9" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="86" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="85"/>
-      <c r="C7" s="85"/>
-      <c r="D7" s="85"/>
-      <c r="E7" s="85"/>
-      <c r="F7" s="85" t="s">
+      <c r="B9" s="86"/>
+      <c r="C9" s="86"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="86"/>
+      <c r="F9" s="86" t="s">
         <v>175</v>
       </c>
-      <c r="G7" s="85"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="86" t="s">
+      <c r="G9" s="86"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="87" t="s">
         <v>330</v>
       </c>
-      <c r="J7" s="86"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="J9" s="87"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="73" t="s">
+      <c r="B10" s="74" t="s">
         <v>227</v>
       </c>
-      <c r="C8" s="73"/>
-      <c r="F8" s="59">
+      <c r="C10" s="74"/>
+      <c r="F10" s="59">
         <v>1380343</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G10" s="6" t="s">
         <v>174</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" s="59">
-        <v>1652909</v>
-      </c>
-      <c r="G9" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" s="59">
-        <v>1652909</v>
-      </c>
-      <c r="G10" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>3</v>
@@ -2505,7 +2527,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>3</v>
@@ -2517,15 +2539,13 @@
         <v>216</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="41" t="s">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
       <c r="F13" s="59">
         <v>1652909</v>
       </c>
@@ -2534,264 +2554,261 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="68" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="42" t="s">
-        <v>87</v>
-      </c>
-      <c r="C14" s="46" t="s">
-        <v>389</v>
+      <c r="A14" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>3</v>
       </c>
       <c r="F14" s="59">
-        <v>1740667</v>
+        <v>1652909</v>
       </c>
       <c r="G14" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="69" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="43" t="s">
-        <v>362</v>
-      </c>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
       <c r="F15" s="59">
-        <v>1414699</v>
+        <v>1652909</v>
       </c>
       <c r="G15" t="s">
-        <v>380</v>
+        <v>216</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="69" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" s="46" t="s">
+        <v>389</v>
+      </c>
+      <c r="F16" s="59">
+        <v>1740667</v>
+      </c>
+      <c r="G16" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="70" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="43" t="s">
+        <v>362</v>
+      </c>
+      <c r="F17" s="59">
+        <v>1414699</v>
+      </c>
+      <c r="G17" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="43" t="s">
+      <c r="B18" s="43" t="s">
         <v>370</v>
       </c>
-      <c r="F16" s="59">
+      <c r="F18" s="59">
         <v>8820066</v>
       </c>
-      <c r="G16" s="73" t="s">
+      <c r="G18" s="74" t="s">
         <v>381</v>
       </c>
-      <c r="H16" s="73"/>
-    </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="70" t="s">
+      <c r="H18" s="74"/>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="44" t="s">
+      <c r="B19" s="44" t="s">
         <v>361</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="F17" s="59">
+      <c r="C19" s="45"/>
+      <c r="F19" s="59">
         <v>1887293</v>
       </c>
-      <c r="G17" s="73" t="s">
+      <c r="G19" s="74" t="s">
         <v>382</v>
       </c>
-      <c r="H17" s="73"/>
-    </row>
-    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="71" t="s">
+      <c r="H19" s="74"/>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="72" t="s">
         <v>366</v>
       </c>
-      <c r="B18" s="35" t="s">
+      <c r="B20" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="39" t="s">
+      <c r="C20" s="39" t="s">
         <v>390</v>
       </c>
-      <c r="F18" s="59">
+      <c r="F20" s="59">
         <v>1414676</v>
       </c>
-      <c r="G18" s="73" t="s">
+      <c r="G20" s="74" t="s">
         <v>224</v>
       </c>
-      <c r="H18" s="73"/>
-      <c r="I18" s="73"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="34"/>
-      <c r="B19" s="37" t="s">
+      <c r="H20" s="74"/>
+      <c r="I20" s="74"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="34"/>
+      <c r="B21" s="37" t="s">
         <v>364</v>
       </c>
-      <c r="C19" s="36"/>
-      <c r="F19" s="59">
+      <c r="C21" s="36"/>
+      <c r="F21" s="59">
         <v>1414668</v>
       </c>
-      <c r="G19" s="73" t="s">
+      <c r="G21" s="74" t="s">
         <v>368</v>
       </c>
-      <c r="H19" s="73"/>
-      <c r="I19" s="73"/>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="30"/>
-      <c r="B20" s="38" t="s">
+      <c r="H21" s="74"/>
+      <c r="I21" s="74"/>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="30"/>
+      <c r="B22" s="38" t="s">
         <v>365</v>
       </c>
-      <c r="C20" s="36"/>
-      <c r="F20" s="59">
+      <c r="C22" s="36"/>
+      <c r="F22" s="59">
         <v>1414685</v>
       </c>
-      <c r="G20" s="73" t="s">
+      <c r="G22" s="74" t="s">
         <v>369</v>
       </c>
-      <c r="H20" s="73"/>
-      <c r="I20" s="73"/>
-    </row>
-    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="71" t="s">
+      <c r="H22" s="74"/>
+      <c r="I22" s="74"/>
+    </row>
+    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="35" t="s">
+      <c r="B23" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="39"/>
-      <c r="F21" s="59">
+      <c r="C23" s="39"/>
+      <c r="F23" s="59">
         <v>1414676</v>
       </c>
-      <c r="G21" s="73" t="s">
+      <c r="G23" s="74" t="s">
         <v>224</v>
       </c>
-      <c r="H21" s="73"/>
-      <c r="I21" s="73"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="32"/>
-      <c r="B22" s="29" t="s">
+      <c r="H23" s="74"/>
+      <c r="I23" s="74"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="32"/>
+      <c r="B24" s="29" t="s">
         <v>364</v>
       </c>
-      <c r="F22" s="59">
+      <c r="F24" s="59">
         <v>1414668</v>
       </c>
-      <c r="G22" s="73" t="s">
+      <c r="G24" s="74" t="s">
         <v>368</v>
       </c>
-      <c r="H22" s="73"/>
-      <c r="I22" s="73"/>
-    </row>
-    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="33"/>
-      <c r="B23" s="31" t="s">
+      <c r="H24" s="74"/>
+      <c r="I24" s="74"/>
+    </row>
+    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="33"/>
+      <c r="B25" s="31" t="s">
         <v>365</v>
       </c>
-      <c r="F23" s="59">
+      <c r="F25" s="59">
         <v>1414685</v>
       </c>
-      <c r="G23" s="73" t="s">
+      <c r="G25" s="74" t="s">
         <v>369</v>
       </c>
-      <c r="H23" s="73"/>
-      <c r="I23" s="73"/>
-    </row>
-    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="26" t="s">
+      <c r="H25" s="74"/>
+      <c r="I25" s="74"/>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="28" t="s">
+      <c r="B26" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="74" t="s">
+      <c r="C26" s="75" t="s">
         <v>391</v>
       </c>
-      <c r="D24" s="73"/>
-      <c r="E24" s="73"/>
-      <c r="F24" s="59">
+      <c r="D26" s="74"/>
+      <c r="E26" s="74"/>
+      <c r="F26" s="59">
         <v>1469858</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G26" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="13"/>
-      <c r="B25" s="27" t="s">
+    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="13"/>
+      <c r="B27" s="27" t="s">
         <v>363</v>
       </c>
-      <c r="C25" s="74" t="s">
+      <c r="C27" s="75" t="s">
         <v>391</v>
       </c>
-      <c r="D25" s="75"/>
-      <c r="E25" s="75"/>
-      <c r="F25" s="59">
+      <c r="D27" s="76"/>
+      <c r="E27" s="76"/>
+      <c r="F27" s="59">
         <v>9332413</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G27" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B26" t="s">
-        <v>18</v>
-      </c>
-      <c r="F26" s="59">
-        <v>1712841</v>
-      </c>
-      <c r="G26" s="73" t="s">
-        <v>219</v>
-      </c>
-      <c r="H26" s="73"/>
-      <c r="I26" s="73"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="F27" s="59">
-        <v>1740667</v>
-      </c>
-      <c r="G27" s="73" t="s">
-        <v>379</v>
-      </c>
-      <c r="H27" s="73"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
-        <v>367</v>
-      </c>
-      <c r="B28" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" t="s">
+        <v>18</v>
+      </c>
+      <c r="F28" s="59">
+        <v>1712841</v>
+      </c>
+      <c r="G28" s="74" t="s">
+        <v>219</v>
+      </c>
+      <c r="H28" s="74"/>
+      <c r="I28" s="74"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="F28" s="59">
+      <c r="F29" s="59">
         <v>1740667</v>
       </c>
-      <c r="G28" s="73" t="s">
+      <c r="G29" s="74" t="s">
         <v>379</v>
       </c>
-      <c r="H28" s="73"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B29" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="C29" s="78" t="s">
-        <v>378</v>
-      </c>
-      <c r="D29" s="78"/>
-      <c r="F29" s="59">
-        <v>1809300</v>
-      </c>
-      <c r="G29" s="66" t="s">
-        <v>209</v>
-      </c>
+      <c r="H29" s="74"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>22</v>
+        <v>367</v>
       </c>
       <c r="B30" s="14" t="s">
         <v>87</v>
@@ -2799,29 +2816,32 @@
       <c r="F30" s="59">
         <v>1740667</v>
       </c>
-      <c r="G30" s="73" t="s">
+      <c r="G30" s="74" t="s">
         <v>379</v>
       </c>
-      <c r="H30" s="73"/>
+      <c r="H30" s="74"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B31" s="14" t="s">
-        <v>87</v>
-      </c>
+      <c r="A31" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C31" s="79" t="s">
+        <v>378</v>
+      </c>
+      <c r="D31" s="79"/>
       <c r="F31" s="59">
-        <v>1740667</v>
-      </c>
-      <c r="G31" s="73" t="s">
-        <v>379</v>
-      </c>
-      <c r="H31" s="73"/>
+        <v>1809300</v>
+      </c>
+      <c r="G31" s="66" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B32" s="14" t="s">
         <v>87</v>
@@ -2829,584 +2849,612 @@
       <c r="F32" s="59">
         <v>1740667</v>
       </c>
-      <c r="G32" s="73" t="s">
+      <c r="G32" s="74" t="s">
         <v>379</v>
       </c>
-      <c r="H32" s="73"/>
+      <c r="H32" s="74"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="9"/>
-      <c r="B33" s="2"/>
-      <c r="F33" s="59"/>
+      <c r="A33" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="F33" s="59">
+        <v>1740667</v>
+      </c>
+      <c r="G33" s="74" t="s">
+        <v>379</v>
+      </c>
+      <c r="H33" s="74"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="88" t="s">
+      <c r="A34" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="F34" s="59">
+        <v>1740667</v>
+      </c>
+      <c r="G34" s="74" t="s">
+        <v>379</v>
+      </c>
+      <c r="H34" s="74"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="9"/>
+      <c r="B35" s="2"/>
+      <c r="F35" s="59"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="89" t="s">
         <v>420</v>
       </c>
-      <c r="B34" s="88"/>
-      <c r="C34" s="88"/>
-      <c r="D34" s="88"/>
-      <c r="E34" s="98" t="s">
+      <c r="B36" s="89"/>
+      <c r="C36" s="89"/>
+      <c r="D36" s="89"/>
+      <c r="E36" s="99" t="s">
         <v>419</v>
       </c>
-      <c r="F34" s="59">
+      <c r="F36" s="59">
         <v>1833277</v>
       </c>
-      <c r="G34" t="s">
+      <c r="G36" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="84" t="s">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="B36" s="84"/>
-      <c r="C36" s="84"/>
-      <c r="D36" s="84"/>
-      <c r="E36" s="84"/>
-      <c r="F36" s="84"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="86" t="s">
+      <c r="B38" s="85"/>
+      <c r="C38" s="85"/>
+      <c r="D38" s="85"/>
+      <c r="E38" s="85"/>
+      <c r="F38" s="85"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="87" t="s">
         <v>331</v>
       </c>
-      <c r="J36" s="86"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="9" t="s">
+      <c r="J38" s="87"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="4"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B39" t="s">
         <v>33</v>
       </c>
-      <c r="F37" s="59">
+      <c r="F39" s="59">
         <v>1146032</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G39" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="48" t="s">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="B38" s="49" t="s">
+      <c r="B40" s="49" t="s">
         <v>20</v>
-      </c>
-      <c r="F38" s="59">
-        <v>8820120</v>
-      </c>
-      <c r="G38" s="73" t="s">
-        <v>218</v>
-      </c>
-      <c r="H38" s="73"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="50"/>
-      <c r="B39" s="51" t="s">
-        <v>36</v>
-      </c>
-      <c r="C39" s="87" t="s">
-        <v>217</v>
-      </c>
-      <c r="D39" s="73"/>
-      <c r="E39" s="73"/>
-      <c r="F39" s="59">
-        <v>1853520</v>
-      </c>
-      <c r="G39" s="73" t="s">
-        <v>383</v>
-      </c>
-      <c r="H39" s="73"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B40" t="s">
-        <v>8</v>
       </c>
       <c r="F40" s="59">
         <v>8820120</v>
       </c>
-      <c r="G40" s="73" t="s">
+      <c r="G40" s="74" t="s">
         <v>218</v>
       </c>
-      <c r="H40" s="73"/>
+      <c r="H40" s="74"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B41" t="s">
-        <v>38</v>
-      </c>
-      <c r="C41" s="52"/>
+      <c r="A41" s="50"/>
+      <c r="B41" s="51" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" s="88" t="s">
+        <v>217</v>
+      </c>
+      <c r="D41" s="74"/>
+      <c r="E41" s="74"/>
       <c r="F41" s="59">
-        <v>9334084</v>
-      </c>
-      <c r="G41" t="s">
-        <v>209</v>
-      </c>
+        <v>1853520</v>
+      </c>
+      <c r="G41" s="74" t="s">
+        <v>383</v>
+      </c>
+      <c r="H41" s="74"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B42" s="73" t="s">
-        <v>41</v>
-      </c>
-      <c r="C42" s="73"/>
-      <c r="D42" s="73"/>
+      <c r="A42" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B42" t="s">
+        <v>8</v>
+      </c>
       <c r="F42" s="59">
-        <v>9406352</v>
-      </c>
-      <c r="G42" s="73" t="s">
-        <v>239</v>
-      </c>
-      <c r="H42" s="73"/>
+        <v>8820120</v>
+      </c>
+      <c r="G42" s="74" t="s">
+        <v>218</v>
+      </c>
+      <c r="H42" s="74"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B43" s="73" t="s">
-        <v>169</v>
-      </c>
-      <c r="C43" s="73"/>
-      <c r="D43" s="73"/>
+        <v>37</v>
+      </c>
+      <c r="B43" t="s">
+        <v>38</v>
+      </c>
+      <c r="C43" s="52"/>
       <c r="F43" s="59">
-        <v>1355761</v>
+        <v>9334084</v>
       </c>
       <c r="G43" t="s">
-        <v>180</v>
+        <v>209</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B44" t="s">
-        <v>44</v>
-      </c>
+      <c r="A44" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B44" s="74" t="s">
+        <v>41</v>
+      </c>
+      <c r="C44" s="74"/>
+      <c r="D44" s="74"/>
       <c r="F44" s="59">
-        <v>1226390</v>
-      </c>
-      <c r="G44" t="s">
-        <v>178</v>
-      </c>
+        <v>9406352</v>
+      </c>
+      <c r="G44" s="74" t="s">
+        <v>239</v>
+      </c>
+      <c r="H44" s="74"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B45" s="74" t="s">
+        <v>169</v>
+      </c>
+      <c r="C45" s="74"/>
+      <c r="D45" s="74"/>
+      <c r="F45" s="59">
+        <v>1355761</v>
+      </c>
+      <c r="G45" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B46" t="s">
+        <v>44</v>
+      </c>
+      <c r="F46" s="59">
+        <v>1226390</v>
+      </c>
+      <c r="G46" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B47" t="s">
         <v>45</v>
       </c>
-      <c r="F45" s="59">
+      <c r="F47" s="59">
         <v>1465996</v>
       </c>
-      <c r="G45" t="s">
+      <c r="G47" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="13" t="s">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B48" t="s">
         <v>48</v>
       </c>
-      <c r="F46" s="59">
+      <c r="F48" s="59">
         <v>1809376</v>
       </c>
-      <c r="G46" t="s">
+      <c r="G48" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="13" t="s">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B49" t="s">
         <v>48</v>
       </c>
-      <c r="F47" s="59">
+      <c r="F49" s="59">
         <v>1809376</v>
       </c>
-      <c r="G47" t="s">
+      <c r="G49" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" s="13"/>
-      <c r="F48" s="59"/>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A49" s="88" t="s">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" s="13"/>
+      <c r="F50" s="59"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" s="89" t="s">
         <v>400</v>
       </c>
-      <c r="B49" s="88"/>
-      <c r="C49" s="88"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="10" t="s">
+      <c r="B51" s="89"/>
+      <c r="C51" s="89"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="10" t="s">
         <v>419</v>
       </c>
-      <c r="F49" s="59">
+      <c r="F51" s="59">
         <v>9558527</v>
       </c>
-      <c r="G49" s="73" t="s">
+      <c r="G51" s="74" t="s">
         <v>399</v>
       </c>
-      <c r="H49" s="73"/>
-      <c r="I49" s="73"/>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25"/>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" s="84" t="s">
+      <c r="H51" s="74"/>
+      <c r="I51" s="74"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" s="85" t="s">
         <v>49</v>
       </c>
-      <c r="B51" s="84"/>
-      <c r="C51" s="84"/>
-      <c r="D51" s="84"/>
-      <c r="E51" s="84"/>
-      <c r="F51" s="84"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-      <c r="I51" s="86" t="s">
+      <c r="B53" s="85"/>
+      <c r="C53" s="85"/>
+      <c r="D53" s="85"/>
+      <c r="E53" s="85"/>
+      <c r="F53" s="85"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+      <c r="I53" s="87" t="s">
         <v>332</v>
       </c>
-      <c r="J51" s="86"/>
-      <c r="K51" s="4"/>
-      <c r="L51" s="4"/>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A52" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B52" t="s">
-        <v>27</v>
-      </c>
-      <c r="F52" s="59">
-        <v>1556741</v>
-      </c>
-      <c r="G52" s="73" t="s">
-        <v>182</v>
-      </c>
-      <c r="H52" s="73"/>
-      <c r="I52" s="73"/>
-      <c r="J52" s="73"/>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A53" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B53" t="s">
-        <v>29</v>
-      </c>
-      <c r="F53" s="59">
-        <v>9229272</v>
-      </c>
-      <c r="G53" s="73" t="s">
-        <v>229</v>
-      </c>
-      <c r="H53" s="73"/>
-      <c r="I53" s="73"/>
-      <c r="J53" s="73"/>
+      <c r="J53" s="87"/>
+      <c r="K53" s="4"/>
+      <c r="L53" s="4"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B54" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F54" s="59">
-        <v>8820120</v>
-      </c>
-      <c r="G54" s="73" t="s">
-        <v>218</v>
-      </c>
-      <c r="H54" s="73"/>
-      <c r="I54" s="73"/>
-      <c r="J54" s="73"/>
+        <v>1556741</v>
+      </c>
+      <c r="G54" s="74" t="s">
+        <v>182</v>
+      </c>
+      <c r="H54" s="74"/>
+      <c r="I54" s="74"/>
+      <c r="J54" s="74"/>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B55" t="s">
-        <v>79</v>
+        <v>29</v>
       </c>
       <c r="F55" s="59">
-        <v>9556915</v>
-      </c>
-      <c r="G55" s="73" t="s">
-        <v>235</v>
-      </c>
-      <c r="H55" s="73"/>
-      <c r="I55" s="73"/>
-      <c r="J55" s="73"/>
+        <v>9229272</v>
+      </c>
+      <c r="G55" s="74" t="s">
+        <v>229</v>
+      </c>
+      <c r="H55" s="74"/>
+      <c r="I55" s="74"/>
+      <c r="J55" s="74"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="B56" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="F56" s="59">
-        <v>1617365</v>
-      </c>
-      <c r="G56" s="73" t="s">
-        <v>228</v>
-      </c>
-      <c r="H56" s="73"/>
-      <c r="I56" s="73"/>
-      <c r="J56" s="73"/>
+        <v>8820120</v>
+      </c>
+      <c r="G56" s="74" t="s">
+        <v>218</v>
+      </c>
+      <c r="H56" s="74"/>
+      <c r="I56" s="74"/>
+      <c r="J56" s="74"/>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B57" t="s">
+        <v>79</v>
+      </c>
+      <c r="F57" s="59">
+        <v>9556915</v>
+      </c>
+      <c r="G57" s="74" t="s">
+        <v>235</v>
+      </c>
+      <c r="H57" s="74"/>
+      <c r="I57" s="74"/>
+      <c r="J57" s="74"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B58" t="s">
+        <v>51</v>
+      </c>
+      <c r="F58" s="59">
+        <v>1617365</v>
+      </c>
+      <c r="G58" s="74" t="s">
+        <v>228</v>
+      </c>
+      <c r="H58" s="74"/>
+      <c r="I58" s="74"/>
+      <c r="J58" s="74"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B59" t="s">
         <v>53</v>
       </c>
-      <c r="F57" s="59">
+      <c r="F59" s="59">
         <v>8820120</v>
       </c>
-      <c r="G57" s="73" t="s">
+      <c r="G59" s="74" t="s">
         <v>218</v>
       </c>
-      <c r="H57" s="73"/>
-      <c r="I57" s="73"/>
-      <c r="J57" s="73"/>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A58" s="10" t="s">
+      <c r="H59" s="74"/>
+      <c r="I59" s="74"/>
+      <c r="J59" s="74"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B60" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C58" s="73" t="s">
+      <c r="C60" s="74" t="s">
         <v>392</v>
       </c>
-      <c r="D58" s="73"/>
-      <c r="E58" s="73"/>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="84" t="s">
+      <c r="D60" s="74"/>
+      <c r="E60" s="74"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="85" t="s">
         <v>56</v>
       </c>
-      <c r="B61" s="84"/>
-      <c r="C61" s="84"/>
-      <c r="D61" s="84"/>
-      <c r="E61" s="84"/>
-      <c r="F61" s="60"/>
-      <c r="G61" s="3"/>
-      <c r="H61" s="3"/>
-      <c r="I61" s="86" t="s">
+      <c r="B63" s="85"/>
+      <c r="C63" s="85"/>
+      <c r="D63" s="85"/>
+      <c r="E63" s="85"/>
+      <c r="F63" s="60"/>
+      <c r="G63" s="3"/>
+      <c r="H63" s="3"/>
+      <c r="I63" s="87" t="s">
         <v>333</v>
       </c>
-      <c r="J61" s="86"/>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A62" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="B62" t="s">
-        <v>60</v>
-      </c>
-      <c r="F62" s="59">
-        <v>9486038</v>
-      </c>
-      <c r="G62" s="79" t="s">
-        <v>356</v>
-      </c>
-      <c r="H62" s="79"/>
-      <c r="I62" s="79"/>
-      <c r="J62" s="79"/>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A63" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B63" t="s">
-        <v>55</v>
-      </c>
-      <c r="F63" s="59">
-        <v>1324152</v>
-      </c>
-      <c r="G63" s="73" t="s">
-        <v>230</v>
-      </c>
-      <c r="H63" s="73"/>
-      <c r="I63" s="73"/>
+      <c r="J63" s="87"/>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B64" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="F64" s="59">
-        <v>1617365</v>
-      </c>
-      <c r="G64" s="73" t="s">
-        <v>228</v>
-      </c>
-      <c r="H64" s="73"/>
-      <c r="I64" s="73"/>
+        <v>9486038</v>
+      </c>
+      <c r="G64" s="80" t="s">
+        <v>356</v>
+      </c>
+      <c r="H64" s="80"/>
+      <c r="I64" s="80"/>
+      <c r="J64" s="80"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B65" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="F65" s="59">
-        <v>8820120</v>
-      </c>
-      <c r="G65" s="73" t="s">
-        <v>218</v>
-      </c>
-      <c r="H65" s="73"/>
-      <c r="I65" s="73"/>
+        <v>1324152</v>
+      </c>
+      <c r="G65" s="74" t="s">
+        <v>230</v>
+      </c>
+      <c r="H65" s="74"/>
+      <c r="I65" s="74"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="F66" s="59">
-        <v>9229272</v>
-      </c>
-      <c r="G66" s="73" t="s">
-        <v>229</v>
-      </c>
-      <c r="H66" s="73"/>
-      <c r="I66" s="73"/>
+        <v>1617365</v>
+      </c>
+      <c r="G66" s="74" t="s">
+        <v>228</v>
+      </c>
+      <c r="H66" s="74"/>
+      <c r="I66" s="74"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="B67" s="24" t="s">
-        <v>51</v>
+      <c r="A67" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>20</v>
       </c>
       <c r="F67" s="59">
-        <v>1617365</v>
-      </c>
-      <c r="G67" s="73" t="s">
-        <v>228</v>
-      </c>
-      <c r="H67" s="73"/>
-      <c r="I67" s="73"/>
+        <v>8820120</v>
+      </c>
+      <c r="G67" s="74" t="s">
+        <v>218</v>
+      </c>
+      <c r="H67" s="74"/>
+      <c r="I67" s="74"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B68" t="s">
+        <v>29</v>
+      </c>
+      <c r="F68" s="59">
+        <v>9229272</v>
+      </c>
+      <c r="G68" s="74" t="s">
+        <v>229</v>
+      </c>
+      <c r="H68" s="74"/>
+      <c r="I68" s="74"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="B69" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="F69" s="59">
+        <v>1617365</v>
+      </c>
+      <c r="G69" s="74" t="s">
+        <v>228</v>
+      </c>
+      <c r="H69" s="74"/>
+      <c r="I69" s="74"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B70" t="s">
         <v>20</v>
       </c>
-      <c r="F68" s="59">
+      <c r="F70" s="59">
         <v>8820120</v>
       </c>
-      <c r="G68" s="73" t="s">
+      <c r="G70" s="74" t="s">
         <v>218</v>
       </c>
-      <c r="H68" s="73"/>
-      <c r="I68" s="73"/>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="9"/>
-      <c r="F69" s="59"/>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="B70" s="88" t="s">
-        <v>291</v>
-      </c>
-      <c r="C70" s="88"/>
-      <c r="D70" s="88"/>
-      <c r="E70" s="88"/>
-      <c r="F70" s="88"/>
+      <c r="H70" s="74"/>
+      <c r="I70" s="74"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="B71" s="88" t="s">
-        <v>291</v>
-      </c>
-      <c r="C71" s="88"/>
-      <c r="D71" s="88"/>
-      <c r="E71" s="88"/>
-      <c r="F71" s="88"/>
+      <c r="A71" s="9"/>
+      <c r="F71" s="59"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B72" s="88" t="s">
+        <v>61</v>
+      </c>
+      <c r="B72" s="89" t="s">
         <v>291</v>
       </c>
-      <c r="C72" s="88"/>
-      <c r="D72" s="88"/>
-      <c r="E72" s="88"/>
-      <c r="F72" s="88"/>
+      <c r="C72" s="89"/>
+      <c r="D72" s="89"/>
+      <c r="E72" s="89"/>
+      <c r="F72" s="89"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="B73" s="88" t="s">
+        <v>62</v>
+      </c>
+      <c r="B73" s="89" t="s">
         <v>291</v>
       </c>
-      <c r="C73" s="88"/>
-      <c r="D73" s="88"/>
-      <c r="E73" s="88"/>
-      <c r="F73" s="88"/>
+      <c r="C73" s="89"/>
+      <c r="D73" s="89"/>
+      <c r="E73" s="89"/>
+      <c r="F73" s="89"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>55</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="B74" s="89" t="s">
+        <v>291</v>
+      </c>
+      <c r="C74" s="89"/>
+      <c r="D74" s="89"/>
+      <c r="E74" s="89"/>
+      <c r="F74" s="89"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B75" s="89" t="s">
+        <v>291</v>
+      </c>
+      <c r="C75" s="89"/>
+      <c r="D75" s="89"/>
+      <c r="E75" s="89"/>
+      <c r="F75" s="89"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B75" s="88" t="s">
+      <c r="B77" s="89" t="s">
         <v>421</v>
       </c>
-      <c r="C75" s="88"/>
-      <c r="D75" s="88"/>
-      <c r="E75" s="88"/>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25"/>
-    <row r="77" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="F77" s="59"/>
-    </row>
-    <row r="78" spans="1:9" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" spans="1:9" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.25"/>
+      <c r="C77" s="89"/>
+      <c r="D77" s="89"/>
+      <c r="E77" s="89"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F79" s="59"/>
+    </row>
+    <row r="80" spans="1:9" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="81" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="82" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="83" hidden="1" x14ac:dyDescent="0.25"/>
@@ -3414,130 +3462,135 @@
     <row r="85" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="86" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="87" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="88" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="89" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="63">
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="G49:I49"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="B75:E75"/>
-    <mergeCell ref="B70:F70"/>
-    <mergeCell ref="B71:F71"/>
+  <mergeCells count="65">
+    <mergeCell ref="G7:L7"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="G51:I51"/>
+    <mergeCell ref="A51:C51"/>
+    <mergeCell ref="B77:E77"/>
     <mergeCell ref="B72:F72"/>
     <mergeCell ref="B73:F73"/>
-    <mergeCell ref="A51:F51"/>
-    <mergeCell ref="A61:E61"/>
-    <mergeCell ref="I61:J61"/>
-    <mergeCell ref="I51:J51"/>
+    <mergeCell ref="B74:F74"/>
+    <mergeCell ref="B75:F75"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="A63:E63"/>
+    <mergeCell ref="I63:J63"/>
+    <mergeCell ref="I53:J53"/>
+    <mergeCell ref="G70:I70"/>
+    <mergeCell ref="G69:I69"/>
     <mergeCell ref="G68:I68"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="A38:F38"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="A36:D36"/>
     <mergeCell ref="G67:I67"/>
     <mergeCell ref="G66:I66"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="A36:F36"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="A34:D34"/>
     <mergeCell ref="G65:I65"/>
-    <mergeCell ref="G64:I64"/>
-    <mergeCell ref="G63:I63"/>
-    <mergeCell ref="G62:J62"/>
+    <mergeCell ref="G64:J64"/>
+    <mergeCell ref="G59:J59"/>
+    <mergeCell ref="G58:J58"/>
     <mergeCell ref="G57:J57"/>
     <mergeCell ref="G56:J56"/>
     <mergeCell ref="G55:J55"/>
     <mergeCell ref="G54:J54"/>
-    <mergeCell ref="G53:J53"/>
-    <mergeCell ref="G52:J52"/>
-    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="G33:H33"/>
     <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G31:H31"/>
     <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="G24:I24"/>
     <mergeCell ref="G23:I23"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="D3:G3"/>
     <mergeCell ref="G22:I22"/>
     <mergeCell ref="G21:I21"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="D3:G3"/>
     <mergeCell ref="G20:I20"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G18:H18"/>
     <mergeCell ref="H3:K3"/>
     <mergeCell ref="H2:K2"/>
     <mergeCell ref="H4:K4"/>
     <mergeCell ref="H5:L5"/>
+    <mergeCell ref="H6:K6"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F8" r:id="rId1" display="http://nz.element14.com/freescale-semiconductor/mc9s12xdp512mal/ic-16bit-microcontroller/dp/1380343"/>
-    <hyperlink ref="F37" r:id="rId2" display="http://nz.element14.com/ftdi/ft232rl/ic-usb-to-uart-smd-ssop28-232/dp/1146032"/>
-    <hyperlink ref="F41" r:id="rId3" display="http://nz.element14.com/multicomp/mc-0-1w-0805-5-2k/resistor-0805-2k/dp/9334084"/>
-    <hyperlink ref="F44" r:id="rId4" display="http://nz.element14.com/osram/lsq976-z/led-smd-red/dp/1226390"/>
-    <hyperlink ref="F45" r:id="rId5" display="http://nz.element14.com/dialight/5988170107f/led-0805-green/dp/1465996"/>
-    <hyperlink ref="F46" r:id="rId6" display="http://nz.element14.com/koa/rk73b2attd471j/resistor-0805-470-ohm-5/dp/1809376"/>
-    <hyperlink ref="F47" r:id="rId7" display="http://nz.element14.com/koa/rk73b2attd471j/resistor-0805-470-ohm-5/dp/1809376"/>
-    <hyperlink ref="F43" r:id="rId8" display="http://nz.element14.com/molex/678038020/socket-mini-usb-otg/dp/1355761"/>
-    <hyperlink ref="F62" r:id="rId9" display="http://nz.element14.com/national-semiconductor/lm2937-5-0/ic-v-reg-ldo-5-0v-2937-to-220-3/dp/9486038"/>
-    <hyperlink ref="F52" r:id="rId10" display="http://nz.element14.com/micrel-semiconductor/mic2954-02ws/ic-reg-ldo-250ma-5v-0-5/dp/1556741"/>
-    <hyperlink ref="F65" r:id="rId11" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
-    <hyperlink ref="F68" r:id="rId12" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
-    <hyperlink ref="F57" r:id="rId13" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
-    <hyperlink ref="F54" r:id="rId14" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
-    <hyperlink ref="F38" r:id="rId15" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
-    <hyperlink ref="F40" r:id="rId16" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
-    <hyperlink ref="F26" r:id="rId17" display="http://nz.element14.com/epson-toyocom/tsx-3225-16mhz-10ppm-9pf/crystal-tsx-3225-16mhz-10ppm-9pf/dp/1712841"/>
-    <hyperlink ref="F18" r:id="rId18" display="http://nz.element14.com/kemet/c0805c220j1gactu/capacitor-0805-22pf-100v-np0/dp/1414676"/>
-    <hyperlink ref="F56" r:id="rId19" display="http://nz.element14.com/vishay-sprague/199d106x9035d1v1e3/capacitor-tant-10uf-35v-radial/dp/1617365"/>
-    <hyperlink ref="F64" r:id="rId20" display="http://nz.element14.com/vishay-sprague/199d106x9035d1v1e3/capacitor-tant-10uf-35v-radial/dp/1617365"/>
-    <hyperlink ref="F66" r:id="rId21" display="http://nz.element14.com/kemet/t495d226k035ate300/capacitor-22uf-35v/dp/9229272"/>
-    <hyperlink ref="F53" r:id="rId22" display="http://nz.element14.com/kemet/t495d226k035ate300/capacitor-22uf-35v/dp/9229272"/>
-    <hyperlink ref="F63" r:id="rId23" display="http://nz.element14.com/fairchild-semiconductor/1n4007/bridge-rectifier-rohs-compliant/dp/9109625"/>
-    <hyperlink ref="F29" r:id="rId24" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
-    <hyperlink ref="F42" r:id="rId25" display="http://nz.element14.com/multicomp/u0805r103kct/capacitor-0805-10nf-50v/dp/9406352"/>
-    <hyperlink ref="F55" r:id="rId26" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
-    <hyperlink ref="F9" r:id="rId27" display="http://nz.element14.com/vishay-draloric/crcw080510k0fkta/thick-film-chip-resistor/dp/1652909"/>
-    <hyperlink ref="F10" r:id="rId28" display="http://nz.element14.com/vishay-draloric/crcw080510k0fkta/thick-film-chip-resistor/dp/1652909"/>
-    <hyperlink ref="F11" r:id="rId29" display="http://nz.element14.com/vishay-draloric/crcw080510k0fkta/thick-film-chip-resistor/dp/1652909"/>
-    <hyperlink ref="F12" r:id="rId30" display="http://nz.element14.com/vishay-draloric/crcw080510k0fkta/thick-film-chip-resistor/dp/1652909"/>
-    <hyperlink ref="F13" r:id="rId31" display="http://nz.element14.com/vishay-draloric/crcw080510k0fkta/thick-film-chip-resistor/dp/1652909"/>
-    <hyperlink ref="F67" r:id="rId32" display="http://nz.element14.com/vishay-sprague/199d106x9035d1v1e3/capacitor-tant-10uf-35v-radial/dp/1617365"/>
-    <hyperlink ref="F21" r:id="rId33" display="http://nz.element14.com/kemet/c0805c220j1gactu/capacitor-0805-22pf-100v-np0/dp/1414676"/>
-    <hyperlink ref="F19" r:id="rId34" display="http://nz.element14.com/kemet/c0805c150j5gactu/capacitor-0805-15pf-50v-np0/dp/1414668"/>
-    <hyperlink ref="F22" r:id="rId35" display="http://nz.element14.com/kemet/c0805c150j5gactu/capacitor-0805-15pf-50v-np0/dp/1414668"/>
-    <hyperlink ref="F20" r:id="rId36" display="http://nz.element14.com/kemet/c0805c330j5gactu/capacitor-0805-33pf-50v-np0/dp/1414685"/>
-    <hyperlink ref="F23" r:id="rId37" display="http://nz.element14.com/kemet/c0805c330j5gactu/capacitor-0805-33pf-50v-np0/dp/1414685"/>
-    <hyperlink ref="F14" r:id="rId38" display="http://nz.element14.com/avx/08053c224jat2a/capacitor-mlcc-0805-25v-220nf/dp/1740667"/>
-    <hyperlink ref="F27" r:id="rId39" display="http://nz.element14.com/avx/08053c224jat2a/capacitor-mlcc-0805-25v-220nf/dp/1740667"/>
-    <hyperlink ref="F28" r:id="rId40" display="http://nz.element14.com/avx/08053c224jat2a/capacitor-mlcc-0805-25v-220nf/dp/1740667"/>
-    <hyperlink ref="F30" r:id="rId41" display="http://nz.element14.com/avx/08053c224jat2a/capacitor-mlcc-0805-25v-220nf/dp/1740667"/>
-    <hyperlink ref="F31" r:id="rId42" display="http://nz.element14.com/avx/08053c224jat2a/capacitor-mlcc-0805-25v-220nf/dp/1740667"/>
-    <hyperlink ref="F32" r:id="rId43" display="http://nz.element14.com/avx/08053c224jat2a/capacitor-mlcc-0805-25v-220nf/dp/1740667"/>
-    <hyperlink ref="F15" r:id="rId44" display="http://nz.element14.com/kemet"/>
-    <hyperlink ref="F16" r:id="rId45" display="http://nz.element14.com/murata/grm2195c1h682ja01d/capacitor-0805-6-8nf-50v/dp/8820066"/>
-    <hyperlink ref="F17" r:id="rId46" display="http://nz.element14.com/multicomp/mcpwr05ftew3301/resistor-0805-3-3k-1-0-125w/dp/1887293"/>
-    <hyperlink ref="F24" r:id="rId47" display="http://nz.element14.com/yageo-phycomp/rc0805fr-0710ml/resistor-rc12h-0805-10m/dp/9238115"/>
-    <hyperlink ref="F25" r:id="rId48" display="http://nz.element14.com/multicomp/mc-0-1w-0805-1-1m/resistor-1mohm-0-1w-1/dp/9332413"/>
-    <hyperlink ref="F39" r:id="rId49" display="http://nz.element14.com/taiyo-yuden/emk212b7475kg-t/capacitor-ceramic-4-7uf-16v-x7r/dp/1853520"/>
+    <hyperlink ref="F10" r:id="rId1" display="http://nz.element14.com/freescale-semiconductor/mc9s12xdp512mal/ic-16bit-microcontroller/dp/1380343"/>
+    <hyperlink ref="F39" r:id="rId2" display="http://nz.element14.com/ftdi/ft232rl/ic-usb-to-uart-smd-ssop28-232/dp/1146032"/>
+    <hyperlink ref="F43" r:id="rId3" display="http://nz.element14.com/multicomp/mc-0-1w-0805-5-2k/resistor-0805-2k/dp/9334084"/>
+    <hyperlink ref="F46" r:id="rId4" display="http://nz.element14.com/osram/lsq976-z/led-smd-red/dp/1226390"/>
+    <hyperlink ref="F47" r:id="rId5" display="http://nz.element14.com/dialight/5988170107f/led-0805-green/dp/1465996"/>
+    <hyperlink ref="F48" r:id="rId6" display="http://nz.element14.com/koa/rk73b2attd471j/resistor-0805-470-ohm-5/dp/1809376"/>
+    <hyperlink ref="F49" r:id="rId7" display="http://nz.element14.com/koa/rk73b2attd471j/resistor-0805-470-ohm-5/dp/1809376"/>
+    <hyperlink ref="F45" r:id="rId8" display="http://nz.element14.com/molex/678038020/socket-mini-usb-otg/dp/1355761"/>
+    <hyperlink ref="F64" r:id="rId9" display="http://nz.element14.com/national-semiconductor/lm2937-5-0/ic-v-reg-ldo-5-0v-2937-to-220-3/dp/9486038"/>
+    <hyperlink ref="F54" r:id="rId10" display="http://nz.element14.com/micrel-semiconductor/mic2954-02ws/ic-reg-ldo-250ma-5v-0-5/dp/1556741"/>
+    <hyperlink ref="F67" r:id="rId11" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
+    <hyperlink ref="F70" r:id="rId12" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
+    <hyperlink ref="F59" r:id="rId13" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
+    <hyperlink ref="F56" r:id="rId14" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
+    <hyperlink ref="F40" r:id="rId15" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
+    <hyperlink ref="F42" r:id="rId16" display="http://nz.element14.com/murata/grm21br71h104ka01l/capacitor-0805-100nf-50v/dp/8820120"/>
+    <hyperlink ref="F28" r:id="rId17" display="http://nz.element14.com/epson-toyocom/tsx-3225-16mhz-10ppm-9pf/crystal-tsx-3225-16mhz-10ppm-9pf/dp/1712841"/>
+    <hyperlink ref="F20" r:id="rId18" display="http://nz.element14.com/kemet/c0805c220j1gactu/capacitor-0805-22pf-100v-np0/dp/1414676"/>
+    <hyperlink ref="F58" r:id="rId19" display="http://nz.element14.com/vishay-sprague/199d106x9035d1v1e3/capacitor-tant-10uf-35v-radial/dp/1617365"/>
+    <hyperlink ref="F66" r:id="rId20" display="http://nz.element14.com/vishay-sprague/199d106x9035d1v1e3/capacitor-tant-10uf-35v-radial/dp/1617365"/>
+    <hyperlink ref="F68" r:id="rId21" display="http://nz.element14.com/kemet/t495d226k035ate300/capacitor-22uf-35v/dp/9229272"/>
+    <hyperlink ref="F55" r:id="rId22" display="http://nz.element14.com/kemet/t495d226k035ate300/capacitor-22uf-35v/dp/9229272"/>
+    <hyperlink ref="F65" r:id="rId23" display="http://nz.element14.com/fairchild-semiconductor/1n4007/bridge-rectifier-rohs-compliant/dp/9109625"/>
+    <hyperlink ref="F31" r:id="rId24" display="http://nz.element14.com/koa/rk73b2attd102j/resistor-0805-1k-ohm-5/dp/1809300"/>
+    <hyperlink ref="F44" r:id="rId25" display="http://nz.element14.com/multicomp/u0805r103kct/capacitor-0805-10nf-50v/dp/9406352"/>
+    <hyperlink ref="F57" r:id="rId26" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
+    <hyperlink ref="F11" r:id="rId27" display="http://nz.element14.com/vishay-draloric/crcw080510k0fkta/thick-film-chip-resistor/dp/1652909"/>
+    <hyperlink ref="F12" r:id="rId28" display="http://nz.element14.com/vishay-draloric/crcw080510k0fkta/thick-film-chip-resistor/dp/1652909"/>
+    <hyperlink ref="F13" r:id="rId29" display="http://nz.element14.com/vishay-draloric/crcw080510k0fkta/thick-film-chip-resistor/dp/1652909"/>
+    <hyperlink ref="F14" r:id="rId30" display="http://nz.element14.com/vishay-draloric/crcw080510k0fkta/thick-film-chip-resistor/dp/1652909"/>
+    <hyperlink ref="F15" r:id="rId31" display="http://nz.element14.com/vishay-draloric/crcw080510k0fkta/thick-film-chip-resistor/dp/1652909"/>
+    <hyperlink ref="F69" r:id="rId32" display="http://nz.element14.com/vishay-sprague/199d106x9035d1v1e3/capacitor-tant-10uf-35v-radial/dp/1617365"/>
+    <hyperlink ref="F23" r:id="rId33" display="http://nz.element14.com/kemet/c0805c220j1gactu/capacitor-0805-22pf-100v-np0/dp/1414676"/>
+    <hyperlink ref="F21" r:id="rId34" display="http://nz.element14.com/kemet/c0805c150j5gactu/capacitor-0805-15pf-50v-np0/dp/1414668"/>
+    <hyperlink ref="F24" r:id="rId35" display="http://nz.element14.com/kemet/c0805c150j5gactu/capacitor-0805-15pf-50v-np0/dp/1414668"/>
+    <hyperlink ref="F22" r:id="rId36" display="http://nz.element14.com/kemet/c0805c330j5gactu/capacitor-0805-33pf-50v-np0/dp/1414685"/>
+    <hyperlink ref="F25" r:id="rId37" display="http://nz.element14.com/kemet/c0805c330j5gactu/capacitor-0805-33pf-50v-np0/dp/1414685"/>
+    <hyperlink ref="F16" r:id="rId38" display="http://nz.element14.com/avx/08053c224jat2a/capacitor-mlcc-0805-25v-220nf/dp/1740667"/>
+    <hyperlink ref="F29" r:id="rId39" display="http://nz.element14.com/avx/08053c224jat2a/capacitor-mlcc-0805-25v-220nf/dp/1740667"/>
+    <hyperlink ref="F30" r:id="rId40" display="http://nz.element14.com/avx/08053c224jat2a/capacitor-mlcc-0805-25v-220nf/dp/1740667"/>
+    <hyperlink ref="F32" r:id="rId41" display="http://nz.element14.com/avx/08053c224jat2a/capacitor-mlcc-0805-25v-220nf/dp/1740667"/>
+    <hyperlink ref="F33" r:id="rId42" display="http://nz.element14.com/avx/08053c224jat2a/capacitor-mlcc-0805-25v-220nf/dp/1740667"/>
+    <hyperlink ref="F34" r:id="rId43" display="http://nz.element14.com/avx/08053c224jat2a/capacitor-mlcc-0805-25v-220nf/dp/1740667"/>
+    <hyperlink ref="F17" r:id="rId44" display="http://nz.element14.com/kemet"/>
+    <hyperlink ref="F18" r:id="rId45" display="http://nz.element14.com/murata/grm2195c1h682ja01d/capacitor-0805-6-8nf-50v/dp/8820066"/>
+    <hyperlink ref="F19" r:id="rId46" display="http://nz.element14.com/multicomp/mcpwr05ftew3301/resistor-0805-3-3k-1-0-125w/dp/1887293"/>
+    <hyperlink ref="F26" r:id="rId47" display="http://nz.element14.com/yageo-phycomp/rc0805fr-0710ml/resistor-rc12h-0805-10m/dp/9238115"/>
+    <hyperlink ref="F27" r:id="rId48" display="http://nz.element14.com/multicomp/mc-0-1w-0805-1-1m/resistor-1mohm-0-1w-1/dp/9332413"/>
+    <hyperlink ref="F41" r:id="rId49" display="http://nz.element14.com/taiyo-yuden/emk212b7475kg-t/capacitor-ceramic-4-7uf-16v-x7r/dp/1853520"/>
     <hyperlink ref="H5" r:id="rId50"/>
-    <hyperlink ref="F34" r:id="rId51" display="http://nz.element14.com/welwyn/mfr3-10kfc/resistor-metal-film-10kohm-400mw/dp/1833277"/>
-    <hyperlink ref="F49" r:id="rId52" display="http://nz.element14.com/on-semiconductor/bc557bzl1g/transistor-pnp-45v-0-1a-to-92/dp/9558527"/>
+    <hyperlink ref="F36" r:id="rId51" display="http://nz.element14.com/welwyn/mfr3-10kfc/resistor-metal-film-10kohm-400mw/dp/1833277"/>
+    <hyperlink ref="F51" r:id="rId52" display="http://nz.element14.com/on-semiconductor/bc557bzl1g/transistor-pnp-45v-0-1a-to-92/dp/9558527"/>
     <hyperlink ref="H3" r:id="rId53"/>
+    <hyperlink ref="G7" r:id="rId54"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" orientation="landscape" r:id="rId54"/>
-  <drawing r:id="rId55"/>
+  <pageSetup paperSize="8" orientation="landscape" r:id="rId55"/>
+  <drawing r:id="rId56"/>
 </worksheet>
 </file>
 
@@ -3560,21 +3613,21 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="86" t="s">
         <v>144</v>
       </c>
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="58"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="86" t="s">
+      <c r="I2" s="87" t="s">
         <v>373</v>
       </c>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
+      <c r="J2" s="87"/>
+      <c r="K2" s="87"/>
       <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -3686,30 +3739,31 @@
   <cols>
     <col min="1" max="5" width="9.140625" customWidth="1"/>
     <col min="6" max="6" width="10.42578125" style="57" customWidth="1"/>
-    <col min="7" max="12" width="9.140625" customWidth="1"/>
+    <col min="7" max="11" width="9.140625" customWidth="1"/>
+    <col min="12" max="12" width="11" customWidth="1"/>
     <col min="13" max="13" width="28.5703125" customWidth="1"/>
-    <col min="14" max="14" width="27.28515625" customWidth="1"/>
+    <col min="14" max="14" width="29.28515625" customWidth="1"/>
     <col min="15" max="15" width="9.140625" hidden="1" customWidth="1"/>
     <col min="16" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="86" t="s">
         <v>145</v>
       </c>
-      <c r="B2" s="85"/>
+      <c r="B2" s="86"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="58"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="86" t="s">
+      <c r="I2" s="87" t="s">
         <v>335</v>
       </c>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
+      <c r="J2" s="87"/>
+      <c r="K2" s="87"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
@@ -3785,9 +3839,10 @@
       <c r="G7" t="s">
         <v>352</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="K7" s="84" t="s">
         <v>349</v>
       </c>
+      <c r="L7" s="84"/>
       <c r="M7" t="s">
         <v>350</v>
       </c>
@@ -3802,21 +3857,21 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="85" t="s">
+      <c r="A10" s="86" t="s">
         <v>154</v>
       </c>
-      <c r="B10" s="85"/>
+      <c r="B10" s="86"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="58"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
-      <c r="I10" s="86" t="s">
+      <c r="I10" s="87" t="s">
         <v>336</v>
       </c>
-      <c r="J10" s="86"/>
-      <c r="K10" s="86"/>
+      <c r="J10" s="87"/>
+      <c r="K10" s="87"/>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
@@ -3892,9 +3947,10 @@
       <c r="G15" t="s">
         <v>352</v>
       </c>
-      <c r="K15" s="5" t="s">
+      <c r="K15" s="84" t="s">
         <v>349</v>
       </c>
+      <c r="L15" s="84"/>
       <c r="M15" t="s">
         <v>350</v>
       </c>
@@ -3912,21 +3968,21 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25"/>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="85" t="s">
+      <c r="A18" s="86" t="s">
         <v>155</v>
       </c>
-      <c r="B18" s="85"/>
+      <c r="B18" s="86"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="58"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
-      <c r="I18" s="86" t="s">
+      <c r="I18" s="87" t="s">
         <v>337</v>
       </c>
-      <c r="J18" s="86"/>
-      <c r="K18" s="86"/>
+      <c r="J18" s="87"/>
+      <c r="K18" s="87"/>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
@@ -4002,9 +4058,10 @@
       <c r="G23" t="s">
         <v>352</v>
       </c>
-      <c r="K23" s="5" t="s">
+      <c r="K23" s="84" t="s">
         <v>349</v>
       </c>
+      <c r="L23" s="84"/>
       <c r="M23" t="s">
         <v>350</v>
       </c>
@@ -4022,21 +4079,21 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="85" t="s">
+      <c r="A26" s="86" t="s">
         <v>156</v>
       </c>
-      <c r="B26" s="85"/>
+      <c r="B26" s="86"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="58"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
-      <c r="I26" s="86" t="s">
+      <c r="I26" s="87" t="s">
         <v>338</v>
       </c>
-      <c r="J26" s="86"/>
-      <c r="K26" s="86"/>
+      <c r="J26" s="87"/>
+      <c r="K26" s="87"/>
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
       <c r="N26" s="4"/>
@@ -4112,9 +4169,10 @@
       <c r="G31" t="s">
         <v>352</v>
       </c>
-      <c r="K31" s="5" t="s">
+      <c r="K31" s="84" t="s">
         <v>349</v>
       </c>
+      <c r="L31" s="84"/>
       <c r="M31" t="s">
         <v>350</v>
       </c>
@@ -4132,21 +4190,21 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25"/>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="85" t="s">
+      <c r="A34" s="86" t="s">
         <v>157</v>
       </c>
-      <c r="B34" s="85"/>
+      <c r="B34" s="86"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="58"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
-      <c r="I34" s="86" t="s">
+      <c r="I34" s="87" t="s">
         <v>339</v>
       </c>
-      <c r="J34" s="86"/>
-      <c r="K34" s="86"/>
+      <c r="J34" s="87"/>
+      <c r="K34" s="87"/>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
@@ -4222,9 +4280,10 @@
       <c r="G39" t="s">
         <v>352</v>
       </c>
-      <c r="K39" s="5" t="s">
+      <c r="K39" s="84" t="s">
         <v>349</v>
       </c>
+      <c r="L39" s="84"/>
       <c r="M39" t="s">
         <v>350</v>
       </c>
@@ -4242,21 +4301,21 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25"/>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" s="85" t="s">
+      <c r="A42" s="86" t="s">
         <v>158</v>
       </c>
-      <c r="B42" s="85"/>
+      <c r="B42" s="86"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
       <c r="F42" s="58"/>
       <c r="G42" s="4"/>
       <c r="H42" s="4"/>
-      <c r="I42" s="86" t="s">
+      <c r="I42" s="87" t="s">
         <v>340</v>
       </c>
-      <c r="J42" s="86"/>
-      <c r="K42" s="86"/>
+      <c r="J42" s="87"/>
+      <c r="K42" s="87"/>
       <c r="L42" s="4"/>
       <c r="M42" s="4"/>
       <c r="N42" s="4"/>
@@ -4332,9 +4391,10 @@
       <c r="G47" t="s">
         <v>352</v>
       </c>
-      <c r="K47" s="5" t="s">
+      <c r="K47" s="84" t="s">
         <v>349</v>
       </c>
+      <c r="L47" s="84"/>
       <c r="M47" t="s">
         <v>350</v>
       </c>
@@ -4352,21 +4412,21 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25"/>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A50" s="85" t="s">
+      <c r="A50" s="86" t="s">
         <v>159</v>
       </c>
-      <c r="B50" s="85"/>
+      <c r="B50" s="86"/>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
       <c r="F50" s="58"/>
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
-      <c r="I50" s="86" t="s">
+      <c r="I50" s="87" t="s">
         <v>341</v>
       </c>
-      <c r="J50" s="86"/>
-      <c r="K50" s="86"/>
+      <c r="J50" s="87"/>
+      <c r="K50" s="87"/>
       <c r="L50" s="4"/>
       <c r="M50" s="4"/>
       <c r="N50" s="4"/>
@@ -4442,9 +4502,10 @@
       <c r="G55" t="s">
         <v>352</v>
       </c>
-      <c r="K55" s="5" t="s">
+      <c r="K55" s="84" t="s">
         <v>349</v>
       </c>
+      <c r="L55" s="84"/>
       <c r="M55" t="s">
         <v>350</v>
       </c>
@@ -4471,21 +4532,21 @@
       <c r="N57" s="2"/>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A58" s="85" t="s">
+      <c r="A58" s="86" t="s">
         <v>160</v>
       </c>
-      <c r="B58" s="85"/>
+      <c r="B58" s="86"/>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
       <c r="E58" s="4"/>
       <c r="F58" s="58"/>
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
-      <c r="I58" s="86" t="s">
+      <c r="I58" s="87" t="s">
         <v>342</v>
       </c>
-      <c r="J58" s="86"/>
-      <c r="K58" s="86"/>
+      <c r="J58" s="87"/>
+      <c r="K58" s="87"/>
       <c r="L58" s="4"/>
       <c r="M58" s="4"/>
       <c r="N58" s="4"/>
@@ -4561,9 +4622,10 @@
       <c r="G63" t="s">
         <v>352</v>
       </c>
-      <c r="K63" s="5" t="s">
+      <c r="K63" s="84" t="s">
         <v>349</v>
       </c>
+      <c r="L63" s="84"/>
       <c r="M63" t="s">
         <v>350</v>
       </c>
@@ -4585,7 +4647,8 @@
     <row r="68" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="69" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="24">
+    <mergeCell ref="K63:L63"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A58:B58"/>
@@ -4602,6 +4665,13 @@
     <mergeCell ref="I26:K26"/>
     <mergeCell ref="I34:K34"/>
     <mergeCell ref="I42:K42"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="K39:L39"/>
+    <mergeCell ref="K47:L47"/>
+    <mergeCell ref="K55:L55"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F4" r:id="rId1" display="http://nz.element14.com/koa/rk73b2attd471j/resistor-0805-470-ohm-5/dp/1809376"/>
@@ -4665,8 +4735,9 @@
     <col min="6" max="6" width="10.28515625" style="57" customWidth="1"/>
     <col min="7" max="10" width="9.140625" customWidth="1"/>
     <col min="11" max="11" width="11.85546875" customWidth="1"/>
-    <col min="12" max="13" width="9.140625" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" customWidth="1"/>
+    <col min="12" max="12" width="8" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" customWidth="1"/>
+    <col min="14" max="14" width="26.7109375" customWidth="1"/>
     <col min="15" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
@@ -4682,11 +4753,11 @@
       <c r="F2" s="58"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="86" t="s">
+      <c r="I2" s="87" t="s">
         <v>343</v>
       </c>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
+      <c r="J2" s="87"/>
+      <c r="K2" s="87"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
@@ -4809,11 +4880,11 @@
       <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="96" t="s">
+      <c r="A12" s="97" t="s">
         <v>394</v>
       </c>
-      <c r="B12" s="96"/>
-      <c r="C12" s="96"/>
+      <c r="B12" s="97"/>
+      <c r="C12" s="97"/>
       <c r="D12" s="16"/>
       <c r="E12" s="25" t="s">
         <v>360</v>
@@ -4826,11 +4897,11 @@
       </c>
     </row>
     <row r="13" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="96" t="s">
+      <c r="A13" s="97" t="s">
         <v>396</v>
       </c>
-      <c r="B13" s="96"/>
-      <c r="C13" s="96"/>
+      <c r="B13" s="97"/>
+      <c r="C13" s="97"/>
       <c r="D13" s="16"/>
       <c r="E13" s="25" t="s">
         <v>416</v>
@@ -4838,13 +4909,13 @@
       <c r="F13" s="59">
         <v>5402608</v>
       </c>
-      <c r="G13" s="73" t="s">
+      <c r="G13" s="74" t="s">
         <v>397</v>
       </c>
-      <c r="H13" s="73"/>
-      <c r="I13" s="73"/>
-      <c r="J13" s="73"/>
-      <c r="K13" s="73"/>
+      <c r="H13" s="74"/>
+      <c r="I13" s="74"/>
+      <c r="J13" s="74"/>
+      <c r="K13" s="74"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -4858,11 +4929,11 @@
       <c r="F15" s="58"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
-      <c r="I15" s="86" t="s">
+      <c r="I15" s="87" t="s">
         <v>344</v>
       </c>
-      <c r="J15" s="86"/>
-      <c r="K15" s="86"/>
+      <c r="J15" s="87"/>
+      <c r="K15" s="87"/>
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
@@ -4880,12 +4951,12 @@
       <c r="G16" t="s">
         <v>209</v>
       </c>
-      <c r="I16" s="82" t="s">
+      <c r="I16" s="83" t="s">
         <v>220</v>
       </c>
-      <c r="J16" s="82"/>
-      <c r="K16" s="82"/>
-      <c r="L16" s="82"/>
+      <c r="J16" s="83"/>
+      <c r="K16" s="83"/>
+      <c r="L16" s="83"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
@@ -4924,12 +4995,14 @@
       <c r="G19" t="s">
         <v>352</v>
       </c>
-      <c r="K19" s="5" t="s">
-        <v>351</v>
-      </c>
-      <c r="L19" t="s">
-        <v>352</v>
-      </c>
+      <c r="K19" s="84" t="s">
+        <v>349</v>
+      </c>
+      <c r="L19" s="84"/>
+      <c r="M19" s="74" t="s">
+        <v>350</v>
+      </c>
+      <c r="N19" s="74"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
@@ -5023,11 +5096,11 @@
       <c r="F28" s="58"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
-      <c r="I28" s="86" t="s">
+      <c r="I28" s="87" t="s">
         <v>345</v>
       </c>
-      <c r="J28" s="86"/>
-      <c r="K28" s="86"/>
+      <c r="J28" s="87"/>
+      <c r="K28" s="87"/>
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
@@ -5045,12 +5118,12 @@
       <c r="G29" t="s">
         <v>209</v>
       </c>
-      <c r="I29" s="82" t="s">
+      <c r="I29" s="83" t="s">
         <v>220</v>
       </c>
-      <c r="J29" s="82"/>
-      <c r="K29" s="82"/>
-      <c r="L29" s="82"/>
+      <c r="J29" s="83"/>
+      <c r="K29" s="83"/>
+      <c r="L29" s="83"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
@@ -5089,12 +5162,14 @@
       <c r="G32" t="s">
         <v>352</v>
       </c>
-      <c r="K32" s="5" t="s">
-        <v>351</v>
-      </c>
-      <c r="L32" t="s">
-        <v>352</v>
-      </c>
+      <c r="K32" s="84" t="s">
+        <v>349</v>
+      </c>
+      <c r="L32" s="84"/>
+      <c r="M32" s="74" t="s">
+        <v>350</v>
+      </c>
+      <c r="N32" s="74"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
@@ -5190,11 +5265,11 @@
       <c r="F41" s="58"/>
       <c r="G41" s="4"/>
       <c r="H41" s="4"/>
-      <c r="I41" s="86" t="s">
+      <c r="I41" s="87" t="s">
         <v>346</v>
       </c>
-      <c r="J41" s="86"/>
-      <c r="K41" s="86"/>
+      <c r="J41" s="87"/>
+      <c r="K41" s="87"/>
       <c r="L41" s="4"/>
       <c r="M41" s="4"/>
       <c r="N41" s="4"/>
@@ -5212,12 +5287,12 @@
       <c r="G42" t="s">
         <v>209</v>
       </c>
-      <c r="I42" s="82" t="s">
+      <c r="I42" s="83" t="s">
         <v>220</v>
       </c>
-      <c r="J42" s="82"/>
-      <c r="K42" s="82"/>
-      <c r="L42" s="82"/>
+      <c r="J42" s="83"/>
+      <c r="K42" s="83"/>
+      <c r="L42" s="83"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
@@ -5257,12 +5332,14 @@
       <c r="G45" t="s">
         <v>352</v>
       </c>
-      <c r="K45" s="5" t="s">
-        <v>351</v>
-      </c>
-      <c r="L45" t="s">
-        <v>352</v>
-      </c>
+      <c r="K45" s="84" t="s">
+        <v>349</v>
+      </c>
+      <c r="L45" s="84"/>
+      <c r="M45" s="74" t="s">
+        <v>350</v>
+      </c>
+      <c r="N45" s="74"/>
       <c r="P45" s="5"/>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
@@ -5360,11 +5437,11 @@
       <c r="F54" s="58"/>
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
-      <c r="I54" s="86" t="s">
+      <c r="I54" s="87" t="s">
         <v>347</v>
       </c>
-      <c r="J54" s="86"/>
-      <c r="K54" s="86"/>
+      <c r="J54" s="87"/>
+      <c r="K54" s="87"/>
       <c r="L54" s="4"/>
       <c r="M54" s="4"/>
       <c r="N54" s="4"/>
@@ -5382,12 +5459,12 @@
       <c r="G55" t="s">
         <v>209</v>
       </c>
-      <c r="I55" s="82" t="s">
+      <c r="I55" s="83" t="s">
         <v>220</v>
       </c>
-      <c r="J55" s="82"/>
-      <c r="K55" s="82"/>
-      <c r="L55" s="82"/>
+      <c r="J55" s="83"/>
+      <c r="K55" s="83"/>
+      <c r="L55" s="83"/>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
@@ -5424,13 +5501,14 @@
       <c r="G58" t="s">
         <v>352</v>
       </c>
-      <c r="K58" s="5" t="s">
-        <v>351</v>
-      </c>
-      <c r="L58" t="s">
-        <v>352</v>
-      </c>
-      <c r="M58" s="5"/>
+      <c r="K58" s="84" t="s">
+        <v>349</v>
+      </c>
+      <c r="L58" s="84"/>
+      <c r="M58" s="74" t="s">
+        <v>350</v>
+      </c>
+      <c r="N58" s="74"/>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
@@ -5524,11 +5602,19 @@
     <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="20">
+    <mergeCell ref="K58:L58"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="M32:N32"/>
+    <mergeCell ref="M45:N45"/>
+    <mergeCell ref="M58:N58"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="G13:K13"/>
     <mergeCell ref="I54:K54"/>
     <mergeCell ref="A13:C13"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="K45:L45"/>
     <mergeCell ref="I15:K15"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="I28:K28"/>
@@ -5570,17 +5656,17 @@
     <hyperlink ref="F49" r:id="rId29" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
     <hyperlink ref="F62" r:id="rId30" display="http://nz.element14.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v/dp/9556915"/>
     <hyperlink ref="F45" r:id="rId31" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
-    <hyperlink ref="K45" r:id="rId32" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
-    <hyperlink ref="F32" r:id="rId33" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
-    <hyperlink ref="K32" r:id="rId34" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
-    <hyperlink ref="F19" r:id="rId35" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
-    <hyperlink ref="K19" r:id="rId36" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
-    <hyperlink ref="F58" r:id="rId37" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
-    <hyperlink ref="K58" r:id="rId38" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
-    <hyperlink ref="F7" r:id="rId39" display="http://nz.element14.com/vishay-draloric/crcw080510k0fkta/thick-film-chip-resistor/dp/1652909"/>
-    <hyperlink ref="F8" r:id="rId40" display="http://nz.element14.com/vishay-draloric/crcw080510k0fkta/thick-film-chip-resistor/dp/1652909"/>
-    <hyperlink ref="F12" r:id="rId41" display="http://nz.element14.com/multicomp/mf12-100k/resistor-0-125w-1-100k/dp/9342427"/>
-    <hyperlink ref="F13" r:id="rId42" display="http://nz.element14.com/vishay-bc-components/pr02000202000jr500/resistor-metal-film-200-ohm-2-w/dp/5402608"/>
+    <hyperlink ref="F32" r:id="rId32" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
+    <hyperlink ref="F19" r:id="rId33" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
+    <hyperlink ref="F58" r:id="rId34" tooltip="Click to repeat search" display="http://newzealand.rs-online.com/web/c/?searchTerm=686-8518P"/>
+    <hyperlink ref="F7" r:id="rId35" display="http://nz.element14.com/vishay-draloric/crcw080510k0fkta/thick-film-chip-resistor/dp/1652909"/>
+    <hyperlink ref="F8" r:id="rId36" display="http://nz.element14.com/vishay-draloric/crcw080510k0fkta/thick-film-chip-resistor/dp/1652909"/>
+    <hyperlink ref="F12" r:id="rId37" display="http://nz.element14.com/multicomp/mf12-100k/resistor-0-125w-1-100k/dp/9342427"/>
+    <hyperlink ref="F13" r:id="rId38" display="http://nz.element14.com/vishay-bc-components/pr02000202000jr500/resistor-metal-film-200-ohm-2-w/dp/5402608"/>
+    <hyperlink ref="K19" r:id="rId39" tooltip="Click to view additional information on this product." display="http://nz.mouser.com/ProductDetail/STMicroelectronics/VNP14NV04-E/?qs=sGAEpiMZZMuCmTIBzycWfOPiiwtMaP0Fv4CVvoRPcP8%3d"/>
+    <hyperlink ref="K32" r:id="rId40" tooltip="Click to view additional information on this product." display="http://nz.mouser.com/ProductDetail/STMicroelectronics/VNP14NV04-E/?qs=sGAEpiMZZMuCmTIBzycWfOPiiwtMaP0Fv4CVvoRPcP8%3d"/>
+    <hyperlink ref="K45" r:id="rId41" tooltip="Click to view additional information on this product." display="http://nz.mouser.com/ProductDetail/STMicroelectronics/VNP14NV04-E/?qs=sGAEpiMZZMuCmTIBzycWfOPiiwtMaP0Fv4CVvoRPcP8%3d"/>
+    <hyperlink ref="K58" r:id="rId42" tooltip="Click to view additional information on this product." display="http://nz.mouser.com/ProductDetail/STMicroelectronics/VNP14NV04-E/?qs=sGAEpiMZZMuCmTIBzycWfOPiiwtMaP0Fv4CVvoRPcP8%3d"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" orientation="landscape" r:id="rId43"/>
@@ -5598,13 +5684,13 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="97" t="s">
+      <c r="B7" s="98" t="s">
         <v>393</v>
       </c>
-      <c r="C7" s="97"/>
-      <c r="D7" s="97"/>
-      <c r="E7" s="97"/>
-      <c r="F7" s="97"/>
+      <c r="C7" s="98"/>
+      <c r="D7" s="98"/>
+      <c r="E7" s="98"/>
+      <c r="F7" s="98"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5634,20 +5720,20 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="85" t="s">
         <v>395</v>
       </c>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="60"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="86" t="s">
+      <c r="I2" s="87" t="s">
         <v>329</v>
       </c>
-      <c r="J2" s="86"/>
+      <c r="J2" s="87"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
     </row>
@@ -5661,10 +5747,10 @@
       <c r="F3" s="59">
         <v>1887296</v>
       </c>
-      <c r="G3" s="73" t="s">
+      <c r="G3" s="74" t="s">
         <v>216</v>
       </c>
-      <c r="H3" s="73"/>
+      <c r="H3" s="74"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
@@ -5676,27 +5762,27 @@
       <c r="F4" s="59">
         <v>1506077</v>
       </c>
-      <c r="G4" s="73" t="s">
+      <c r="G4" s="74" t="s">
         <v>221</v>
       </c>
-      <c r="H4" s="73"/>
+      <c r="H4" s="74"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="74" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
       <c r="F5" s="59">
         <v>1809596</v>
       </c>
-      <c r="G5" s="73" t="s">
+      <c r="G5" s="74" t="s">
         <v>208</v>
       </c>
-      <c r="H5" s="73"/>
+      <c r="H5" s="74"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
@@ -5708,11 +5794,11 @@
       <c r="F6" s="59">
         <v>1759172</v>
       </c>
-      <c r="G6" s="73" t="s">
+      <c r="G6" s="74" t="s">
         <v>223</v>
       </c>
-      <c r="H6" s="73"/>
-      <c r="I6" s="73"/>
+      <c r="H6" s="74"/>
+      <c r="I6" s="74"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
@@ -5724,13 +5810,13 @@
       <c r="F7" s="59">
         <v>9556915</v>
       </c>
-      <c r="G7" s="73" t="s">
+      <c r="G7" s="74" t="s">
         <v>235</v>
       </c>
-      <c r="H7" s="73"/>
-      <c r="I7" s="73"/>
-      <c r="J7" s="73"/>
-      <c r="K7" s="73"/>
+      <c r="H7" s="74"/>
+      <c r="I7" s="74"/>
+      <c r="J7" s="74"/>
+      <c r="K7" s="74"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
@@ -5742,13 +5828,13 @@
       <c r="F8" s="59">
         <v>9556915</v>
       </c>
-      <c r="G8" s="73" t="s">
+      <c r="G8" s="74" t="s">
         <v>235</v>
       </c>
-      <c r="H8" s="73"/>
-      <c r="I8" s="73"/>
-      <c r="J8" s="73"/>
-      <c r="K8" s="73"/>
+      <c r="H8" s="74"/>
+      <c r="I8" s="74"/>
+      <c r="J8" s="74"/>
+      <c r="K8" s="74"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
@@ -5761,10 +5847,10 @@
       <c r="F9" s="59">
         <v>1809376</v>
       </c>
-      <c r="G9" s="73" t="s">
+      <c r="G9" s="74" t="s">
         <v>209</v>
       </c>
-      <c r="H9" s="73"/>
+      <c r="H9" s="74"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
@@ -5816,30 +5902,30 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="85" t="s">
         <v>358</v>
       </c>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
       <c r="E2" s="3"/>
       <c r="F2" s="60"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="86" t="s">
+      <c r="I2" s="87" t="s">
         <v>354</v>
       </c>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
+      <c r="J2" s="87"/>
+      <c r="K2" s="87"/>
       <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="89" t="s">
+      <c r="A3" s="90" t="s">
         <v>406</v>
       </c>
-      <c r="B3" s="89"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
+      <c r="B3" s="90"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
       <c r="E3" s="3"/>
       <c r="F3" s="60"/>
       <c r="G3" s="4"/>
@@ -5859,11 +5945,11 @@
       <c r="F4" s="59">
         <v>8820120</v>
       </c>
-      <c r="G4" s="73" t="s">
+      <c r="G4" s="74" t="s">
         <v>218</v>
       </c>
-      <c r="H4" s="73"/>
-      <c r="I4" s="73"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
@@ -5875,11 +5961,11 @@
       <c r="F5" s="59">
         <v>1759199</v>
       </c>
-      <c r="G5" s="73" t="s">
+      <c r="G5" s="74" t="s">
         <v>222</v>
       </c>
-      <c r="H5" s="73"/>
-      <c r="I5" s="73"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
@@ -5891,11 +5977,11 @@
       <c r="F6" s="59">
         <v>1759172</v>
       </c>
-      <c r="G6" s="73" t="s">
+      <c r="G6" s="74" t="s">
         <v>223</v>
       </c>
-      <c r="H6" s="73"/>
-      <c r="I6" s="73"/>
+      <c r="H6" s="74"/>
+      <c r="I6" s="74"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
@@ -5907,10 +5993,10 @@
       <c r="F7" s="59">
         <v>1809376</v>
       </c>
-      <c r="G7" s="73" t="s">
+      <c r="G7" s="74" t="s">
         <v>209</v>
       </c>
-      <c r="H7" s="73"/>
+      <c r="H7" s="74"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
@@ -5922,10 +6008,10 @@
       <c r="F8" s="59">
         <v>1809596</v>
       </c>
-      <c r="G8" s="73" t="s">
+      <c r="G8" s="74" t="s">
         <v>208</v>
       </c>
-      <c r="H8" s="73"/>
+      <c r="H8" s="74"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
@@ -5937,20 +6023,20 @@
       <c r="F9" s="59">
         <v>1809596</v>
       </c>
-      <c r="G9" s="73" t="s">
+      <c r="G9" s="74" t="s">
         <v>208</v>
       </c>
-      <c r="H9" s="73"/>
+      <c r="H9" s="74"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>371</v>
       </c>
-      <c r="B10" s="73" t="s">
+      <c r="B10" s="74" t="s">
         <v>95</v>
       </c>
-      <c r="C10" s="73"/>
-      <c r="D10" s="73"/>
+      <c r="C10" s="74"/>
+      <c r="D10" s="74"/>
       <c r="F10" s="59"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -5958,93 +6044,93 @@
       <c r="F11" s="59"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="90" t="s">
+      <c r="A12" s="91" t="s">
         <v>401</v>
       </c>
-      <c r="B12" s="90"/>
-      <c r="C12" s="90"/>
-      <c r="D12" s="90"/>
-      <c r="E12" s="90"/>
-      <c r="F12" s="90"/>
-      <c r="G12" s="90"/>
-      <c r="H12" s="90"/>
-      <c r="I12" s="90"/>
-      <c r="J12" s="90"/>
-      <c r="K12" s="90"/>
-      <c r="L12" s="90"/>
+      <c r="B12" s="91"/>
+      <c r="C12" s="91"/>
+      <c r="D12" s="91"/>
+      <c r="E12" s="91"/>
+      <c r="F12" s="91"/>
+      <c r="G12" s="91"/>
+      <c r="H12" s="91"/>
+      <c r="I12" s="91"/>
+      <c r="J12" s="91"/>
+      <c r="K12" s="91"/>
+      <c r="L12" s="91"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="B13" s="73" t="s">
+      <c r="B13" s="74" t="s">
         <v>82</v>
       </c>
-      <c r="C13" s="73"/>
+      <c r="C13" s="74"/>
       <c r="F13" s="59">
         <v>1457153</v>
       </c>
-      <c r="G13" s="73" t="s">
+      <c r="G13" s="74" t="s">
         <v>183</v>
       </c>
-      <c r="H13" s="73"/>
-      <c r="I13" s="73"/>
+      <c r="H13" s="74"/>
+      <c r="I13" s="74"/>
       <c r="J13" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="K13" s="91" t="s">
+      <c r="K13" s="92" t="s">
         <v>233</v>
       </c>
-      <c r="L13" s="91"/>
+      <c r="L13" s="92"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="B14" s="73" t="s">
+      <c r="B14" s="74" t="s">
         <v>95</v>
       </c>
-      <c r="C14" s="73"/>
-      <c r="D14" s="73"/>
+      <c r="C14" s="74"/>
+      <c r="D14" s="74"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="B15" s="73" t="s">
+      <c r="B15" s="74" t="s">
         <v>95</v>
       </c>
-      <c r="C15" s="73"/>
-      <c r="D15" s="73"/>
+      <c r="C15" s="74"/>
+      <c r="D15" s="74"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="B16" s="73" t="s">
+      <c r="B16" s="74" t="s">
         <v>95</v>
       </c>
-      <c r="C16" s="73"/>
-      <c r="D16" s="73"/>
+      <c r="C16" s="74"/>
+      <c r="D16" s="74"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
     </row>
     <row r="18" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="92" t="s">
+      <c r="A18" s="93" t="s">
         <v>402</v>
       </c>
-      <c r="B18" s="92"/>
-      <c r="C18" s="92"/>
-      <c r="D18" s="92"/>
-      <c r="E18" s="92"/>
-      <c r="F18" s="92"/>
-      <c r="G18" s="92"/>
-      <c r="H18" s="92"/>
-      <c r="I18" s="92"/>
-      <c r="J18" s="92"/>
-      <c r="K18" s="92"/>
-      <c r="L18" s="92"/>
+      <c r="B18" s="93"/>
+      <c r="C18" s="93"/>
+      <c r="D18" s="93"/>
+      <c r="E18" s="93"/>
+      <c r="F18" s="93"/>
+      <c r="G18" s="93"/>
+      <c r="H18" s="93"/>
+      <c r="I18" s="93"/>
+      <c r="J18" s="93"/>
+      <c r="K18" s="93"/>
+      <c r="L18" s="93"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
@@ -6059,13 +6145,13 @@
       <c r="F19" s="61">
         <v>9556915</v>
       </c>
-      <c r="G19" s="93" t="s">
+      <c r="G19" s="94" t="s">
         <v>235</v>
       </c>
-      <c r="H19" s="93"/>
-      <c r="I19" s="93"/>
-      <c r="J19" s="93"/>
-      <c r="K19" s="93"/>
+      <c r="H19" s="94"/>
+      <c r="I19" s="94"/>
+      <c r="J19" s="94"/>
+      <c r="K19" s="94"/>
       <c r="L19" s="22"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -6081,13 +6167,13 @@
       <c r="F20" s="61">
         <v>9556915</v>
       </c>
-      <c r="G20" s="93" t="s">
+      <c r="G20" s="94" t="s">
         <v>235</v>
       </c>
-      <c r="H20" s="93"/>
-      <c r="I20" s="93"/>
-      <c r="J20" s="93"/>
-      <c r="K20" s="93"/>
+      <c r="H20" s="94"/>
+      <c r="I20" s="94"/>
+      <c r="J20" s="94"/>
+      <c r="K20" s="94"/>
       <c r="L20" s="22"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -6103,11 +6189,11 @@
       <c r="F21" s="61">
         <v>8820120</v>
       </c>
-      <c r="G21" s="93" t="s">
+      <c r="G21" s="94" t="s">
         <v>218</v>
       </c>
-      <c r="H21" s="93"/>
-      <c r="I21" s="93"/>
+      <c r="H21" s="94"/>
+      <c r="I21" s="94"/>
       <c r="J21" s="22"/>
       <c r="K21" s="22"/>
       <c r="L21" s="22"/>
@@ -6190,29 +6276,29 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="85" t="s">
         <v>348</v>
       </c>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
       <c r="E2" s="3"/>
       <c r="F2" s="60"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="86" t="s">
+      <c r="I2" s="87" t="s">
         <v>355</v>
       </c>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
+      <c r="J2" s="87"/>
+      <c r="K2" s="87"/>
       <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="94" t="s">
+      <c r="A3" s="95" t="s">
         <v>405</v>
       </c>
-      <c r="B3" s="94"/>
-      <c r="C3" s="94"/>
+      <c r="B3" s="95"/>
+      <c r="C3" s="95"/>
       <c r="F3" s="58"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -6225,21 +6311,21 @@
       <c r="F4" s="59">
         <v>8820120</v>
       </c>
-      <c r="G4" s="73" t="s">
+      <c r="G4" s="74" t="s">
         <v>218</v>
       </c>
-      <c r="H4" s="73"/>
-      <c r="I4" s="73"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="74" t="s">
         <v>95</v>
       </c>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
       <c r="F5" s="59"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -6252,11 +6338,11 @@
       <c r="F6" s="59">
         <v>1759199</v>
       </c>
-      <c r="G6" s="73" t="s">
+      <c r="G6" s="74" t="s">
         <v>222</v>
       </c>
-      <c r="H6" s="73"/>
-      <c r="I6" s="73"/>
+      <c r="H6" s="74"/>
+      <c r="I6" s="74"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
@@ -6268,11 +6354,11 @@
       <c r="F7" s="59">
         <v>1759172</v>
       </c>
-      <c r="G7" s="73" t="s">
+      <c r="G7" s="74" t="s">
         <v>223</v>
       </c>
-      <c r="H7" s="73"/>
-      <c r="I7" s="73"/>
+      <c r="H7" s="74"/>
+      <c r="I7" s="74"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
@@ -6284,10 +6370,10 @@
       <c r="F8" s="59">
         <v>1809376</v>
       </c>
-      <c r="G8" s="73" t="s">
+      <c r="G8" s="74" t="s">
         <v>209</v>
       </c>
-      <c r="H8" s="73"/>
+      <c r="H8" s="74"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
@@ -6299,92 +6385,92 @@
       <c r="F9" s="59">
         <v>1809596</v>
       </c>
-      <c r="G9" s="73" t="s">
+      <c r="G9" s="74" t="s">
         <v>208</v>
       </c>
-      <c r="H9" s="73"/>
+      <c r="H9" s="74"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
       <c r="F10" s="59"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="90" t="s">
+      <c r="A11" s="91" t="s">
         <v>403</v>
       </c>
-      <c r="B11" s="90"/>
-      <c r="C11" s="90"/>
-      <c r="D11" s="90"/>
-      <c r="E11" s="90"/>
-      <c r="F11" s="90"/>
-      <c r="G11" s="90"/>
-      <c r="H11" s="90"/>
-      <c r="I11" s="90"/>
-      <c r="J11" s="90"/>
-      <c r="K11" s="90"/>
-      <c r="L11" s="90"/>
+      <c r="B11" s="91"/>
+      <c r="C11" s="91"/>
+      <c r="D11" s="91"/>
+      <c r="E11" s="91"/>
+      <c r="F11" s="91"/>
+      <c r="G11" s="91"/>
+      <c r="H11" s="91"/>
+      <c r="I11" s="91"/>
+      <c r="J11" s="91"/>
+      <c r="K11" s="91"/>
+      <c r="L11" s="91"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="B12" s="73" t="s">
+      <c r="B12" s="74" t="s">
         <v>96</v>
       </c>
-      <c r="C12" s="73"/>
+      <c r="C12" s="74"/>
       <c r="F12" s="67">
         <v>1703477</v>
       </c>
-      <c r="G12" s="73" t="s">
+      <c r="G12" s="74" t="s">
         <v>407</v>
       </c>
-      <c r="H12" s="73"/>
-      <c r="I12" s="73"/>
+      <c r="H12" s="74"/>
+      <c r="I12" s="74"/>
       <c r="J12" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="K12" s="91" t="s">
+      <c r="K12" s="92" t="s">
         <v>408</v>
       </c>
-      <c r="L12" s="91"/>
+      <c r="L12" s="92"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="B13" s="73" t="s">
+      <c r="B13" s="74" t="s">
         <v>95</v>
       </c>
-      <c r="C13" s="73"/>
-      <c r="D13" s="73"/>
+      <c r="C13" s="74"/>
+      <c r="D13" s="74"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="B14" s="73" t="s">
+      <c r="B14" s="74" t="s">
         <v>95</v>
       </c>
-      <c r="C14" s="73"/>
-      <c r="D14" s="73"/>
+      <c r="C14" s="74"/>
+      <c r="D14" s="74"/>
       <c r="F14" s="59"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="B15" s="78" t="s">
+      <c r="B15" s="79" t="s">
         <v>95</v>
       </c>
-      <c r="C15" s="78"/>
-      <c r="D15" s="78"/>
+      <c r="C15" s="79"/>
+      <c r="D15" s="79"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
       <c r="F16" s="59"/>
     </row>
-    <row r="17" spans="1:12" s="92" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="92" t="s">
+    <row r="17" spans="1:12" s="93" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="93" t="s">
         <v>404</v>
       </c>
     </row>
@@ -6401,12 +6487,12 @@
       <c r="F18" s="61">
         <v>9556915</v>
       </c>
-      <c r="G18" s="93" t="s">
+      <c r="G18" s="94" t="s">
         <v>235</v>
       </c>
-      <c r="H18" s="93"/>
-      <c r="I18" s="93"/>
-      <c r="J18" s="93"/>
+      <c r="H18" s="94"/>
+      <c r="I18" s="94"/>
+      <c r="J18" s="94"/>
       <c r="K18" s="22"/>
       <c r="L18" s="22"/>
     </row>
@@ -6423,12 +6509,12 @@
       <c r="F19" s="61">
         <v>9556915</v>
       </c>
-      <c r="G19" s="93" t="s">
+      <c r="G19" s="94" t="s">
         <v>235</v>
       </c>
-      <c r="H19" s="93"/>
-      <c r="I19" s="93"/>
-      <c r="J19" s="93"/>
+      <c r="H19" s="94"/>
+      <c r="I19" s="94"/>
+      <c r="J19" s="94"/>
       <c r="K19" s="22"/>
       <c r="L19" s="22"/>
     </row>
@@ -6445,11 +6531,11 @@
       <c r="F20" s="61">
         <v>8820120</v>
       </c>
-      <c r="G20" s="93" t="s">
+      <c r="G20" s="94" t="s">
         <v>218</v>
       </c>
-      <c r="H20" s="93"/>
-      <c r="I20" s="93"/>
+      <c r="H20" s="94"/>
+      <c r="I20" s="94"/>
       <c r="J20" s="62"/>
       <c r="K20" s="22"/>
       <c r="L20" s="22"/>
@@ -6515,9 +6601,7 @@
   </sheetPr>
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19:I19"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6533,21 +6617,21 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="85" t="s">
         <v>118</v>
       </c>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
       <c r="D2" s="3"/>
       <c r="E2" s="4"/>
       <c r="F2" s="58"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="86" t="s">
+      <c r="I2" s="87" t="s">
         <v>417</v>
       </c>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
+      <c r="J2" s="87"/>
+      <c r="K2" s="87"/>
       <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -6561,18 +6645,18 @@
       <c r="F3" s="63">
         <v>1845719</v>
       </c>
-      <c r="G3" s="95" t="s">
+      <c r="G3" s="96" t="s">
         <v>181</v>
       </c>
-      <c r="H3" s="95"/>
-      <c r="I3" s="95"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
       <c r="J3" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="K3" s="91" t="s">
+      <c r="K3" s="92" t="s">
         <v>231</v>
       </c>
-      <c r="L3" s="91"/>
+      <c r="L3" s="92"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
@@ -6584,10 +6668,10 @@
       <c r="F4" s="59">
         <v>1652909</v>
       </c>
-      <c r="G4" s="73" t="s">
+      <c r="G4" s="74" t="s">
         <v>216</v>
       </c>
-      <c r="H4" s="73"/>
+      <c r="H4" s="74"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
@@ -6599,12 +6683,12 @@
       <c r="F5" s="59">
         <v>8820120</v>
       </c>
-      <c r="G5" s="73" t="s">
+      <c r="G5" s="74" t="s">
         <v>218</v>
       </c>
-      <c r="H5" s="73"/>
-      <c r="I5" s="73"/>
-      <c r="J5" s="73"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="74"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
@@ -6616,12 +6700,12 @@
       <c r="F6" s="59">
         <v>1414659</v>
       </c>
-      <c r="G6" s="73" t="s">
+      <c r="G6" s="74" t="s">
         <v>225</v>
       </c>
-      <c r="H6" s="73"/>
-      <c r="I6" s="73"/>
-      <c r="J6" s="73"/>
+      <c r="H6" s="74"/>
+      <c r="I6" s="74"/>
+      <c r="J6" s="74"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
@@ -6636,11 +6720,11 @@
       <c r="F7" s="59">
         <v>1618242</v>
       </c>
-      <c r="G7" s="73" t="s">
+      <c r="G7" s="74" t="s">
         <v>237</v>
       </c>
-      <c r="H7" s="73"/>
-      <c r="I7" s="73"/>
+      <c r="H7" s="74"/>
+      <c r="I7" s="74"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
@@ -6655,11 +6739,11 @@
       <c r="F8" s="59">
         <v>1618242</v>
       </c>
-      <c r="G8" s="73" t="s">
+      <c r="G8" s="74" t="s">
         <v>237</v>
       </c>
-      <c r="H8" s="73"/>
-      <c r="I8" s="73"/>
+      <c r="H8" s="74"/>
+      <c r="I8" s="74"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
@@ -6671,10 +6755,10 @@
       <c r="F9" s="59">
         <v>1809300</v>
       </c>
-      <c r="G9" s="73" t="s">
+      <c r="G9" s="74" t="s">
         <v>209</v>
       </c>
-      <c r="H9" s="73"/>
+      <c r="H9" s="74"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
@@ -6686,38 +6770,38 @@
       <c r="F10" s="65">
         <v>1809596</v>
       </c>
-      <c r="G10" s="73" t="s">
+      <c r="G10" s="74" t="s">
         <v>208</v>
       </c>
-      <c r="H10" s="73"/>
+      <c r="H10" s="74"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>411</v>
       </c>
-      <c r="B11" s="73" t="s">
+      <c r="B11" s="74" t="s">
         <v>412</v>
       </c>
-      <c r="C11" s="73"/>
+      <c r="C11" s="74"/>
       <c r="F11" s="59"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="84" t="s">
+      <c r="A13" s="85" t="s">
         <v>119</v>
       </c>
-      <c r="B13" s="84"/>
-      <c r="C13" s="84"/>
+      <c r="B13" s="85"/>
+      <c r="C13" s="85"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="58"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
-      <c r="I13" s="86" t="s">
+      <c r="I13" s="87" t="s">
         <v>418</v>
       </c>
-      <c r="J13" s="86"/>
-      <c r="K13" s="86"/>
+      <c r="J13" s="87"/>
+      <c r="K13" s="87"/>
       <c r="L13" s="4"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -6731,18 +6815,18 @@
       <c r="F14" s="63">
         <v>1845719</v>
       </c>
-      <c r="G14" s="95" t="s">
+      <c r="G14" s="96" t="s">
         <v>181</v>
       </c>
-      <c r="H14" s="95"/>
-      <c r="I14" s="95"/>
+      <c r="H14" s="96"/>
+      <c r="I14" s="96"/>
       <c r="J14" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="K14" s="91" t="s">
+      <c r="K14" s="92" t="s">
         <v>231</v>
       </c>
-      <c r="L14" s="91"/>
+      <c r="L14" s="92"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
@@ -6754,10 +6838,10 @@
       <c r="F15" s="59">
         <v>1652909</v>
       </c>
-      <c r="G15" s="73" t="s">
+      <c r="G15" s="74" t="s">
         <v>216</v>
       </c>
-      <c r="H15" s="73"/>
+      <c r="H15" s="74"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
@@ -6769,11 +6853,11 @@
       <c r="F16" s="59">
         <v>8820120</v>
       </c>
-      <c r="G16" s="73" t="s">
+      <c r="G16" s="74" t="s">
         <v>218</v>
       </c>
-      <c r="H16" s="73"/>
-      <c r="I16" s="73"/>
+      <c r="H16" s="74"/>
+      <c r="I16" s="74"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
@@ -6785,12 +6869,12 @@
       <c r="F17" s="59">
         <v>1414659</v>
       </c>
-      <c r="G17" s="73" t="s">
+      <c r="G17" s="74" t="s">
         <v>225</v>
       </c>
-      <c r="H17" s="73"/>
-      <c r="I17" s="73"/>
-      <c r="J17" s="73"/>
+      <c r="H17" s="74"/>
+      <c r="I17" s="74"/>
+      <c r="J17" s="74"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
@@ -6805,11 +6889,11 @@
       <c r="F18" s="59">
         <v>1618242</v>
       </c>
-      <c r="G18" s="73" t="s">
+      <c r="G18" s="74" t="s">
         <v>237</v>
       </c>
-      <c r="H18" s="73"/>
-      <c r="I18" s="73"/>
+      <c r="H18" s="74"/>
+      <c r="I18" s="74"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
@@ -6824,11 +6908,11 @@
       <c r="F19" s="59">
         <v>1618242</v>
       </c>
-      <c r="G19" s="73" t="s">
+      <c r="G19" s="74" t="s">
         <v>237</v>
       </c>
-      <c r="H19" s="73"/>
-      <c r="I19" s="73"/>
+      <c r="H19" s="74"/>
+      <c r="I19" s="74"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
@@ -6840,10 +6924,10 @@
       <c r="F20" s="59">
         <v>1809300</v>
       </c>
-      <c r="G20" s="73" t="s">
+      <c r="G20" s="74" t="s">
         <v>209</v>
       </c>
-      <c r="H20" s="73"/>
+      <c r="H20" s="74"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
@@ -6855,19 +6939,19 @@
       <c r="F21" s="65">
         <v>1809596</v>
       </c>
-      <c r="G21" s="73" t="s">
+      <c r="G21" s="74" t="s">
         <v>208</v>
       </c>
-      <c r="H21" s="73"/>
+      <c r="H21" s="74"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>415</v>
       </c>
-      <c r="B22" s="73" t="s">
+      <c r="B22" s="74" t="s">
         <v>412</v>
       </c>
-      <c r="C22" s="73"/>
+      <c r="C22" s="74"/>
       <c r="F22" s="59"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25"/>
@@ -6946,17 +7030,17 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="85" t="s">
         <v>310</v>
       </c>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
@@ -7092,21 +7176,21 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="85" t="s">
         <v>359</v>
       </c>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
       <c r="E2" s="3"/>
       <c r="F2" s="58"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="86" t="s">
+      <c r="I2" s="87" t="s">
         <v>327</v>
       </c>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
+      <c r="J2" s="87"/>
+      <c r="K2" s="87"/>
       <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -7294,21 +7378,21 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="85" t="s">
         <v>131</v>
       </c>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
       <c r="E2" s="3"/>
       <c r="F2" s="60"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="86" t="s">
+      <c r="I2" s="87" t="s">
         <v>334</v>
       </c>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
+      <c r="J2" s="87"/>
+      <c r="K2" s="87"/>
       <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -7497,21 +7581,21 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="86" t="s">
         <v>137</v>
       </c>
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="58"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="86" t="s">
+      <c r="I2" s="87" t="s">
         <v>328</v>
       </c>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
+      <c r="J2" s="87"/>
+      <c r="K2" s="87"/>
       <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>